<commit_message>
Add Sprint 2 changes tab
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -5,29 +5,31 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Desktop\CDISC\DDF\DDF_Phase 2\CT Work Sprint 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3E4F66-B7ED-4A82-ADD6-FA56B254A648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6088B859-F4CC-4BEC-A868-E480CB51A829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="370" windowWidth="17720" windowHeight="9730" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2240" yWindow="1390" windowWidth="16590" windowHeight="8590" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
     <sheet name="DDF Terminology 2022-09-30" sheetId="1" r:id="rId2"/>
-    <sheet name="Terminology Changes Sp1 - new" sheetId="3" r:id="rId3"/>
-    <sheet name="Terminology Changes Sp1 - chg" sheetId="4" r:id="rId4"/>
+    <sheet name="Terminology Changes Sp2 - new" sheetId="6" r:id="rId3"/>
+    <sheet name="Terminology Changes Sp2 - chg" sheetId="5" r:id="rId4"/>
+    <sheet name="Terminology Changes Sp1 - new" sheetId="3" r:id="rId5"/>
+    <sheet name="Terminology Changes Sp1 - chg" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DDF Terminology 2022-09-30'!$A$1:$H$255</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Terminology Changes Sp1 - new'!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Terminology Changes Sp1 - new'!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="1006">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1723" uniqueCount="1010">
   <si>
     <t>Code</t>
   </si>
@@ -3170,12 +3172,24 @@
   <si>
     <t>Business Therapeutic Areas</t>
   </si>
+  <si>
+    <t>Remove attribute 'transitionStartRule' from Encounter Class</t>
+  </si>
+  <si>
+    <t>Remove attribute 'transitionEndRule' from Encounter Class</t>
+  </si>
+  <si>
+    <t>Remove attribute 'transitionStartRule' from StudyElement Class</t>
+  </si>
+  <si>
+    <t>Remove attribute 'transitionEndRule' from StudyElement Class</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3253,6 +3267,13 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF262626"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -3396,7 +3417,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -3512,6 +3533,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -9648,13 +9684,961 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC60F93F-DDE7-4577-BCA7-BDCFD0F8A197}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA8CB9F-21CB-4CA7-BF40-DA6BB340EB8E}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.26953125" style="44" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="44"/>
+    <col min="3" max="3" width="17" style="44" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" style="44" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" style="44" customWidth="1"/>
+    <col min="6" max="6" width="13.90625" style="44" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="44"/>
+    <col min="8" max="8" width="17.90625" style="44" customWidth="1"/>
+    <col min="9" max="9" width="8.7265625" style="44"/>
+    <col min="10" max="10" width="53.6328125" style="44" customWidth="1"/>
+    <col min="11" max="255" width="8.7265625" style="44"/>
+    <col min="256" max="256" width="10.90625" style="44" customWidth="1"/>
+    <col min="257" max="257" width="22.26953125" style="44" customWidth="1"/>
+    <col min="258" max="258" width="8.7265625" style="44"/>
+    <col min="259" max="259" width="17" style="44" customWidth="1"/>
+    <col min="260" max="260" width="13.90625" style="44" customWidth="1"/>
+    <col min="261" max="261" width="20.26953125" style="44" customWidth="1"/>
+    <col min="262" max="262" width="13.90625" style="44" customWidth="1"/>
+    <col min="263" max="263" width="8.7265625" style="44"/>
+    <col min="264" max="264" width="17.90625" style="44" customWidth="1"/>
+    <col min="265" max="265" width="8.7265625" style="44"/>
+    <col min="266" max="266" width="53.6328125" style="44" customWidth="1"/>
+    <col min="267" max="511" width="8.7265625" style="44"/>
+    <col min="512" max="512" width="10.90625" style="44" customWidth="1"/>
+    <col min="513" max="513" width="22.26953125" style="44" customWidth="1"/>
+    <col min="514" max="514" width="8.7265625" style="44"/>
+    <col min="515" max="515" width="17" style="44" customWidth="1"/>
+    <col min="516" max="516" width="13.90625" style="44" customWidth="1"/>
+    <col min="517" max="517" width="20.26953125" style="44" customWidth="1"/>
+    <col min="518" max="518" width="13.90625" style="44" customWidth="1"/>
+    <col min="519" max="519" width="8.7265625" style="44"/>
+    <col min="520" max="520" width="17.90625" style="44" customWidth="1"/>
+    <col min="521" max="521" width="8.7265625" style="44"/>
+    <col min="522" max="522" width="53.6328125" style="44" customWidth="1"/>
+    <col min="523" max="767" width="8.7265625" style="44"/>
+    <col min="768" max="768" width="10.90625" style="44" customWidth="1"/>
+    <col min="769" max="769" width="22.26953125" style="44" customWidth="1"/>
+    <col min="770" max="770" width="8.7265625" style="44"/>
+    <col min="771" max="771" width="17" style="44" customWidth="1"/>
+    <col min="772" max="772" width="13.90625" style="44" customWidth="1"/>
+    <col min="773" max="773" width="20.26953125" style="44" customWidth="1"/>
+    <col min="774" max="774" width="13.90625" style="44" customWidth="1"/>
+    <col min="775" max="775" width="8.7265625" style="44"/>
+    <col min="776" max="776" width="17.90625" style="44" customWidth="1"/>
+    <col min="777" max="777" width="8.7265625" style="44"/>
+    <col min="778" max="778" width="53.6328125" style="44" customWidth="1"/>
+    <col min="779" max="1023" width="8.7265625" style="44"/>
+    <col min="1024" max="1024" width="10.90625" style="44" customWidth="1"/>
+    <col min="1025" max="1025" width="22.26953125" style="44" customWidth="1"/>
+    <col min="1026" max="1026" width="8.7265625" style="44"/>
+    <col min="1027" max="1027" width="17" style="44" customWidth="1"/>
+    <col min="1028" max="1028" width="13.90625" style="44" customWidth="1"/>
+    <col min="1029" max="1029" width="20.26953125" style="44" customWidth="1"/>
+    <col min="1030" max="1030" width="13.90625" style="44" customWidth="1"/>
+    <col min="1031" max="1031" width="8.7265625" style="44"/>
+    <col min="1032" max="1032" width="17.90625" style="44" customWidth="1"/>
+    <col min="1033" max="1033" width="8.7265625" style="44"/>
+    <col min="1034" max="1034" width="53.6328125" style="44" customWidth="1"/>
+    <col min="1035" max="1279" width="8.7265625" style="44"/>
+    <col min="1280" max="1280" width="10.90625" style="44" customWidth="1"/>
+    <col min="1281" max="1281" width="22.26953125" style="44" customWidth="1"/>
+    <col min="1282" max="1282" width="8.7265625" style="44"/>
+    <col min="1283" max="1283" width="17" style="44" customWidth="1"/>
+    <col min="1284" max="1284" width="13.90625" style="44" customWidth="1"/>
+    <col min="1285" max="1285" width="20.26953125" style="44" customWidth="1"/>
+    <col min="1286" max="1286" width="13.90625" style="44" customWidth="1"/>
+    <col min="1287" max="1287" width="8.7265625" style="44"/>
+    <col min="1288" max="1288" width="17.90625" style="44" customWidth="1"/>
+    <col min="1289" max="1289" width="8.7265625" style="44"/>
+    <col min="1290" max="1290" width="53.6328125" style="44" customWidth="1"/>
+    <col min="1291" max="1535" width="8.7265625" style="44"/>
+    <col min="1536" max="1536" width="10.90625" style="44" customWidth="1"/>
+    <col min="1537" max="1537" width="22.26953125" style="44" customWidth="1"/>
+    <col min="1538" max="1538" width="8.7265625" style="44"/>
+    <col min="1539" max="1539" width="17" style="44" customWidth="1"/>
+    <col min="1540" max="1540" width="13.90625" style="44" customWidth="1"/>
+    <col min="1541" max="1541" width="20.26953125" style="44" customWidth="1"/>
+    <col min="1542" max="1542" width="13.90625" style="44" customWidth="1"/>
+    <col min="1543" max="1543" width="8.7265625" style="44"/>
+    <col min="1544" max="1544" width="17.90625" style="44" customWidth="1"/>
+    <col min="1545" max="1545" width="8.7265625" style="44"/>
+    <col min="1546" max="1546" width="53.6328125" style="44" customWidth="1"/>
+    <col min="1547" max="1791" width="8.7265625" style="44"/>
+    <col min="1792" max="1792" width="10.90625" style="44" customWidth="1"/>
+    <col min="1793" max="1793" width="22.26953125" style="44" customWidth="1"/>
+    <col min="1794" max="1794" width="8.7265625" style="44"/>
+    <col min="1795" max="1795" width="17" style="44" customWidth="1"/>
+    <col min="1796" max="1796" width="13.90625" style="44" customWidth="1"/>
+    <col min="1797" max="1797" width="20.26953125" style="44" customWidth="1"/>
+    <col min="1798" max="1798" width="13.90625" style="44" customWidth="1"/>
+    <col min="1799" max="1799" width="8.7265625" style="44"/>
+    <col min="1800" max="1800" width="17.90625" style="44" customWidth="1"/>
+    <col min="1801" max="1801" width="8.7265625" style="44"/>
+    <col min="1802" max="1802" width="53.6328125" style="44" customWidth="1"/>
+    <col min="1803" max="2047" width="8.7265625" style="44"/>
+    <col min="2048" max="2048" width="10.90625" style="44" customWidth="1"/>
+    <col min="2049" max="2049" width="22.26953125" style="44" customWidth="1"/>
+    <col min="2050" max="2050" width="8.7265625" style="44"/>
+    <col min="2051" max="2051" width="17" style="44" customWidth="1"/>
+    <col min="2052" max="2052" width="13.90625" style="44" customWidth="1"/>
+    <col min="2053" max="2053" width="20.26953125" style="44" customWidth="1"/>
+    <col min="2054" max="2054" width="13.90625" style="44" customWidth="1"/>
+    <col min="2055" max="2055" width="8.7265625" style="44"/>
+    <col min="2056" max="2056" width="17.90625" style="44" customWidth="1"/>
+    <col min="2057" max="2057" width="8.7265625" style="44"/>
+    <col min="2058" max="2058" width="53.6328125" style="44" customWidth="1"/>
+    <col min="2059" max="2303" width="8.7265625" style="44"/>
+    <col min="2304" max="2304" width="10.90625" style="44" customWidth="1"/>
+    <col min="2305" max="2305" width="22.26953125" style="44" customWidth="1"/>
+    <col min="2306" max="2306" width="8.7265625" style="44"/>
+    <col min="2307" max="2307" width="17" style="44" customWidth="1"/>
+    <col min="2308" max="2308" width="13.90625" style="44" customWidth="1"/>
+    <col min="2309" max="2309" width="20.26953125" style="44" customWidth="1"/>
+    <col min="2310" max="2310" width="13.90625" style="44" customWidth="1"/>
+    <col min="2311" max="2311" width="8.7265625" style="44"/>
+    <col min="2312" max="2312" width="17.90625" style="44" customWidth="1"/>
+    <col min="2313" max="2313" width="8.7265625" style="44"/>
+    <col min="2314" max="2314" width="53.6328125" style="44" customWidth="1"/>
+    <col min="2315" max="2559" width="8.7265625" style="44"/>
+    <col min="2560" max="2560" width="10.90625" style="44" customWidth="1"/>
+    <col min="2561" max="2561" width="22.26953125" style="44" customWidth="1"/>
+    <col min="2562" max="2562" width="8.7265625" style="44"/>
+    <col min="2563" max="2563" width="17" style="44" customWidth="1"/>
+    <col min="2564" max="2564" width="13.90625" style="44" customWidth="1"/>
+    <col min="2565" max="2565" width="20.26953125" style="44" customWidth="1"/>
+    <col min="2566" max="2566" width="13.90625" style="44" customWidth="1"/>
+    <col min="2567" max="2567" width="8.7265625" style="44"/>
+    <col min="2568" max="2568" width="17.90625" style="44" customWidth="1"/>
+    <col min="2569" max="2569" width="8.7265625" style="44"/>
+    <col min="2570" max="2570" width="53.6328125" style="44" customWidth="1"/>
+    <col min="2571" max="2815" width="8.7265625" style="44"/>
+    <col min="2816" max="2816" width="10.90625" style="44" customWidth="1"/>
+    <col min="2817" max="2817" width="22.26953125" style="44" customWidth="1"/>
+    <col min="2818" max="2818" width="8.7265625" style="44"/>
+    <col min="2819" max="2819" width="17" style="44" customWidth="1"/>
+    <col min="2820" max="2820" width="13.90625" style="44" customWidth="1"/>
+    <col min="2821" max="2821" width="20.26953125" style="44" customWidth="1"/>
+    <col min="2822" max="2822" width="13.90625" style="44" customWidth="1"/>
+    <col min="2823" max="2823" width="8.7265625" style="44"/>
+    <col min="2824" max="2824" width="17.90625" style="44" customWidth="1"/>
+    <col min="2825" max="2825" width="8.7265625" style="44"/>
+    <col min="2826" max="2826" width="53.6328125" style="44" customWidth="1"/>
+    <col min="2827" max="3071" width="8.7265625" style="44"/>
+    <col min="3072" max="3072" width="10.90625" style="44" customWidth="1"/>
+    <col min="3073" max="3073" width="22.26953125" style="44" customWidth="1"/>
+    <col min="3074" max="3074" width="8.7265625" style="44"/>
+    <col min="3075" max="3075" width="17" style="44" customWidth="1"/>
+    <col min="3076" max="3076" width="13.90625" style="44" customWidth="1"/>
+    <col min="3077" max="3077" width="20.26953125" style="44" customWidth="1"/>
+    <col min="3078" max="3078" width="13.90625" style="44" customWidth="1"/>
+    <col min="3079" max="3079" width="8.7265625" style="44"/>
+    <col min="3080" max="3080" width="17.90625" style="44" customWidth="1"/>
+    <col min="3081" max="3081" width="8.7265625" style="44"/>
+    <col min="3082" max="3082" width="53.6328125" style="44" customWidth="1"/>
+    <col min="3083" max="3327" width="8.7265625" style="44"/>
+    <col min="3328" max="3328" width="10.90625" style="44" customWidth="1"/>
+    <col min="3329" max="3329" width="22.26953125" style="44" customWidth="1"/>
+    <col min="3330" max="3330" width="8.7265625" style="44"/>
+    <col min="3331" max="3331" width="17" style="44" customWidth="1"/>
+    <col min="3332" max="3332" width="13.90625" style="44" customWidth="1"/>
+    <col min="3333" max="3333" width="20.26953125" style="44" customWidth="1"/>
+    <col min="3334" max="3334" width="13.90625" style="44" customWidth="1"/>
+    <col min="3335" max="3335" width="8.7265625" style="44"/>
+    <col min="3336" max="3336" width="17.90625" style="44" customWidth="1"/>
+    <col min="3337" max="3337" width="8.7265625" style="44"/>
+    <col min="3338" max="3338" width="53.6328125" style="44" customWidth="1"/>
+    <col min="3339" max="3583" width="8.7265625" style="44"/>
+    <col min="3584" max="3584" width="10.90625" style="44" customWidth="1"/>
+    <col min="3585" max="3585" width="22.26953125" style="44" customWidth="1"/>
+    <col min="3586" max="3586" width="8.7265625" style="44"/>
+    <col min="3587" max="3587" width="17" style="44" customWidth="1"/>
+    <col min="3588" max="3588" width="13.90625" style="44" customWidth="1"/>
+    <col min="3589" max="3589" width="20.26953125" style="44" customWidth="1"/>
+    <col min="3590" max="3590" width="13.90625" style="44" customWidth="1"/>
+    <col min="3591" max="3591" width="8.7265625" style="44"/>
+    <col min="3592" max="3592" width="17.90625" style="44" customWidth="1"/>
+    <col min="3593" max="3593" width="8.7265625" style="44"/>
+    <col min="3594" max="3594" width="53.6328125" style="44" customWidth="1"/>
+    <col min="3595" max="3839" width="8.7265625" style="44"/>
+    <col min="3840" max="3840" width="10.90625" style="44" customWidth="1"/>
+    <col min="3841" max="3841" width="22.26953125" style="44" customWidth="1"/>
+    <col min="3842" max="3842" width="8.7265625" style="44"/>
+    <col min="3843" max="3843" width="17" style="44" customWidth="1"/>
+    <col min="3844" max="3844" width="13.90625" style="44" customWidth="1"/>
+    <col min="3845" max="3845" width="20.26953125" style="44" customWidth="1"/>
+    <col min="3846" max="3846" width="13.90625" style="44" customWidth="1"/>
+    <col min="3847" max="3847" width="8.7265625" style="44"/>
+    <col min="3848" max="3848" width="17.90625" style="44" customWidth="1"/>
+    <col min="3849" max="3849" width="8.7265625" style="44"/>
+    <col min="3850" max="3850" width="53.6328125" style="44" customWidth="1"/>
+    <col min="3851" max="4095" width="8.7265625" style="44"/>
+    <col min="4096" max="4096" width="10.90625" style="44" customWidth="1"/>
+    <col min="4097" max="4097" width="22.26953125" style="44" customWidth="1"/>
+    <col min="4098" max="4098" width="8.7265625" style="44"/>
+    <col min="4099" max="4099" width="17" style="44" customWidth="1"/>
+    <col min="4100" max="4100" width="13.90625" style="44" customWidth="1"/>
+    <col min="4101" max="4101" width="20.26953125" style="44" customWidth="1"/>
+    <col min="4102" max="4102" width="13.90625" style="44" customWidth="1"/>
+    <col min="4103" max="4103" width="8.7265625" style="44"/>
+    <col min="4104" max="4104" width="17.90625" style="44" customWidth="1"/>
+    <col min="4105" max="4105" width="8.7265625" style="44"/>
+    <col min="4106" max="4106" width="53.6328125" style="44" customWidth="1"/>
+    <col min="4107" max="4351" width="8.7265625" style="44"/>
+    <col min="4352" max="4352" width="10.90625" style="44" customWidth="1"/>
+    <col min="4353" max="4353" width="22.26953125" style="44" customWidth="1"/>
+    <col min="4354" max="4354" width="8.7265625" style="44"/>
+    <col min="4355" max="4355" width="17" style="44" customWidth="1"/>
+    <col min="4356" max="4356" width="13.90625" style="44" customWidth="1"/>
+    <col min="4357" max="4357" width="20.26953125" style="44" customWidth="1"/>
+    <col min="4358" max="4358" width="13.90625" style="44" customWidth="1"/>
+    <col min="4359" max="4359" width="8.7265625" style="44"/>
+    <col min="4360" max="4360" width="17.90625" style="44" customWidth="1"/>
+    <col min="4361" max="4361" width="8.7265625" style="44"/>
+    <col min="4362" max="4362" width="53.6328125" style="44" customWidth="1"/>
+    <col min="4363" max="4607" width="8.7265625" style="44"/>
+    <col min="4608" max="4608" width="10.90625" style="44" customWidth="1"/>
+    <col min="4609" max="4609" width="22.26953125" style="44" customWidth="1"/>
+    <col min="4610" max="4610" width="8.7265625" style="44"/>
+    <col min="4611" max="4611" width="17" style="44" customWidth="1"/>
+    <col min="4612" max="4612" width="13.90625" style="44" customWidth="1"/>
+    <col min="4613" max="4613" width="20.26953125" style="44" customWidth="1"/>
+    <col min="4614" max="4614" width="13.90625" style="44" customWidth="1"/>
+    <col min="4615" max="4615" width="8.7265625" style="44"/>
+    <col min="4616" max="4616" width="17.90625" style="44" customWidth="1"/>
+    <col min="4617" max="4617" width="8.7265625" style="44"/>
+    <col min="4618" max="4618" width="53.6328125" style="44" customWidth="1"/>
+    <col min="4619" max="4863" width="8.7265625" style="44"/>
+    <col min="4864" max="4864" width="10.90625" style="44" customWidth="1"/>
+    <col min="4865" max="4865" width="22.26953125" style="44" customWidth="1"/>
+    <col min="4866" max="4866" width="8.7265625" style="44"/>
+    <col min="4867" max="4867" width="17" style="44" customWidth="1"/>
+    <col min="4868" max="4868" width="13.90625" style="44" customWidth="1"/>
+    <col min="4869" max="4869" width="20.26953125" style="44" customWidth="1"/>
+    <col min="4870" max="4870" width="13.90625" style="44" customWidth="1"/>
+    <col min="4871" max="4871" width="8.7265625" style="44"/>
+    <col min="4872" max="4872" width="17.90625" style="44" customWidth="1"/>
+    <col min="4873" max="4873" width="8.7265625" style="44"/>
+    <col min="4874" max="4874" width="53.6328125" style="44" customWidth="1"/>
+    <col min="4875" max="5119" width="8.7265625" style="44"/>
+    <col min="5120" max="5120" width="10.90625" style="44" customWidth="1"/>
+    <col min="5121" max="5121" width="22.26953125" style="44" customWidth="1"/>
+    <col min="5122" max="5122" width="8.7265625" style="44"/>
+    <col min="5123" max="5123" width="17" style="44" customWidth="1"/>
+    <col min="5124" max="5124" width="13.90625" style="44" customWidth="1"/>
+    <col min="5125" max="5125" width="20.26953125" style="44" customWidth="1"/>
+    <col min="5126" max="5126" width="13.90625" style="44" customWidth="1"/>
+    <col min="5127" max="5127" width="8.7265625" style="44"/>
+    <col min="5128" max="5128" width="17.90625" style="44" customWidth="1"/>
+    <col min="5129" max="5129" width="8.7265625" style="44"/>
+    <col min="5130" max="5130" width="53.6328125" style="44" customWidth="1"/>
+    <col min="5131" max="5375" width="8.7265625" style="44"/>
+    <col min="5376" max="5376" width="10.90625" style="44" customWidth="1"/>
+    <col min="5377" max="5377" width="22.26953125" style="44" customWidth="1"/>
+    <col min="5378" max="5378" width="8.7265625" style="44"/>
+    <col min="5379" max="5379" width="17" style="44" customWidth="1"/>
+    <col min="5380" max="5380" width="13.90625" style="44" customWidth="1"/>
+    <col min="5381" max="5381" width="20.26953125" style="44" customWidth="1"/>
+    <col min="5382" max="5382" width="13.90625" style="44" customWidth="1"/>
+    <col min="5383" max="5383" width="8.7265625" style="44"/>
+    <col min="5384" max="5384" width="17.90625" style="44" customWidth="1"/>
+    <col min="5385" max="5385" width="8.7265625" style="44"/>
+    <col min="5386" max="5386" width="53.6328125" style="44" customWidth="1"/>
+    <col min="5387" max="5631" width="8.7265625" style="44"/>
+    <col min="5632" max="5632" width="10.90625" style="44" customWidth="1"/>
+    <col min="5633" max="5633" width="22.26953125" style="44" customWidth="1"/>
+    <col min="5634" max="5634" width="8.7265625" style="44"/>
+    <col min="5635" max="5635" width="17" style="44" customWidth="1"/>
+    <col min="5636" max="5636" width="13.90625" style="44" customWidth="1"/>
+    <col min="5637" max="5637" width="20.26953125" style="44" customWidth="1"/>
+    <col min="5638" max="5638" width="13.90625" style="44" customWidth="1"/>
+    <col min="5639" max="5639" width="8.7265625" style="44"/>
+    <col min="5640" max="5640" width="17.90625" style="44" customWidth="1"/>
+    <col min="5641" max="5641" width="8.7265625" style="44"/>
+    <col min="5642" max="5642" width="53.6328125" style="44" customWidth="1"/>
+    <col min="5643" max="5887" width="8.7265625" style="44"/>
+    <col min="5888" max="5888" width="10.90625" style="44" customWidth="1"/>
+    <col min="5889" max="5889" width="22.26953125" style="44" customWidth="1"/>
+    <col min="5890" max="5890" width="8.7265625" style="44"/>
+    <col min="5891" max="5891" width="17" style="44" customWidth="1"/>
+    <col min="5892" max="5892" width="13.90625" style="44" customWidth="1"/>
+    <col min="5893" max="5893" width="20.26953125" style="44" customWidth="1"/>
+    <col min="5894" max="5894" width="13.90625" style="44" customWidth="1"/>
+    <col min="5895" max="5895" width="8.7265625" style="44"/>
+    <col min="5896" max="5896" width="17.90625" style="44" customWidth="1"/>
+    <col min="5897" max="5897" width="8.7265625" style="44"/>
+    <col min="5898" max="5898" width="53.6328125" style="44" customWidth="1"/>
+    <col min="5899" max="6143" width="8.7265625" style="44"/>
+    <col min="6144" max="6144" width="10.90625" style="44" customWidth="1"/>
+    <col min="6145" max="6145" width="22.26953125" style="44" customWidth="1"/>
+    <col min="6146" max="6146" width="8.7265625" style="44"/>
+    <col min="6147" max="6147" width="17" style="44" customWidth="1"/>
+    <col min="6148" max="6148" width="13.90625" style="44" customWidth="1"/>
+    <col min="6149" max="6149" width="20.26953125" style="44" customWidth="1"/>
+    <col min="6150" max="6150" width="13.90625" style="44" customWidth="1"/>
+    <col min="6151" max="6151" width="8.7265625" style="44"/>
+    <col min="6152" max="6152" width="17.90625" style="44" customWidth="1"/>
+    <col min="6153" max="6153" width="8.7265625" style="44"/>
+    <col min="6154" max="6154" width="53.6328125" style="44" customWidth="1"/>
+    <col min="6155" max="6399" width="8.7265625" style="44"/>
+    <col min="6400" max="6400" width="10.90625" style="44" customWidth="1"/>
+    <col min="6401" max="6401" width="22.26953125" style="44" customWidth="1"/>
+    <col min="6402" max="6402" width="8.7265625" style="44"/>
+    <col min="6403" max="6403" width="17" style="44" customWidth="1"/>
+    <col min="6404" max="6404" width="13.90625" style="44" customWidth="1"/>
+    <col min="6405" max="6405" width="20.26953125" style="44" customWidth="1"/>
+    <col min="6406" max="6406" width="13.90625" style="44" customWidth="1"/>
+    <col min="6407" max="6407" width="8.7265625" style="44"/>
+    <col min="6408" max="6408" width="17.90625" style="44" customWidth="1"/>
+    <col min="6409" max="6409" width="8.7265625" style="44"/>
+    <col min="6410" max="6410" width="53.6328125" style="44" customWidth="1"/>
+    <col min="6411" max="6655" width="8.7265625" style="44"/>
+    <col min="6656" max="6656" width="10.90625" style="44" customWidth="1"/>
+    <col min="6657" max="6657" width="22.26953125" style="44" customWidth="1"/>
+    <col min="6658" max="6658" width="8.7265625" style="44"/>
+    <col min="6659" max="6659" width="17" style="44" customWidth="1"/>
+    <col min="6660" max="6660" width="13.90625" style="44" customWidth="1"/>
+    <col min="6661" max="6661" width="20.26953125" style="44" customWidth="1"/>
+    <col min="6662" max="6662" width="13.90625" style="44" customWidth="1"/>
+    <col min="6663" max="6663" width="8.7265625" style="44"/>
+    <col min="6664" max="6664" width="17.90625" style="44" customWidth="1"/>
+    <col min="6665" max="6665" width="8.7265625" style="44"/>
+    <col min="6666" max="6666" width="53.6328125" style="44" customWidth="1"/>
+    <col min="6667" max="6911" width="8.7265625" style="44"/>
+    <col min="6912" max="6912" width="10.90625" style="44" customWidth="1"/>
+    <col min="6913" max="6913" width="22.26953125" style="44" customWidth="1"/>
+    <col min="6914" max="6914" width="8.7265625" style="44"/>
+    <col min="6915" max="6915" width="17" style="44" customWidth="1"/>
+    <col min="6916" max="6916" width="13.90625" style="44" customWidth="1"/>
+    <col min="6917" max="6917" width="20.26953125" style="44" customWidth="1"/>
+    <col min="6918" max="6918" width="13.90625" style="44" customWidth="1"/>
+    <col min="6919" max="6919" width="8.7265625" style="44"/>
+    <col min="6920" max="6920" width="17.90625" style="44" customWidth="1"/>
+    <col min="6921" max="6921" width="8.7265625" style="44"/>
+    <col min="6922" max="6922" width="53.6328125" style="44" customWidth="1"/>
+    <col min="6923" max="7167" width="8.7265625" style="44"/>
+    <col min="7168" max="7168" width="10.90625" style="44" customWidth="1"/>
+    <col min="7169" max="7169" width="22.26953125" style="44" customWidth="1"/>
+    <col min="7170" max="7170" width="8.7265625" style="44"/>
+    <col min="7171" max="7171" width="17" style="44" customWidth="1"/>
+    <col min="7172" max="7172" width="13.90625" style="44" customWidth="1"/>
+    <col min="7173" max="7173" width="20.26953125" style="44" customWidth="1"/>
+    <col min="7174" max="7174" width="13.90625" style="44" customWidth="1"/>
+    <col min="7175" max="7175" width="8.7265625" style="44"/>
+    <col min="7176" max="7176" width="17.90625" style="44" customWidth="1"/>
+    <col min="7177" max="7177" width="8.7265625" style="44"/>
+    <col min="7178" max="7178" width="53.6328125" style="44" customWidth="1"/>
+    <col min="7179" max="7423" width="8.7265625" style="44"/>
+    <col min="7424" max="7424" width="10.90625" style="44" customWidth="1"/>
+    <col min="7425" max="7425" width="22.26953125" style="44" customWidth="1"/>
+    <col min="7426" max="7426" width="8.7265625" style="44"/>
+    <col min="7427" max="7427" width="17" style="44" customWidth="1"/>
+    <col min="7428" max="7428" width="13.90625" style="44" customWidth="1"/>
+    <col min="7429" max="7429" width="20.26953125" style="44" customWidth="1"/>
+    <col min="7430" max="7430" width="13.90625" style="44" customWidth="1"/>
+    <col min="7431" max="7431" width="8.7265625" style="44"/>
+    <col min="7432" max="7432" width="17.90625" style="44" customWidth="1"/>
+    <col min="7433" max="7433" width="8.7265625" style="44"/>
+    <col min="7434" max="7434" width="53.6328125" style="44" customWidth="1"/>
+    <col min="7435" max="7679" width="8.7265625" style="44"/>
+    <col min="7680" max="7680" width="10.90625" style="44" customWidth="1"/>
+    <col min="7681" max="7681" width="22.26953125" style="44" customWidth="1"/>
+    <col min="7682" max="7682" width="8.7265625" style="44"/>
+    <col min="7683" max="7683" width="17" style="44" customWidth="1"/>
+    <col min="7684" max="7684" width="13.90625" style="44" customWidth="1"/>
+    <col min="7685" max="7685" width="20.26953125" style="44" customWidth="1"/>
+    <col min="7686" max="7686" width="13.90625" style="44" customWidth="1"/>
+    <col min="7687" max="7687" width="8.7265625" style="44"/>
+    <col min="7688" max="7688" width="17.90625" style="44" customWidth="1"/>
+    <col min="7689" max="7689" width="8.7265625" style="44"/>
+    <col min="7690" max="7690" width="53.6328125" style="44" customWidth="1"/>
+    <col min="7691" max="7935" width="8.7265625" style="44"/>
+    <col min="7936" max="7936" width="10.90625" style="44" customWidth="1"/>
+    <col min="7937" max="7937" width="22.26953125" style="44" customWidth="1"/>
+    <col min="7938" max="7938" width="8.7265625" style="44"/>
+    <col min="7939" max="7939" width="17" style="44" customWidth="1"/>
+    <col min="7940" max="7940" width="13.90625" style="44" customWidth="1"/>
+    <col min="7941" max="7941" width="20.26953125" style="44" customWidth="1"/>
+    <col min="7942" max="7942" width="13.90625" style="44" customWidth="1"/>
+    <col min="7943" max="7943" width="8.7265625" style="44"/>
+    <col min="7944" max="7944" width="17.90625" style="44" customWidth="1"/>
+    <col min="7945" max="7945" width="8.7265625" style="44"/>
+    <col min="7946" max="7946" width="53.6328125" style="44" customWidth="1"/>
+    <col min="7947" max="8191" width="8.7265625" style="44"/>
+    <col min="8192" max="8192" width="10.90625" style="44" customWidth="1"/>
+    <col min="8193" max="8193" width="22.26953125" style="44" customWidth="1"/>
+    <col min="8194" max="8194" width="8.7265625" style="44"/>
+    <col min="8195" max="8195" width="17" style="44" customWidth="1"/>
+    <col min="8196" max="8196" width="13.90625" style="44" customWidth="1"/>
+    <col min="8197" max="8197" width="20.26953125" style="44" customWidth="1"/>
+    <col min="8198" max="8198" width="13.90625" style="44" customWidth="1"/>
+    <col min="8199" max="8199" width="8.7265625" style="44"/>
+    <col min="8200" max="8200" width="17.90625" style="44" customWidth="1"/>
+    <col min="8201" max="8201" width="8.7265625" style="44"/>
+    <col min="8202" max="8202" width="53.6328125" style="44" customWidth="1"/>
+    <col min="8203" max="8447" width="8.7265625" style="44"/>
+    <col min="8448" max="8448" width="10.90625" style="44" customWidth="1"/>
+    <col min="8449" max="8449" width="22.26953125" style="44" customWidth="1"/>
+    <col min="8450" max="8450" width="8.7265625" style="44"/>
+    <col min="8451" max="8451" width="17" style="44" customWidth="1"/>
+    <col min="8452" max="8452" width="13.90625" style="44" customWidth="1"/>
+    <col min="8453" max="8453" width="20.26953125" style="44" customWidth="1"/>
+    <col min="8454" max="8454" width="13.90625" style="44" customWidth="1"/>
+    <col min="8455" max="8455" width="8.7265625" style="44"/>
+    <col min="8456" max="8456" width="17.90625" style="44" customWidth="1"/>
+    <col min="8457" max="8457" width="8.7265625" style="44"/>
+    <col min="8458" max="8458" width="53.6328125" style="44" customWidth="1"/>
+    <col min="8459" max="8703" width="8.7265625" style="44"/>
+    <col min="8704" max="8704" width="10.90625" style="44" customWidth="1"/>
+    <col min="8705" max="8705" width="22.26953125" style="44" customWidth="1"/>
+    <col min="8706" max="8706" width="8.7265625" style="44"/>
+    <col min="8707" max="8707" width="17" style="44" customWidth="1"/>
+    <col min="8708" max="8708" width="13.90625" style="44" customWidth="1"/>
+    <col min="8709" max="8709" width="20.26953125" style="44" customWidth="1"/>
+    <col min="8710" max="8710" width="13.90625" style="44" customWidth="1"/>
+    <col min="8711" max="8711" width="8.7265625" style="44"/>
+    <col min="8712" max="8712" width="17.90625" style="44" customWidth="1"/>
+    <col min="8713" max="8713" width="8.7265625" style="44"/>
+    <col min="8714" max="8714" width="53.6328125" style="44" customWidth="1"/>
+    <col min="8715" max="8959" width="8.7265625" style="44"/>
+    <col min="8960" max="8960" width="10.90625" style="44" customWidth="1"/>
+    <col min="8961" max="8961" width="22.26953125" style="44" customWidth="1"/>
+    <col min="8962" max="8962" width="8.7265625" style="44"/>
+    <col min="8963" max="8963" width="17" style="44" customWidth="1"/>
+    <col min="8964" max="8964" width="13.90625" style="44" customWidth="1"/>
+    <col min="8965" max="8965" width="20.26953125" style="44" customWidth="1"/>
+    <col min="8966" max="8966" width="13.90625" style="44" customWidth="1"/>
+    <col min="8967" max="8967" width="8.7265625" style="44"/>
+    <col min="8968" max="8968" width="17.90625" style="44" customWidth="1"/>
+    <col min="8969" max="8969" width="8.7265625" style="44"/>
+    <col min="8970" max="8970" width="53.6328125" style="44" customWidth="1"/>
+    <col min="8971" max="9215" width="8.7265625" style="44"/>
+    <col min="9216" max="9216" width="10.90625" style="44" customWidth="1"/>
+    <col min="9217" max="9217" width="22.26953125" style="44" customWidth="1"/>
+    <col min="9218" max="9218" width="8.7265625" style="44"/>
+    <col min="9219" max="9219" width="17" style="44" customWidth="1"/>
+    <col min="9220" max="9220" width="13.90625" style="44" customWidth="1"/>
+    <col min="9221" max="9221" width="20.26953125" style="44" customWidth="1"/>
+    <col min="9222" max="9222" width="13.90625" style="44" customWidth="1"/>
+    <col min="9223" max="9223" width="8.7265625" style="44"/>
+    <col min="9224" max="9224" width="17.90625" style="44" customWidth="1"/>
+    <col min="9225" max="9225" width="8.7265625" style="44"/>
+    <col min="9226" max="9226" width="53.6328125" style="44" customWidth="1"/>
+    <col min="9227" max="9471" width="8.7265625" style="44"/>
+    <col min="9472" max="9472" width="10.90625" style="44" customWidth="1"/>
+    <col min="9473" max="9473" width="22.26953125" style="44" customWidth="1"/>
+    <col min="9474" max="9474" width="8.7265625" style="44"/>
+    <col min="9475" max="9475" width="17" style="44" customWidth="1"/>
+    <col min="9476" max="9476" width="13.90625" style="44" customWidth="1"/>
+    <col min="9477" max="9477" width="20.26953125" style="44" customWidth="1"/>
+    <col min="9478" max="9478" width="13.90625" style="44" customWidth="1"/>
+    <col min="9479" max="9479" width="8.7265625" style="44"/>
+    <col min="9480" max="9480" width="17.90625" style="44" customWidth="1"/>
+    <col min="9481" max="9481" width="8.7265625" style="44"/>
+    <col min="9482" max="9482" width="53.6328125" style="44" customWidth="1"/>
+    <col min="9483" max="9727" width="8.7265625" style="44"/>
+    <col min="9728" max="9728" width="10.90625" style="44" customWidth="1"/>
+    <col min="9729" max="9729" width="22.26953125" style="44" customWidth="1"/>
+    <col min="9730" max="9730" width="8.7265625" style="44"/>
+    <col min="9731" max="9731" width="17" style="44" customWidth="1"/>
+    <col min="9732" max="9732" width="13.90625" style="44" customWidth="1"/>
+    <col min="9733" max="9733" width="20.26953125" style="44" customWidth="1"/>
+    <col min="9734" max="9734" width="13.90625" style="44" customWidth="1"/>
+    <col min="9735" max="9735" width="8.7265625" style="44"/>
+    <col min="9736" max="9736" width="17.90625" style="44" customWidth="1"/>
+    <col min="9737" max="9737" width="8.7265625" style="44"/>
+    <col min="9738" max="9738" width="53.6328125" style="44" customWidth="1"/>
+    <col min="9739" max="9983" width="8.7265625" style="44"/>
+    <col min="9984" max="9984" width="10.90625" style="44" customWidth="1"/>
+    <col min="9985" max="9985" width="22.26953125" style="44" customWidth="1"/>
+    <col min="9986" max="9986" width="8.7265625" style="44"/>
+    <col min="9987" max="9987" width="17" style="44" customWidth="1"/>
+    <col min="9988" max="9988" width="13.90625" style="44" customWidth="1"/>
+    <col min="9989" max="9989" width="20.26953125" style="44" customWidth="1"/>
+    <col min="9990" max="9990" width="13.90625" style="44" customWidth="1"/>
+    <col min="9991" max="9991" width="8.7265625" style="44"/>
+    <col min="9992" max="9992" width="17.90625" style="44" customWidth="1"/>
+    <col min="9993" max="9993" width="8.7265625" style="44"/>
+    <col min="9994" max="9994" width="53.6328125" style="44" customWidth="1"/>
+    <col min="9995" max="10239" width="8.7265625" style="44"/>
+    <col min="10240" max="10240" width="10.90625" style="44" customWidth="1"/>
+    <col min="10241" max="10241" width="22.26953125" style="44" customWidth="1"/>
+    <col min="10242" max="10242" width="8.7265625" style="44"/>
+    <col min="10243" max="10243" width="17" style="44" customWidth="1"/>
+    <col min="10244" max="10244" width="13.90625" style="44" customWidth="1"/>
+    <col min="10245" max="10245" width="20.26953125" style="44" customWidth="1"/>
+    <col min="10246" max="10246" width="13.90625" style="44" customWidth="1"/>
+    <col min="10247" max="10247" width="8.7265625" style="44"/>
+    <col min="10248" max="10248" width="17.90625" style="44" customWidth="1"/>
+    <col min="10249" max="10249" width="8.7265625" style="44"/>
+    <col min="10250" max="10250" width="53.6328125" style="44" customWidth="1"/>
+    <col min="10251" max="10495" width="8.7265625" style="44"/>
+    <col min="10496" max="10496" width="10.90625" style="44" customWidth="1"/>
+    <col min="10497" max="10497" width="22.26953125" style="44" customWidth="1"/>
+    <col min="10498" max="10498" width="8.7265625" style="44"/>
+    <col min="10499" max="10499" width="17" style="44" customWidth="1"/>
+    <col min="10500" max="10500" width="13.90625" style="44" customWidth="1"/>
+    <col min="10501" max="10501" width="20.26953125" style="44" customWidth="1"/>
+    <col min="10502" max="10502" width="13.90625" style="44" customWidth="1"/>
+    <col min="10503" max="10503" width="8.7265625" style="44"/>
+    <col min="10504" max="10504" width="17.90625" style="44" customWidth="1"/>
+    <col min="10505" max="10505" width="8.7265625" style="44"/>
+    <col min="10506" max="10506" width="53.6328125" style="44" customWidth="1"/>
+    <col min="10507" max="10751" width="8.7265625" style="44"/>
+    <col min="10752" max="10752" width="10.90625" style="44" customWidth="1"/>
+    <col min="10753" max="10753" width="22.26953125" style="44" customWidth="1"/>
+    <col min="10754" max="10754" width="8.7265625" style="44"/>
+    <col min="10755" max="10755" width="17" style="44" customWidth="1"/>
+    <col min="10756" max="10756" width="13.90625" style="44" customWidth="1"/>
+    <col min="10757" max="10757" width="20.26953125" style="44" customWidth="1"/>
+    <col min="10758" max="10758" width="13.90625" style="44" customWidth="1"/>
+    <col min="10759" max="10759" width="8.7265625" style="44"/>
+    <col min="10760" max="10760" width="17.90625" style="44" customWidth="1"/>
+    <col min="10761" max="10761" width="8.7265625" style="44"/>
+    <col min="10762" max="10762" width="53.6328125" style="44" customWidth="1"/>
+    <col min="10763" max="11007" width="8.7265625" style="44"/>
+    <col min="11008" max="11008" width="10.90625" style="44" customWidth="1"/>
+    <col min="11009" max="11009" width="22.26953125" style="44" customWidth="1"/>
+    <col min="11010" max="11010" width="8.7265625" style="44"/>
+    <col min="11011" max="11011" width="17" style="44" customWidth="1"/>
+    <col min="11012" max="11012" width="13.90625" style="44" customWidth="1"/>
+    <col min="11013" max="11013" width="20.26953125" style="44" customWidth="1"/>
+    <col min="11014" max="11014" width="13.90625" style="44" customWidth="1"/>
+    <col min="11015" max="11015" width="8.7265625" style="44"/>
+    <col min="11016" max="11016" width="17.90625" style="44" customWidth="1"/>
+    <col min="11017" max="11017" width="8.7265625" style="44"/>
+    <col min="11018" max="11018" width="53.6328125" style="44" customWidth="1"/>
+    <col min="11019" max="11263" width="8.7265625" style="44"/>
+    <col min="11264" max="11264" width="10.90625" style="44" customWidth="1"/>
+    <col min="11265" max="11265" width="22.26953125" style="44" customWidth="1"/>
+    <col min="11266" max="11266" width="8.7265625" style="44"/>
+    <col min="11267" max="11267" width="17" style="44" customWidth="1"/>
+    <col min="11268" max="11268" width="13.90625" style="44" customWidth="1"/>
+    <col min="11269" max="11269" width="20.26953125" style="44" customWidth="1"/>
+    <col min="11270" max="11270" width="13.90625" style="44" customWidth="1"/>
+    <col min="11271" max="11271" width="8.7265625" style="44"/>
+    <col min="11272" max="11272" width="17.90625" style="44" customWidth="1"/>
+    <col min="11273" max="11273" width="8.7265625" style="44"/>
+    <col min="11274" max="11274" width="53.6328125" style="44" customWidth="1"/>
+    <col min="11275" max="11519" width="8.7265625" style="44"/>
+    <col min="11520" max="11520" width="10.90625" style="44" customWidth="1"/>
+    <col min="11521" max="11521" width="22.26953125" style="44" customWidth="1"/>
+    <col min="11522" max="11522" width="8.7265625" style="44"/>
+    <col min="11523" max="11523" width="17" style="44" customWidth="1"/>
+    <col min="11524" max="11524" width="13.90625" style="44" customWidth="1"/>
+    <col min="11525" max="11525" width="20.26953125" style="44" customWidth="1"/>
+    <col min="11526" max="11526" width="13.90625" style="44" customWidth="1"/>
+    <col min="11527" max="11527" width="8.7265625" style="44"/>
+    <col min="11528" max="11528" width="17.90625" style="44" customWidth="1"/>
+    <col min="11529" max="11529" width="8.7265625" style="44"/>
+    <col min="11530" max="11530" width="53.6328125" style="44" customWidth="1"/>
+    <col min="11531" max="11775" width="8.7265625" style="44"/>
+    <col min="11776" max="11776" width="10.90625" style="44" customWidth="1"/>
+    <col min="11777" max="11777" width="22.26953125" style="44" customWidth="1"/>
+    <col min="11778" max="11778" width="8.7265625" style="44"/>
+    <col min="11779" max="11779" width="17" style="44" customWidth="1"/>
+    <col min="11780" max="11780" width="13.90625" style="44" customWidth="1"/>
+    <col min="11781" max="11781" width="20.26953125" style="44" customWidth="1"/>
+    <col min="11782" max="11782" width="13.90625" style="44" customWidth="1"/>
+    <col min="11783" max="11783" width="8.7265625" style="44"/>
+    <col min="11784" max="11784" width="17.90625" style="44" customWidth="1"/>
+    <col min="11785" max="11785" width="8.7265625" style="44"/>
+    <col min="11786" max="11786" width="53.6328125" style="44" customWidth="1"/>
+    <col min="11787" max="12031" width="8.7265625" style="44"/>
+    <col min="12032" max="12032" width="10.90625" style="44" customWidth="1"/>
+    <col min="12033" max="12033" width="22.26953125" style="44" customWidth="1"/>
+    <col min="12034" max="12034" width="8.7265625" style="44"/>
+    <col min="12035" max="12035" width="17" style="44" customWidth="1"/>
+    <col min="12036" max="12036" width="13.90625" style="44" customWidth="1"/>
+    <col min="12037" max="12037" width="20.26953125" style="44" customWidth="1"/>
+    <col min="12038" max="12038" width="13.90625" style="44" customWidth="1"/>
+    <col min="12039" max="12039" width="8.7265625" style="44"/>
+    <col min="12040" max="12040" width="17.90625" style="44" customWidth="1"/>
+    <col min="12041" max="12041" width="8.7265625" style="44"/>
+    <col min="12042" max="12042" width="53.6328125" style="44" customWidth="1"/>
+    <col min="12043" max="12287" width="8.7265625" style="44"/>
+    <col min="12288" max="12288" width="10.90625" style="44" customWidth="1"/>
+    <col min="12289" max="12289" width="22.26953125" style="44" customWidth="1"/>
+    <col min="12290" max="12290" width="8.7265625" style="44"/>
+    <col min="12291" max="12291" width="17" style="44" customWidth="1"/>
+    <col min="12292" max="12292" width="13.90625" style="44" customWidth="1"/>
+    <col min="12293" max="12293" width="20.26953125" style="44" customWidth="1"/>
+    <col min="12294" max="12294" width="13.90625" style="44" customWidth="1"/>
+    <col min="12295" max="12295" width="8.7265625" style="44"/>
+    <col min="12296" max="12296" width="17.90625" style="44" customWidth="1"/>
+    <col min="12297" max="12297" width="8.7265625" style="44"/>
+    <col min="12298" max="12298" width="53.6328125" style="44" customWidth="1"/>
+    <col min="12299" max="12543" width="8.7265625" style="44"/>
+    <col min="12544" max="12544" width="10.90625" style="44" customWidth="1"/>
+    <col min="12545" max="12545" width="22.26953125" style="44" customWidth="1"/>
+    <col min="12546" max="12546" width="8.7265625" style="44"/>
+    <col min="12547" max="12547" width="17" style="44" customWidth="1"/>
+    <col min="12548" max="12548" width="13.90625" style="44" customWidth="1"/>
+    <col min="12549" max="12549" width="20.26953125" style="44" customWidth="1"/>
+    <col min="12550" max="12550" width="13.90625" style="44" customWidth="1"/>
+    <col min="12551" max="12551" width="8.7265625" style="44"/>
+    <col min="12552" max="12552" width="17.90625" style="44" customWidth="1"/>
+    <col min="12553" max="12553" width="8.7265625" style="44"/>
+    <col min="12554" max="12554" width="53.6328125" style="44" customWidth="1"/>
+    <col min="12555" max="12799" width="8.7265625" style="44"/>
+    <col min="12800" max="12800" width="10.90625" style="44" customWidth="1"/>
+    <col min="12801" max="12801" width="22.26953125" style="44" customWidth="1"/>
+    <col min="12802" max="12802" width="8.7265625" style="44"/>
+    <col min="12803" max="12803" width="17" style="44" customWidth="1"/>
+    <col min="12804" max="12804" width="13.90625" style="44" customWidth="1"/>
+    <col min="12805" max="12805" width="20.26953125" style="44" customWidth="1"/>
+    <col min="12806" max="12806" width="13.90625" style="44" customWidth="1"/>
+    <col min="12807" max="12807" width="8.7265625" style="44"/>
+    <col min="12808" max="12808" width="17.90625" style="44" customWidth="1"/>
+    <col min="12809" max="12809" width="8.7265625" style="44"/>
+    <col min="12810" max="12810" width="53.6328125" style="44" customWidth="1"/>
+    <col min="12811" max="13055" width="8.7265625" style="44"/>
+    <col min="13056" max="13056" width="10.90625" style="44" customWidth="1"/>
+    <col min="13057" max="13057" width="22.26953125" style="44" customWidth="1"/>
+    <col min="13058" max="13058" width="8.7265625" style="44"/>
+    <col min="13059" max="13059" width="17" style="44" customWidth="1"/>
+    <col min="13060" max="13060" width="13.90625" style="44" customWidth="1"/>
+    <col min="13061" max="13061" width="20.26953125" style="44" customWidth="1"/>
+    <col min="13062" max="13062" width="13.90625" style="44" customWidth="1"/>
+    <col min="13063" max="13063" width="8.7265625" style="44"/>
+    <col min="13064" max="13064" width="17.90625" style="44" customWidth="1"/>
+    <col min="13065" max="13065" width="8.7265625" style="44"/>
+    <col min="13066" max="13066" width="53.6328125" style="44" customWidth="1"/>
+    <col min="13067" max="13311" width="8.7265625" style="44"/>
+    <col min="13312" max="13312" width="10.90625" style="44" customWidth="1"/>
+    <col min="13313" max="13313" width="22.26953125" style="44" customWidth="1"/>
+    <col min="13314" max="13314" width="8.7265625" style="44"/>
+    <col min="13315" max="13315" width="17" style="44" customWidth="1"/>
+    <col min="13316" max="13316" width="13.90625" style="44" customWidth="1"/>
+    <col min="13317" max="13317" width="20.26953125" style="44" customWidth="1"/>
+    <col min="13318" max="13318" width="13.90625" style="44" customWidth="1"/>
+    <col min="13319" max="13319" width="8.7265625" style="44"/>
+    <col min="13320" max="13320" width="17.90625" style="44" customWidth="1"/>
+    <col min="13321" max="13321" width="8.7265625" style="44"/>
+    <col min="13322" max="13322" width="53.6328125" style="44" customWidth="1"/>
+    <col min="13323" max="13567" width="8.7265625" style="44"/>
+    <col min="13568" max="13568" width="10.90625" style="44" customWidth="1"/>
+    <col min="13569" max="13569" width="22.26953125" style="44" customWidth="1"/>
+    <col min="13570" max="13570" width="8.7265625" style="44"/>
+    <col min="13571" max="13571" width="17" style="44" customWidth="1"/>
+    <col min="13572" max="13572" width="13.90625" style="44" customWidth="1"/>
+    <col min="13573" max="13573" width="20.26953125" style="44" customWidth="1"/>
+    <col min="13574" max="13574" width="13.90625" style="44" customWidth="1"/>
+    <col min="13575" max="13575" width="8.7265625" style="44"/>
+    <col min="13576" max="13576" width="17.90625" style="44" customWidth="1"/>
+    <col min="13577" max="13577" width="8.7265625" style="44"/>
+    <col min="13578" max="13578" width="53.6328125" style="44" customWidth="1"/>
+    <col min="13579" max="13823" width="8.7265625" style="44"/>
+    <col min="13824" max="13824" width="10.90625" style="44" customWidth="1"/>
+    <col min="13825" max="13825" width="22.26953125" style="44" customWidth="1"/>
+    <col min="13826" max="13826" width="8.7265625" style="44"/>
+    <col min="13827" max="13827" width="17" style="44" customWidth="1"/>
+    <col min="13828" max="13828" width="13.90625" style="44" customWidth="1"/>
+    <col min="13829" max="13829" width="20.26953125" style="44" customWidth="1"/>
+    <col min="13830" max="13830" width="13.90625" style="44" customWidth="1"/>
+    <col min="13831" max="13831" width="8.7265625" style="44"/>
+    <col min="13832" max="13832" width="17.90625" style="44" customWidth="1"/>
+    <col min="13833" max="13833" width="8.7265625" style="44"/>
+    <col min="13834" max="13834" width="53.6328125" style="44" customWidth="1"/>
+    <col min="13835" max="14079" width="8.7265625" style="44"/>
+    <col min="14080" max="14080" width="10.90625" style="44" customWidth="1"/>
+    <col min="14081" max="14081" width="22.26953125" style="44" customWidth="1"/>
+    <col min="14082" max="14082" width="8.7265625" style="44"/>
+    <col min="14083" max="14083" width="17" style="44" customWidth="1"/>
+    <col min="14084" max="14084" width="13.90625" style="44" customWidth="1"/>
+    <col min="14085" max="14085" width="20.26953125" style="44" customWidth="1"/>
+    <col min="14086" max="14086" width="13.90625" style="44" customWidth="1"/>
+    <col min="14087" max="14087" width="8.7265625" style="44"/>
+    <col min="14088" max="14088" width="17.90625" style="44" customWidth="1"/>
+    <col min="14089" max="14089" width="8.7265625" style="44"/>
+    <col min="14090" max="14090" width="53.6328125" style="44" customWidth="1"/>
+    <col min="14091" max="14335" width="8.7265625" style="44"/>
+    <col min="14336" max="14336" width="10.90625" style="44" customWidth="1"/>
+    <col min="14337" max="14337" width="22.26953125" style="44" customWidth="1"/>
+    <col min="14338" max="14338" width="8.7265625" style="44"/>
+    <col min="14339" max="14339" width="17" style="44" customWidth="1"/>
+    <col min="14340" max="14340" width="13.90625" style="44" customWidth="1"/>
+    <col min="14341" max="14341" width="20.26953125" style="44" customWidth="1"/>
+    <col min="14342" max="14342" width="13.90625" style="44" customWidth="1"/>
+    <col min="14343" max="14343" width="8.7265625" style="44"/>
+    <col min="14344" max="14344" width="17.90625" style="44" customWidth="1"/>
+    <col min="14345" max="14345" width="8.7265625" style="44"/>
+    <col min="14346" max="14346" width="53.6328125" style="44" customWidth="1"/>
+    <col min="14347" max="14591" width="8.7265625" style="44"/>
+    <col min="14592" max="14592" width="10.90625" style="44" customWidth="1"/>
+    <col min="14593" max="14593" width="22.26953125" style="44" customWidth="1"/>
+    <col min="14594" max="14594" width="8.7265625" style="44"/>
+    <col min="14595" max="14595" width="17" style="44" customWidth="1"/>
+    <col min="14596" max="14596" width="13.90625" style="44" customWidth="1"/>
+    <col min="14597" max="14597" width="20.26953125" style="44" customWidth="1"/>
+    <col min="14598" max="14598" width="13.90625" style="44" customWidth="1"/>
+    <col min="14599" max="14599" width="8.7265625" style="44"/>
+    <col min="14600" max="14600" width="17.90625" style="44" customWidth="1"/>
+    <col min="14601" max="14601" width="8.7265625" style="44"/>
+    <col min="14602" max="14602" width="53.6328125" style="44" customWidth="1"/>
+    <col min="14603" max="14847" width="8.7265625" style="44"/>
+    <col min="14848" max="14848" width="10.90625" style="44" customWidth="1"/>
+    <col min="14849" max="14849" width="22.26953125" style="44" customWidth="1"/>
+    <col min="14850" max="14850" width="8.7265625" style="44"/>
+    <col min="14851" max="14851" width="17" style="44" customWidth="1"/>
+    <col min="14852" max="14852" width="13.90625" style="44" customWidth="1"/>
+    <col min="14853" max="14853" width="20.26953125" style="44" customWidth="1"/>
+    <col min="14854" max="14854" width="13.90625" style="44" customWidth="1"/>
+    <col min="14855" max="14855" width="8.7265625" style="44"/>
+    <col min="14856" max="14856" width="17.90625" style="44" customWidth="1"/>
+    <col min="14857" max="14857" width="8.7265625" style="44"/>
+    <col min="14858" max="14858" width="53.6328125" style="44" customWidth="1"/>
+    <col min="14859" max="15103" width="8.7265625" style="44"/>
+    <col min="15104" max="15104" width="10.90625" style="44" customWidth="1"/>
+    <col min="15105" max="15105" width="22.26953125" style="44" customWidth="1"/>
+    <col min="15106" max="15106" width="8.7265625" style="44"/>
+    <col min="15107" max="15107" width="17" style="44" customWidth="1"/>
+    <col min="15108" max="15108" width="13.90625" style="44" customWidth="1"/>
+    <col min="15109" max="15109" width="20.26953125" style="44" customWidth="1"/>
+    <col min="15110" max="15110" width="13.90625" style="44" customWidth="1"/>
+    <col min="15111" max="15111" width="8.7265625" style="44"/>
+    <col min="15112" max="15112" width="17.90625" style="44" customWidth="1"/>
+    <col min="15113" max="15113" width="8.7265625" style="44"/>
+    <col min="15114" max="15114" width="53.6328125" style="44" customWidth="1"/>
+    <col min="15115" max="15359" width="8.7265625" style="44"/>
+    <col min="15360" max="15360" width="10.90625" style="44" customWidth="1"/>
+    <col min="15361" max="15361" width="22.26953125" style="44" customWidth="1"/>
+    <col min="15362" max="15362" width="8.7265625" style="44"/>
+    <col min="15363" max="15363" width="17" style="44" customWidth="1"/>
+    <col min="15364" max="15364" width="13.90625" style="44" customWidth="1"/>
+    <col min="15365" max="15365" width="20.26953125" style="44" customWidth="1"/>
+    <col min="15366" max="15366" width="13.90625" style="44" customWidth="1"/>
+    <col min="15367" max="15367" width="8.7265625" style="44"/>
+    <col min="15368" max="15368" width="17.90625" style="44" customWidth="1"/>
+    <col min="15369" max="15369" width="8.7265625" style="44"/>
+    <col min="15370" max="15370" width="53.6328125" style="44" customWidth="1"/>
+    <col min="15371" max="15615" width="8.7265625" style="44"/>
+    <col min="15616" max="15616" width="10.90625" style="44" customWidth="1"/>
+    <col min="15617" max="15617" width="22.26953125" style="44" customWidth="1"/>
+    <col min="15618" max="15618" width="8.7265625" style="44"/>
+    <col min="15619" max="15619" width="17" style="44" customWidth="1"/>
+    <col min="15620" max="15620" width="13.90625" style="44" customWidth="1"/>
+    <col min="15621" max="15621" width="20.26953125" style="44" customWidth="1"/>
+    <col min="15622" max="15622" width="13.90625" style="44" customWidth="1"/>
+    <col min="15623" max="15623" width="8.7265625" style="44"/>
+    <col min="15624" max="15624" width="17.90625" style="44" customWidth="1"/>
+    <col min="15625" max="15625" width="8.7265625" style="44"/>
+    <col min="15626" max="15626" width="53.6328125" style="44" customWidth="1"/>
+    <col min="15627" max="15871" width="8.7265625" style="44"/>
+    <col min="15872" max="15872" width="10.90625" style="44" customWidth="1"/>
+    <col min="15873" max="15873" width="22.26953125" style="44" customWidth="1"/>
+    <col min="15874" max="15874" width="8.7265625" style="44"/>
+    <col min="15875" max="15875" width="17" style="44" customWidth="1"/>
+    <col min="15876" max="15876" width="13.90625" style="44" customWidth="1"/>
+    <col min="15877" max="15877" width="20.26953125" style="44" customWidth="1"/>
+    <col min="15878" max="15878" width="13.90625" style="44" customWidth="1"/>
+    <col min="15879" max="15879" width="8.7265625" style="44"/>
+    <col min="15880" max="15880" width="17.90625" style="44" customWidth="1"/>
+    <col min="15881" max="15881" width="8.7265625" style="44"/>
+    <col min="15882" max="15882" width="53.6328125" style="44" customWidth="1"/>
+    <col min="15883" max="16127" width="8.7265625" style="44"/>
+    <col min="16128" max="16128" width="10.90625" style="44" customWidth="1"/>
+    <col min="16129" max="16129" width="22.26953125" style="44" customWidth="1"/>
+    <col min="16130" max="16130" width="8.7265625" style="44"/>
+    <col min="16131" max="16131" width="17" style="44" customWidth="1"/>
+    <col min="16132" max="16132" width="13.90625" style="44" customWidth="1"/>
+    <col min="16133" max="16133" width="20.26953125" style="44" customWidth="1"/>
+    <col min="16134" max="16134" width="13.90625" style="44" customWidth="1"/>
+    <col min="16135" max="16135" width="8.7265625" style="44"/>
+    <col min="16136" max="16136" width="17.90625" style="44" customWidth="1"/>
+    <col min="16137" max="16137" width="8.7265625" style="44"/>
+    <col min="16138" max="16138" width="53.6328125" style="44" customWidth="1"/>
+    <col min="16139" max="16384" width="8.7265625" style="44"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>980</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>981</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>982</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>975</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>976</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>977</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>993</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>987</v>
+      </c>
+      <c r="F2" s="43" t="s">
+        <v>974</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>978</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>985</v>
+      </c>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>993</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>988</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>974</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>978</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>986</v>
+      </c>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="38.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>347</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>348</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>994</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>987</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>974</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>978</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>985</v>
+      </c>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="39.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="40" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>347</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>348</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>994</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>988</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>974</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>978</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>986</v>
+      </c>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41" t="s">
+        <v>996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft"/>
@@ -9926,11 +10910,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Added Sprint 2 changes new tab contents
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6088B859-F4CC-4BEC-A868-E480CB51A829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82BC453-615B-49C3-ADD4-473B1344DB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="1390" windowWidth="16590" windowHeight="8590" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="360" windowWidth="16590" windowHeight="8590" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1723" uniqueCount="1010">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1776" uniqueCount="1029">
   <si>
     <t>Code</t>
   </si>
@@ -3183,6 +3183,64 @@
   </si>
   <si>
     <t>Remove attribute 'transitionEndRule' from StudyElement Class</t>
+  </si>
+  <si>
+    <t>Add relationship to StudyDesign class</t>
+  </si>
+  <si>
+    <t>encounters</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>activities</t>
+  </si>
+  <si>
+    <t>Add attribute to StudyDesign Class</t>
+  </si>
+  <si>
+    <t>studyDesignName</t>
+  </si>
+  <si>
+    <t>Study Design Name</t>
+  </si>
+  <si>
+    <t>The literal identifier (i.e., distinctive designation) of the study design.</t>
+  </si>
+  <si>
+    <t>studyDesignDesc</t>
+  </si>
+  <si>
+    <t>Study Design Description</t>
+  </si>
+  <si>
+    <t>The textual representation of the study design.</t>
+  </si>
+  <si>
+    <t>Add new Class</t>
+  </si>
+  <si>
+    <t>AliasCode</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Alias Code</t>
+  </si>
+  <si>
+    <t>Add relationship to AliasCode class</t>
+  </si>
+  <si>
+    <t>standardCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standardCodeAliases
+</t>
+  </si>
+  <si>
+    <t>An alternative symbol or combination of symbols which is assigned to the members of a collection.</t>
   </si>
 </sst>
 </file>
@@ -3334,7 +3392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -3411,13 +3469,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -3525,15 +3596,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -3548,6 +3610,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3843,10 +3929,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="42" t="s">
         <v>973</v>
       </c>
-      <c r="B1" s="38"/>
+      <c r="B1" s="43"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -9685,14 +9771,232 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC60F93F-DDE7-4577-BCA7-BDCFD0F8A197}">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.90625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15" style="4" customWidth="1"/>
+    <col min="5" max="5" width="19.36328125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.90625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="22.453125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.36328125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="75" style="4" customWidth="1"/>
+    <col min="11" max="11" width="4.36328125" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>980</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>981</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>982</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>975</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>976</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>977</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="37" t="s">
+        <v>979</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>1012</v>
+      </c>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+    </row>
+    <row r="3" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="37" t="s">
+        <v>979</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>1012</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" ht="44.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>323</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>324</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>979</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>1015</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>974</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>978</v>
+      </c>
+      <c r="H4" s="37" t="s">
+        <v>1016</v>
+      </c>
+      <c r="I4" s="18"/>
+      <c r="J4" s="37" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="41" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>323</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>324</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>979</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>974</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>978</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>1019</v>
+      </c>
+      <c r="I5" s="18"/>
+      <c r="J5" s="37" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="41" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>1023</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>978</v>
+      </c>
+      <c r="H6" s="48" t="s">
+        <v>1024</v>
+      </c>
+      <c r="I6" s="48"/>
+      <c r="J6" s="49" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="41" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>1026</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>1012</v>
+      </c>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="37"/>
+    </row>
+    <row r="8" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="37" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>1027</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>1012</v>
+      </c>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9704,777 +10008,777 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.26953125" style="44" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="44"/>
-    <col min="3" max="3" width="17" style="44" customWidth="1"/>
-    <col min="4" max="4" width="13.90625" style="44" customWidth="1"/>
-    <col min="5" max="5" width="20.26953125" style="44" customWidth="1"/>
-    <col min="6" max="6" width="13.90625" style="44" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="44"/>
-    <col min="8" max="8" width="17.90625" style="44" customWidth="1"/>
-    <col min="9" max="9" width="8.7265625" style="44"/>
-    <col min="10" max="10" width="53.6328125" style="44" customWidth="1"/>
-    <col min="11" max="255" width="8.7265625" style="44"/>
-    <col min="256" max="256" width="10.90625" style="44" customWidth="1"/>
-    <col min="257" max="257" width="22.26953125" style="44" customWidth="1"/>
-    <col min="258" max="258" width="8.7265625" style="44"/>
-    <col min="259" max="259" width="17" style="44" customWidth="1"/>
-    <col min="260" max="260" width="13.90625" style="44" customWidth="1"/>
-    <col min="261" max="261" width="20.26953125" style="44" customWidth="1"/>
-    <col min="262" max="262" width="13.90625" style="44" customWidth="1"/>
-    <col min="263" max="263" width="8.7265625" style="44"/>
-    <col min="264" max="264" width="17.90625" style="44" customWidth="1"/>
-    <col min="265" max="265" width="8.7265625" style="44"/>
-    <col min="266" max="266" width="53.6328125" style="44" customWidth="1"/>
-    <col min="267" max="511" width="8.7265625" style="44"/>
-    <col min="512" max="512" width="10.90625" style="44" customWidth="1"/>
-    <col min="513" max="513" width="22.26953125" style="44" customWidth="1"/>
-    <col min="514" max="514" width="8.7265625" style="44"/>
-    <col min="515" max="515" width="17" style="44" customWidth="1"/>
-    <col min="516" max="516" width="13.90625" style="44" customWidth="1"/>
-    <col min="517" max="517" width="20.26953125" style="44" customWidth="1"/>
-    <col min="518" max="518" width="13.90625" style="44" customWidth="1"/>
-    <col min="519" max="519" width="8.7265625" style="44"/>
-    <col min="520" max="520" width="17.90625" style="44" customWidth="1"/>
-    <col min="521" max="521" width="8.7265625" style="44"/>
-    <col min="522" max="522" width="53.6328125" style="44" customWidth="1"/>
-    <col min="523" max="767" width="8.7265625" style="44"/>
-    <col min="768" max="768" width="10.90625" style="44" customWidth="1"/>
-    <col min="769" max="769" width="22.26953125" style="44" customWidth="1"/>
-    <col min="770" max="770" width="8.7265625" style="44"/>
-    <col min="771" max="771" width="17" style="44" customWidth="1"/>
-    <col min="772" max="772" width="13.90625" style="44" customWidth="1"/>
-    <col min="773" max="773" width="20.26953125" style="44" customWidth="1"/>
-    <col min="774" max="774" width="13.90625" style="44" customWidth="1"/>
-    <col min="775" max="775" width="8.7265625" style="44"/>
-    <col min="776" max="776" width="17.90625" style="44" customWidth="1"/>
-    <col min="777" max="777" width="8.7265625" style="44"/>
-    <col min="778" max="778" width="53.6328125" style="44" customWidth="1"/>
-    <col min="779" max="1023" width="8.7265625" style="44"/>
-    <col min="1024" max="1024" width="10.90625" style="44" customWidth="1"/>
-    <col min="1025" max="1025" width="22.26953125" style="44" customWidth="1"/>
-    <col min="1026" max="1026" width="8.7265625" style="44"/>
-    <col min="1027" max="1027" width="17" style="44" customWidth="1"/>
-    <col min="1028" max="1028" width="13.90625" style="44" customWidth="1"/>
-    <col min="1029" max="1029" width="20.26953125" style="44" customWidth="1"/>
-    <col min="1030" max="1030" width="13.90625" style="44" customWidth="1"/>
-    <col min="1031" max="1031" width="8.7265625" style="44"/>
-    <col min="1032" max="1032" width="17.90625" style="44" customWidth="1"/>
-    <col min="1033" max="1033" width="8.7265625" style="44"/>
-    <col min="1034" max="1034" width="53.6328125" style="44" customWidth="1"/>
-    <col min="1035" max="1279" width="8.7265625" style="44"/>
-    <col min="1280" max="1280" width="10.90625" style="44" customWidth="1"/>
-    <col min="1281" max="1281" width="22.26953125" style="44" customWidth="1"/>
-    <col min="1282" max="1282" width="8.7265625" style="44"/>
-    <col min="1283" max="1283" width="17" style="44" customWidth="1"/>
-    <col min="1284" max="1284" width="13.90625" style="44" customWidth="1"/>
-    <col min="1285" max="1285" width="20.26953125" style="44" customWidth="1"/>
-    <col min="1286" max="1286" width="13.90625" style="44" customWidth="1"/>
-    <col min="1287" max="1287" width="8.7265625" style="44"/>
-    <col min="1288" max="1288" width="17.90625" style="44" customWidth="1"/>
-    <col min="1289" max="1289" width="8.7265625" style="44"/>
-    <col min="1290" max="1290" width="53.6328125" style="44" customWidth="1"/>
-    <col min="1291" max="1535" width="8.7265625" style="44"/>
-    <col min="1536" max="1536" width="10.90625" style="44" customWidth="1"/>
-    <col min="1537" max="1537" width="22.26953125" style="44" customWidth="1"/>
-    <col min="1538" max="1538" width="8.7265625" style="44"/>
-    <col min="1539" max="1539" width="17" style="44" customWidth="1"/>
-    <col min="1540" max="1540" width="13.90625" style="44" customWidth="1"/>
-    <col min="1541" max="1541" width="20.26953125" style="44" customWidth="1"/>
-    <col min="1542" max="1542" width="13.90625" style="44" customWidth="1"/>
-    <col min="1543" max="1543" width="8.7265625" style="44"/>
-    <col min="1544" max="1544" width="17.90625" style="44" customWidth="1"/>
-    <col min="1545" max="1545" width="8.7265625" style="44"/>
-    <col min="1546" max="1546" width="53.6328125" style="44" customWidth="1"/>
-    <col min="1547" max="1791" width="8.7265625" style="44"/>
-    <col min="1792" max="1792" width="10.90625" style="44" customWidth="1"/>
-    <col min="1793" max="1793" width="22.26953125" style="44" customWidth="1"/>
-    <col min="1794" max="1794" width="8.7265625" style="44"/>
-    <col min="1795" max="1795" width="17" style="44" customWidth="1"/>
-    <col min="1796" max="1796" width="13.90625" style="44" customWidth="1"/>
-    <col min="1797" max="1797" width="20.26953125" style="44" customWidth="1"/>
-    <col min="1798" max="1798" width="13.90625" style="44" customWidth="1"/>
-    <col min="1799" max="1799" width="8.7265625" style="44"/>
-    <col min="1800" max="1800" width="17.90625" style="44" customWidth="1"/>
-    <col min="1801" max="1801" width="8.7265625" style="44"/>
-    <col min="1802" max="1802" width="53.6328125" style="44" customWidth="1"/>
-    <col min="1803" max="2047" width="8.7265625" style="44"/>
-    <col min="2048" max="2048" width="10.90625" style="44" customWidth="1"/>
-    <col min="2049" max="2049" width="22.26953125" style="44" customWidth="1"/>
-    <col min="2050" max="2050" width="8.7265625" style="44"/>
-    <col min="2051" max="2051" width="17" style="44" customWidth="1"/>
-    <col min="2052" max="2052" width="13.90625" style="44" customWidth="1"/>
-    <col min="2053" max="2053" width="20.26953125" style="44" customWidth="1"/>
-    <col min="2054" max="2054" width="13.90625" style="44" customWidth="1"/>
-    <col min="2055" max="2055" width="8.7265625" style="44"/>
-    <col min="2056" max="2056" width="17.90625" style="44" customWidth="1"/>
-    <col min="2057" max="2057" width="8.7265625" style="44"/>
-    <col min="2058" max="2058" width="53.6328125" style="44" customWidth="1"/>
-    <col min="2059" max="2303" width="8.7265625" style="44"/>
-    <col min="2304" max="2304" width="10.90625" style="44" customWidth="1"/>
-    <col min="2305" max="2305" width="22.26953125" style="44" customWidth="1"/>
-    <col min="2306" max="2306" width="8.7265625" style="44"/>
-    <col min="2307" max="2307" width="17" style="44" customWidth="1"/>
-    <col min="2308" max="2308" width="13.90625" style="44" customWidth="1"/>
-    <col min="2309" max="2309" width="20.26953125" style="44" customWidth="1"/>
-    <col min="2310" max="2310" width="13.90625" style="44" customWidth="1"/>
-    <col min="2311" max="2311" width="8.7265625" style="44"/>
-    <col min="2312" max="2312" width="17.90625" style="44" customWidth="1"/>
-    <col min="2313" max="2313" width="8.7265625" style="44"/>
-    <col min="2314" max="2314" width="53.6328125" style="44" customWidth="1"/>
-    <col min="2315" max="2559" width="8.7265625" style="44"/>
-    <col min="2560" max="2560" width="10.90625" style="44" customWidth="1"/>
-    <col min="2561" max="2561" width="22.26953125" style="44" customWidth="1"/>
-    <col min="2562" max="2562" width="8.7265625" style="44"/>
-    <col min="2563" max="2563" width="17" style="44" customWidth="1"/>
-    <col min="2564" max="2564" width="13.90625" style="44" customWidth="1"/>
-    <col min="2565" max="2565" width="20.26953125" style="44" customWidth="1"/>
-    <col min="2566" max="2566" width="13.90625" style="44" customWidth="1"/>
-    <col min="2567" max="2567" width="8.7265625" style="44"/>
-    <col min="2568" max="2568" width="17.90625" style="44" customWidth="1"/>
-    <col min="2569" max="2569" width="8.7265625" style="44"/>
-    <col min="2570" max="2570" width="53.6328125" style="44" customWidth="1"/>
-    <col min="2571" max="2815" width="8.7265625" style="44"/>
-    <col min="2816" max="2816" width="10.90625" style="44" customWidth="1"/>
-    <col min="2817" max="2817" width="22.26953125" style="44" customWidth="1"/>
-    <col min="2818" max="2818" width="8.7265625" style="44"/>
-    <col min="2819" max="2819" width="17" style="44" customWidth="1"/>
-    <col min="2820" max="2820" width="13.90625" style="44" customWidth="1"/>
-    <col min="2821" max="2821" width="20.26953125" style="44" customWidth="1"/>
-    <col min="2822" max="2822" width="13.90625" style="44" customWidth="1"/>
-    <col min="2823" max="2823" width="8.7265625" style="44"/>
-    <col min="2824" max="2824" width="17.90625" style="44" customWidth="1"/>
-    <col min="2825" max="2825" width="8.7265625" style="44"/>
-    <col min="2826" max="2826" width="53.6328125" style="44" customWidth="1"/>
-    <col min="2827" max="3071" width="8.7265625" style="44"/>
-    <col min="3072" max="3072" width="10.90625" style="44" customWidth="1"/>
-    <col min="3073" max="3073" width="22.26953125" style="44" customWidth="1"/>
-    <col min="3074" max="3074" width="8.7265625" style="44"/>
-    <col min="3075" max="3075" width="17" style="44" customWidth="1"/>
-    <col min="3076" max="3076" width="13.90625" style="44" customWidth="1"/>
-    <col min="3077" max="3077" width="20.26953125" style="44" customWidth="1"/>
-    <col min="3078" max="3078" width="13.90625" style="44" customWidth="1"/>
-    <col min="3079" max="3079" width="8.7265625" style="44"/>
-    <col min="3080" max="3080" width="17.90625" style="44" customWidth="1"/>
-    <col min="3081" max="3081" width="8.7265625" style="44"/>
-    <col min="3082" max="3082" width="53.6328125" style="44" customWidth="1"/>
-    <col min="3083" max="3327" width="8.7265625" style="44"/>
-    <col min="3328" max="3328" width="10.90625" style="44" customWidth="1"/>
-    <col min="3329" max="3329" width="22.26953125" style="44" customWidth="1"/>
-    <col min="3330" max="3330" width="8.7265625" style="44"/>
-    <col min="3331" max="3331" width="17" style="44" customWidth="1"/>
-    <col min="3332" max="3332" width="13.90625" style="44" customWidth="1"/>
-    <col min="3333" max="3333" width="20.26953125" style="44" customWidth="1"/>
-    <col min="3334" max="3334" width="13.90625" style="44" customWidth="1"/>
-    <col min="3335" max="3335" width="8.7265625" style="44"/>
-    <col min="3336" max="3336" width="17.90625" style="44" customWidth="1"/>
-    <col min="3337" max="3337" width="8.7265625" style="44"/>
-    <col min="3338" max="3338" width="53.6328125" style="44" customWidth="1"/>
-    <col min="3339" max="3583" width="8.7265625" style="44"/>
-    <col min="3584" max="3584" width="10.90625" style="44" customWidth="1"/>
-    <col min="3585" max="3585" width="22.26953125" style="44" customWidth="1"/>
-    <col min="3586" max="3586" width="8.7265625" style="44"/>
-    <col min="3587" max="3587" width="17" style="44" customWidth="1"/>
-    <col min="3588" max="3588" width="13.90625" style="44" customWidth="1"/>
-    <col min="3589" max="3589" width="20.26953125" style="44" customWidth="1"/>
-    <col min="3590" max="3590" width="13.90625" style="44" customWidth="1"/>
-    <col min="3591" max="3591" width="8.7265625" style="44"/>
-    <col min="3592" max="3592" width="17.90625" style="44" customWidth="1"/>
-    <col min="3593" max="3593" width="8.7265625" style="44"/>
-    <col min="3594" max="3594" width="53.6328125" style="44" customWidth="1"/>
-    <col min="3595" max="3839" width="8.7265625" style="44"/>
-    <col min="3840" max="3840" width="10.90625" style="44" customWidth="1"/>
-    <col min="3841" max="3841" width="22.26953125" style="44" customWidth="1"/>
-    <col min="3842" max="3842" width="8.7265625" style="44"/>
-    <col min="3843" max="3843" width="17" style="44" customWidth="1"/>
-    <col min="3844" max="3844" width="13.90625" style="44" customWidth="1"/>
-    <col min="3845" max="3845" width="20.26953125" style="44" customWidth="1"/>
-    <col min="3846" max="3846" width="13.90625" style="44" customWidth="1"/>
-    <col min="3847" max="3847" width="8.7265625" style="44"/>
-    <col min="3848" max="3848" width="17.90625" style="44" customWidth="1"/>
-    <col min="3849" max="3849" width="8.7265625" style="44"/>
-    <col min="3850" max="3850" width="53.6328125" style="44" customWidth="1"/>
-    <col min="3851" max="4095" width="8.7265625" style="44"/>
-    <col min="4096" max="4096" width="10.90625" style="44" customWidth="1"/>
-    <col min="4097" max="4097" width="22.26953125" style="44" customWidth="1"/>
-    <col min="4098" max="4098" width="8.7265625" style="44"/>
-    <col min="4099" max="4099" width="17" style="44" customWidth="1"/>
-    <col min="4100" max="4100" width="13.90625" style="44" customWidth="1"/>
-    <col min="4101" max="4101" width="20.26953125" style="44" customWidth="1"/>
-    <col min="4102" max="4102" width="13.90625" style="44" customWidth="1"/>
-    <col min="4103" max="4103" width="8.7265625" style="44"/>
-    <col min="4104" max="4104" width="17.90625" style="44" customWidth="1"/>
-    <col min="4105" max="4105" width="8.7265625" style="44"/>
-    <col min="4106" max="4106" width="53.6328125" style="44" customWidth="1"/>
-    <col min="4107" max="4351" width="8.7265625" style="44"/>
-    <col min="4352" max="4352" width="10.90625" style="44" customWidth="1"/>
-    <col min="4353" max="4353" width="22.26953125" style="44" customWidth="1"/>
-    <col min="4354" max="4354" width="8.7265625" style="44"/>
-    <col min="4355" max="4355" width="17" style="44" customWidth="1"/>
-    <col min="4356" max="4356" width="13.90625" style="44" customWidth="1"/>
-    <col min="4357" max="4357" width="20.26953125" style="44" customWidth="1"/>
-    <col min="4358" max="4358" width="13.90625" style="44" customWidth="1"/>
-    <col min="4359" max="4359" width="8.7265625" style="44"/>
-    <col min="4360" max="4360" width="17.90625" style="44" customWidth="1"/>
-    <col min="4361" max="4361" width="8.7265625" style="44"/>
-    <col min="4362" max="4362" width="53.6328125" style="44" customWidth="1"/>
-    <col min="4363" max="4607" width="8.7265625" style="44"/>
-    <col min="4608" max="4608" width="10.90625" style="44" customWidth="1"/>
-    <col min="4609" max="4609" width="22.26953125" style="44" customWidth="1"/>
-    <col min="4610" max="4610" width="8.7265625" style="44"/>
-    <col min="4611" max="4611" width="17" style="44" customWidth="1"/>
-    <col min="4612" max="4612" width="13.90625" style="44" customWidth="1"/>
-    <col min="4613" max="4613" width="20.26953125" style="44" customWidth="1"/>
-    <col min="4614" max="4614" width="13.90625" style="44" customWidth="1"/>
-    <col min="4615" max="4615" width="8.7265625" style="44"/>
-    <col min="4616" max="4616" width="17.90625" style="44" customWidth="1"/>
-    <col min="4617" max="4617" width="8.7265625" style="44"/>
-    <col min="4618" max="4618" width="53.6328125" style="44" customWidth="1"/>
-    <col min="4619" max="4863" width="8.7265625" style="44"/>
-    <col min="4864" max="4864" width="10.90625" style="44" customWidth="1"/>
-    <col min="4865" max="4865" width="22.26953125" style="44" customWidth="1"/>
-    <col min="4866" max="4866" width="8.7265625" style="44"/>
-    <col min="4867" max="4867" width="17" style="44" customWidth="1"/>
-    <col min="4868" max="4868" width="13.90625" style="44" customWidth="1"/>
-    <col min="4869" max="4869" width="20.26953125" style="44" customWidth="1"/>
-    <col min="4870" max="4870" width="13.90625" style="44" customWidth="1"/>
-    <col min="4871" max="4871" width="8.7265625" style="44"/>
-    <col min="4872" max="4872" width="17.90625" style="44" customWidth="1"/>
-    <col min="4873" max="4873" width="8.7265625" style="44"/>
-    <col min="4874" max="4874" width="53.6328125" style="44" customWidth="1"/>
-    <col min="4875" max="5119" width="8.7265625" style="44"/>
-    <col min="5120" max="5120" width="10.90625" style="44" customWidth="1"/>
-    <col min="5121" max="5121" width="22.26953125" style="44" customWidth="1"/>
-    <col min="5122" max="5122" width="8.7265625" style="44"/>
-    <col min="5123" max="5123" width="17" style="44" customWidth="1"/>
-    <col min="5124" max="5124" width="13.90625" style="44" customWidth="1"/>
-    <col min="5125" max="5125" width="20.26953125" style="44" customWidth="1"/>
-    <col min="5126" max="5126" width="13.90625" style="44" customWidth="1"/>
-    <col min="5127" max="5127" width="8.7265625" style="44"/>
-    <col min="5128" max="5128" width="17.90625" style="44" customWidth="1"/>
-    <col min="5129" max="5129" width="8.7265625" style="44"/>
-    <col min="5130" max="5130" width="53.6328125" style="44" customWidth="1"/>
-    <col min="5131" max="5375" width="8.7265625" style="44"/>
-    <col min="5376" max="5376" width="10.90625" style="44" customWidth="1"/>
-    <col min="5377" max="5377" width="22.26953125" style="44" customWidth="1"/>
-    <col min="5378" max="5378" width="8.7265625" style="44"/>
-    <col min="5379" max="5379" width="17" style="44" customWidth="1"/>
-    <col min="5380" max="5380" width="13.90625" style="44" customWidth="1"/>
-    <col min="5381" max="5381" width="20.26953125" style="44" customWidth="1"/>
-    <col min="5382" max="5382" width="13.90625" style="44" customWidth="1"/>
-    <col min="5383" max="5383" width="8.7265625" style="44"/>
-    <col min="5384" max="5384" width="17.90625" style="44" customWidth="1"/>
-    <col min="5385" max="5385" width="8.7265625" style="44"/>
-    <col min="5386" max="5386" width="53.6328125" style="44" customWidth="1"/>
-    <col min="5387" max="5631" width="8.7265625" style="44"/>
-    <col min="5632" max="5632" width="10.90625" style="44" customWidth="1"/>
-    <col min="5633" max="5633" width="22.26953125" style="44" customWidth="1"/>
-    <col min="5634" max="5634" width="8.7265625" style="44"/>
-    <col min="5635" max="5635" width="17" style="44" customWidth="1"/>
-    <col min="5636" max="5636" width="13.90625" style="44" customWidth="1"/>
-    <col min="5637" max="5637" width="20.26953125" style="44" customWidth="1"/>
-    <col min="5638" max="5638" width="13.90625" style="44" customWidth="1"/>
-    <col min="5639" max="5639" width="8.7265625" style="44"/>
-    <col min="5640" max="5640" width="17.90625" style="44" customWidth="1"/>
-    <col min="5641" max="5641" width="8.7265625" style="44"/>
-    <col min="5642" max="5642" width="53.6328125" style="44" customWidth="1"/>
-    <col min="5643" max="5887" width="8.7265625" style="44"/>
-    <col min="5888" max="5888" width="10.90625" style="44" customWidth="1"/>
-    <col min="5889" max="5889" width="22.26953125" style="44" customWidth="1"/>
-    <col min="5890" max="5890" width="8.7265625" style="44"/>
-    <col min="5891" max="5891" width="17" style="44" customWidth="1"/>
-    <col min="5892" max="5892" width="13.90625" style="44" customWidth="1"/>
-    <col min="5893" max="5893" width="20.26953125" style="44" customWidth="1"/>
-    <col min="5894" max="5894" width="13.90625" style="44" customWidth="1"/>
-    <col min="5895" max="5895" width="8.7265625" style="44"/>
-    <col min="5896" max="5896" width="17.90625" style="44" customWidth="1"/>
-    <col min="5897" max="5897" width="8.7265625" style="44"/>
-    <col min="5898" max="5898" width="53.6328125" style="44" customWidth="1"/>
-    <col min="5899" max="6143" width="8.7265625" style="44"/>
-    <col min="6144" max="6144" width="10.90625" style="44" customWidth="1"/>
-    <col min="6145" max="6145" width="22.26953125" style="44" customWidth="1"/>
-    <col min="6146" max="6146" width="8.7265625" style="44"/>
-    <col min="6147" max="6147" width="17" style="44" customWidth="1"/>
-    <col min="6148" max="6148" width="13.90625" style="44" customWidth="1"/>
-    <col min="6149" max="6149" width="20.26953125" style="44" customWidth="1"/>
-    <col min="6150" max="6150" width="13.90625" style="44" customWidth="1"/>
-    <col min="6151" max="6151" width="8.7265625" style="44"/>
-    <col min="6152" max="6152" width="17.90625" style="44" customWidth="1"/>
-    <col min="6153" max="6153" width="8.7265625" style="44"/>
-    <col min="6154" max="6154" width="53.6328125" style="44" customWidth="1"/>
-    <col min="6155" max="6399" width="8.7265625" style="44"/>
-    <col min="6400" max="6400" width="10.90625" style="44" customWidth="1"/>
-    <col min="6401" max="6401" width="22.26953125" style="44" customWidth="1"/>
-    <col min="6402" max="6402" width="8.7265625" style="44"/>
-    <col min="6403" max="6403" width="17" style="44" customWidth="1"/>
-    <col min="6404" max="6404" width="13.90625" style="44" customWidth="1"/>
-    <col min="6405" max="6405" width="20.26953125" style="44" customWidth="1"/>
-    <col min="6406" max="6406" width="13.90625" style="44" customWidth="1"/>
-    <col min="6407" max="6407" width="8.7265625" style="44"/>
-    <col min="6408" max="6408" width="17.90625" style="44" customWidth="1"/>
-    <col min="6409" max="6409" width="8.7265625" style="44"/>
-    <col min="6410" max="6410" width="53.6328125" style="44" customWidth="1"/>
-    <col min="6411" max="6655" width="8.7265625" style="44"/>
-    <col min="6656" max="6656" width="10.90625" style="44" customWidth="1"/>
-    <col min="6657" max="6657" width="22.26953125" style="44" customWidth="1"/>
-    <col min="6658" max="6658" width="8.7265625" style="44"/>
-    <col min="6659" max="6659" width="17" style="44" customWidth="1"/>
-    <col min="6660" max="6660" width="13.90625" style="44" customWidth="1"/>
-    <col min="6661" max="6661" width="20.26953125" style="44" customWidth="1"/>
-    <col min="6662" max="6662" width="13.90625" style="44" customWidth="1"/>
-    <col min="6663" max="6663" width="8.7265625" style="44"/>
-    <col min="6664" max="6664" width="17.90625" style="44" customWidth="1"/>
-    <col min="6665" max="6665" width="8.7265625" style="44"/>
-    <col min="6666" max="6666" width="53.6328125" style="44" customWidth="1"/>
-    <col min="6667" max="6911" width="8.7265625" style="44"/>
-    <col min="6912" max="6912" width="10.90625" style="44" customWidth="1"/>
-    <col min="6913" max="6913" width="22.26953125" style="44" customWidth="1"/>
-    <col min="6914" max="6914" width="8.7265625" style="44"/>
-    <col min="6915" max="6915" width="17" style="44" customWidth="1"/>
-    <col min="6916" max="6916" width="13.90625" style="44" customWidth="1"/>
-    <col min="6917" max="6917" width="20.26953125" style="44" customWidth="1"/>
-    <col min="6918" max="6918" width="13.90625" style="44" customWidth="1"/>
-    <col min="6919" max="6919" width="8.7265625" style="44"/>
-    <col min="6920" max="6920" width="17.90625" style="44" customWidth="1"/>
-    <col min="6921" max="6921" width="8.7265625" style="44"/>
-    <col min="6922" max="6922" width="53.6328125" style="44" customWidth="1"/>
-    <col min="6923" max="7167" width="8.7265625" style="44"/>
-    <col min="7168" max="7168" width="10.90625" style="44" customWidth="1"/>
-    <col min="7169" max="7169" width="22.26953125" style="44" customWidth="1"/>
-    <col min="7170" max="7170" width="8.7265625" style="44"/>
-    <col min="7171" max="7171" width="17" style="44" customWidth="1"/>
-    <col min="7172" max="7172" width="13.90625" style="44" customWidth="1"/>
-    <col min="7173" max="7173" width="20.26953125" style="44" customWidth="1"/>
-    <col min="7174" max="7174" width="13.90625" style="44" customWidth="1"/>
-    <col min="7175" max="7175" width="8.7265625" style="44"/>
-    <col min="7176" max="7176" width="17.90625" style="44" customWidth="1"/>
-    <col min="7177" max="7177" width="8.7265625" style="44"/>
-    <col min="7178" max="7178" width="53.6328125" style="44" customWidth="1"/>
-    <col min="7179" max="7423" width="8.7265625" style="44"/>
-    <col min="7424" max="7424" width="10.90625" style="44" customWidth="1"/>
-    <col min="7425" max="7425" width="22.26953125" style="44" customWidth="1"/>
-    <col min="7426" max="7426" width="8.7265625" style="44"/>
-    <col min="7427" max="7427" width="17" style="44" customWidth="1"/>
-    <col min="7428" max="7428" width="13.90625" style="44" customWidth="1"/>
-    <col min="7429" max="7429" width="20.26953125" style="44" customWidth="1"/>
-    <col min="7430" max="7430" width="13.90625" style="44" customWidth="1"/>
-    <col min="7431" max="7431" width="8.7265625" style="44"/>
-    <col min="7432" max="7432" width="17.90625" style="44" customWidth="1"/>
-    <col min="7433" max="7433" width="8.7265625" style="44"/>
-    <col min="7434" max="7434" width="53.6328125" style="44" customWidth="1"/>
-    <col min="7435" max="7679" width="8.7265625" style="44"/>
-    <col min="7680" max="7680" width="10.90625" style="44" customWidth="1"/>
-    <col min="7681" max="7681" width="22.26953125" style="44" customWidth="1"/>
-    <col min="7682" max="7682" width="8.7265625" style="44"/>
-    <col min="7683" max="7683" width="17" style="44" customWidth="1"/>
-    <col min="7684" max="7684" width="13.90625" style="44" customWidth="1"/>
-    <col min="7685" max="7685" width="20.26953125" style="44" customWidth="1"/>
-    <col min="7686" max="7686" width="13.90625" style="44" customWidth="1"/>
-    <col min="7687" max="7687" width="8.7265625" style="44"/>
-    <col min="7688" max="7688" width="17.90625" style="44" customWidth="1"/>
-    <col min="7689" max="7689" width="8.7265625" style="44"/>
-    <col min="7690" max="7690" width="53.6328125" style="44" customWidth="1"/>
-    <col min="7691" max="7935" width="8.7265625" style="44"/>
-    <col min="7936" max="7936" width="10.90625" style="44" customWidth="1"/>
-    <col min="7937" max="7937" width="22.26953125" style="44" customWidth="1"/>
-    <col min="7938" max="7938" width="8.7265625" style="44"/>
-    <col min="7939" max="7939" width="17" style="44" customWidth="1"/>
-    <col min="7940" max="7940" width="13.90625" style="44" customWidth="1"/>
-    <col min="7941" max="7941" width="20.26953125" style="44" customWidth="1"/>
-    <col min="7942" max="7942" width="13.90625" style="44" customWidth="1"/>
-    <col min="7943" max="7943" width="8.7265625" style="44"/>
-    <col min="7944" max="7944" width="17.90625" style="44" customWidth="1"/>
-    <col min="7945" max="7945" width="8.7265625" style="44"/>
-    <col min="7946" max="7946" width="53.6328125" style="44" customWidth="1"/>
-    <col min="7947" max="8191" width="8.7265625" style="44"/>
-    <col min="8192" max="8192" width="10.90625" style="44" customWidth="1"/>
-    <col min="8193" max="8193" width="22.26953125" style="44" customWidth="1"/>
-    <col min="8194" max="8194" width="8.7265625" style="44"/>
-    <col min="8195" max="8195" width="17" style="44" customWidth="1"/>
-    <col min="8196" max="8196" width="13.90625" style="44" customWidth="1"/>
-    <col min="8197" max="8197" width="20.26953125" style="44" customWidth="1"/>
-    <col min="8198" max="8198" width="13.90625" style="44" customWidth="1"/>
-    <col min="8199" max="8199" width="8.7265625" style="44"/>
-    <col min="8200" max="8200" width="17.90625" style="44" customWidth="1"/>
-    <col min="8201" max="8201" width="8.7265625" style="44"/>
-    <col min="8202" max="8202" width="53.6328125" style="44" customWidth="1"/>
-    <col min="8203" max="8447" width="8.7265625" style="44"/>
-    <col min="8448" max="8448" width="10.90625" style="44" customWidth="1"/>
-    <col min="8449" max="8449" width="22.26953125" style="44" customWidth="1"/>
-    <col min="8450" max="8450" width="8.7265625" style="44"/>
-    <col min="8451" max="8451" width="17" style="44" customWidth="1"/>
-    <col min="8452" max="8452" width="13.90625" style="44" customWidth="1"/>
-    <col min="8453" max="8453" width="20.26953125" style="44" customWidth="1"/>
-    <col min="8454" max="8454" width="13.90625" style="44" customWidth="1"/>
-    <col min="8455" max="8455" width="8.7265625" style="44"/>
-    <col min="8456" max="8456" width="17.90625" style="44" customWidth="1"/>
-    <col min="8457" max="8457" width="8.7265625" style="44"/>
-    <col min="8458" max="8458" width="53.6328125" style="44" customWidth="1"/>
-    <col min="8459" max="8703" width="8.7265625" style="44"/>
-    <col min="8704" max="8704" width="10.90625" style="44" customWidth="1"/>
-    <col min="8705" max="8705" width="22.26953125" style="44" customWidth="1"/>
-    <col min="8706" max="8706" width="8.7265625" style="44"/>
-    <col min="8707" max="8707" width="17" style="44" customWidth="1"/>
-    <col min="8708" max="8708" width="13.90625" style="44" customWidth="1"/>
-    <col min="8709" max="8709" width="20.26953125" style="44" customWidth="1"/>
-    <col min="8710" max="8710" width="13.90625" style="44" customWidth="1"/>
-    <col min="8711" max="8711" width="8.7265625" style="44"/>
-    <col min="8712" max="8712" width="17.90625" style="44" customWidth="1"/>
-    <col min="8713" max="8713" width="8.7265625" style="44"/>
-    <col min="8714" max="8714" width="53.6328125" style="44" customWidth="1"/>
-    <col min="8715" max="8959" width="8.7265625" style="44"/>
-    <col min="8960" max="8960" width="10.90625" style="44" customWidth="1"/>
-    <col min="8961" max="8961" width="22.26953125" style="44" customWidth="1"/>
-    <col min="8962" max="8962" width="8.7265625" style="44"/>
-    <col min="8963" max="8963" width="17" style="44" customWidth="1"/>
-    <col min="8964" max="8964" width="13.90625" style="44" customWidth="1"/>
-    <col min="8965" max="8965" width="20.26953125" style="44" customWidth="1"/>
-    <col min="8966" max="8966" width="13.90625" style="44" customWidth="1"/>
-    <col min="8967" max="8967" width="8.7265625" style="44"/>
-    <col min="8968" max="8968" width="17.90625" style="44" customWidth="1"/>
-    <col min="8969" max="8969" width="8.7265625" style="44"/>
-    <col min="8970" max="8970" width="53.6328125" style="44" customWidth="1"/>
-    <col min="8971" max="9215" width="8.7265625" style="44"/>
-    <col min="9216" max="9216" width="10.90625" style="44" customWidth="1"/>
-    <col min="9217" max="9217" width="22.26953125" style="44" customWidth="1"/>
-    <col min="9218" max="9218" width="8.7265625" style="44"/>
-    <col min="9219" max="9219" width="17" style="44" customWidth="1"/>
-    <col min="9220" max="9220" width="13.90625" style="44" customWidth="1"/>
-    <col min="9221" max="9221" width="20.26953125" style="44" customWidth="1"/>
-    <col min="9222" max="9222" width="13.90625" style="44" customWidth="1"/>
-    <col min="9223" max="9223" width="8.7265625" style="44"/>
-    <col min="9224" max="9224" width="17.90625" style="44" customWidth="1"/>
-    <col min="9225" max="9225" width="8.7265625" style="44"/>
-    <col min="9226" max="9226" width="53.6328125" style="44" customWidth="1"/>
-    <col min="9227" max="9471" width="8.7265625" style="44"/>
-    <col min="9472" max="9472" width="10.90625" style="44" customWidth="1"/>
-    <col min="9473" max="9473" width="22.26953125" style="44" customWidth="1"/>
-    <col min="9474" max="9474" width="8.7265625" style="44"/>
-    <col min="9475" max="9475" width="17" style="44" customWidth="1"/>
-    <col min="9476" max="9476" width="13.90625" style="44" customWidth="1"/>
-    <col min="9477" max="9477" width="20.26953125" style="44" customWidth="1"/>
-    <col min="9478" max="9478" width="13.90625" style="44" customWidth="1"/>
-    <col min="9479" max="9479" width="8.7265625" style="44"/>
-    <col min="9480" max="9480" width="17.90625" style="44" customWidth="1"/>
-    <col min="9481" max="9481" width="8.7265625" style="44"/>
-    <col min="9482" max="9482" width="53.6328125" style="44" customWidth="1"/>
-    <col min="9483" max="9727" width="8.7265625" style="44"/>
-    <col min="9728" max="9728" width="10.90625" style="44" customWidth="1"/>
-    <col min="9729" max="9729" width="22.26953125" style="44" customWidth="1"/>
-    <col min="9730" max="9730" width="8.7265625" style="44"/>
-    <col min="9731" max="9731" width="17" style="44" customWidth="1"/>
-    <col min="9732" max="9732" width="13.90625" style="44" customWidth="1"/>
-    <col min="9733" max="9733" width="20.26953125" style="44" customWidth="1"/>
-    <col min="9734" max="9734" width="13.90625" style="44" customWidth="1"/>
-    <col min="9735" max="9735" width="8.7265625" style="44"/>
-    <col min="9736" max="9736" width="17.90625" style="44" customWidth="1"/>
-    <col min="9737" max="9737" width="8.7265625" style="44"/>
-    <col min="9738" max="9738" width="53.6328125" style="44" customWidth="1"/>
-    <col min="9739" max="9983" width="8.7265625" style="44"/>
-    <col min="9984" max="9984" width="10.90625" style="44" customWidth="1"/>
-    <col min="9985" max="9985" width="22.26953125" style="44" customWidth="1"/>
-    <col min="9986" max="9986" width="8.7265625" style="44"/>
-    <col min="9987" max="9987" width="17" style="44" customWidth="1"/>
-    <col min="9988" max="9988" width="13.90625" style="44" customWidth="1"/>
-    <col min="9989" max="9989" width="20.26953125" style="44" customWidth="1"/>
-    <col min="9990" max="9990" width="13.90625" style="44" customWidth="1"/>
-    <col min="9991" max="9991" width="8.7265625" style="44"/>
-    <col min="9992" max="9992" width="17.90625" style="44" customWidth="1"/>
-    <col min="9993" max="9993" width="8.7265625" style="44"/>
-    <col min="9994" max="9994" width="53.6328125" style="44" customWidth="1"/>
-    <col min="9995" max="10239" width="8.7265625" style="44"/>
-    <col min="10240" max="10240" width="10.90625" style="44" customWidth="1"/>
-    <col min="10241" max="10241" width="22.26953125" style="44" customWidth="1"/>
-    <col min="10242" max="10242" width="8.7265625" style="44"/>
-    <col min="10243" max="10243" width="17" style="44" customWidth="1"/>
-    <col min="10244" max="10244" width="13.90625" style="44" customWidth="1"/>
-    <col min="10245" max="10245" width="20.26953125" style="44" customWidth="1"/>
-    <col min="10246" max="10246" width="13.90625" style="44" customWidth="1"/>
-    <col min="10247" max="10247" width="8.7265625" style="44"/>
-    <col min="10248" max="10248" width="17.90625" style="44" customWidth="1"/>
-    <col min="10249" max="10249" width="8.7265625" style="44"/>
-    <col min="10250" max="10250" width="53.6328125" style="44" customWidth="1"/>
-    <col min="10251" max="10495" width="8.7265625" style="44"/>
-    <col min="10496" max="10496" width="10.90625" style="44" customWidth="1"/>
-    <col min="10497" max="10497" width="22.26953125" style="44" customWidth="1"/>
-    <col min="10498" max="10498" width="8.7265625" style="44"/>
-    <col min="10499" max="10499" width="17" style="44" customWidth="1"/>
-    <col min="10500" max="10500" width="13.90625" style="44" customWidth="1"/>
-    <col min="10501" max="10501" width="20.26953125" style="44" customWidth="1"/>
-    <col min="10502" max="10502" width="13.90625" style="44" customWidth="1"/>
-    <col min="10503" max="10503" width="8.7265625" style="44"/>
-    <col min="10504" max="10504" width="17.90625" style="44" customWidth="1"/>
-    <col min="10505" max="10505" width="8.7265625" style="44"/>
-    <col min="10506" max="10506" width="53.6328125" style="44" customWidth="1"/>
-    <col min="10507" max="10751" width="8.7265625" style="44"/>
-    <col min="10752" max="10752" width="10.90625" style="44" customWidth="1"/>
-    <col min="10753" max="10753" width="22.26953125" style="44" customWidth="1"/>
-    <col min="10754" max="10754" width="8.7265625" style="44"/>
-    <col min="10755" max="10755" width="17" style="44" customWidth="1"/>
-    <col min="10756" max="10756" width="13.90625" style="44" customWidth="1"/>
-    <col min="10757" max="10757" width="20.26953125" style="44" customWidth="1"/>
-    <col min="10758" max="10758" width="13.90625" style="44" customWidth="1"/>
-    <col min="10759" max="10759" width="8.7265625" style="44"/>
-    <col min="10760" max="10760" width="17.90625" style="44" customWidth="1"/>
-    <col min="10761" max="10761" width="8.7265625" style="44"/>
-    <col min="10762" max="10762" width="53.6328125" style="44" customWidth="1"/>
-    <col min="10763" max="11007" width="8.7265625" style="44"/>
-    <col min="11008" max="11008" width="10.90625" style="44" customWidth="1"/>
-    <col min="11009" max="11009" width="22.26953125" style="44" customWidth="1"/>
-    <col min="11010" max="11010" width="8.7265625" style="44"/>
-    <col min="11011" max="11011" width="17" style="44" customWidth="1"/>
-    <col min="11012" max="11012" width="13.90625" style="44" customWidth="1"/>
-    <col min="11013" max="11013" width="20.26953125" style="44" customWidth="1"/>
-    <col min="11014" max="11014" width="13.90625" style="44" customWidth="1"/>
-    <col min="11015" max="11015" width="8.7265625" style="44"/>
-    <col min="11016" max="11016" width="17.90625" style="44" customWidth="1"/>
-    <col min="11017" max="11017" width="8.7265625" style="44"/>
-    <col min="11018" max="11018" width="53.6328125" style="44" customWidth="1"/>
-    <col min="11019" max="11263" width="8.7265625" style="44"/>
-    <col min="11264" max="11264" width="10.90625" style="44" customWidth="1"/>
-    <col min="11265" max="11265" width="22.26953125" style="44" customWidth="1"/>
-    <col min="11266" max="11266" width="8.7265625" style="44"/>
-    <col min="11267" max="11267" width="17" style="44" customWidth="1"/>
-    <col min="11268" max="11268" width="13.90625" style="44" customWidth="1"/>
-    <col min="11269" max="11269" width="20.26953125" style="44" customWidth="1"/>
-    <col min="11270" max="11270" width="13.90625" style="44" customWidth="1"/>
-    <col min="11271" max="11271" width="8.7265625" style="44"/>
-    <col min="11272" max="11272" width="17.90625" style="44" customWidth="1"/>
-    <col min="11273" max="11273" width="8.7265625" style="44"/>
-    <col min="11274" max="11274" width="53.6328125" style="44" customWidth="1"/>
-    <col min="11275" max="11519" width="8.7265625" style="44"/>
-    <col min="11520" max="11520" width="10.90625" style="44" customWidth="1"/>
-    <col min="11521" max="11521" width="22.26953125" style="44" customWidth="1"/>
-    <col min="11522" max="11522" width="8.7265625" style="44"/>
-    <col min="11523" max="11523" width="17" style="44" customWidth="1"/>
-    <col min="11524" max="11524" width="13.90625" style="44" customWidth="1"/>
-    <col min="11525" max="11525" width="20.26953125" style="44" customWidth="1"/>
-    <col min="11526" max="11526" width="13.90625" style="44" customWidth="1"/>
-    <col min="11527" max="11527" width="8.7265625" style="44"/>
-    <col min="11528" max="11528" width="17.90625" style="44" customWidth="1"/>
-    <col min="11529" max="11529" width="8.7265625" style="44"/>
-    <col min="11530" max="11530" width="53.6328125" style="44" customWidth="1"/>
-    <col min="11531" max="11775" width="8.7265625" style="44"/>
-    <col min="11776" max="11776" width="10.90625" style="44" customWidth="1"/>
-    <col min="11777" max="11777" width="22.26953125" style="44" customWidth="1"/>
-    <col min="11778" max="11778" width="8.7265625" style="44"/>
-    <col min="11779" max="11779" width="17" style="44" customWidth="1"/>
-    <col min="11780" max="11780" width="13.90625" style="44" customWidth="1"/>
-    <col min="11781" max="11781" width="20.26953125" style="44" customWidth="1"/>
-    <col min="11782" max="11782" width="13.90625" style="44" customWidth="1"/>
-    <col min="11783" max="11783" width="8.7265625" style="44"/>
-    <col min="11784" max="11784" width="17.90625" style="44" customWidth="1"/>
-    <col min="11785" max="11785" width="8.7265625" style="44"/>
-    <col min="11786" max="11786" width="53.6328125" style="44" customWidth="1"/>
-    <col min="11787" max="12031" width="8.7265625" style="44"/>
-    <col min="12032" max="12032" width="10.90625" style="44" customWidth="1"/>
-    <col min="12033" max="12033" width="22.26953125" style="44" customWidth="1"/>
-    <col min="12034" max="12034" width="8.7265625" style="44"/>
-    <col min="12035" max="12035" width="17" style="44" customWidth="1"/>
-    <col min="12036" max="12036" width="13.90625" style="44" customWidth="1"/>
-    <col min="12037" max="12037" width="20.26953125" style="44" customWidth="1"/>
-    <col min="12038" max="12038" width="13.90625" style="44" customWidth="1"/>
-    <col min="12039" max="12039" width="8.7265625" style="44"/>
-    <col min="12040" max="12040" width="17.90625" style="44" customWidth="1"/>
-    <col min="12041" max="12041" width="8.7265625" style="44"/>
-    <col min="12042" max="12042" width="53.6328125" style="44" customWidth="1"/>
-    <col min="12043" max="12287" width="8.7265625" style="44"/>
-    <col min="12288" max="12288" width="10.90625" style="44" customWidth="1"/>
-    <col min="12289" max="12289" width="22.26953125" style="44" customWidth="1"/>
-    <col min="12290" max="12290" width="8.7265625" style="44"/>
-    <col min="12291" max="12291" width="17" style="44" customWidth="1"/>
-    <col min="12292" max="12292" width="13.90625" style="44" customWidth="1"/>
-    <col min="12293" max="12293" width="20.26953125" style="44" customWidth="1"/>
-    <col min="12294" max="12294" width="13.90625" style="44" customWidth="1"/>
-    <col min="12295" max="12295" width="8.7265625" style="44"/>
-    <col min="12296" max="12296" width="17.90625" style="44" customWidth="1"/>
-    <col min="12297" max="12297" width="8.7265625" style="44"/>
-    <col min="12298" max="12298" width="53.6328125" style="44" customWidth="1"/>
-    <col min="12299" max="12543" width="8.7265625" style="44"/>
-    <col min="12544" max="12544" width="10.90625" style="44" customWidth="1"/>
-    <col min="12545" max="12545" width="22.26953125" style="44" customWidth="1"/>
-    <col min="12546" max="12546" width="8.7265625" style="44"/>
-    <col min="12547" max="12547" width="17" style="44" customWidth="1"/>
-    <col min="12548" max="12548" width="13.90625" style="44" customWidth="1"/>
-    <col min="12549" max="12549" width="20.26953125" style="44" customWidth="1"/>
-    <col min="12550" max="12550" width="13.90625" style="44" customWidth="1"/>
-    <col min="12551" max="12551" width="8.7265625" style="44"/>
-    <col min="12552" max="12552" width="17.90625" style="44" customWidth="1"/>
-    <col min="12553" max="12553" width="8.7265625" style="44"/>
-    <col min="12554" max="12554" width="53.6328125" style="44" customWidth="1"/>
-    <col min="12555" max="12799" width="8.7265625" style="44"/>
-    <col min="12800" max="12800" width="10.90625" style="44" customWidth="1"/>
-    <col min="12801" max="12801" width="22.26953125" style="44" customWidth="1"/>
-    <col min="12802" max="12802" width="8.7265625" style="44"/>
-    <col min="12803" max="12803" width="17" style="44" customWidth="1"/>
-    <col min="12804" max="12804" width="13.90625" style="44" customWidth="1"/>
-    <col min="12805" max="12805" width="20.26953125" style="44" customWidth="1"/>
-    <col min="12806" max="12806" width="13.90625" style="44" customWidth="1"/>
-    <col min="12807" max="12807" width="8.7265625" style="44"/>
-    <col min="12808" max="12808" width="17.90625" style="44" customWidth="1"/>
-    <col min="12809" max="12809" width="8.7265625" style="44"/>
-    <col min="12810" max="12810" width="53.6328125" style="44" customWidth="1"/>
-    <col min="12811" max="13055" width="8.7265625" style="44"/>
-    <col min="13056" max="13056" width="10.90625" style="44" customWidth="1"/>
-    <col min="13057" max="13057" width="22.26953125" style="44" customWidth="1"/>
-    <col min="13058" max="13058" width="8.7265625" style="44"/>
-    <col min="13059" max="13059" width="17" style="44" customWidth="1"/>
-    <col min="13060" max="13060" width="13.90625" style="44" customWidth="1"/>
-    <col min="13061" max="13061" width="20.26953125" style="44" customWidth="1"/>
-    <col min="13062" max="13062" width="13.90625" style="44" customWidth="1"/>
-    <col min="13063" max="13063" width="8.7265625" style="44"/>
-    <col min="13064" max="13064" width="17.90625" style="44" customWidth="1"/>
-    <col min="13065" max="13065" width="8.7265625" style="44"/>
-    <col min="13066" max="13066" width="53.6328125" style="44" customWidth="1"/>
-    <col min="13067" max="13311" width="8.7265625" style="44"/>
-    <col min="13312" max="13312" width="10.90625" style="44" customWidth="1"/>
-    <col min="13313" max="13313" width="22.26953125" style="44" customWidth="1"/>
-    <col min="13314" max="13314" width="8.7265625" style="44"/>
-    <col min="13315" max="13315" width="17" style="44" customWidth="1"/>
-    <col min="13316" max="13316" width="13.90625" style="44" customWidth="1"/>
-    <col min="13317" max="13317" width="20.26953125" style="44" customWidth="1"/>
-    <col min="13318" max="13318" width="13.90625" style="44" customWidth="1"/>
-    <col min="13319" max="13319" width="8.7265625" style="44"/>
-    <col min="13320" max="13320" width="17.90625" style="44" customWidth="1"/>
-    <col min="13321" max="13321" width="8.7265625" style="44"/>
-    <col min="13322" max="13322" width="53.6328125" style="44" customWidth="1"/>
-    <col min="13323" max="13567" width="8.7265625" style="44"/>
-    <col min="13568" max="13568" width="10.90625" style="44" customWidth="1"/>
-    <col min="13569" max="13569" width="22.26953125" style="44" customWidth="1"/>
-    <col min="13570" max="13570" width="8.7265625" style="44"/>
-    <col min="13571" max="13571" width="17" style="44" customWidth="1"/>
-    <col min="13572" max="13572" width="13.90625" style="44" customWidth="1"/>
-    <col min="13573" max="13573" width="20.26953125" style="44" customWidth="1"/>
-    <col min="13574" max="13574" width="13.90625" style="44" customWidth="1"/>
-    <col min="13575" max="13575" width="8.7265625" style="44"/>
-    <col min="13576" max="13576" width="17.90625" style="44" customWidth="1"/>
-    <col min="13577" max="13577" width="8.7265625" style="44"/>
-    <col min="13578" max="13578" width="53.6328125" style="44" customWidth="1"/>
-    <col min="13579" max="13823" width="8.7265625" style="44"/>
-    <col min="13824" max="13824" width="10.90625" style="44" customWidth="1"/>
-    <col min="13825" max="13825" width="22.26953125" style="44" customWidth="1"/>
-    <col min="13826" max="13826" width="8.7265625" style="44"/>
-    <col min="13827" max="13827" width="17" style="44" customWidth="1"/>
-    <col min="13828" max="13828" width="13.90625" style="44" customWidth="1"/>
-    <col min="13829" max="13829" width="20.26953125" style="44" customWidth="1"/>
-    <col min="13830" max="13830" width="13.90625" style="44" customWidth="1"/>
-    <col min="13831" max="13831" width="8.7265625" style="44"/>
-    <col min="13832" max="13832" width="17.90625" style="44" customWidth="1"/>
-    <col min="13833" max="13833" width="8.7265625" style="44"/>
-    <col min="13834" max="13834" width="53.6328125" style="44" customWidth="1"/>
-    <col min="13835" max="14079" width="8.7265625" style="44"/>
-    <col min="14080" max="14080" width="10.90625" style="44" customWidth="1"/>
-    <col min="14081" max="14081" width="22.26953125" style="44" customWidth="1"/>
-    <col min="14082" max="14082" width="8.7265625" style="44"/>
-    <col min="14083" max="14083" width="17" style="44" customWidth="1"/>
-    <col min="14084" max="14084" width="13.90625" style="44" customWidth="1"/>
-    <col min="14085" max="14085" width="20.26953125" style="44" customWidth="1"/>
-    <col min="14086" max="14086" width="13.90625" style="44" customWidth="1"/>
-    <col min="14087" max="14087" width="8.7265625" style="44"/>
-    <col min="14088" max="14088" width="17.90625" style="44" customWidth="1"/>
-    <col min="14089" max="14089" width="8.7265625" style="44"/>
-    <col min="14090" max="14090" width="53.6328125" style="44" customWidth="1"/>
-    <col min="14091" max="14335" width="8.7265625" style="44"/>
-    <col min="14336" max="14336" width="10.90625" style="44" customWidth="1"/>
-    <col min="14337" max="14337" width="22.26953125" style="44" customWidth="1"/>
-    <col min="14338" max="14338" width="8.7265625" style="44"/>
-    <col min="14339" max="14339" width="17" style="44" customWidth="1"/>
-    <col min="14340" max="14340" width="13.90625" style="44" customWidth="1"/>
-    <col min="14341" max="14341" width="20.26953125" style="44" customWidth="1"/>
-    <col min="14342" max="14342" width="13.90625" style="44" customWidth="1"/>
-    <col min="14343" max="14343" width="8.7265625" style="44"/>
-    <col min="14344" max="14344" width="17.90625" style="44" customWidth="1"/>
-    <col min="14345" max="14345" width="8.7265625" style="44"/>
-    <col min="14346" max="14346" width="53.6328125" style="44" customWidth="1"/>
-    <col min="14347" max="14591" width="8.7265625" style="44"/>
-    <col min="14592" max="14592" width="10.90625" style="44" customWidth="1"/>
-    <col min="14593" max="14593" width="22.26953125" style="44" customWidth="1"/>
-    <col min="14594" max="14594" width="8.7265625" style="44"/>
-    <col min="14595" max="14595" width="17" style="44" customWidth="1"/>
-    <col min="14596" max="14596" width="13.90625" style="44" customWidth="1"/>
-    <col min="14597" max="14597" width="20.26953125" style="44" customWidth="1"/>
-    <col min="14598" max="14598" width="13.90625" style="44" customWidth="1"/>
-    <col min="14599" max="14599" width="8.7265625" style="44"/>
-    <col min="14600" max="14600" width="17.90625" style="44" customWidth="1"/>
-    <col min="14601" max="14601" width="8.7265625" style="44"/>
-    <col min="14602" max="14602" width="53.6328125" style="44" customWidth="1"/>
-    <col min="14603" max="14847" width="8.7265625" style="44"/>
-    <col min="14848" max="14848" width="10.90625" style="44" customWidth="1"/>
-    <col min="14849" max="14849" width="22.26953125" style="44" customWidth="1"/>
-    <col min="14850" max="14850" width="8.7265625" style="44"/>
-    <col min="14851" max="14851" width="17" style="44" customWidth="1"/>
-    <col min="14852" max="14852" width="13.90625" style="44" customWidth="1"/>
-    <col min="14853" max="14853" width="20.26953125" style="44" customWidth="1"/>
-    <col min="14854" max="14854" width="13.90625" style="44" customWidth="1"/>
-    <col min="14855" max="14855" width="8.7265625" style="44"/>
-    <col min="14856" max="14856" width="17.90625" style="44" customWidth="1"/>
-    <col min="14857" max="14857" width="8.7265625" style="44"/>
-    <col min="14858" max="14858" width="53.6328125" style="44" customWidth="1"/>
-    <col min="14859" max="15103" width="8.7265625" style="44"/>
-    <col min="15104" max="15104" width="10.90625" style="44" customWidth="1"/>
-    <col min="15105" max="15105" width="22.26953125" style="44" customWidth="1"/>
-    <col min="15106" max="15106" width="8.7265625" style="44"/>
-    <col min="15107" max="15107" width="17" style="44" customWidth="1"/>
-    <col min="15108" max="15108" width="13.90625" style="44" customWidth="1"/>
-    <col min="15109" max="15109" width="20.26953125" style="44" customWidth="1"/>
-    <col min="15110" max="15110" width="13.90625" style="44" customWidth="1"/>
-    <col min="15111" max="15111" width="8.7265625" style="44"/>
-    <col min="15112" max="15112" width="17.90625" style="44" customWidth="1"/>
-    <col min="15113" max="15113" width="8.7265625" style="44"/>
-    <col min="15114" max="15114" width="53.6328125" style="44" customWidth="1"/>
-    <col min="15115" max="15359" width="8.7265625" style="44"/>
-    <col min="15360" max="15360" width="10.90625" style="44" customWidth="1"/>
-    <col min="15361" max="15361" width="22.26953125" style="44" customWidth="1"/>
-    <col min="15362" max="15362" width="8.7265625" style="44"/>
-    <col min="15363" max="15363" width="17" style="44" customWidth="1"/>
-    <col min="15364" max="15364" width="13.90625" style="44" customWidth="1"/>
-    <col min="15365" max="15365" width="20.26953125" style="44" customWidth="1"/>
-    <col min="15366" max="15366" width="13.90625" style="44" customWidth="1"/>
-    <col min="15367" max="15367" width="8.7265625" style="44"/>
-    <col min="15368" max="15368" width="17.90625" style="44" customWidth="1"/>
-    <col min="15369" max="15369" width="8.7265625" style="44"/>
-    <col min="15370" max="15370" width="53.6328125" style="44" customWidth="1"/>
-    <col min="15371" max="15615" width="8.7265625" style="44"/>
-    <col min="15616" max="15616" width="10.90625" style="44" customWidth="1"/>
-    <col min="15617" max="15617" width="22.26953125" style="44" customWidth="1"/>
-    <col min="15618" max="15618" width="8.7265625" style="44"/>
-    <col min="15619" max="15619" width="17" style="44" customWidth="1"/>
-    <col min="15620" max="15620" width="13.90625" style="44" customWidth="1"/>
-    <col min="15621" max="15621" width="20.26953125" style="44" customWidth="1"/>
-    <col min="15622" max="15622" width="13.90625" style="44" customWidth="1"/>
-    <col min="15623" max="15623" width="8.7265625" style="44"/>
-    <col min="15624" max="15624" width="17.90625" style="44" customWidth="1"/>
-    <col min="15625" max="15625" width="8.7265625" style="44"/>
-    <col min="15626" max="15626" width="53.6328125" style="44" customWidth="1"/>
-    <col min="15627" max="15871" width="8.7265625" style="44"/>
-    <col min="15872" max="15872" width="10.90625" style="44" customWidth="1"/>
-    <col min="15873" max="15873" width="22.26953125" style="44" customWidth="1"/>
-    <col min="15874" max="15874" width="8.7265625" style="44"/>
-    <col min="15875" max="15875" width="17" style="44" customWidth="1"/>
-    <col min="15876" max="15876" width="13.90625" style="44" customWidth="1"/>
-    <col min="15877" max="15877" width="20.26953125" style="44" customWidth="1"/>
-    <col min="15878" max="15878" width="13.90625" style="44" customWidth="1"/>
-    <col min="15879" max="15879" width="8.7265625" style="44"/>
-    <col min="15880" max="15880" width="17.90625" style="44" customWidth="1"/>
-    <col min="15881" max="15881" width="8.7265625" style="44"/>
-    <col min="15882" max="15882" width="53.6328125" style="44" customWidth="1"/>
-    <col min="15883" max="16127" width="8.7265625" style="44"/>
-    <col min="16128" max="16128" width="10.90625" style="44" customWidth="1"/>
-    <col min="16129" max="16129" width="22.26953125" style="44" customWidth="1"/>
-    <col min="16130" max="16130" width="8.7265625" style="44"/>
-    <col min="16131" max="16131" width="17" style="44" customWidth="1"/>
-    <col min="16132" max="16132" width="13.90625" style="44" customWidth="1"/>
-    <col min="16133" max="16133" width="20.26953125" style="44" customWidth="1"/>
-    <col min="16134" max="16134" width="13.90625" style="44" customWidth="1"/>
-    <col min="16135" max="16135" width="8.7265625" style="44"/>
-    <col min="16136" max="16136" width="17.90625" style="44" customWidth="1"/>
-    <col min="16137" max="16137" width="8.7265625" style="44"/>
-    <col min="16138" max="16138" width="53.6328125" style="44" customWidth="1"/>
-    <col min="16139" max="16384" width="8.7265625" style="44"/>
+    <col min="1" max="1" width="22.26953125" style="41" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="41"/>
+    <col min="3" max="3" width="17" style="41" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" style="41" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" style="41" customWidth="1"/>
+    <col min="6" max="6" width="13.90625" style="41" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="41"/>
+    <col min="8" max="8" width="17.90625" style="41" customWidth="1"/>
+    <col min="9" max="9" width="8.7265625" style="41"/>
+    <col min="10" max="10" width="53.6328125" style="41" customWidth="1"/>
+    <col min="11" max="255" width="8.7265625" style="41"/>
+    <col min="256" max="256" width="10.90625" style="41" customWidth="1"/>
+    <col min="257" max="257" width="22.26953125" style="41" customWidth="1"/>
+    <col min="258" max="258" width="8.7265625" style="41"/>
+    <col min="259" max="259" width="17" style="41" customWidth="1"/>
+    <col min="260" max="260" width="13.90625" style="41" customWidth="1"/>
+    <col min="261" max="261" width="20.26953125" style="41" customWidth="1"/>
+    <col min="262" max="262" width="13.90625" style="41" customWidth="1"/>
+    <col min="263" max="263" width="8.7265625" style="41"/>
+    <col min="264" max="264" width="17.90625" style="41" customWidth="1"/>
+    <col min="265" max="265" width="8.7265625" style="41"/>
+    <col min="266" max="266" width="53.6328125" style="41" customWidth="1"/>
+    <col min="267" max="511" width="8.7265625" style="41"/>
+    <col min="512" max="512" width="10.90625" style="41" customWidth="1"/>
+    <col min="513" max="513" width="22.26953125" style="41" customWidth="1"/>
+    <col min="514" max="514" width="8.7265625" style="41"/>
+    <col min="515" max="515" width="17" style="41" customWidth="1"/>
+    <col min="516" max="516" width="13.90625" style="41" customWidth="1"/>
+    <col min="517" max="517" width="20.26953125" style="41" customWidth="1"/>
+    <col min="518" max="518" width="13.90625" style="41" customWidth="1"/>
+    <col min="519" max="519" width="8.7265625" style="41"/>
+    <col min="520" max="520" width="17.90625" style="41" customWidth="1"/>
+    <col min="521" max="521" width="8.7265625" style="41"/>
+    <col min="522" max="522" width="53.6328125" style="41" customWidth="1"/>
+    <col min="523" max="767" width="8.7265625" style="41"/>
+    <col min="768" max="768" width="10.90625" style="41" customWidth="1"/>
+    <col min="769" max="769" width="22.26953125" style="41" customWidth="1"/>
+    <col min="770" max="770" width="8.7265625" style="41"/>
+    <col min="771" max="771" width="17" style="41" customWidth="1"/>
+    <col min="772" max="772" width="13.90625" style="41" customWidth="1"/>
+    <col min="773" max="773" width="20.26953125" style="41" customWidth="1"/>
+    <col min="774" max="774" width="13.90625" style="41" customWidth="1"/>
+    <col min="775" max="775" width="8.7265625" style="41"/>
+    <col min="776" max="776" width="17.90625" style="41" customWidth="1"/>
+    <col min="777" max="777" width="8.7265625" style="41"/>
+    <col min="778" max="778" width="53.6328125" style="41" customWidth="1"/>
+    <col min="779" max="1023" width="8.7265625" style="41"/>
+    <col min="1024" max="1024" width="10.90625" style="41" customWidth="1"/>
+    <col min="1025" max="1025" width="22.26953125" style="41" customWidth="1"/>
+    <col min="1026" max="1026" width="8.7265625" style="41"/>
+    <col min="1027" max="1027" width="17" style="41" customWidth="1"/>
+    <col min="1028" max="1028" width="13.90625" style="41" customWidth="1"/>
+    <col min="1029" max="1029" width="20.26953125" style="41" customWidth="1"/>
+    <col min="1030" max="1030" width="13.90625" style="41" customWidth="1"/>
+    <col min="1031" max="1031" width="8.7265625" style="41"/>
+    <col min="1032" max="1032" width="17.90625" style="41" customWidth="1"/>
+    <col min="1033" max="1033" width="8.7265625" style="41"/>
+    <col min="1034" max="1034" width="53.6328125" style="41" customWidth="1"/>
+    <col min="1035" max="1279" width="8.7265625" style="41"/>
+    <col min="1280" max="1280" width="10.90625" style="41" customWidth="1"/>
+    <col min="1281" max="1281" width="22.26953125" style="41" customWidth="1"/>
+    <col min="1282" max="1282" width="8.7265625" style="41"/>
+    <col min="1283" max="1283" width="17" style="41" customWidth="1"/>
+    <col min="1284" max="1284" width="13.90625" style="41" customWidth="1"/>
+    <col min="1285" max="1285" width="20.26953125" style="41" customWidth="1"/>
+    <col min="1286" max="1286" width="13.90625" style="41" customWidth="1"/>
+    <col min="1287" max="1287" width="8.7265625" style="41"/>
+    <col min="1288" max="1288" width="17.90625" style="41" customWidth="1"/>
+    <col min="1289" max="1289" width="8.7265625" style="41"/>
+    <col min="1290" max="1290" width="53.6328125" style="41" customWidth="1"/>
+    <col min="1291" max="1535" width="8.7265625" style="41"/>
+    <col min="1536" max="1536" width="10.90625" style="41" customWidth="1"/>
+    <col min="1537" max="1537" width="22.26953125" style="41" customWidth="1"/>
+    <col min="1538" max="1538" width="8.7265625" style="41"/>
+    <col min="1539" max="1539" width="17" style="41" customWidth="1"/>
+    <col min="1540" max="1540" width="13.90625" style="41" customWidth="1"/>
+    <col min="1541" max="1541" width="20.26953125" style="41" customWidth="1"/>
+    <col min="1542" max="1542" width="13.90625" style="41" customWidth="1"/>
+    <col min="1543" max="1543" width="8.7265625" style="41"/>
+    <col min="1544" max="1544" width="17.90625" style="41" customWidth="1"/>
+    <col min="1545" max="1545" width="8.7265625" style="41"/>
+    <col min="1546" max="1546" width="53.6328125" style="41" customWidth="1"/>
+    <col min="1547" max="1791" width="8.7265625" style="41"/>
+    <col min="1792" max="1792" width="10.90625" style="41" customWidth="1"/>
+    <col min="1793" max="1793" width="22.26953125" style="41" customWidth="1"/>
+    <col min="1794" max="1794" width="8.7265625" style="41"/>
+    <col min="1795" max="1795" width="17" style="41" customWidth="1"/>
+    <col min="1796" max="1796" width="13.90625" style="41" customWidth="1"/>
+    <col min="1797" max="1797" width="20.26953125" style="41" customWidth="1"/>
+    <col min="1798" max="1798" width="13.90625" style="41" customWidth="1"/>
+    <col min="1799" max="1799" width="8.7265625" style="41"/>
+    <col min="1800" max="1800" width="17.90625" style="41" customWidth="1"/>
+    <col min="1801" max="1801" width="8.7265625" style="41"/>
+    <col min="1802" max="1802" width="53.6328125" style="41" customWidth="1"/>
+    <col min="1803" max="2047" width="8.7265625" style="41"/>
+    <col min="2048" max="2048" width="10.90625" style="41" customWidth="1"/>
+    <col min="2049" max="2049" width="22.26953125" style="41" customWidth="1"/>
+    <col min="2050" max="2050" width="8.7265625" style="41"/>
+    <col min="2051" max="2051" width="17" style="41" customWidth="1"/>
+    <col min="2052" max="2052" width="13.90625" style="41" customWidth="1"/>
+    <col min="2053" max="2053" width="20.26953125" style="41" customWidth="1"/>
+    <col min="2054" max="2054" width="13.90625" style="41" customWidth="1"/>
+    <col min="2055" max="2055" width="8.7265625" style="41"/>
+    <col min="2056" max="2056" width="17.90625" style="41" customWidth="1"/>
+    <col min="2057" max="2057" width="8.7265625" style="41"/>
+    <col min="2058" max="2058" width="53.6328125" style="41" customWidth="1"/>
+    <col min="2059" max="2303" width="8.7265625" style="41"/>
+    <col min="2304" max="2304" width="10.90625" style="41" customWidth="1"/>
+    <col min="2305" max="2305" width="22.26953125" style="41" customWidth="1"/>
+    <col min="2306" max="2306" width="8.7265625" style="41"/>
+    <col min="2307" max="2307" width="17" style="41" customWidth="1"/>
+    <col min="2308" max="2308" width="13.90625" style="41" customWidth="1"/>
+    <col min="2309" max="2309" width="20.26953125" style="41" customWidth="1"/>
+    <col min="2310" max="2310" width="13.90625" style="41" customWidth="1"/>
+    <col min="2311" max="2311" width="8.7265625" style="41"/>
+    <col min="2312" max="2312" width="17.90625" style="41" customWidth="1"/>
+    <col min="2313" max="2313" width="8.7265625" style="41"/>
+    <col min="2314" max="2314" width="53.6328125" style="41" customWidth="1"/>
+    <col min="2315" max="2559" width="8.7265625" style="41"/>
+    <col min="2560" max="2560" width="10.90625" style="41" customWidth="1"/>
+    <col min="2561" max="2561" width="22.26953125" style="41" customWidth="1"/>
+    <col min="2562" max="2562" width="8.7265625" style="41"/>
+    <col min="2563" max="2563" width="17" style="41" customWidth="1"/>
+    <col min="2564" max="2564" width="13.90625" style="41" customWidth="1"/>
+    <col min="2565" max="2565" width="20.26953125" style="41" customWidth="1"/>
+    <col min="2566" max="2566" width="13.90625" style="41" customWidth="1"/>
+    <col min="2567" max="2567" width="8.7265625" style="41"/>
+    <col min="2568" max="2568" width="17.90625" style="41" customWidth="1"/>
+    <col min="2569" max="2569" width="8.7265625" style="41"/>
+    <col min="2570" max="2570" width="53.6328125" style="41" customWidth="1"/>
+    <col min="2571" max="2815" width="8.7265625" style="41"/>
+    <col min="2816" max="2816" width="10.90625" style="41" customWidth="1"/>
+    <col min="2817" max="2817" width="22.26953125" style="41" customWidth="1"/>
+    <col min="2818" max="2818" width="8.7265625" style="41"/>
+    <col min="2819" max="2819" width="17" style="41" customWidth="1"/>
+    <col min="2820" max="2820" width="13.90625" style="41" customWidth="1"/>
+    <col min="2821" max="2821" width="20.26953125" style="41" customWidth="1"/>
+    <col min="2822" max="2822" width="13.90625" style="41" customWidth="1"/>
+    <col min="2823" max="2823" width="8.7265625" style="41"/>
+    <col min="2824" max="2824" width="17.90625" style="41" customWidth="1"/>
+    <col min="2825" max="2825" width="8.7265625" style="41"/>
+    <col min="2826" max="2826" width="53.6328125" style="41" customWidth="1"/>
+    <col min="2827" max="3071" width="8.7265625" style="41"/>
+    <col min="3072" max="3072" width="10.90625" style="41" customWidth="1"/>
+    <col min="3073" max="3073" width="22.26953125" style="41" customWidth="1"/>
+    <col min="3074" max="3074" width="8.7265625" style="41"/>
+    <col min="3075" max="3075" width="17" style="41" customWidth="1"/>
+    <col min="3076" max="3076" width="13.90625" style="41" customWidth="1"/>
+    <col min="3077" max="3077" width="20.26953125" style="41" customWidth="1"/>
+    <col min="3078" max="3078" width="13.90625" style="41" customWidth="1"/>
+    <col min="3079" max="3079" width="8.7265625" style="41"/>
+    <col min="3080" max="3080" width="17.90625" style="41" customWidth="1"/>
+    <col min="3081" max="3081" width="8.7265625" style="41"/>
+    <col min="3082" max="3082" width="53.6328125" style="41" customWidth="1"/>
+    <col min="3083" max="3327" width="8.7265625" style="41"/>
+    <col min="3328" max="3328" width="10.90625" style="41" customWidth="1"/>
+    <col min="3329" max="3329" width="22.26953125" style="41" customWidth="1"/>
+    <col min="3330" max="3330" width="8.7265625" style="41"/>
+    <col min="3331" max="3331" width="17" style="41" customWidth="1"/>
+    <col min="3332" max="3332" width="13.90625" style="41" customWidth="1"/>
+    <col min="3333" max="3333" width="20.26953125" style="41" customWidth="1"/>
+    <col min="3334" max="3334" width="13.90625" style="41" customWidth="1"/>
+    <col min="3335" max="3335" width="8.7265625" style="41"/>
+    <col min="3336" max="3336" width="17.90625" style="41" customWidth="1"/>
+    <col min="3337" max="3337" width="8.7265625" style="41"/>
+    <col min="3338" max="3338" width="53.6328125" style="41" customWidth="1"/>
+    <col min="3339" max="3583" width="8.7265625" style="41"/>
+    <col min="3584" max="3584" width="10.90625" style="41" customWidth="1"/>
+    <col min="3585" max="3585" width="22.26953125" style="41" customWidth="1"/>
+    <col min="3586" max="3586" width="8.7265625" style="41"/>
+    <col min="3587" max="3587" width="17" style="41" customWidth="1"/>
+    <col min="3588" max="3588" width="13.90625" style="41" customWidth="1"/>
+    <col min="3589" max="3589" width="20.26953125" style="41" customWidth="1"/>
+    <col min="3590" max="3590" width="13.90625" style="41" customWidth="1"/>
+    <col min="3591" max="3591" width="8.7265625" style="41"/>
+    <col min="3592" max="3592" width="17.90625" style="41" customWidth="1"/>
+    <col min="3593" max="3593" width="8.7265625" style="41"/>
+    <col min="3594" max="3594" width="53.6328125" style="41" customWidth="1"/>
+    <col min="3595" max="3839" width="8.7265625" style="41"/>
+    <col min="3840" max="3840" width="10.90625" style="41" customWidth="1"/>
+    <col min="3841" max="3841" width="22.26953125" style="41" customWidth="1"/>
+    <col min="3842" max="3842" width="8.7265625" style="41"/>
+    <col min="3843" max="3843" width="17" style="41" customWidth="1"/>
+    <col min="3844" max="3844" width="13.90625" style="41" customWidth="1"/>
+    <col min="3845" max="3845" width="20.26953125" style="41" customWidth="1"/>
+    <col min="3846" max="3846" width="13.90625" style="41" customWidth="1"/>
+    <col min="3847" max="3847" width="8.7265625" style="41"/>
+    <col min="3848" max="3848" width="17.90625" style="41" customWidth="1"/>
+    <col min="3849" max="3849" width="8.7265625" style="41"/>
+    <col min="3850" max="3850" width="53.6328125" style="41" customWidth="1"/>
+    <col min="3851" max="4095" width="8.7265625" style="41"/>
+    <col min="4096" max="4096" width="10.90625" style="41" customWidth="1"/>
+    <col min="4097" max="4097" width="22.26953125" style="41" customWidth="1"/>
+    <col min="4098" max="4098" width="8.7265625" style="41"/>
+    <col min="4099" max="4099" width="17" style="41" customWidth="1"/>
+    <col min="4100" max="4100" width="13.90625" style="41" customWidth="1"/>
+    <col min="4101" max="4101" width="20.26953125" style="41" customWidth="1"/>
+    <col min="4102" max="4102" width="13.90625" style="41" customWidth="1"/>
+    <col min="4103" max="4103" width="8.7265625" style="41"/>
+    <col min="4104" max="4104" width="17.90625" style="41" customWidth="1"/>
+    <col min="4105" max="4105" width="8.7265625" style="41"/>
+    <col min="4106" max="4106" width="53.6328125" style="41" customWidth="1"/>
+    <col min="4107" max="4351" width="8.7265625" style="41"/>
+    <col min="4352" max="4352" width="10.90625" style="41" customWidth="1"/>
+    <col min="4353" max="4353" width="22.26953125" style="41" customWidth="1"/>
+    <col min="4354" max="4354" width="8.7265625" style="41"/>
+    <col min="4355" max="4355" width="17" style="41" customWidth="1"/>
+    <col min="4356" max="4356" width="13.90625" style="41" customWidth="1"/>
+    <col min="4357" max="4357" width="20.26953125" style="41" customWidth="1"/>
+    <col min="4358" max="4358" width="13.90625" style="41" customWidth="1"/>
+    <col min="4359" max="4359" width="8.7265625" style="41"/>
+    <col min="4360" max="4360" width="17.90625" style="41" customWidth="1"/>
+    <col min="4361" max="4361" width="8.7265625" style="41"/>
+    <col min="4362" max="4362" width="53.6328125" style="41" customWidth="1"/>
+    <col min="4363" max="4607" width="8.7265625" style="41"/>
+    <col min="4608" max="4608" width="10.90625" style="41" customWidth="1"/>
+    <col min="4609" max="4609" width="22.26953125" style="41" customWidth="1"/>
+    <col min="4610" max="4610" width="8.7265625" style="41"/>
+    <col min="4611" max="4611" width="17" style="41" customWidth="1"/>
+    <col min="4612" max="4612" width="13.90625" style="41" customWidth="1"/>
+    <col min="4613" max="4613" width="20.26953125" style="41" customWidth="1"/>
+    <col min="4614" max="4614" width="13.90625" style="41" customWidth="1"/>
+    <col min="4615" max="4615" width="8.7265625" style="41"/>
+    <col min="4616" max="4616" width="17.90625" style="41" customWidth="1"/>
+    <col min="4617" max="4617" width="8.7265625" style="41"/>
+    <col min="4618" max="4618" width="53.6328125" style="41" customWidth="1"/>
+    <col min="4619" max="4863" width="8.7265625" style="41"/>
+    <col min="4864" max="4864" width="10.90625" style="41" customWidth="1"/>
+    <col min="4865" max="4865" width="22.26953125" style="41" customWidth="1"/>
+    <col min="4866" max="4866" width="8.7265625" style="41"/>
+    <col min="4867" max="4867" width="17" style="41" customWidth="1"/>
+    <col min="4868" max="4868" width="13.90625" style="41" customWidth="1"/>
+    <col min="4869" max="4869" width="20.26953125" style="41" customWidth="1"/>
+    <col min="4870" max="4870" width="13.90625" style="41" customWidth="1"/>
+    <col min="4871" max="4871" width="8.7265625" style="41"/>
+    <col min="4872" max="4872" width="17.90625" style="41" customWidth="1"/>
+    <col min="4873" max="4873" width="8.7265625" style="41"/>
+    <col min="4874" max="4874" width="53.6328125" style="41" customWidth="1"/>
+    <col min="4875" max="5119" width="8.7265625" style="41"/>
+    <col min="5120" max="5120" width="10.90625" style="41" customWidth="1"/>
+    <col min="5121" max="5121" width="22.26953125" style="41" customWidth="1"/>
+    <col min="5122" max="5122" width="8.7265625" style="41"/>
+    <col min="5123" max="5123" width="17" style="41" customWidth="1"/>
+    <col min="5124" max="5124" width="13.90625" style="41" customWidth="1"/>
+    <col min="5125" max="5125" width="20.26953125" style="41" customWidth="1"/>
+    <col min="5126" max="5126" width="13.90625" style="41" customWidth="1"/>
+    <col min="5127" max="5127" width="8.7265625" style="41"/>
+    <col min="5128" max="5128" width="17.90625" style="41" customWidth="1"/>
+    <col min="5129" max="5129" width="8.7265625" style="41"/>
+    <col min="5130" max="5130" width="53.6328125" style="41" customWidth="1"/>
+    <col min="5131" max="5375" width="8.7265625" style="41"/>
+    <col min="5376" max="5376" width="10.90625" style="41" customWidth="1"/>
+    <col min="5377" max="5377" width="22.26953125" style="41" customWidth="1"/>
+    <col min="5378" max="5378" width="8.7265625" style="41"/>
+    <col min="5379" max="5379" width="17" style="41" customWidth="1"/>
+    <col min="5380" max="5380" width="13.90625" style="41" customWidth="1"/>
+    <col min="5381" max="5381" width="20.26953125" style="41" customWidth="1"/>
+    <col min="5382" max="5382" width="13.90625" style="41" customWidth="1"/>
+    <col min="5383" max="5383" width="8.7265625" style="41"/>
+    <col min="5384" max="5384" width="17.90625" style="41" customWidth="1"/>
+    <col min="5385" max="5385" width="8.7265625" style="41"/>
+    <col min="5386" max="5386" width="53.6328125" style="41" customWidth="1"/>
+    <col min="5387" max="5631" width="8.7265625" style="41"/>
+    <col min="5632" max="5632" width="10.90625" style="41" customWidth="1"/>
+    <col min="5633" max="5633" width="22.26953125" style="41" customWidth="1"/>
+    <col min="5634" max="5634" width="8.7265625" style="41"/>
+    <col min="5635" max="5635" width="17" style="41" customWidth="1"/>
+    <col min="5636" max="5636" width="13.90625" style="41" customWidth="1"/>
+    <col min="5637" max="5637" width="20.26953125" style="41" customWidth="1"/>
+    <col min="5638" max="5638" width="13.90625" style="41" customWidth="1"/>
+    <col min="5639" max="5639" width="8.7265625" style="41"/>
+    <col min="5640" max="5640" width="17.90625" style="41" customWidth="1"/>
+    <col min="5641" max="5641" width="8.7265625" style="41"/>
+    <col min="5642" max="5642" width="53.6328125" style="41" customWidth="1"/>
+    <col min="5643" max="5887" width="8.7265625" style="41"/>
+    <col min="5888" max="5888" width="10.90625" style="41" customWidth="1"/>
+    <col min="5889" max="5889" width="22.26953125" style="41" customWidth="1"/>
+    <col min="5890" max="5890" width="8.7265625" style="41"/>
+    <col min="5891" max="5891" width="17" style="41" customWidth="1"/>
+    <col min="5892" max="5892" width="13.90625" style="41" customWidth="1"/>
+    <col min="5893" max="5893" width="20.26953125" style="41" customWidth="1"/>
+    <col min="5894" max="5894" width="13.90625" style="41" customWidth="1"/>
+    <col min="5895" max="5895" width="8.7265625" style="41"/>
+    <col min="5896" max="5896" width="17.90625" style="41" customWidth="1"/>
+    <col min="5897" max="5897" width="8.7265625" style="41"/>
+    <col min="5898" max="5898" width="53.6328125" style="41" customWidth="1"/>
+    <col min="5899" max="6143" width="8.7265625" style="41"/>
+    <col min="6144" max="6144" width="10.90625" style="41" customWidth="1"/>
+    <col min="6145" max="6145" width="22.26953125" style="41" customWidth="1"/>
+    <col min="6146" max="6146" width="8.7265625" style="41"/>
+    <col min="6147" max="6147" width="17" style="41" customWidth="1"/>
+    <col min="6148" max="6148" width="13.90625" style="41" customWidth="1"/>
+    <col min="6149" max="6149" width="20.26953125" style="41" customWidth="1"/>
+    <col min="6150" max="6150" width="13.90625" style="41" customWidth="1"/>
+    <col min="6151" max="6151" width="8.7265625" style="41"/>
+    <col min="6152" max="6152" width="17.90625" style="41" customWidth="1"/>
+    <col min="6153" max="6153" width="8.7265625" style="41"/>
+    <col min="6154" max="6154" width="53.6328125" style="41" customWidth="1"/>
+    <col min="6155" max="6399" width="8.7265625" style="41"/>
+    <col min="6400" max="6400" width="10.90625" style="41" customWidth="1"/>
+    <col min="6401" max="6401" width="22.26953125" style="41" customWidth="1"/>
+    <col min="6402" max="6402" width="8.7265625" style="41"/>
+    <col min="6403" max="6403" width="17" style="41" customWidth="1"/>
+    <col min="6404" max="6404" width="13.90625" style="41" customWidth="1"/>
+    <col min="6405" max="6405" width="20.26953125" style="41" customWidth="1"/>
+    <col min="6406" max="6406" width="13.90625" style="41" customWidth="1"/>
+    <col min="6407" max="6407" width="8.7265625" style="41"/>
+    <col min="6408" max="6408" width="17.90625" style="41" customWidth="1"/>
+    <col min="6409" max="6409" width="8.7265625" style="41"/>
+    <col min="6410" max="6410" width="53.6328125" style="41" customWidth="1"/>
+    <col min="6411" max="6655" width="8.7265625" style="41"/>
+    <col min="6656" max="6656" width="10.90625" style="41" customWidth="1"/>
+    <col min="6657" max="6657" width="22.26953125" style="41" customWidth="1"/>
+    <col min="6658" max="6658" width="8.7265625" style="41"/>
+    <col min="6659" max="6659" width="17" style="41" customWidth="1"/>
+    <col min="6660" max="6660" width="13.90625" style="41" customWidth="1"/>
+    <col min="6661" max="6661" width="20.26953125" style="41" customWidth="1"/>
+    <col min="6662" max="6662" width="13.90625" style="41" customWidth="1"/>
+    <col min="6663" max="6663" width="8.7265625" style="41"/>
+    <col min="6664" max="6664" width="17.90625" style="41" customWidth="1"/>
+    <col min="6665" max="6665" width="8.7265625" style="41"/>
+    <col min="6666" max="6666" width="53.6328125" style="41" customWidth="1"/>
+    <col min="6667" max="6911" width="8.7265625" style="41"/>
+    <col min="6912" max="6912" width="10.90625" style="41" customWidth="1"/>
+    <col min="6913" max="6913" width="22.26953125" style="41" customWidth="1"/>
+    <col min="6914" max="6914" width="8.7265625" style="41"/>
+    <col min="6915" max="6915" width="17" style="41" customWidth="1"/>
+    <col min="6916" max="6916" width="13.90625" style="41" customWidth="1"/>
+    <col min="6917" max="6917" width="20.26953125" style="41" customWidth="1"/>
+    <col min="6918" max="6918" width="13.90625" style="41" customWidth="1"/>
+    <col min="6919" max="6919" width="8.7265625" style="41"/>
+    <col min="6920" max="6920" width="17.90625" style="41" customWidth="1"/>
+    <col min="6921" max="6921" width="8.7265625" style="41"/>
+    <col min="6922" max="6922" width="53.6328125" style="41" customWidth="1"/>
+    <col min="6923" max="7167" width="8.7265625" style="41"/>
+    <col min="7168" max="7168" width="10.90625" style="41" customWidth="1"/>
+    <col min="7169" max="7169" width="22.26953125" style="41" customWidth="1"/>
+    <col min="7170" max="7170" width="8.7265625" style="41"/>
+    <col min="7171" max="7171" width="17" style="41" customWidth="1"/>
+    <col min="7172" max="7172" width="13.90625" style="41" customWidth="1"/>
+    <col min="7173" max="7173" width="20.26953125" style="41" customWidth="1"/>
+    <col min="7174" max="7174" width="13.90625" style="41" customWidth="1"/>
+    <col min="7175" max="7175" width="8.7265625" style="41"/>
+    <col min="7176" max="7176" width="17.90625" style="41" customWidth="1"/>
+    <col min="7177" max="7177" width="8.7265625" style="41"/>
+    <col min="7178" max="7178" width="53.6328125" style="41" customWidth="1"/>
+    <col min="7179" max="7423" width="8.7265625" style="41"/>
+    <col min="7424" max="7424" width="10.90625" style="41" customWidth="1"/>
+    <col min="7425" max="7425" width="22.26953125" style="41" customWidth="1"/>
+    <col min="7426" max="7426" width="8.7265625" style="41"/>
+    <col min="7427" max="7427" width="17" style="41" customWidth="1"/>
+    <col min="7428" max="7428" width="13.90625" style="41" customWidth="1"/>
+    <col min="7429" max="7429" width="20.26953125" style="41" customWidth="1"/>
+    <col min="7430" max="7430" width="13.90625" style="41" customWidth="1"/>
+    <col min="7431" max="7431" width="8.7265625" style="41"/>
+    <col min="7432" max="7432" width="17.90625" style="41" customWidth="1"/>
+    <col min="7433" max="7433" width="8.7265625" style="41"/>
+    <col min="7434" max="7434" width="53.6328125" style="41" customWidth="1"/>
+    <col min="7435" max="7679" width="8.7265625" style="41"/>
+    <col min="7680" max="7680" width="10.90625" style="41" customWidth="1"/>
+    <col min="7681" max="7681" width="22.26953125" style="41" customWidth="1"/>
+    <col min="7682" max="7682" width="8.7265625" style="41"/>
+    <col min="7683" max="7683" width="17" style="41" customWidth="1"/>
+    <col min="7684" max="7684" width="13.90625" style="41" customWidth="1"/>
+    <col min="7685" max="7685" width="20.26953125" style="41" customWidth="1"/>
+    <col min="7686" max="7686" width="13.90625" style="41" customWidth="1"/>
+    <col min="7687" max="7687" width="8.7265625" style="41"/>
+    <col min="7688" max="7688" width="17.90625" style="41" customWidth="1"/>
+    <col min="7689" max="7689" width="8.7265625" style="41"/>
+    <col min="7690" max="7690" width="53.6328125" style="41" customWidth="1"/>
+    <col min="7691" max="7935" width="8.7265625" style="41"/>
+    <col min="7936" max="7936" width="10.90625" style="41" customWidth="1"/>
+    <col min="7937" max="7937" width="22.26953125" style="41" customWidth="1"/>
+    <col min="7938" max="7938" width="8.7265625" style="41"/>
+    <col min="7939" max="7939" width="17" style="41" customWidth="1"/>
+    <col min="7940" max="7940" width="13.90625" style="41" customWidth="1"/>
+    <col min="7941" max="7941" width="20.26953125" style="41" customWidth="1"/>
+    <col min="7942" max="7942" width="13.90625" style="41" customWidth="1"/>
+    <col min="7943" max="7943" width="8.7265625" style="41"/>
+    <col min="7944" max="7944" width="17.90625" style="41" customWidth="1"/>
+    <col min="7945" max="7945" width="8.7265625" style="41"/>
+    <col min="7946" max="7946" width="53.6328125" style="41" customWidth="1"/>
+    <col min="7947" max="8191" width="8.7265625" style="41"/>
+    <col min="8192" max="8192" width="10.90625" style="41" customWidth="1"/>
+    <col min="8193" max="8193" width="22.26953125" style="41" customWidth="1"/>
+    <col min="8194" max="8194" width="8.7265625" style="41"/>
+    <col min="8195" max="8195" width="17" style="41" customWidth="1"/>
+    <col min="8196" max="8196" width="13.90625" style="41" customWidth="1"/>
+    <col min="8197" max="8197" width="20.26953125" style="41" customWidth="1"/>
+    <col min="8198" max="8198" width="13.90625" style="41" customWidth="1"/>
+    <col min="8199" max="8199" width="8.7265625" style="41"/>
+    <col min="8200" max="8200" width="17.90625" style="41" customWidth="1"/>
+    <col min="8201" max="8201" width="8.7265625" style="41"/>
+    <col min="8202" max="8202" width="53.6328125" style="41" customWidth="1"/>
+    <col min="8203" max="8447" width="8.7265625" style="41"/>
+    <col min="8448" max="8448" width="10.90625" style="41" customWidth="1"/>
+    <col min="8449" max="8449" width="22.26953125" style="41" customWidth="1"/>
+    <col min="8450" max="8450" width="8.7265625" style="41"/>
+    <col min="8451" max="8451" width="17" style="41" customWidth="1"/>
+    <col min="8452" max="8452" width="13.90625" style="41" customWidth="1"/>
+    <col min="8453" max="8453" width="20.26953125" style="41" customWidth="1"/>
+    <col min="8454" max="8454" width="13.90625" style="41" customWidth="1"/>
+    <col min="8455" max="8455" width="8.7265625" style="41"/>
+    <col min="8456" max="8456" width="17.90625" style="41" customWidth="1"/>
+    <col min="8457" max="8457" width="8.7265625" style="41"/>
+    <col min="8458" max="8458" width="53.6328125" style="41" customWidth="1"/>
+    <col min="8459" max="8703" width="8.7265625" style="41"/>
+    <col min="8704" max="8704" width="10.90625" style="41" customWidth="1"/>
+    <col min="8705" max="8705" width="22.26953125" style="41" customWidth="1"/>
+    <col min="8706" max="8706" width="8.7265625" style="41"/>
+    <col min="8707" max="8707" width="17" style="41" customWidth="1"/>
+    <col min="8708" max="8708" width="13.90625" style="41" customWidth="1"/>
+    <col min="8709" max="8709" width="20.26953125" style="41" customWidth="1"/>
+    <col min="8710" max="8710" width="13.90625" style="41" customWidth="1"/>
+    <col min="8711" max="8711" width="8.7265625" style="41"/>
+    <col min="8712" max="8712" width="17.90625" style="41" customWidth="1"/>
+    <col min="8713" max="8713" width="8.7265625" style="41"/>
+    <col min="8714" max="8714" width="53.6328125" style="41" customWidth="1"/>
+    <col min="8715" max="8959" width="8.7265625" style="41"/>
+    <col min="8960" max="8960" width="10.90625" style="41" customWidth="1"/>
+    <col min="8961" max="8961" width="22.26953125" style="41" customWidth="1"/>
+    <col min="8962" max="8962" width="8.7265625" style="41"/>
+    <col min="8963" max="8963" width="17" style="41" customWidth="1"/>
+    <col min="8964" max="8964" width="13.90625" style="41" customWidth="1"/>
+    <col min="8965" max="8965" width="20.26953125" style="41" customWidth="1"/>
+    <col min="8966" max="8966" width="13.90625" style="41" customWidth="1"/>
+    <col min="8967" max="8967" width="8.7265625" style="41"/>
+    <col min="8968" max="8968" width="17.90625" style="41" customWidth="1"/>
+    <col min="8969" max="8969" width="8.7265625" style="41"/>
+    <col min="8970" max="8970" width="53.6328125" style="41" customWidth="1"/>
+    <col min="8971" max="9215" width="8.7265625" style="41"/>
+    <col min="9216" max="9216" width="10.90625" style="41" customWidth="1"/>
+    <col min="9217" max="9217" width="22.26953125" style="41" customWidth="1"/>
+    <col min="9218" max="9218" width="8.7265625" style="41"/>
+    <col min="9219" max="9219" width="17" style="41" customWidth="1"/>
+    <col min="9220" max="9220" width="13.90625" style="41" customWidth="1"/>
+    <col min="9221" max="9221" width="20.26953125" style="41" customWidth="1"/>
+    <col min="9222" max="9222" width="13.90625" style="41" customWidth="1"/>
+    <col min="9223" max="9223" width="8.7265625" style="41"/>
+    <col min="9224" max="9224" width="17.90625" style="41" customWidth="1"/>
+    <col min="9225" max="9225" width="8.7265625" style="41"/>
+    <col min="9226" max="9226" width="53.6328125" style="41" customWidth="1"/>
+    <col min="9227" max="9471" width="8.7265625" style="41"/>
+    <col min="9472" max="9472" width="10.90625" style="41" customWidth="1"/>
+    <col min="9473" max="9473" width="22.26953125" style="41" customWidth="1"/>
+    <col min="9474" max="9474" width="8.7265625" style="41"/>
+    <col min="9475" max="9475" width="17" style="41" customWidth="1"/>
+    <col min="9476" max="9476" width="13.90625" style="41" customWidth="1"/>
+    <col min="9477" max="9477" width="20.26953125" style="41" customWidth="1"/>
+    <col min="9478" max="9478" width="13.90625" style="41" customWidth="1"/>
+    <col min="9479" max="9479" width="8.7265625" style="41"/>
+    <col min="9480" max="9480" width="17.90625" style="41" customWidth="1"/>
+    <col min="9481" max="9481" width="8.7265625" style="41"/>
+    <col min="9482" max="9482" width="53.6328125" style="41" customWidth="1"/>
+    <col min="9483" max="9727" width="8.7265625" style="41"/>
+    <col min="9728" max="9728" width="10.90625" style="41" customWidth="1"/>
+    <col min="9729" max="9729" width="22.26953125" style="41" customWidth="1"/>
+    <col min="9730" max="9730" width="8.7265625" style="41"/>
+    <col min="9731" max="9731" width="17" style="41" customWidth="1"/>
+    <col min="9732" max="9732" width="13.90625" style="41" customWidth="1"/>
+    <col min="9733" max="9733" width="20.26953125" style="41" customWidth="1"/>
+    <col min="9734" max="9734" width="13.90625" style="41" customWidth="1"/>
+    <col min="9735" max="9735" width="8.7265625" style="41"/>
+    <col min="9736" max="9736" width="17.90625" style="41" customWidth="1"/>
+    <col min="9737" max="9737" width="8.7265625" style="41"/>
+    <col min="9738" max="9738" width="53.6328125" style="41" customWidth="1"/>
+    <col min="9739" max="9983" width="8.7265625" style="41"/>
+    <col min="9984" max="9984" width="10.90625" style="41" customWidth="1"/>
+    <col min="9985" max="9985" width="22.26953125" style="41" customWidth="1"/>
+    <col min="9986" max="9986" width="8.7265625" style="41"/>
+    <col min="9987" max="9987" width="17" style="41" customWidth="1"/>
+    <col min="9988" max="9988" width="13.90625" style="41" customWidth="1"/>
+    <col min="9989" max="9989" width="20.26953125" style="41" customWidth="1"/>
+    <col min="9990" max="9990" width="13.90625" style="41" customWidth="1"/>
+    <col min="9991" max="9991" width="8.7265625" style="41"/>
+    <col min="9992" max="9992" width="17.90625" style="41" customWidth="1"/>
+    <col min="9993" max="9993" width="8.7265625" style="41"/>
+    <col min="9994" max="9994" width="53.6328125" style="41" customWidth="1"/>
+    <col min="9995" max="10239" width="8.7265625" style="41"/>
+    <col min="10240" max="10240" width="10.90625" style="41" customWidth="1"/>
+    <col min="10241" max="10241" width="22.26953125" style="41" customWidth="1"/>
+    <col min="10242" max="10242" width="8.7265625" style="41"/>
+    <col min="10243" max="10243" width="17" style="41" customWidth="1"/>
+    <col min="10244" max="10244" width="13.90625" style="41" customWidth="1"/>
+    <col min="10245" max="10245" width="20.26953125" style="41" customWidth="1"/>
+    <col min="10246" max="10246" width="13.90625" style="41" customWidth="1"/>
+    <col min="10247" max="10247" width="8.7265625" style="41"/>
+    <col min="10248" max="10248" width="17.90625" style="41" customWidth="1"/>
+    <col min="10249" max="10249" width="8.7265625" style="41"/>
+    <col min="10250" max="10250" width="53.6328125" style="41" customWidth="1"/>
+    <col min="10251" max="10495" width="8.7265625" style="41"/>
+    <col min="10496" max="10496" width="10.90625" style="41" customWidth="1"/>
+    <col min="10497" max="10497" width="22.26953125" style="41" customWidth="1"/>
+    <col min="10498" max="10498" width="8.7265625" style="41"/>
+    <col min="10499" max="10499" width="17" style="41" customWidth="1"/>
+    <col min="10500" max="10500" width="13.90625" style="41" customWidth="1"/>
+    <col min="10501" max="10501" width="20.26953125" style="41" customWidth="1"/>
+    <col min="10502" max="10502" width="13.90625" style="41" customWidth="1"/>
+    <col min="10503" max="10503" width="8.7265625" style="41"/>
+    <col min="10504" max="10504" width="17.90625" style="41" customWidth="1"/>
+    <col min="10505" max="10505" width="8.7265625" style="41"/>
+    <col min="10506" max="10506" width="53.6328125" style="41" customWidth="1"/>
+    <col min="10507" max="10751" width="8.7265625" style="41"/>
+    <col min="10752" max="10752" width="10.90625" style="41" customWidth="1"/>
+    <col min="10753" max="10753" width="22.26953125" style="41" customWidth="1"/>
+    <col min="10754" max="10754" width="8.7265625" style="41"/>
+    <col min="10755" max="10755" width="17" style="41" customWidth="1"/>
+    <col min="10756" max="10756" width="13.90625" style="41" customWidth="1"/>
+    <col min="10757" max="10757" width="20.26953125" style="41" customWidth="1"/>
+    <col min="10758" max="10758" width="13.90625" style="41" customWidth="1"/>
+    <col min="10759" max="10759" width="8.7265625" style="41"/>
+    <col min="10760" max="10760" width="17.90625" style="41" customWidth="1"/>
+    <col min="10761" max="10761" width="8.7265625" style="41"/>
+    <col min="10762" max="10762" width="53.6328125" style="41" customWidth="1"/>
+    <col min="10763" max="11007" width="8.7265625" style="41"/>
+    <col min="11008" max="11008" width="10.90625" style="41" customWidth="1"/>
+    <col min="11009" max="11009" width="22.26953125" style="41" customWidth="1"/>
+    <col min="11010" max="11010" width="8.7265625" style="41"/>
+    <col min="11011" max="11011" width="17" style="41" customWidth="1"/>
+    <col min="11012" max="11012" width="13.90625" style="41" customWidth="1"/>
+    <col min="11013" max="11013" width="20.26953125" style="41" customWidth="1"/>
+    <col min="11014" max="11014" width="13.90625" style="41" customWidth="1"/>
+    <col min="11015" max="11015" width="8.7265625" style="41"/>
+    <col min="11016" max="11016" width="17.90625" style="41" customWidth="1"/>
+    <col min="11017" max="11017" width="8.7265625" style="41"/>
+    <col min="11018" max="11018" width="53.6328125" style="41" customWidth="1"/>
+    <col min="11019" max="11263" width="8.7265625" style="41"/>
+    <col min="11264" max="11264" width="10.90625" style="41" customWidth="1"/>
+    <col min="11265" max="11265" width="22.26953125" style="41" customWidth="1"/>
+    <col min="11266" max="11266" width="8.7265625" style="41"/>
+    <col min="11267" max="11267" width="17" style="41" customWidth="1"/>
+    <col min="11268" max="11268" width="13.90625" style="41" customWidth="1"/>
+    <col min="11269" max="11269" width="20.26953125" style="41" customWidth="1"/>
+    <col min="11270" max="11270" width="13.90625" style="41" customWidth="1"/>
+    <col min="11271" max="11271" width="8.7265625" style="41"/>
+    <col min="11272" max="11272" width="17.90625" style="41" customWidth="1"/>
+    <col min="11273" max="11273" width="8.7265625" style="41"/>
+    <col min="11274" max="11274" width="53.6328125" style="41" customWidth="1"/>
+    <col min="11275" max="11519" width="8.7265625" style="41"/>
+    <col min="11520" max="11520" width="10.90625" style="41" customWidth="1"/>
+    <col min="11521" max="11521" width="22.26953125" style="41" customWidth="1"/>
+    <col min="11522" max="11522" width="8.7265625" style="41"/>
+    <col min="11523" max="11523" width="17" style="41" customWidth="1"/>
+    <col min="11524" max="11524" width="13.90625" style="41" customWidth="1"/>
+    <col min="11525" max="11525" width="20.26953125" style="41" customWidth="1"/>
+    <col min="11526" max="11526" width="13.90625" style="41" customWidth="1"/>
+    <col min="11527" max="11527" width="8.7265625" style="41"/>
+    <col min="11528" max="11528" width="17.90625" style="41" customWidth="1"/>
+    <col min="11529" max="11529" width="8.7265625" style="41"/>
+    <col min="11530" max="11530" width="53.6328125" style="41" customWidth="1"/>
+    <col min="11531" max="11775" width="8.7265625" style="41"/>
+    <col min="11776" max="11776" width="10.90625" style="41" customWidth="1"/>
+    <col min="11777" max="11777" width="22.26953125" style="41" customWidth="1"/>
+    <col min="11778" max="11778" width="8.7265625" style="41"/>
+    <col min="11779" max="11779" width="17" style="41" customWidth="1"/>
+    <col min="11780" max="11780" width="13.90625" style="41" customWidth="1"/>
+    <col min="11781" max="11781" width="20.26953125" style="41" customWidth="1"/>
+    <col min="11782" max="11782" width="13.90625" style="41" customWidth="1"/>
+    <col min="11783" max="11783" width="8.7265625" style="41"/>
+    <col min="11784" max="11784" width="17.90625" style="41" customWidth="1"/>
+    <col min="11785" max="11785" width="8.7265625" style="41"/>
+    <col min="11786" max="11786" width="53.6328125" style="41" customWidth="1"/>
+    <col min="11787" max="12031" width="8.7265625" style="41"/>
+    <col min="12032" max="12032" width="10.90625" style="41" customWidth="1"/>
+    <col min="12033" max="12033" width="22.26953125" style="41" customWidth="1"/>
+    <col min="12034" max="12034" width="8.7265625" style="41"/>
+    <col min="12035" max="12035" width="17" style="41" customWidth="1"/>
+    <col min="12036" max="12036" width="13.90625" style="41" customWidth="1"/>
+    <col min="12037" max="12037" width="20.26953125" style="41" customWidth="1"/>
+    <col min="12038" max="12038" width="13.90625" style="41" customWidth="1"/>
+    <col min="12039" max="12039" width="8.7265625" style="41"/>
+    <col min="12040" max="12040" width="17.90625" style="41" customWidth="1"/>
+    <col min="12041" max="12041" width="8.7265625" style="41"/>
+    <col min="12042" max="12042" width="53.6328125" style="41" customWidth="1"/>
+    <col min="12043" max="12287" width="8.7265625" style="41"/>
+    <col min="12288" max="12288" width="10.90625" style="41" customWidth="1"/>
+    <col min="12289" max="12289" width="22.26953125" style="41" customWidth="1"/>
+    <col min="12290" max="12290" width="8.7265625" style="41"/>
+    <col min="12291" max="12291" width="17" style="41" customWidth="1"/>
+    <col min="12292" max="12292" width="13.90625" style="41" customWidth="1"/>
+    <col min="12293" max="12293" width="20.26953125" style="41" customWidth="1"/>
+    <col min="12294" max="12294" width="13.90625" style="41" customWidth="1"/>
+    <col min="12295" max="12295" width="8.7265625" style="41"/>
+    <col min="12296" max="12296" width="17.90625" style="41" customWidth="1"/>
+    <col min="12297" max="12297" width="8.7265625" style="41"/>
+    <col min="12298" max="12298" width="53.6328125" style="41" customWidth="1"/>
+    <col min="12299" max="12543" width="8.7265625" style="41"/>
+    <col min="12544" max="12544" width="10.90625" style="41" customWidth="1"/>
+    <col min="12545" max="12545" width="22.26953125" style="41" customWidth="1"/>
+    <col min="12546" max="12546" width="8.7265625" style="41"/>
+    <col min="12547" max="12547" width="17" style="41" customWidth="1"/>
+    <col min="12548" max="12548" width="13.90625" style="41" customWidth="1"/>
+    <col min="12549" max="12549" width="20.26953125" style="41" customWidth="1"/>
+    <col min="12550" max="12550" width="13.90625" style="41" customWidth="1"/>
+    <col min="12551" max="12551" width="8.7265625" style="41"/>
+    <col min="12552" max="12552" width="17.90625" style="41" customWidth="1"/>
+    <col min="12553" max="12553" width="8.7265625" style="41"/>
+    <col min="12554" max="12554" width="53.6328125" style="41" customWidth="1"/>
+    <col min="12555" max="12799" width="8.7265625" style="41"/>
+    <col min="12800" max="12800" width="10.90625" style="41" customWidth="1"/>
+    <col min="12801" max="12801" width="22.26953125" style="41" customWidth="1"/>
+    <col min="12802" max="12802" width="8.7265625" style="41"/>
+    <col min="12803" max="12803" width="17" style="41" customWidth="1"/>
+    <col min="12804" max="12804" width="13.90625" style="41" customWidth="1"/>
+    <col min="12805" max="12805" width="20.26953125" style="41" customWidth="1"/>
+    <col min="12806" max="12806" width="13.90625" style="41" customWidth="1"/>
+    <col min="12807" max="12807" width="8.7265625" style="41"/>
+    <col min="12808" max="12808" width="17.90625" style="41" customWidth="1"/>
+    <col min="12809" max="12809" width="8.7265625" style="41"/>
+    <col min="12810" max="12810" width="53.6328125" style="41" customWidth="1"/>
+    <col min="12811" max="13055" width="8.7265625" style="41"/>
+    <col min="13056" max="13056" width="10.90625" style="41" customWidth="1"/>
+    <col min="13057" max="13057" width="22.26953125" style="41" customWidth="1"/>
+    <col min="13058" max="13058" width="8.7265625" style="41"/>
+    <col min="13059" max="13059" width="17" style="41" customWidth="1"/>
+    <col min="13060" max="13060" width="13.90625" style="41" customWidth="1"/>
+    <col min="13061" max="13061" width="20.26953125" style="41" customWidth="1"/>
+    <col min="13062" max="13062" width="13.90625" style="41" customWidth="1"/>
+    <col min="13063" max="13063" width="8.7265625" style="41"/>
+    <col min="13064" max="13064" width="17.90625" style="41" customWidth="1"/>
+    <col min="13065" max="13065" width="8.7265625" style="41"/>
+    <col min="13066" max="13066" width="53.6328125" style="41" customWidth="1"/>
+    <col min="13067" max="13311" width="8.7265625" style="41"/>
+    <col min="13312" max="13312" width="10.90625" style="41" customWidth="1"/>
+    <col min="13313" max="13313" width="22.26953125" style="41" customWidth="1"/>
+    <col min="13314" max="13314" width="8.7265625" style="41"/>
+    <col min="13315" max="13315" width="17" style="41" customWidth="1"/>
+    <col min="13316" max="13316" width="13.90625" style="41" customWidth="1"/>
+    <col min="13317" max="13317" width="20.26953125" style="41" customWidth="1"/>
+    <col min="13318" max="13318" width="13.90625" style="41" customWidth="1"/>
+    <col min="13319" max="13319" width="8.7265625" style="41"/>
+    <col min="13320" max="13320" width="17.90625" style="41" customWidth="1"/>
+    <col min="13321" max="13321" width="8.7265625" style="41"/>
+    <col min="13322" max="13322" width="53.6328125" style="41" customWidth="1"/>
+    <col min="13323" max="13567" width="8.7265625" style="41"/>
+    <col min="13568" max="13568" width="10.90625" style="41" customWidth="1"/>
+    <col min="13569" max="13569" width="22.26953125" style="41" customWidth="1"/>
+    <col min="13570" max="13570" width="8.7265625" style="41"/>
+    <col min="13571" max="13571" width="17" style="41" customWidth="1"/>
+    <col min="13572" max="13572" width="13.90625" style="41" customWidth="1"/>
+    <col min="13573" max="13573" width="20.26953125" style="41" customWidth="1"/>
+    <col min="13574" max="13574" width="13.90625" style="41" customWidth="1"/>
+    <col min="13575" max="13575" width="8.7265625" style="41"/>
+    <col min="13576" max="13576" width="17.90625" style="41" customWidth="1"/>
+    <col min="13577" max="13577" width="8.7265625" style="41"/>
+    <col min="13578" max="13578" width="53.6328125" style="41" customWidth="1"/>
+    <col min="13579" max="13823" width="8.7265625" style="41"/>
+    <col min="13824" max="13824" width="10.90625" style="41" customWidth="1"/>
+    <col min="13825" max="13825" width="22.26953125" style="41" customWidth="1"/>
+    <col min="13826" max="13826" width="8.7265625" style="41"/>
+    <col min="13827" max="13827" width="17" style="41" customWidth="1"/>
+    <col min="13828" max="13828" width="13.90625" style="41" customWidth="1"/>
+    <col min="13829" max="13829" width="20.26953125" style="41" customWidth="1"/>
+    <col min="13830" max="13830" width="13.90625" style="41" customWidth="1"/>
+    <col min="13831" max="13831" width="8.7265625" style="41"/>
+    <col min="13832" max="13832" width="17.90625" style="41" customWidth="1"/>
+    <col min="13833" max="13833" width="8.7265625" style="41"/>
+    <col min="13834" max="13834" width="53.6328125" style="41" customWidth="1"/>
+    <col min="13835" max="14079" width="8.7265625" style="41"/>
+    <col min="14080" max="14080" width="10.90625" style="41" customWidth="1"/>
+    <col min="14081" max="14081" width="22.26953125" style="41" customWidth="1"/>
+    <col min="14082" max="14082" width="8.7265625" style="41"/>
+    <col min="14083" max="14083" width="17" style="41" customWidth="1"/>
+    <col min="14084" max="14084" width="13.90625" style="41" customWidth="1"/>
+    <col min="14085" max="14085" width="20.26953125" style="41" customWidth="1"/>
+    <col min="14086" max="14086" width="13.90625" style="41" customWidth="1"/>
+    <col min="14087" max="14087" width="8.7265625" style="41"/>
+    <col min="14088" max="14088" width="17.90625" style="41" customWidth="1"/>
+    <col min="14089" max="14089" width="8.7265625" style="41"/>
+    <col min="14090" max="14090" width="53.6328125" style="41" customWidth="1"/>
+    <col min="14091" max="14335" width="8.7265625" style="41"/>
+    <col min="14336" max="14336" width="10.90625" style="41" customWidth="1"/>
+    <col min="14337" max="14337" width="22.26953125" style="41" customWidth="1"/>
+    <col min="14338" max="14338" width="8.7265625" style="41"/>
+    <col min="14339" max="14339" width="17" style="41" customWidth="1"/>
+    <col min="14340" max="14340" width="13.90625" style="41" customWidth="1"/>
+    <col min="14341" max="14341" width="20.26953125" style="41" customWidth="1"/>
+    <col min="14342" max="14342" width="13.90625" style="41" customWidth="1"/>
+    <col min="14343" max="14343" width="8.7265625" style="41"/>
+    <col min="14344" max="14344" width="17.90625" style="41" customWidth="1"/>
+    <col min="14345" max="14345" width="8.7265625" style="41"/>
+    <col min="14346" max="14346" width="53.6328125" style="41" customWidth="1"/>
+    <col min="14347" max="14591" width="8.7265625" style="41"/>
+    <col min="14592" max="14592" width="10.90625" style="41" customWidth="1"/>
+    <col min="14593" max="14593" width="22.26953125" style="41" customWidth="1"/>
+    <col min="14594" max="14594" width="8.7265625" style="41"/>
+    <col min="14595" max="14595" width="17" style="41" customWidth="1"/>
+    <col min="14596" max="14596" width="13.90625" style="41" customWidth="1"/>
+    <col min="14597" max="14597" width="20.26953125" style="41" customWidth="1"/>
+    <col min="14598" max="14598" width="13.90625" style="41" customWidth="1"/>
+    <col min="14599" max="14599" width="8.7265625" style="41"/>
+    <col min="14600" max="14600" width="17.90625" style="41" customWidth="1"/>
+    <col min="14601" max="14601" width="8.7265625" style="41"/>
+    <col min="14602" max="14602" width="53.6328125" style="41" customWidth="1"/>
+    <col min="14603" max="14847" width="8.7265625" style="41"/>
+    <col min="14848" max="14848" width="10.90625" style="41" customWidth="1"/>
+    <col min="14849" max="14849" width="22.26953125" style="41" customWidth="1"/>
+    <col min="14850" max="14850" width="8.7265625" style="41"/>
+    <col min="14851" max="14851" width="17" style="41" customWidth="1"/>
+    <col min="14852" max="14852" width="13.90625" style="41" customWidth="1"/>
+    <col min="14853" max="14853" width="20.26953125" style="41" customWidth="1"/>
+    <col min="14854" max="14854" width="13.90625" style="41" customWidth="1"/>
+    <col min="14855" max="14855" width="8.7265625" style="41"/>
+    <col min="14856" max="14856" width="17.90625" style="41" customWidth="1"/>
+    <col min="14857" max="14857" width="8.7265625" style="41"/>
+    <col min="14858" max="14858" width="53.6328125" style="41" customWidth="1"/>
+    <col min="14859" max="15103" width="8.7265625" style="41"/>
+    <col min="15104" max="15104" width="10.90625" style="41" customWidth="1"/>
+    <col min="15105" max="15105" width="22.26953125" style="41" customWidth="1"/>
+    <col min="15106" max="15106" width="8.7265625" style="41"/>
+    <col min="15107" max="15107" width="17" style="41" customWidth="1"/>
+    <col min="15108" max="15108" width="13.90625" style="41" customWidth="1"/>
+    <col min="15109" max="15109" width="20.26953125" style="41" customWidth="1"/>
+    <col min="15110" max="15110" width="13.90625" style="41" customWidth="1"/>
+    <col min="15111" max="15111" width="8.7265625" style="41"/>
+    <col min="15112" max="15112" width="17.90625" style="41" customWidth="1"/>
+    <col min="15113" max="15113" width="8.7265625" style="41"/>
+    <col min="15114" max="15114" width="53.6328125" style="41" customWidth="1"/>
+    <col min="15115" max="15359" width="8.7265625" style="41"/>
+    <col min="15360" max="15360" width="10.90625" style="41" customWidth="1"/>
+    <col min="15361" max="15361" width="22.26953125" style="41" customWidth="1"/>
+    <col min="15362" max="15362" width="8.7265625" style="41"/>
+    <col min="15363" max="15363" width="17" style="41" customWidth="1"/>
+    <col min="15364" max="15364" width="13.90625" style="41" customWidth="1"/>
+    <col min="15365" max="15365" width="20.26953125" style="41" customWidth="1"/>
+    <col min="15366" max="15366" width="13.90625" style="41" customWidth="1"/>
+    <col min="15367" max="15367" width="8.7265625" style="41"/>
+    <col min="15368" max="15368" width="17.90625" style="41" customWidth="1"/>
+    <col min="15369" max="15369" width="8.7265625" style="41"/>
+    <col min="15370" max="15370" width="53.6328125" style="41" customWidth="1"/>
+    <col min="15371" max="15615" width="8.7265625" style="41"/>
+    <col min="15616" max="15616" width="10.90625" style="41" customWidth="1"/>
+    <col min="15617" max="15617" width="22.26953125" style="41" customWidth="1"/>
+    <col min="15618" max="15618" width="8.7265625" style="41"/>
+    <col min="15619" max="15619" width="17" style="41" customWidth="1"/>
+    <col min="15620" max="15620" width="13.90625" style="41" customWidth="1"/>
+    <col min="15621" max="15621" width="20.26953125" style="41" customWidth="1"/>
+    <col min="15622" max="15622" width="13.90625" style="41" customWidth="1"/>
+    <col min="15623" max="15623" width="8.7265625" style="41"/>
+    <col min="15624" max="15624" width="17.90625" style="41" customWidth="1"/>
+    <col min="15625" max="15625" width="8.7265625" style="41"/>
+    <col min="15626" max="15626" width="53.6328125" style="41" customWidth="1"/>
+    <col min="15627" max="15871" width="8.7265625" style="41"/>
+    <col min="15872" max="15872" width="10.90625" style="41" customWidth="1"/>
+    <col min="15873" max="15873" width="22.26953125" style="41" customWidth="1"/>
+    <col min="15874" max="15874" width="8.7265625" style="41"/>
+    <col min="15875" max="15875" width="17" style="41" customWidth="1"/>
+    <col min="15876" max="15876" width="13.90625" style="41" customWidth="1"/>
+    <col min="15877" max="15877" width="20.26953125" style="41" customWidth="1"/>
+    <col min="15878" max="15878" width="13.90625" style="41" customWidth="1"/>
+    <col min="15879" max="15879" width="8.7265625" style="41"/>
+    <col min="15880" max="15880" width="17.90625" style="41" customWidth="1"/>
+    <col min="15881" max="15881" width="8.7265625" style="41"/>
+    <col min="15882" max="15882" width="53.6328125" style="41" customWidth="1"/>
+    <col min="15883" max="16127" width="8.7265625" style="41"/>
+    <col min="16128" max="16128" width="10.90625" style="41" customWidth="1"/>
+    <col min="16129" max="16129" width="22.26953125" style="41" customWidth="1"/>
+    <col min="16130" max="16130" width="8.7265625" style="41"/>
+    <col min="16131" max="16131" width="17" style="41" customWidth="1"/>
+    <col min="16132" max="16132" width="13.90625" style="41" customWidth="1"/>
+    <col min="16133" max="16133" width="20.26953125" style="41" customWidth="1"/>
+    <col min="16134" max="16134" width="13.90625" style="41" customWidth="1"/>
+    <col min="16135" max="16135" width="8.7265625" style="41"/>
+    <col min="16136" max="16136" width="17.90625" style="41" customWidth="1"/>
+    <col min="16137" max="16137" width="8.7265625" style="41"/>
+    <col min="16138" max="16138" width="53.6328125" style="41" customWidth="1"/>
+    <col min="16139" max="16384" width="8.7265625" style="41"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.25">
@@ -10510,122 +10814,122 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="37" t="s">
         <v>1006</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="39" t="s">
         <v>993</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="39" t="s">
         <v>987</v>
       </c>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="40" t="s">
         <v>974</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="38" t="s">
         <v>978</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="38" t="s">
         <v>985</v>
       </c>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41" t="s">
+      <c r="I2" s="38"/>
+      <c r="J2" s="38" t="s">
         <v>995</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="37" t="s">
         <v>1007</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="39" t="s">
         <v>993</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="39" t="s">
         <v>988</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="40" t="s">
         <v>974</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="38" t="s">
         <v>978</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="38" t="s">
         <v>986</v>
       </c>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41" t="s">
+      <c r="I3" s="38"/>
+      <c r="J3" s="38" t="s">
         <v>996</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="38.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="37" t="s">
         <v>1008</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="38" t="s">
         <v>347</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="38" t="s">
         <v>348</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="39" t="s">
         <v>994</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="39" t="s">
         <v>987</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="40" t="s">
         <v>974</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="38" t="s">
         <v>978</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="38" t="s">
         <v>985</v>
       </c>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41" t="s">
+      <c r="I4" s="38"/>
+      <c r="J4" s="38" t="s">
         <v>995</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="39.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="37" t="s">
         <v>1009</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="38" t="s">
         <v>347</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="38" t="s">
         <v>348</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="39" t="s">
         <v>994</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="39" t="s">
         <v>988</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="40" t="s">
         <v>974</v>
       </c>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="38" t="s">
         <v>978</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="38" t="s">
         <v>986</v>
       </c>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41" t="s">
+      <c r="I5" s="38"/>
+      <c r="J5" s="38" t="s">
         <v>996</v>
       </c>
     </row>
@@ -10641,7 +10945,7 @@
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -10924,11 +11228,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="44" t="s">
         <v>992</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Removed yellow from cells in changes new tab
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82BC453-615B-49C3-ADD4-473B1344DB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BF6498-66F2-48F6-8F32-3725C38906E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="360" windowWidth="16590" windowHeight="8590" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1760" yWindow="1050" windowWidth="16590" windowHeight="8590" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -3488,7 +3488,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -3611,20 +3611,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3634,6 +3622,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3929,10 +3926,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="46" t="s">
         <v>973</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="47"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -9830,32 +9827,32 @@
       <c r="A2" s="36" t="s">
         <v>1010</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
       <c r="D2" s="37" t="s">
         <v>979</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="44" t="s">
         <v>1011</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>1012</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>1010</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
       <c r="D3" s="37" t="s">
         <v>979</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="44" t="s">
         <v>1013</v>
       </c>
       <c r="F3" s="37" t="s">
@@ -9870,10 +9867,10 @@
       <c r="A4" s="36" t="s">
         <v>1014</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="42" t="s">
         <v>323</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="42" t="s">
         <v>324</v>
       </c>
       <c r="D4" s="37" t="s">
@@ -9900,10 +9897,10 @@
       <c r="A5" s="36" t="s">
         <v>1014</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="42" t="s">
         <v>323</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="42" t="s">
         <v>324</v>
       </c>
       <c r="D5" s="37" t="s">
@@ -9945,14 +9942,14 @@
       <c r="F6" s="37" t="s">
         <v>1023</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="44" t="s">
         <v>978</v>
       </c>
-      <c r="H6" s="48" t="s">
+      <c r="H6" s="44" t="s">
         <v>1024</v>
       </c>
-      <c r="I6" s="48"/>
-      <c r="J6" s="49" t="s">
+      <c r="I6" s="44"/>
+      <c r="J6" s="45" t="s">
         <v>1028</v>
       </c>
     </row>
@@ -11228,11 +11225,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="48" t="s">
         <v>992</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Desc updated to Description
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82BC453-615B-49C3-ADD4-473B1344DB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EEA6D9-A6BE-4013-8823-029918143733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="360" windowWidth="16590" windowHeight="8590" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="17790" windowHeight="8850" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1776" uniqueCount="1029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1909" uniqueCount="1064">
   <si>
     <t>Code</t>
   </si>
@@ -3242,12 +3242,585 @@
   <si>
     <t>An alternative symbol or combination of symbols which is assigned to the members of a collection.</t>
   </si>
+  <si>
+    <t>InvestigationalInterventions</t>
+  </si>
+  <si>
+    <t>Indication</t>
+  </si>
+  <si>
+    <t>The condition, disease or disorder that the clinical trial is intended to investigate or address.</t>
+  </si>
+  <si>
+    <t>StudyDesignPopulation</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Endpoint</t>
+  </si>
+  <si>
+    <t>StudyArm</t>
+  </si>
+  <si>
+    <t>The textual representation of the study arm.</t>
+  </si>
+  <si>
+    <t>StudyEpoch</t>
+  </si>
+  <si>
+    <t>StudyElement</t>
+  </si>
+  <si>
+    <t>TransitionRule</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>StudyData</t>
+  </si>
+  <si>
+    <t>WorkflowItem</t>
+  </si>
+  <si>
+    <t>AnalysisPopulation</t>
+  </si>
+  <si>
+    <t>IntercurrentEvent</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyDesignDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyDesignDescription</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>interventionDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>interventionDescription</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>indicationDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>indicationDescription</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>populationDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>populationDescription</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectiveDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectiveDescription</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>endpointDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>endpointDescription</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>endpointPurposeDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>endpointPurposeDesciption</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyArmDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyArmDescription</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyArmDataOriginDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyArmDataOriginDescription</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyEpochDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyEpochDescription</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyElementDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyElementDescription</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>transitionRuleDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>transitionRuleDescription</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>encounterDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>encounterDescription</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>activityDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>activityDescription</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyDataDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyDataDescription</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>workflowDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>workflowDescription</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>workflowItemDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>workflowItemDescription</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>intercurrentEventDesc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>intercurrentEventDescription</t>
+    </r>
+  </si>
+  <si>
+    <t>Update Attribute Name in USDM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3335,8 +3908,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3388,6 +3967,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3488,7 +4073,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -3611,6 +4196,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3620,20 +4217,14 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3929,10 +4520,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="46" t="s">
         <v>973</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="47"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -9830,32 +10421,32 @@
       <c r="A2" s="36" t="s">
         <v>1010</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
       <c r="D2" s="37" t="s">
         <v>979</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="44" t="s">
         <v>1011</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>1012</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>1010</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
       <c r="D3" s="37" t="s">
         <v>979</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="44" t="s">
         <v>1013</v>
       </c>
       <c r="F3" s="37" t="s">
@@ -9870,10 +10461,10 @@
       <c r="A4" s="36" t="s">
         <v>1014</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="42" t="s">
         <v>323</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="42" t="s">
         <v>324</v>
       </c>
       <c r="D4" s="37" t="s">
@@ -9900,10 +10491,10 @@
       <c r="A5" s="36" t="s">
         <v>1014</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="42" t="s">
         <v>323</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="42" t="s">
         <v>324</v>
       </c>
       <c r="D5" s="37" t="s">
@@ -9945,14 +10536,14 @@
       <c r="F6" s="37" t="s">
         <v>1023</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="44" t="s">
         <v>978</v>
       </c>
-      <c r="H6" s="48" t="s">
+      <c r="H6" s="44" t="s">
         <v>1024</v>
       </c>
-      <c r="I6" s="48"/>
-      <c r="J6" s="49" t="s">
+      <c r="I6" s="44"/>
+      <c r="J6" s="45" t="s">
         <v>1028</v>
       </c>
     </row>
@@ -10006,9 +10597,9 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10933,8 +11524,503 @@
         <v>996</v>
       </c>
     </row>
+    <row r="6" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="E6" s="49" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G6" s="37" t="s">
+        <v>978</v>
+      </c>
+      <c r="H6" s="37" t="s">
+        <v>1019</v>
+      </c>
+      <c r="I6" s="50"/>
+      <c r="J6" s="37" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+      <c r="A7" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="35" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E7" s="49" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="50" x14ac:dyDescent="0.25">
+      <c r="A8" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="35" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E8" s="49" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="35" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E9" s="49" t="s">
+        <v>1048</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>344</v>
+      </c>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+      <c r="A10" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="35" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>1049</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="35" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>1050</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="H11" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="I11" s="37"/>
+      <c r="J11" s="35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="35" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>1051</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+      <c r="A13" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="35" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E13" s="49" t="s">
+        <v>1052</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G13" s="37" t="s">
+        <v>298</v>
+      </c>
+      <c r="H13" s="35" t="s">
+        <v>299</v>
+      </c>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="50" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="35" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>293</v>
+      </c>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="35" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>1054</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>367</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>368</v>
+      </c>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="35" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>351</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>352</v>
+      </c>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="35" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E17" s="49" t="s">
+        <v>1056</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>415</v>
+      </c>
+      <c r="H17" s="35" t="s">
+        <v>416</v>
+      </c>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+      <c r="A18" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="35" t="s">
+        <v>993</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>1057</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="35" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>1058</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G19" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="35"/>
+      <c r="J19" s="37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+      <c r="A20" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="35" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>313</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>314</v>
+      </c>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+      <c r="A21" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="E21" s="49" t="s">
+        <v>1060</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>422</v>
+      </c>
+      <c r="H21" s="35" t="s">
+        <v>423</v>
+      </c>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="35" t="s">
+        <v>1042</v>
+      </c>
+      <c r="E22" s="51" t="s">
+        <v>1061</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="H22" s="35" t="s">
+        <v>209</v>
+      </c>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="35" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E23" s="49" t="s">
+        <v>1048</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G23" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="35" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>1062</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="G24" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="H24" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35" t="s">
+        <v>234</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11228,11 +12314,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="48" t="s">
         <v>992</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Sprint 11 QC changes from Dave
Backlog item numbers 70 and 89 from Dave QC of sprint 11 deliverables completed.
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0066D1-1C38-4F91-9C9E-6BECE226AF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F850B2DF-CA43-4CD7-A561-51CA56F647F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="70" windowWidth="18200" windowHeight="9820" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="310" yWindow="0" windowWidth="18200" windowHeight="9820" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3641" uniqueCount="1570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3653" uniqueCount="1570">
   <si>
     <t>Code</t>
   </si>
@@ -19420,7 +19420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2261BAFA-DB40-4742-A275-AC9B4F4BE353}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -20052,7 +20052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26159E6B-EDF9-4EC9-8B9E-0CC93771A6CC}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -21724,7 +21724,9 @@
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
+      <c r="K27" s="32" t="s">
+        <v>1196</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
@@ -21792,6 +21794,9 @@
       <c r="J29" s="31" t="s">
         <v>738</v>
       </c>
+      <c r="K29" s="32" t="s">
+        <v>1196</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
@@ -21822,6 +21827,9 @@
       <c r="J30" s="31" t="s">
         <v>741</v>
       </c>
+      <c r="K30" s="32" t="s">
+        <v>1196</v>
+      </c>
     </row>
     <row r="31" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
@@ -21852,6 +21860,9 @@
       <c r="J31" s="31" t="s">
         <v>745</v>
       </c>
+      <c r="K31" s="32" t="s">
+        <v>1196</v>
+      </c>
     </row>
     <row r="32" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
@@ -21882,8 +21893,11 @@
       <c r="J32" s="31" t="s">
         <v>749</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="K32" s="32" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
         <v>1569</v>
       </c>
@@ -21912,8 +21926,11 @@
       <c r="J33" s="31" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="K33" s="32" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
         <v>1569</v>
       </c>
@@ -21942,8 +21959,11 @@
       <c r="J34" s="31" t="s">
         <v>757</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="K34" s="32" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
         <v>1569</v>
       </c>
@@ -21972,8 +21992,11 @@
       <c r="J35" s="31" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="K35" s="32" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>1569</v>
       </c>
@@ -22004,8 +22027,11 @@
       <c r="J36" s="31" t="s">
         <v>766</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="K36" s="32" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>1569</v>
       </c>
@@ -22034,8 +22060,11 @@
       <c r="J37" s="31" t="s">
         <v>769</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="K37" s="32" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>1569</v>
       </c>
@@ -22064,8 +22093,11 @@
       <c r="J38" s="31" t="s">
         <v>773</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="K38" s="32" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>1569</v>
       </c>
@@ -22095,6 +22127,9 @@
       </c>
       <c r="J39" s="31" t="s">
         <v>777</v>
+      </c>
+      <c r="K39" s="32" t="s">
+        <v>1196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to USDM CT deliverable
Add, remove, and change as applicable to the sprint.
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C11EC5-54E4-43B6-9103-299057F917F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AB92D6-0BDD-43D1-8AAE-019209D6ADC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="15960" windowHeight="8670" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="15960" windowHeight="8670" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
     <sheet name="DDF Terminology 2023-03-31" sheetId="1" r:id="rId2"/>
-    <sheet name="Terminology Changes Sp12 - new" sheetId="24" r:id="rId3"/>
-    <sheet name="Terminology Changes Sp12 - chg" sheetId="23" r:id="rId4"/>
+    <sheet name="Terminology Changes Sp13 - new" sheetId="24" r:id="rId3"/>
+    <sheet name="Terminology Changes Sp13 - chg" sheetId="23" r:id="rId4"/>
     <sheet name="Terminology Changes Sp11 - new" sheetId="22" r:id="rId5"/>
     <sheet name="Terminology Changes Sp11 - chg" sheetId="21" r:id="rId6"/>
     <sheet name="Terminology Changes Sp10 - new" sheetId="19" r:id="rId7"/>
@@ -6991,6 +6991,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6999,12 +7005,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7300,10 +7300,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>966</v>
       </c>
-      <c r="B1" s="95"/>
+      <c r="B1" s="97"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -21668,11 +21668,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="98" t="s">
         <v>985</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -22914,7 +22914,7 @@
       <c r="D4" s="14" t="s">
         <v>1326</v>
       </c>
-      <c r="E4" s="97" t="s">
+      <c r="E4" s="94" t="s">
         <v>1340</v>
       </c>
       <c r="F4" s="14" t="s">
@@ -22964,7 +22964,7 @@
       <c r="D6" s="32" t="s">
         <v>1326</v>
       </c>
-      <c r="E6" s="98" t="s">
+      <c r="E6" s="95" t="s">
         <v>1331</v>
       </c>
       <c r="F6" s="54" t="s">

</xml_diff>

<commit_message>
Updates based on Berber email
•	in entity studyCell "id" not removed from relationships: studyArmId, studyEpochId and studyElementIds
•	in entity studyEpoch "id" not removed from names: previousStudyEpochId and nextStudyEpochId
•	in entity encounter "id" not removed from names: previousEncounterId and nextEncounterId
•	in entity biomedicalConceptCategory "id" not removed from bcCategoryMemberIds
•	in entity scheduledInstance "id" not removed from defaultConditionId
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E667F5A-5714-4B2B-AA88-D812109C5A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF157314-C1D8-441C-8BDC-1BF78EA910DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="770" windowWidth="14620" windowHeight="9320" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="470" windowWidth="18660" windowHeight="9820" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DDF Terminology 2023-06-30'!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Terminology Changes Sp1 - chg'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Terminology Changes Sp1 - chg'!$A$1:$K$58</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="1125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="1135">
   <si>
     <t>Code</t>
   </si>
@@ -5192,6 +5192,280 @@
         <family val="2"/>
       </rPr>
       <t>A health problem or disease that is identified as likely to be benefited by a therapy being studied in clinical trials.</t>
+    </r>
+  </si>
+  <si>
+    <t>StudyCell</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyEpochId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyEpoch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyArmId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyArm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyElementIds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>studyElement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>previousStudyEpochId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>previousStudyEpoch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>nextStudyEpochId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>nextStudyEpoch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>previousEncounterId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>previousEncounter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>nextEncounterId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>nextEncounter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>bcCategoryMemberIds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>bcCategoryMembers</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>defaultConditionId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>defaultCondition</t>
     </r>
   </si>
 </sst>
@@ -5491,7 +5765,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -5640,6 +5914,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -12295,9 +12572,9 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -12655,32 +12932,26 @@
         <v>1055</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>971</v>
+        <v>997</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>998</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>1078</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>967</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>971</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>1000</v>
-      </c>
+        <v>1003</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>978</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
       <c r="I12" s="17"/>
-      <c r="J12" s="17" t="s">
-        <v>1001</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>996</v>
+      <c r="J12" s="17"/>
+      <c r="K12" s="14" t="s">
+        <v>997</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="50" x14ac:dyDescent="0.25">
@@ -12697,7 +12968,7 @@
         <v>998</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>967</v>
@@ -12706,11 +12977,11 @@
         <v>971</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="I13" s="17"/>
       <c r="J13" s="17" t="s">
-        <v>1080</v>
+        <v>1001</v>
       </c>
       <c r="K13" s="17" t="s">
         <v>996</v>
@@ -12721,62 +12992,62 @@
         <v>1055</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>997</v>
+        <v>971</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>976</v>
-      </c>
-      <c r="E14" s="40" t="s">
-        <v>1061</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>978</v>
-      </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+        <v>998</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17" t="s">
+        <v>1080</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>1055</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>84</v>
+        <v>997</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>85</v>
+        <v>997</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>976</v>
       </c>
-      <c r="E15" s="19" t="s">
-        <v>1081</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>967</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="K15" s="16" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+      <c r="E15" s="40" t="s">
+        <v>1061</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>978</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>1055</v>
       </c>
@@ -12790,121 +13061,121 @@
         <v>976</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>967</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I16" s="16"/>
       <c r="J16" s="16" t="s">
-        <v>1083</v>
-      </c>
-      <c r="K16" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="K16" s="16" t="s">
         <v>996</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>1055</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>111</v>
+      <c r="B17" s="22" t="s">
+        <v>84</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>985</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>1108</v>
+        <v>976</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>1082</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>967</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="I17" s="17"/>
+        <v>88</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" s="16"/>
       <c r="J17" s="16" t="s">
-        <v>1109</v>
+        <v>1083</v>
       </c>
       <c r="K17" s="17" t="s">
         <v>996</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="160" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>1055</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>219</v>
+      <c r="B18" s="22" t="s">
+        <v>84</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>220</v>
+        <v>85</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>982</v>
+        <v>976</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>1110</v>
+        <v>1131</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>967</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>201</v>
+        <v>107</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>202</v>
+        <v>108</v>
       </c>
       <c r="I18" s="16"/>
       <c r="J18" s="16" t="s">
-        <v>1111</v>
-      </c>
-      <c r="K18" s="16" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>1113</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>219</v>
+        <v>1055</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>84</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>220</v>
+        <v>85</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>982</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>982</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>1012</v>
+        <v>976</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>1132</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>967</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>1114</v>
+        <v>103</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>1115</v>
+        <v>104</v>
       </c>
       <c r="I19" s="16"/>
       <c r="J19" s="16" t="s">
-        <v>1124</v>
-      </c>
-      <c r="K19" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="K19" s="17" t="s">
         <v>996</v>
       </c>
     </row>
@@ -12912,98 +13183,98 @@
       <c r="A20" s="16" t="s">
         <v>1055</v>
       </c>
-      <c r="B20" s="22" t="s">
-        <v>226</v>
+      <c r="B20" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>227</v>
+        <v>112</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>992</v>
-      </c>
-      <c r="E20" s="42" t="s">
-        <v>1084</v>
+        <v>985</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>1108</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>967</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>233</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="I20" s="16"/>
+        <v>115</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="I20" s="17"/>
       <c r="J20" s="16" t="s">
-        <v>235</v>
+        <v>1109</v>
       </c>
       <c r="K20" s="17" t="s">
         <v>996</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="160" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>1055</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>226</v>
+      <c r="B21" s="14" t="s">
+        <v>219</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>992</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>1085</v>
+        <v>982</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>1110</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>967</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="I21" s="16"/>
       <c r="J21" s="16" t="s">
-        <v>1086</v>
-      </c>
-      <c r="K21" s="17" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+        <v>1111</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>1055</v>
+        <v>1113</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>1020</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>1116</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>967</v>
+        <v>982</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>982</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>1012</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>243</v>
+        <v>1114</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="I22" s="16"/>
       <c r="J22" s="16" t="s">
-        <v>1118</v>
-      </c>
-      <c r="K22" s="17" t="s">
+        <v>1124</v>
+      </c>
+      <c r="K22" s="16" t="s">
         <v>996</v>
       </c>
     </row>
@@ -13011,32 +13282,32 @@
       <c r="A23" s="16" t="s">
         <v>1055</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>249</v>
+      <c r="B23" s="22" t="s">
+        <v>226</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>250</v>
+        <v>227</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>984</v>
+        <v>992</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>1119</v>
+        <v>1084</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>967</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="I23" s="16"/>
       <c r="J23" s="16" t="s">
-        <v>1120</v>
-      </c>
-      <c r="K23" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="K23" s="17" t="s">
         <v>996</v>
       </c>
     </row>
@@ -13045,149 +13316,167 @@
         <v>1055</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>275</v>
+        <v>226</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>276</v>
+        <v>227</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>1087</v>
+        <v>992</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>1085</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>967</v>
       </c>
-      <c r="G24" s="17" t="s">
-        <v>971</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>1022</v>
-      </c>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23" t="s">
-        <v>1023</v>
+      <c r="G24" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16" t="s">
+        <v>1086</v>
       </c>
       <c r="K24" s="17" t="s">
         <v>996</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>1055</v>
       </c>
-      <c r="B25" s="22" t="s">
-        <v>275</v>
+      <c r="B25" s="14" t="s">
+        <v>239</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>276</v>
+        <v>240</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>1088</v>
+        <v>1020</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>1116</v>
       </c>
       <c r="F25" s="16" t="s">
         <v>967</v>
       </c>
-      <c r="G25" s="17" t="s">
-        <v>971</v>
-      </c>
-      <c r="H25" s="23" t="s">
-        <v>1024</v>
-      </c>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23" t="s">
-        <v>1089</v>
+      <c r="G25" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>1117</v>
+      </c>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16" t="s">
+        <v>1118</v>
       </c>
       <c r="K25" s="17" t="s">
         <v>996</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>1055</v>
       </c>
-      <c r="B26" s="22" t="s">
-        <v>997</v>
+      <c r="B26" s="14" t="s">
+        <v>249</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>997</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>1011</v>
-      </c>
-      <c r="E26" s="40" t="s">
-        <v>1062</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>978</v>
-      </c>
-      <c r="G26" s="22"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>984</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16" t="s">
+        <v>1120</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>1055</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>997</v>
+        <v>275</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>997</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>1011</v>
-      </c>
-      <c r="E27" s="40" t="s">
-        <v>1063</v>
-      </c>
-      <c r="F27" s="22" t="s">
-        <v>978</v>
-      </c>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>1022</v>
+      </c>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23" t="s">
+        <v>1023</v>
+      </c>
+      <c r="K27" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>1064</v>
+        <v>1055</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>997</v>
+        <v>275</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>997</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>1013</v>
-      </c>
-      <c r="E28" s="31" t="s">
-        <v>1014</v>
-      </c>
-      <c r="F28" s="25" t="s">
-        <v>978</v>
-      </c>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>1088</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>1024</v>
+      </c>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23" t="s">
+        <v>1089</v>
+      </c>
+      <c r="K28" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>1055</v>
       </c>
@@ -13197,16 +13486,16 @@
       <c r="C29" s="22" t="s">
         <v>997</v>
       </c>
-      <c r="D29" s="23" t="s">
-        <v>1013</v>
-      </c>
-      <c r="E29" s="39" t="s">
-        <v>1065</v>
+      <c r="D29" s="22" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E29" s="40" t="s">
+        <v>1062</v>
       </c>
       <c r="F29" s="22" t="s">
         <v>978</v>
       </c>
-      <c r="G29" s="14"/>
+      <c r="G29" s="22"/>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
@@ -13214,7 +13503,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>1055</v>
       </c>
@@ -13224,11 +13513,11 @@
       <c r="C30" s="22" t="s">
         <v>997</v>
       </c>
-      <c r="D30" s="23" t="s">
-        <v>1013</v>
-      </c>
-      <c r="E30" s="39" t="s">
-        <v>1066</v>
+      <c r="D30" s="22" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E30" s="40" t="s">
+        <v>1063</v>
       </c>
       <c r="F30" s="22" t="s">
         <v>978</v>
@@ -13243,7 +13532,7 @@
     </row>
     <row r="31" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>1055</v>
+        <v>1064</v>
       </c>
       <c r="B31" s="22" t="s">
         <v>997</v>
@@ -13251,13 +13540,13 @@
       <c r="C31" s="22" t="s">
         <v>997</v>
       </c>
-      <c r="D31" s="23" t="s">
+      <c r="D31" s="29" t="s">
         <v>1013</v>
       </c>
-      <c r="E31" s="39" t="s">
-        <v>1067</v>
-      </c>
-      <c r="F31" s="22" t="s">
+      <c r="E31" s="31" t="s">
+        <v>1014</v>
+      </c>
+      <c r="F31" s="25" t="s">
         <v>978</v>
       </c>
       <c r="G31" s="14"/>
@@ -13268,7 +13557,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>1055</v>
       </c>
@@ -13278,11 +13567,11 @@
       <c r="C32" s="22" t="s">
         <v>997</v>
       </c>
-      <c r="D32" s="22" t="s">
-        <v>1015</v>
-      </c>
-      <c r="E32" s="40" t="s">
-        <v>1068</v>
+      <c r="D32" s="23" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E32" s="39" t="s">
+        <v>1065</v>
       </c>
       <c r="F32" s="22" t="s">
         <v>978</v>
@@ -13295,70 +13584,58 @@
         <v>997</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>1055</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>971</v>
+        <v>997</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>1039</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>1015</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>1090</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>967</v>
-      </c>
-      <c r="G33" s="23" t="s">
-        <v>971</v>
-      </c>
-      <c r="H33" s="22" t="s">
-        <v>1016</v>
-      </c>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23" t="s">
-        <v>1017</v>
-      </c>
-      <c r="K33" s="23" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+        <v>997</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E33" s="39" t="s">
+        <v>1066</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>978</v>
+      </c>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>1055</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>971</v>
+        <v>997</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>1039</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>1015</v>
-      </c>
-      <c r="E34" s="43" t="s">
-        <v>1091</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>967</v>
-      </c>
-      <c r="G34" s="23" t="s">
-        <v>971</v>
-      </c>
-      <c r="H34" s="22" t="s">
-        <v>1018</v>
-      </c>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23" t="s">
-        <v>1092</v>
-      </c>
-      <c r="K34" s="23" t="s">
-        <v>996</v>
+        <v>997</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E34" s="39" t="s">
+        <v>1067</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>978</v>
+      </c>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14" t="s">
+        <v>997</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
@@ -13366,146 +13643,152 @@
         <v>1055</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>286</v>
+        <v>997</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>287</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>986</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>1093</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>967</v>
-      </c>
-      <c r="G35" s="16" t="s">
-        <v>300</v>
-      </c>
-      <c r="H35" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16" t="s">
-        <v>302</v>
-      </c>
-      <c r="K35" s="16" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+        <v>997</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E35" s="39" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>978</v>
+      </c>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>1055</v>
       </c>
       <c r="B36" s="22" t="s">
+        <v>997</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>997</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E36" s="40" t="s">
+        <v>1068</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>978</v>
+      </c>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>971</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G37" s="23" t="s">
+        <v>971</v>
+      </c>
+      <c r="H37" s="22" t="s">
+        <v>1016</v>
+      </c>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23" t="s">
+        <v>1017</v>
+      </c>
+      <c r="K37" s="23" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>971</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E38" s="43" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>971</v>
+      </c>
+      <c r="H38" s="22" t="s">
+        <v>1018</v>
+      </c>
+      <c r="I38" s="23"/>
+      <c r="J38" s="23" t="s">
+        <v>1092</v>
+      </c>
+      <c r="K38" s="23" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B39" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C39" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D39" s="16" t="s">
         <v>986</v>
       </c>
-      <c r="E36" s="19" t="s">
-        <v>1094</v>
-      </c>
-      <c r="F36" s="16" t="s">
+      <c r="E39" s="19" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F39" s="16" t="s">
         <v>967</v>
       </c>
-      <c r="G36" s="17" t="s">
-        <v>296</v>
-      </c>
-      <c r="H36" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16" t="s">
-        <v>1095</v>
-      </c>
-      <c r="K36" s="16" t="s">
+      <c r="G39" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="K39" s="16" t="s">
         <v>996</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="25" x14ac:dyDescent="0.25">
-      <c r="A37" s="41" t="s">
-        <v>1069</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>997</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>997</v>
-      </c>
-      <c r="D37" s="25" t="s">
-        <v>972</v>
-      </c>
-      <c r="E37" s="28" t="s">
-        <v>1008</v>
-      </c>
-      <c r="F37" s="25" t="s">
-        <v>978</v>
-      </c>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="14" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="25" x14ac:dyDescent="0.25">
-      <c r="A38" s="41" t="s">
-        <v>1069</v>
-      </c>
-      <c r="B38" s="22" t="s">
-        <v>997</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>997</v>
-      </c>
-      <c r="D38" s="47" t="s">
-        <v>972</v>
-      </c>
-      <c r="E38" s="48" t="s">
-        <v>1009</v>
-      </c>
-      <c r="F38" s="25" t="s">
-        <v>978</v>
-      </c>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="25" x14ac:dyDescent="0.25">
-      <c r="A39" s="41" t="s">
-        <v>1069</v>
-      </c>
-      <c r="B39" s="22" t="s">
-        <v>997</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>997</v>
-      </c>
-      <c r="D39" s="47" t="s">
-        <v>972</v>
-      </c>
-      <c r="E39" s="48" t="s">
-        <v>1010</v>
-      </c>
-      <c r="F39" s="25" t="s">
-        <v>978</v>
-      </c>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14" t="s">
-        <v>997</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
@@ -13513,194 +13796,176 @@
         <v>1055</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>321</v>
+        <v>286</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>322</v>
-      </c>
-      <c r="D40" s="27" t="s">
-        <v>972</v>
+        <v>287</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>986</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="F40" s="16" t="s">
         <v>967</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>971</v>
-      </c>
-      <c r="H40" s="17" t="s">
-        <v>979</v>
-      </c>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17" t="s">
-        <v>980</v>
+        <v>296</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>297</v>
+      </c>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16" t="s">
+        <v>1095</v>
       </c>
       <c r="K40" s="16" t="s">
         <v>996</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
-        <v>1055</v>
+      <c r="A41" s="41" t="s">
+        <v>1069</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>321</v>
+        <v>997</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>322</v>
-      </c>
-      <c r="D41" s="16" t="s">
+        <v>997</v>
+      </c>
+      <c r="D41" s="25" t="s">
         <v>972</v>
       </c>
-      <c r="E41" s="19" t="s">
-        <v>1097</v>
-      </c>
-      <c r="F41" s="16" t="s">
-        <v>967</v>
-      </c>
-      <c r="G41" s="17" t="s">
-        <v>971</v>
-      </c>
-      <c r="H41" s="17" t="s">
-        <v>981</v>
-      </c>
-      <c r="I41" s="17"/>
-      <c r="J41" s="17" t="s">
-        <v>1098</v>
-      </c>
-      <c r="K41" s="16" t="s">
-        <v>996</v>
+      <c r="E41" s="28" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F41" s="25" t="s">
+        <v>978</v>
+      </c>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="14" t="s">
+        <v>997</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
-        <v>1055</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>337</v>
+      <c r="A42" s="41" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>997</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>338</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>983</v>
-      </c>
-      <c r="E42" s="42" t="s">
-        <v>1106</v>
-      </c>
-      <c r="F42" s="16" t="s">
-        <v>967</v>
-      </c>
-      <c r="G42" s="16" t="s">
-        <v>341</v>
-      </c>
-      <c r="H42" s="16" t="s">
-        <v>342</v>
-      </c>
-      <c r="I42" s="16"/>
-      <c r="J42" s="16" t="s">
-        <v>1121</v>
-      </c>
-      <c r="K42" s="17" t="s">
-        <v>996</v>
+        <v>997</v>
+      </c>
+      <c r="D42" s="47" t="s">
+        <v>972</v>
+      </c>
+      <c r="E42" s="48" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F42" s="25" t="s">
+        <v>978</v>
+      </c>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14" t="s">
+        <v>997</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="s">
-        <v>1055</v>
+      <c r="A43" s="41" t="s">
+        <v>1069</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>345</v>
+        <v>997</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>346</v>
-      </c>
-      <c r="D43" s="44" t="s">
-        <v>988</v>
-      </c>
-      <c r="E43" s="45" t="s">
-        <v>1099</v>
-      </c>
-      <c r="F43" s="46" t="s">
-        <v>967</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>352</v>
-      </c>
-      <c r="H43" s="16" t="s">
-        <v>353</v>
-      </c>
-      <c r="I43" s="16"/>
-      <c r="J43" s="16" t="s">
-        <v>354</v>
-      </c>
-      <c r="K43" s="16" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+        <v>997</v>
+      </c>
+      <c r="D43" s="47" t="s">
+        <v>972</v>
+      </c>
+      <c r="E43" s="48" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F43" s="25" t="s">
+        <v>978</v>
+      </c>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>1055</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>346</v>
-      </c>
-      <c r="D44" s="44" t="s">
-        <v>988</v>
-      </c>
-      <c r="E44" s="45" t="s">
-        <v>1100</v>
-      </c>
-      <c r="F44" s="46" t="s">
+        <v>322</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>972</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>1096</v>
+      </c>
+      <c r="F44" s="16" t="s">
         <v>967</v>
       </c>
-      <c r="G44" s="16" t="s">
-        <v>349</v>
-      </c>
-      <c r="H44" s="16" t="s">
-        <v>350</v>
-      </c>
-      <c r="I44" s="16"/>
-      <c r="J44" s="16" t="s">
-        <v>1101</v>
+      <c r="G44" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="H44" s="17" t="s">
+        <v>979</v>
+      </c>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17" t="s">
+        <v>980</v>
       </c>
       <c r="K44" s="16" t="s">
         <v>996</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>1055</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>355</v>
+        <v>321</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>356</v>
+        <v>322</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>987</v>
+        <v>972</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>1102</v>
+        <v>1097</v>
       </c>
       <c r="F45" s="16" t="s">
         <v>967</v>
       </c>
-      <c r="G45" s="16" t="s">
-        <v>369</v>
-      </c>
-      <c r="H45" s="16" t="s">
-        <v>370</v>
-      </c>
-      <c r="I45" s="16"/>
+      <c r="G45" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="H45" s="17" t="s">
+        <v>981</v>
+      </c>
+      <c r="I45" s="17"/>
       <c r="J45" s="17" t="s">
-        <v>1103</v>
+        <v>1098</v>
       </c>
       <c r="K45" s="16" t="s">
         <v>996</v>
@@ -13710,60 +13975,66 @@
       <c r="A46" s="16" t="s">
         <v>1055</v>
       </c>
-      <c r="B46" s="22" t="s">
-        <v>355</v>
+      <c r="B46" s="14" t="s">
+        <v>337</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>356</v>
+        <v>338</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>987</v>
-      </c>
-      <c r="E46" s="19" t="s">
-        <v>1104</v>
+        <v>983</v>
+      </c>
+      <c r="E46" s="42" t="s">
+        <v>1106</v>
       </c>
       <c r="F46" s="16" t="s">
         <v>967</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="I46" s="16"/>
       <c r="J46" s="16" t="s">
-        <v>1105</v>
+        <v>1121</v>
       </c>
       <c r="K46" s="17" t="s">
         <v>996</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>1055</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>997</v>
+        <v>345</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>997</v>
-      </c>
-      <c r="D47" s="22" t="s">
-        <v>1019</v>
-      </c>
-      <c r="E47" s="40" t="s">
-        <v>1070</v>
-      </c>
-      <c r="F47" s="22" t="s">
-        <v>978</v>
-      </c>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14" t="s">
-        <v>997</v>
+        <v>346</v>
+      </c>
+      <c r="D47" s="44" t="s">
+        <v>988</v>
+      </c>
+      <c r="E47" s="45" t="s">
+        <v>1099</v>
+      </c>
+      <c r="F47" s="46" t="s">
+        <v>967</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>352</v>
+      </c>
+      <c r="H47" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="K47" s="16" t="s">
+        <v>996</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="50" x14ac:dyDescent="0.25">
@@ -13771,67 +14042,341 @@
         <v>1055</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>997</v>
+        <v>345</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>997</v>
-      </c>
-      <c r="D48" s="22" t="s">
-        <v>1019</v>
-      </c>
-      <c r="E48" s="40" t="s">
-        <v>1071</v>
-      </c>
-      <c r="F48" s="22" t="s">
-        <v>978</v>
-      </c>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+      <c r="D48" s="44" t="s">
+        <v>988</v>
+      </c>
+      <c r="E48" s="45" t="s">
+        <v>1100</v>
+      </c>
+      <c r="F48" s="46" t="s">
+        <v>967</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>349</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16" t="s">
+        <v>1101</v>
+      </c>
+      <c r="K48" s="16" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>1055</v>
       </c>
-      <c r="B49" s="14" t="s">
-        <v>409</v>
+      <c r="B49" s="22" t="s">
+        <v>355</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>410</v>
+        <v>356</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>1122</v>
+        <v>1102</v>
       </c>
       <c r="F49" s="16" t="s">
         <v>967</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>413</v>
+        <v>369</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>414</v>
+        <v>370</v>
       </c>
       <c r="I49" s="16"/>
-      <c r="J49" s="16" t="s">
-        <v>1123</v>
+      <c r="J49" s="17" t="s">
+        <v>1103</v>
       </c>
       <c r="K49" s="16" t="s">
         <v>996</v>
       </c>
     </row>
+    <row r="50" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>987</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>1104</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G50" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="H50" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16" t="s">
+        <v>1105</v>
+      </c>
+      <c r="K50" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>987</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F51" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G51" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="H51" s="16" t="s">
+        <v>363</v>
+      </c>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="K51" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>987</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F52" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G52" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="H52" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="K52" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>997</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>997</v>
+      </c>
+      <c r="D53" s="22" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E53" s="40" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F53" s="22" t="s">
+        <v>978</v>
+      </c>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="14" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>997</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>997</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E54" s="40" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F54" s="22" t="s">
+        <v>978</v>
+      </c>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>409</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>410</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>989</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>1122</v>
+      </c>
+      <c r="F55" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G55" s="16" t="s">
+        <v>413</v>
+      </c>
+      <c r="H55" s="16" t="s">
+        <v>414</v>
+      </c>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16" t="s">
+        <v>1123</v>
+      </c>
+      <c r="K55" s="16" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A56" s="16" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>997</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>997</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>1125</v>
+      </c>
+      <c r="E56" s="51" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F56" s="22" t="s">
+        <v>978</v>
+      </c>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="14" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A57" s="16" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>997</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>997</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>1125</v>
+      </c>
+      <c r="E57" s="51" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F57" s="22" t="s">
+        <v>978</v>
+      </c>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="14" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>997</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>997</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>1125</v>
+      </c>
+      <c r="E58" s="51" t="s">
+        <v>1128</v>
+      </c>
+      <c r="F58" s="22" t="s">
+        <v>978</v>
+      </c>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="14" t="s">
+        <v>997</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K1" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <autoFilter ref="A1:K58" xr:uid="{00000000-0001-0000-0300-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K51">
       <sortCondition ref="D1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update USDM CT changes file for sprint 2
117, 122
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,19 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E9BB9D-F61C-4E79-AE52-CC41FE1179CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435FBE2F-7BF8-428C-8642-8EA99F4B4FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="590" windowWidth="18960" windowHeight="9820" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1430" yWindow="350" windowWidth="16160" windowHeight="9850" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
     <sheet name="DDF Terminology 2023-06-30" sheetId="26" r:id="rId2"/>
-    <sheet name="Terminology Changes sp1 - new" sheetId="25" r:id="rId3"/>
-    <sheet name="Terminology Changes Sp1 - chg" sheetId="4" r:id="rId4"/>
+    <sheet name="Terminology Changes sp2 - new" sheetId="27" r:id="rId3"/>
+    <sheet name="Terminology Changes sp 2 - chg" sheetId="28" r:id="rId4"/>
+    <sheet name="Terminology Changes sp1 - new" sheetId="25" r:id="rId5"/>
+    <sheet name="Terminology Changes Sp1 - chg" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DDF Terminology 2023-06-30'!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Terminology Changes Sp1 - chg'!$A$1:$K$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Terminology Changes sp 2 - chg'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Terminology Changes Sp1 - chg'!$A$1:$K$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Terminology Changes sp2 - new'!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="1140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2342" uniqueCount="1190">
   <si>
     <t>Code</t>
   </si>
@@ -5586,13 +5590,391 @@
   </si>
   <si>
     <t>Rename UML Item Name. Change UML Item from an Attribute to a Relationship</t>
+  </si>
+  <si>
+    <t>Addition of new Entity</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>C44476</t>
+  </si>
+  <si>
+    <t>Everything that is included in a collection, container, or communication.</t>
+  </si>
+  <si>
+    <t>Addition of new Attribute</t>
+  </si>
+  <si>
+    <t>DDF Content Attribute Terminology</t>
+  </si>
+  <si>
+    <t>sectionNumber</t>
+  </si>
+  <si>
+    <t>Section Number</t>
+  </si>
+  <si>
+    <t>The numeric identifier assigned to a particular document section.</t>
+  </si>
+  <si>
+    <t>sectionTitle</t>
+  </si>
+  <si>
+    <t>Section Title</t>
+  </si>
+  <si>
+    <t>An identifying designation for the document section.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Content Name</t>
+  </si>
+  <si>
+    <t>The literal identifier (i.e., distinctive designation) of the content.</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Content Text</t>
+  </si>
+  <si>
+    <t>A textual representation of the content.</t>
+  </si>
+  <si>
+    <t>Addition of new Relationship</t>
+  </si>
+  <si>
+    <t>contentChildren</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Disease Indication Name</t>
+  </si>
+  <si>
+    <t>The literal identifier (i.e., distinctive designation) of the disease indication.</t>
+  </si>
+  <si>
+    <t>Target Study Population Name</t>
+  </si>
+  <si>
+    <t>The literal identifier (i.e., distinctive designation) of the target study population.</t>
+  </si>
+  <si>
+    <t>Study Objective Name</t>
+  </si>
+  <si>
+    <t>The literal identifier (i.e., distinctive designation) of the study objective.</t>
+  </si>
+  <si>
+    <t>DDF Timing Attribute Terminology</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Timing Label</t>
+  </si>
+  <si>
+    <t>The identifying or descriptive marker that is attached to the timing.</t>
+  </si>
+  <si>
+    <t>Timing Name</t>
+  </si>
+  <si>
+    <t>The literal identifier (i.e., distinctive designation) of the timing.</t>
+  </si>
+  <si>
+    <t>Update USDM Model attribute name</t>
+  </si>
+  <si>
+    <t>DDF Biomedical Concept Attribute Terminology</t>
+  </si>
+  <si>
+    <t>BiomedicalConcept</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>bcName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+  </si>
+  <si>
+    <t>Biomedical Concept Name</t>
+  </si>
+  <si>
+    <t>The literal identifier (i.e., distinctive designation) of the biomedical concept.</t>
+  </si>
+  <si>
+    <t>BiomedicalConceptProperty</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>bcPropertyName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+  </si>
+  <si>
+    <t>Biomedical Concept Property Name</t>
+  </si>
+  <si>
+    <t>The literal identifier (i.e., distinctive designation) of the biomedical concept property.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>organizationName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color rgb="FF1F2328"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>timingDescription</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF1F2328"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>description</t>
+    </r>
+  </si>
+  <si>
+    <t>Timing Description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The textual representation of the chronological relationship between temporal events.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A narrative representation of the biomedical concept category.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>endpointPurposeDescription</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>purpose</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Study Endpoint Purpose Description</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Study Endpoint Purpose</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The textual representation of the study endpoint purpose.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The reason or intention for the study endpoint.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -5691,8 +6073,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F2328"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FF1F2328"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5765,8 +6160,20 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -5878,13 +6285,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -6022,12 +6440,6 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6038,6 +6450,30 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6334,10 +6770,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="51" t="s">
         <v>966</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="52"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -12669,10 +13105,663 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D1745F-094B-493C-A13B-22B89A7AABE3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{503195DC-D1D8-4668-937F-5F13E0D1E503}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.36328125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" style="18" customWidth="1"/>
+    <col min="5" max="6" width="17.81640625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="12.6328125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="22.453125" style="18" customWidth="1"/>
+    <col min="9" max="9" width="14.36328125" style="18" customWidth="1"/>
+    <col min="10" max="10" width="43.54296875" style="18" customWidth="1"/>
+    <col min="11" max="11" width="17" style="18" customWidth="1"/>
+    <col min="12" max="16384" width="8.6328125" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="41.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
+        <v>977</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>973</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>974</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>975</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>968</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>969</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>970</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A2" s="54" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>1141</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>1012</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>1142</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>1141</v>
+      </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="17" t="s">
+        <v>1143</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A3" s="54" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>971</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>967</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>1147</v>
+      </c>
+      <c r="I3" s="14"/>
+      <c r="J3" s="17" t="s">
+        <v>1148</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A4" s="54" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>971</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E4" s="56" t="s">
+        <v>1149</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>967</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>1150</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17" t="s">
+        <v>1151</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A5" s="54" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>971</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E5" s="57" t="s">
+        <v>1152</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>967</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>1153</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17" t="s">
+        <v>1154</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A6" s="54" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>971</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>967</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>1156</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="17" t="s">
+        <v>1157</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="54" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>997</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>997</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>978</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>982</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>967</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>1161</v>
+      </c>
+      <c r="I8" s="14"/>
+      <c r="J8" s="16" t="s">
+        <v>1162</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>338</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>983</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>967</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>1163</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="16" t="s">
+        <v>1164</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>984</v>
+      </c>
+      <c r="E10" s="56" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>967</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>1165</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="16" t="s">
+        <v>1166</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>967</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>1169</v>
+      </c>
+      <c r="I11" s="14"/>
+      <c r="J11" s="17" t="s">
+        <v>1170</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>967</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>1171</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="16" t="s">
+        <v>1172</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:N1" xr:uid="{503195DC-D1D8-4668-937F-5F13E0D1E503}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6613B91-9C94-4373-A8CA-806726FA647F}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.36328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6328125" style="1" customWidth="1"/>
+    <col min="4" max="6" width="14.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6328125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="21.7265625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="42.90625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.81640625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>977</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>973</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>974</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>975</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>968</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>969</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>970</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="37" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>967</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17" t="s">
+        <v>1178</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>1180</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>967</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>1181</v>
+      </c>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17" t="s">
+        <v>1182</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>967</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E5" s="58" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>967</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>971</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>1185</v>
+      </c>
+      <c r="I5" s="23"/>
+      <c r="J5" s="17" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K5" s="23" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>985</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>967</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>1188</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16" t="s">
+        <v>1189</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>996</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:K1" xr:uid="{D6613B91-9C94-4373-A8CA-806726FA647F}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D1745F-094B-493C-A13B-22B89A7AABE3}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12689,16 +13778,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -13293,10 +14379,10 @@
       <c r="A20" s="16" t="s">
         <v>1139</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="47" t="s">
         <v>85</v>
       </c>
       <c r="D20" s="16" t="s">
@@ -13326,10 +14412,10 @@
       <c r="A21" s="16" t="s">
         <v>1139</v>
       </c>
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="47" t="s">
         <v>85</v>
       </c>
       <c r="D21" s="16" t="s">
@@ -14037,10 +15123,10 @@
       <c r="C44" s="22" t="s">
         <v>997</v>
       </c>
-      <c r="D44" s="51" t="s">
+      <c r="D44" s="49" t="s">
         <v>1125</v>
       </c>
-      <c r="E44" s="52" t="s">
+      <c r="E44" s="50" t="s">
         <v>1126</v>
       </c>
       <c r="F44" s="22" t="s">
@@ -14064,10 +15150,10 @@
       <c r="C45" s="22" t="s">
         <v>997</v>
       </c>
-      <c r="D45" s="51" t="s">
+      <c r="D45" s="49" t="s">
         <v>1125</v>
       </c>
-      <c r="E45" s="52" t="s">
+      <c r="E45" s="50" t="s">
         <v>1128</v>
       </c>
       <c r="F45" s="22" t="s">
@@ -14091,7 +15177,7 @@
       <c r="C46" s="22" t="s">
         <v>997</v>
       </c>
-      <c r="D46" s="50" t="s">
+      <c r="D46" s="48" t="s">
         <v>972</v>
       </c>
       <c r="E46" s="27" t="s">
@@ -14397,10 +15483,10 @@
       <c r="A56" s="16" t="s">
         <v>1139</v>
       </c>
-      <c r="B56" s="49" t="s">
+      <c r="B56" s="47" t="s">
         <v>355</v>
       </c>
-      <c r="C56" s="49" t="s">
+      <c r="C56" s="47" t="s">
         <v>356</v>
       </c>
       <c r="D56" s="16" t="s">
@@ -14430,10 +15516,10 @@
       <c r="A57" s="16" t="s">
         <v>1139</v>
       </c>
-      <c r="B57" s="49" t="s">
+      <c r="B57" s="47" t="s">
         <v>355</v>
       </c>
-      <c r="C57" s="49" t="s">
+      <c r="C57" s="47" t="s">
         <v>356</v>
       </c>
       <c r="D57" s="16" t="s">

</xml_diff>

<commit_message>
CT Deliverables for Release 2.3.0
125, 141, 135
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6823D3EE-2844-4B84-B47D-3041198038C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C098E779-F4CF-4C5F-8698-9271A7BF9ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="80" windowWidth="15610" windowHeight="9780" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="420" windowWidth="18760" windowHeight="9780" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2800" uniqueCount="1297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2790" uniqueCount="1297">
   <si>
     <t>Code</t>
   </si>
@@ -7137,12 +7137,6 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -7163,6 +7157,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7458,10 +7458,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="62" t="s">
         <v>966</v>
       </c>
-      <c r="B1" s="56"/>
+      <c r="B1" s="63"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -13733,7 +13733,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -13800,7 +13800,7 @@
       <c r="D2" s="13" t="s">
         <v>1231</v>
       </c>
-      <c r="E2" s="61" t="s">
+      <c r="E2" s="59" t="s">
         <v>1231</v>
       </c>
       <c r="F2" s="16" t="s">
@@ -13833,7 +13833,7 @@
       <c r="D3" s="13" t="s">
         <v>1231</v>
       </c>
-      <c r="E3" s="62" t="s">
+      <c r="E3" s="60" t="s">
         <v>1160</v>
       </c>
       <c r="F3" s="16" t="s">
@@ -13866,7 +13866,7 @@
       <c r="D4" s="13" t="s">
         <v>1231</v>
       </c>
-      <c r="E4" s="62" t="s">
+      <c r="E4" s="60" t="s">
         <v>1236</v>
       </c>
       <c r="F4" s="16" t="s">
@@ -13998,7 +13998,7 @@
       <c r="D8" s="16" t="s">
         <v>1244</v>
       </c>
-      <c r="E8" s="62" t="s">
+      <c r="E8" s="60" t="s">
         <v>1160</v>
       </c>
       <c r="F8" s="16" t="s">
@@ -14031,7 +14031,7 @@
       <c r="D9" s="16" t="s">
         <v>1244</v>
       </c>
-      <c r="E9" s="62" t="s">
+      <c r="E9" s="60" t="s">
         <v>1239</v>
       </c>
       <c r="F9" s="16" t="s">
@@ -14064,7 +14064,7 @@
       <c r="D10" s="16" t="s">
         <v>1244</v>
       </c>
-      <c r="E10" s="62" t="s">
+      <c r="E10" s="60" t="s">
         <v>1168</v>
       </c>
       <c r="F10" s="16" t="s">
@@ -14097,7 +14097,7 @@
       <c r="D11" s="16" t="s">
         <v>1244</v>
       </c>
-      <c r="E11" s="62" t="s">
+      <c r="E11" s="60" t="s">
         <v>1253</v>
       </c>
       <c r="F11" s="16" t="s">
@@ -14130,7 +14130,7 @@
       <c r="D12" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="E12" s="62" t="s">
+      <c r="E12" s="60" t="s">
         <v>1168</v>
       </c>
       <c r="F12" s="15" t="s">
@@ -14163,7 +14163,7 @@
       <c r="D13" s="15" t="s">
         <v>972</v>
       </c>
-      <c r="E13" s="62" t="s">
+      <c r="E13" s="60" t="s">
         <v>1168</v>
       </c>
       <c r="F13" s="15" t="s">
@@ -14196,7 +14196,7 @@
       <c r="D14" s="15" t="s">
         <v>982</v>
       </c>
-      <c r="E14" s="62" t="s">
+      <c r="E14" s="60" t="s">
         <v>1168</v>
       </c>
       <c r="F14" s="15" t="s">
@@ -14229,7 +14229,7 @@
       <c r="D15" s="15" t="s">
         <v>983</v>
       </c>
-      <c r="E15" s="62" t="s">
+      <c r="E15" s="60" t="s">
         <v>1168</v>
       </c>
       <c r="F15" s="15" t="s">
@@ -14262,7 +14262,7 @@
       <c r="D16" s="15" t="s">
         <v>984</v>
       </c>
-      <c r="E16" s="62" t="s">
+      <c r="E16" s="60" t="s">
         <v>1168</v>
       </c>
       <c r="F16" s="15" t="s">
@@ -14295,7 +14295,7 @@
       <c r="D17" s="15" t="s">
         <v>986</v>
       </c>
-      <c r="E17" s="62" t="s">
+      <c r="E17" s="60" t="s">
         <v>1168</v>
       </c>
       <c r="F17" s="15" t="s">
@@ -14328,7 +14328,7 @@
       <c r="D18" s="15" t="s">
         <v>987</v>
       </c>
-      <c r="E18" s="62" t="s">
+      <c r="E18" s="60" t="s">
         <v>1168</v>
       </c>
       <c r="F18" s="15" t="s">
@@ -14361,7 +14361,7 @@
       <c r="D19" s="15" t="s">
         <v>988</v>
       </c>
-      <c r="E19" s="62" t="s">
+      <c r="E19" s="60" t="s">
         <v>1168</v>
       </c>
       <c r="F19" s="15" t="s">
@@ -14394,7 +14394,7 @@
       <c r="D20" s="15" t="s">
         <v>976</v>
       </c>
-      <c r="E20" s="62" t="s">
+      <c r="E20" s="60" t="s">
         <v>1168</v>
       </c>
       <c r="F20" s="15" t="s">
@@ -14427,7 +14427,7 @@
       <c r="D21" s="15" t="s">
         <v>990</v>
       </c>
-      <c r="E21" s="62" t="s">
+      <c r="E21" s="60" t="s">
         <v>1168</v>
       </c>
       <c r="F21" s="15" t="s">
@@ -14460,7 +14460,7 @@
       <c r="D22" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="E22" s="62" t="s">
+      <c r="E22" s="60" t="s">
         <v>1168</v>
       </c>
       <c r="F22" s="15" t="s">
@@ -14493,7 +14493,7 @@
       <c r="D23" s="15" t="s">
         <v>992</v>
       </c>
-      <c r="E23" s="62" t="s">
+      <c r="E23" s="60" t="s">
         <v>1168</v>
       </c>
       <c r="F23" s="15" t="s">
@@ -14526,10 +14526,10 @@
       <c r="D24" s="15" t="s">
         <v>1175</v>
       </c>
-      <c r="E24" s="62" t="s">
+      <c r="E24" s="60" t="s">
         <v>1168</v>
       </c>
-      <c r="F24" s="63" t="s">
+      <c r="F24" s="61" t="s">
         <v>967</v>
       </c>
       <c r="G24" s="16" t="s">
@@ -14559,10 +14559,10 @@
       <c r="D25" s="15" t="s">
         <v>1179</v>
       </c>
-      <c r="E25" s="62" t="s">
+      <c r="E25" s="60" t="s">
         <v>1168</v>
       </c>
-      <c r="F25" s="63" t="s">
+      <c r="F25" s="61" t="s">
         <v>967</v>
       </c>
       <c r="G25" s="16" t="s">
@@ -14592,10 +14592,10 @@
       <c r="D26" s="15" t="s">
         <v>998</v>
       </c>
-      <c r="E26" s="62" t="s">
+      <c r="E26" s="60" t="s">
         <v>1168</v>
       </c>
-      <c r="F26" s="63" t="s">
+      <c r="F26" s="61" t="s">
         <v>967</v>
       </c>
       <c r="G26" s="16" t="s">
@@ -14625,10 +14625,10 @@
       <c r="D27" s="15" t="s">
         <v>1003</v>
       </c>
-      <c r="E27" s="62" t="s">
+      <c r="E27" s="60" t="s">
         <v>1168</v>
       </c>
-      <c r="F27" s="63" t="s">
+      <c r="F27" s="61" t="s">
         <v>967</v>
       </c>
       <c r="G27" s="16" t="s">
@@ -14655,13 +14655,13 @@
       <c r="C28" s="16" t="s">
         <v>1039</v>
       </c>
-      <c r="D28" s="60" t="s">
+      <c r="D28" s="58" t="s">
         <v>1015</v>
       </c>
-      <c r="E28" s="62" t="s">
+      <c r="E28" s="60" t="s">
         <v>1168</v>
       </c>
-      <c r="F28" s="59" t="s">
+      <c r="F28" s="57" t="s">
         <v>967</v>
       </c>
       <c r="G28" s="16" t="s">
@@ -14686,61 +14686,28 @@
         <v>971</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>1167</v>
-      </c>
-      <c r="D29" s="60" t="s">
-        <v>1019</v>
-      </c>
-      <c r="E29" s="62" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D29" s="58" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E29" s="60" t="s">
         <v>1168</v>
       </c>
-      <c r="F29" s="59" t="s">
+      <c r="F29" s="57" t="s">
         <v>967</v>
       </c>
       <c r="G29" s="16" t="s">
         <v>971</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>1169</v>
+        <v>1290</v>
       </c>
       <c r="I29" s="13"/>
       <c r="J29" s="13" t="s">
-        <v>1170</v>
+        <v>1291</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
-        <v>1296</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>971</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>1145</v>
-      </c>
-      <c r="D30" s="60" t="s">
-        <v>1141</v>
-      </c>
-      <c r="E30" s="62" t="s">
-        <v>1168</v>
-      </c>
-      <c r="F30" s="59" t="s">
-        <v>967</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>971</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>1290</v>
-      </c>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13" t="s">
-        <v>1291</v>
-      </c>
-      <c r="K30" s="13" t="s">
         <v>996</v>
       </c>
     </row>
@@ -15017,7 +14984,7 @@
       <c r="D8" s="13" t="s">
         <v>1013</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="55" t="s">
         <v>1211</v>
       </c>
       <c r="F8" s="13" t="s">
@@ -15219,20 +15186,20 @@
       <c r="D14" s="13" t="s">
         <v>1019</v>
       </c>
-      <c r="E14" s="58" t="s">
+      <c r="E14" s="56" t="s">
         <v>1214</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>967</v>
       </c>
-      <c r="G14" s="59" t="s">
+      <c r="G14" s="57" t="s">
         <v>971</v>
       </c>
-      <c r="H14" s="60" t="s">
+      <c r="H14" s="58" t="s">
         <v>1215</v>
       </c>
       <c r="I14" s="13"/>
-      <c r="J14" s="59" t="s">
+      <c r="J14" s="57" t="s">
         <v>1216</v>
       </c>
       <c r="K14" s="16" t="s">

</xml_diff>

<commit_message>
Changes from Ticket 144
Changes from Ticket 144
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -1,36 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0398FD-1305-479F-A285-DD5C6A10D17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CE08D9-8C3C-4C1B-B751-10AFE01E5309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="60" windowWidth="17410" windowHeight="9990" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="17480" windowHeight="9700" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
     <sheet name="DDF Terminology 2023-06-30" sheetId="26" r:id="rId2"/>
-    <sheet name="Terminology Changes sp 5 - new" sheetId="31" r:id="rId3"/>
-    <sheet name="Terminology Changes sp 5 - chg" sheetId="32" r:id="rId4"/>
-    <sheet name="Terminology Changes sp 4 - new" sheetId="30" r:id="rId5"/>
-    <sheet name="Terminology Changes sp 4 - chg" sheetId="29" r:id="rId6"/>
-    <sheet name="Terminology Changes sp2 - new" sheetId="27" r:id="rId7"/>
-    <sheet name="Terminology Changes sp 2 - chg" sheetId="28" r:id="rId8"/>
-    <sheet name="Terminology Changes sp1 - new" sheetId="25" r:id="rId9"/>
-    <sheet name="Terminology Changes Sp1 - chg" sheetId="4" r:id="rId10"/>
+    <sheet name="Terminology Changes sp 6 - new" sheetId="34" r:id="rId3"/>
+    <sheet name="Terminology Changes sp 6 - chg" sheetId="33" r:id="rId4"/>
+    <sheet name="Terminology Changes sp 5 - new" sheetId="31" r:id="rId5"/>
+    <sheet name="Terminology Changes sp 5 - chg" sheetId="32" r:id="rId6"/>
+    <sheet name="Terminology Changes sp 4 - new" sheetId="30" r:id="rId7"/>
+    <sheet name="Terminology Changes sp 4 - chg" sheetId="29" r:id="rId8"/>
+    <sheet name="Terminology Changes sp2 - new" sheetId="27" r:id="rId9"/>
+    <sheet name="Terminology Changes sp 2 - chg" sheetId="28" r:id="rId10"/>
+    <sheet name="Terminology Changes sp1 - new" sheetId="25" r:id="rId11"/>
+    <sheet name="Terminology Changes Sp1 - chg" sheetId="4" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DDF Terminology 2023-06-30'!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Terminology Changes sp 2 - chg'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Terminology Changes sp 4 - chg'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Terminology Changes sp 4 - new'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Terminology Changes Sp1 - chg'!$A$1:$K$60</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Terminology Changes sp2 - new'!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Terminology Changes sp 2 - chg'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Terminology Changes sp 4 - chg'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Terminology Changes sp 4 - new'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Terminology Changes Sp1 - chg'!$A$1:$K$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Terminology Changes sp2 - new'!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3010" uniqueCount="1352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3112" uniqueCount="1372">
   <si>
     <t>Code</t>
   </si>
@@ -7154,13 +7156,129 @@
   </si>
   <si>
     <t>Y (C188726)</t>
+  </si>
+  <si>
+    <t>Add new attribute to TransitionRule entity</t>
+  </si>
+  <si>
+    <t>Add new attribute to AnalysisPopulation entity</t>
+  </si>
+  <si>
+    <t>Transition Rule Name</t>
+  </si>
+  <si>
+    <t>The literal identifier (i.e., distinctive designation) of the transition rule.</t>
+  </si>
+  <si>
+    <t>Transition Rule Label</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the transition rule.</t>
+  </si>
+  <si>
+    <t>Transition Rule Text</t>
+  </si>
+  <si>
+    <t>An instance of unstructured text that represents the transition rule.</t>
+  </si>
+  <si>
+    <t>Analysis Population Name</t>
+  </si>
+  <si>
+    <t>The literal identifier (i.e., distinctive designation) of the analysis population.</t>
+  </si>
+  <si>
+    <t>Analysis Population Label</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the analysis population.</t>
+  </si>
+  <si>
+    <t>Analysis Population Text</t>
+  </si>
+  <si>
+    <t>An instance of unstructured text that represents the analysis population.</t>
+  </si>
+  <si>
+    <t>Investigational Intervention Description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A narrative representation of the study intervention.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A narrative representation of the investigational intervention.</t>
+    </r>
+  </si>
+  <si>
+    <t>A narrative representation of the condition, disease or disorder that the clinical trial is intended to investigate or address.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Y (point out to multiple Biomedical coding dictionaries such as SNOMEDCT (for FDA), MedDRA, NCIt, ICD's, etc.)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N</t>
+    </r>
+  </si>
+  <si>
+    <t>Update Attribute Definition</t>
+  </si>
+  <si>
+    <t>Update Valid Value set information</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -7284,8 +7402,29 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7368,6 +7507,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -7495,12 +7639,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -7689,12 +7834,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -7707,8 +7846,24 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 6" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -8001,10 +8156,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="68" t="s">
         <v>966</v>
       </c>
-      <c r="B1" s="65"/>
+      <c r="B1" s="69"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -8099,6 +8254,251 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6613B91-9C94-4373-A8CA-806726FA647F}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.36328125" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.6328125" customWidth="1"/>
+    <col min="4" max="6" width="14.81640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6328125" customWidth="1"/>
+    <col min="8" max="9" width="21.81640625" customWidth="1"/>
+    <col min="10" max="10" width="42.90625" customWidth="1"/>
+    <col min="11" max="11" width="9.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>977</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>973</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>974</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>975</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>968</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>969</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>970</v>
+      </c>
+      <c r="J1" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="35" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>971</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>971</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16" t="s">
+        <v>1178</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>971</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>1180</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>971</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>1181</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16" t="s">
+        <v>1182</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>971</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E5" s="54" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>971</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>1185</v>
+      </c>
+      <c r="I5" s="21"/>
+      <c r="J5" s="16" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>985</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>1188</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15" t="s">
+        <v>1189</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>996</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:K1" xr:uid="{D6613B91-9C94-4373-A8CA-806726FA647F}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D1745F-094B-493C-A13B-22B89A7AABE3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K60"/>
   <sheetViews>
@@ -9967,8 +10367,8 @@
   <dimension ref="A1:H260"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -10432,12 +10832,12 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="70" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="70" t="s">
         <v>39</v>
       </c>
       <c r="E7" s="30" t="s">
@@ -11590,12 +11990,12 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A59" s="30" t="s">
+      <c r="A59" s="70" t="s">
         <v>219</v>
       </c>
       <c r="B59" s="30"/>
       <c r="C59" s="30"/>
-      <c r="D59" s="30" t="s">
+      <c r="D59" s="70" t="s">
         <v>220</v>
       </c>
       <c r="E59" s="30" t="s">
@@ -11746,12 +12146,12 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A66" s="30" t="s">
+      <c r="A66" s="70" t="s">
         <v>239</v>
       </c>
       <c r="B66" s="30"/>
       <c r="C66" s="30"/>
-      <c r="D66" s="30" t="s">
+      <c r="D66" s="70" t="s">
         <v>240</v>
       </c>
       <c r="E66" s="30" t="s">
@@ -12856,12 +13256,12 @@
       </c>
     </row>
     <row r="116" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A116" s="30" t="s">
+      <c r="A116" s="70" t="s">
         <v>409</v>
       </c>
       <c r="B116" s="30"/>
       <c r="C116" s="30"/>
-      <c r="D116" s="30" t="s">
+      <c r="D116" s="70" t="s">
         <v>410</v>
       </c>
       <c r="E116" s="30" t="s">
@@ -16136,11 +16536,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3BAEC7F-C9CC-43EF-BB4E-AEB1F505CF02}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA34DB14-F4B9-4494-BF11-CA9C6DF92515}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -16198,6 +16598,398 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>989</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>971</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>1354</v>
+      </c>
+      <c r="I2" s="13"/>
+      <c r="J2" s="16" t="s">
+        <v>1355</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>989</v>
+      </c>
+      <c r="E3" s="52" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>971</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>1356</v>
+      </c>
+      <c r="I3" s="13"/>
+      <c r="J3" s="16" t="s">
+        <v>1357</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>989</v>
+      </c>
+      <c r="E4" s="52" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>971</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>1358</v>
+      </c>
+      <c r="I4" s="13"/>
+      <c r="J4" s="16" t="s">
+        <v>1359</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>991</v>
+      </c>
+      <c r="E5" s="52" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>967</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>971</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>1360</v>
+      </c>
+      <c r="I5" s="13"/>
+      <c r="J5" s="16" t="s">
+        <v>1361</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>991</v>
+      </c>
+      <c r="E6" s="52" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>971</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>1362</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="16" t="s">
+        <v>1363</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>991</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>971</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>1364</v>
+      </c>
+      <c r="I7" s="13"/>
+      <c r="J7" s="16" t="s">
+        <v>1365</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9D468B-E509-4E37-947E-729EC706743D}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.36328125" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.6328125" customWidth="1"/>
+    <col min="4" max="6" width="14.81640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6328125" customWidth="1"/>
+    <col min="8" max="9" width="21.81640625" customWidth="1"/>
+    <col min="10" max="10" width="42.90625" customWidth="1"/>
+    <col min="11" max="11" width="18.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="42.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>977</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>973</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>974</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>975</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>968</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>969</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>970</v>
+      </c>
+      <c r="J1" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="35" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="63.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>967</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>1366</v>
+      </c>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15" t="s">
+        <v>1367</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>1371</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>982</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>967</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15" t="s">
+        <v>1368</v>
+      </c>
+      <c r="K3" s="72" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3BAEC7F-C9CC-43EF-BB4E-AEB1F505CF02}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6328125" customWidth="1"/>
+    <col min="8" max="8" width="22.453125" customWidth="1"/>
+    <col min="9" max="9" width="14.36328125" customWidth="1"/>
+    <col min="10" max="10" width="43.54296875" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="41.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>977</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>973</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>974</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>975</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>968</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>969</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>970</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>1140</v>
       </c>
@@ -16223,7 +17015,7 @@
       <c r="K2" s="16"/>
     </row>
     <row r="3" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="64" t="s">
         <v>1302</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -16256,7 +17048,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="64" t="s">
         <v>1302</v>
       </c>
       <c r="B4" s="13" t="s">
@@ -16289,7 +17081,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="64" t="s">
         <v>1302</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -16322,7 +17114,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="64" t="s">
         <v>1302</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -16334,7 +17126,7 @@
       <c r="D6" s="13" t="s">
         <v>1301</v>
       </c>
-      <c r="E6" s="67" t="s">
+      <c r="E6" s="65" t="s">
         <v>1311</v>
       </c>
       <c r="F6" s="16" t="s">
@@ -16355,7 +17147,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="64" t="s">
         <v>1302</v>
       </c>
       <c r="B7" s="13" t="s">
@@ -16388,7 +17180,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="64" t="s">
         <v>1304</v>
       </c>
       <c r="B8" s="13" t="s">
@@ -16415,7 +17207,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="64" t="s">
         <v>1304</v>
       </c>
       <c r="B9" s="13" t="s">
@@ -16578,14 +17370,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DBA91A-E718-4980-9E9A-18D4DBF2CD50}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16647,7 +17438,7 @@
       <c r="D2" s="57" t="s">
         <v>1337</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="66" t="s">
         <v>1337</v>
       </c>
       <c r="F2" s="57" t="s">
@@ -16746,7 +17537,7 @@
       <c r="D5" s="57" t="s">
         <v>1337</v>
       </c>
-      <c r="E5" s="69" t="s">
+      <c r="E5" s="67" t="s">
         <v>1160</v>
       </c>
       <c r="F5" s="56" t="s">
@@ -16897,7 +17688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF8CAFD-EC7B-4D13-AF47-091182230DA0}">
   <dimension ref="A1:K29"/>
   <sheetViews>
@@ -17879,7 +18670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1C8570-9E8C-4EEF-9B82-79DBE6082DD9}">
   <dimension ref="A1:K16"/>
   <sheetViews>
@@ -18432,7 +19223,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{503195DC-D1D8-4668-937F-5F13E0D1E503}">
   <dimension ref="A1:K14"/>
   <sheetViews>
@@ -18906,249 +19697,4 @@
   <autoFilter ref="A1:N1" xr:uid="{503195DC-D1D8-4668-937F-5F13E0D1E503}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6613B91-9C94-4373-A8CA-806726FA647F}">
-  <dimension ref="A1:K6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.36328125" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" customWidth="1"/>
-    <col min="3" max="3" width="17.6328125" customWidth="1"/>
-    <col min="4" max="6" width="14.81640625" customWidth="1"/>
-    <col min="7" max="7" width="10.6328125" customWidth="1"/>
-    <col min="8" max="9" width="21.81640625" customWidth="1"/>
-    <col min="10" max="10" width="42.90625" customWidth="1"/>
-    <col min="11" max="11" width="9.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>977</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>973</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>974</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>975</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>968</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>969</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>970</v>
-      </c>
-      <c r="J1" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="35" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>1173</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>971</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>1174</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>1175</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>1176</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>967</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>971</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>1177</v>
-      </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16" t="s">
-        <v>1178</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>1173</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>971</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>1174</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>1179</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>1180</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>967</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>971</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>1181</v>
-      </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16" t="s">
-        <v>1182</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>1173</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>259</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>1183</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>967</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="50" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>1173</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>971</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>1167</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>1019</v>
-      </c>
-      <c r="E5" s="54" t="s">
-        <v>1184</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>967</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>971</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>1185</v>
-      </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="16" t="s">
-        <v>1186</v>
-      </c>
-      <c r="K5" s="21" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>1173</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>985</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>1187</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>967</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>1188</v>
-      </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15" t="s">
-        <v>1189</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>996</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:K1" xr:uid="{D6613B91-9C94-4373-A8CA-806726FA647F}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D1745F-094B-493C-A13B-22B89A7AABE3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update to USDM CT Changes file
item 163
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CE08D9-8C3C-4C1B-B751-10AFE01E5309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28EF8D7-072F-4E8D-B6A8-D475DCE7C343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="17480" windowHeight="9700" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="260" windowWidth="16650" windowHeight="10010" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3112" uniqueCount="1372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3122" uniqueCount="1378">
   <si>
     <t>Code</t>
   </si>
@@ -7272,6 +7272,24 @@
   </si>
   <si>
     <t>Update Valid Value set information</t>
+  </si>
+  <si>
+    <t>Add new valid value to Objective.level valid value set</t>
+  </si>
+  <si>
+    <t>Objective.level</t>
+  </si>
+  <si>
+    <t>Exploratory Objective</t>
+  </si>
+  <si>
+    <t>valid value</t>
+  </si>
+  <si>
+    <t>C163559</t>
+  </si>
+  <si>
+    <t>The exploratory reason for performing a study in terms of the scientific questions to be answered by the analysis of data collected during the study.</t>
   </si>
 </sst>
 </file>
@@ -7846,12 +7864,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -7861,6 +7873,12 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -7868,7 +7886,18 @@
     <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 6" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -8156,10 +8185,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="71" t="s">
         <v>966</v>
       </c>
-      <c r="B1" s="69"/>
+      <c r="B1" s="72"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -10832,12 +10861,12 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="68" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
-      <c r="D7" s="70" t="s">
+      <c r="D7" s="68" t="s">
         <v>39</v>
       </c>
       <c r="E7" s="30" t="s">
@@ -11990,12 +12019,12 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A59" s="70" t="s">
+      <c r="A59" s="68" t="s">
         <v>219</v>
       </c>
       <c r="B59" s="30"/>
       <c r="C59" s="30"/>
-      <c r="D59" s="70" t="s">
+      <c r="D59" s="68" t="s">
         <v>220</v>
       </c>
       <c r="E59" s="30" t="s">
@@ -12146,12 +12175,12 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A66" s="70" t="s">
+      <c r="A66" s="68" t="s">
         <v>239</v>
       </c>
       <c r="B66" s="30"/>
       <c r="C66" s="30"/>
-      <c r="D66" s="70" t="s">
+      <c r="D66" s="68" t="s">
         <v>240</v>
       </c>
       <c r="E66" s="30" t="s">
@@ -13256,12 +13285,12 @@
       </c>
     </row>
     <row r="116" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A116" s="70" t="s">
+      <c r="A116" s="68" t="s">
         <v>409</v>
       </c>
       <c r="B116" s="30"/>
       <c r="C116" s="30"/>
-      <c r="D116" s="70" t="s">
+      <c r="D116" s="68" t="s">
         <v>410</v>
       </c>
       <c r="E116" s="30" t="s">
@@ -16540,7 +16569,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -16795,7 +16824,43 @@
         <v>996</v>
       </c>
     </row>
+    <row r="8" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>1373</v>
+      </c>
+      <c r="E8" s="52" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>1375</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>1376</v>
+      </c>
+      <c r="H8" s="57" t="s">
+        <v>1374</v>
+      </c>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15" t="s">
+        <v>1377</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>997</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -16869,7 +16934,7 @@
       <c r="C2" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="69" t="s">
         <v>1020</v>
       </c>
       <c r="E2" s="17" t="s">
@@ -16921,7 +16986,7 @@
       <c r="J3" s="15" t="s">
         <v>1368</v>
       </c>
-      <c r="K3" s="72" t="s">
+      <c r="K3" s="70" t="s">
         <v>1369</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes based on Berber QC
Remove name, label, description attributes from Objective, Endpoint, and EligibilityCriteria classes. Remove 'content' relationship from StudyDesign.
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36691CBF-2C43-4266-B81D-01F20549E409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA30488-433A-4578-AC77-21B70F5833F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="310" yWindow="450" windowWidth="17330" windowHeight="9230" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="17320" windowHeight="9730" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4161" uniqueCount="1576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4258" uniqueCount="1579">
   <si>
     <t>Code</t>
   </si>
@@ -7991,6 +7991,15 @@
   </si>
   <si>
     <t>Update class name in valid value set tab</t>
+  </si>
+  <si>
+    <t>Remove Relationship from existing Entity</t>
+  </si>
+  <si>
+    <t>A narrative representation of the study objective. (BRIDG)</t>
+  </si>
+  <si>
+    <t>A narrative representation of the study endpoint.</t>
   </si>
 </sst>
 </file>
@@ -8376,7 +8385,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -8589,12 +8598,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -8634,11 +8637,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -8647,17 +8668,7 @@
     <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 6" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -8976,10 +8987,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="85" t="s">
         <v>966</v>
       </c>
-      <c r="B1" s="73"/>
+      <c r="B1" s="86"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -18640,7 +18651,7 @@
       <c r="J7" s="16" t="s">
         <v>1469</v>
       </c>
-      <c r="K7" s="88" t="s">
+      <c r="K7" s="16" t="s">
         <v>1560</v>
       </c>
     </row>
@@ -19176,7 +19187,7 @@
       <c r="D25" s="15" t="s">
         <v>1503</v>
       </c>
-      <c r="E25" s="85" t="s">
+      <c r="E25" s="83" t="s">
         <v>1503</v>
       </c>
       <c r="F25" s="16" t="s">
@@ -19595,7 +19606,7 @@
       <c r="F38" s="16" t="s">
         <v>967</v>
       </c>
-      <c r="G38" s="86" t="s">
+      <c r="G38" s="84" t="s">
         <v>1405</v>
       </c>
       <c r="H38" s="16" t="s">
@@ -19628,7 +19639,7 @@
       <c r="F39" s="16" t="s">
         <v>967</v>
       </c>
-      <c r="G39" s="86" t="s">
+      <c r="G39" s="84" t="s">
         <v>1409</v>
       </c>
       <c r="H39" s="16" t="s">
@@ -19906,7 +19917,7 @@
         <v>1529</v>
       </c>
       <c r="I48" s="15"/>
-      <c r="J48" s="87" t="s">
+      <c r="J48" s="15" t="s">
         <v>1549</v>
       </c>
       <c r="K48" s="16" t="s">
@@ -19942,7 +19953,7 @@
       <c r="J49" s="13" t="s">
         <v>1531</v>
       </c>
-      <c r="K49" s="88" t="s">
+      <c r="K49" s="16" t="s">
         <v>1573</v>
       </c>
     </row>
@@ -20185,7 +20196,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -20285,7 +20296,7 @@
       <c r="D3" s="15" t="s">
         <v>1382</v>
       </c>
-      <c r="E3" s="74" t="s">
+      <c r="E3" s="72" t="s">
         <v>1384</v>
       </c>
       <c r="F3" s="63" t="s">
@@ -20318,7 +20329,7 @@
       <c r="D4" s="15" t="s">
         <v>1382</v>
       </c>
-      <c r="E4" s="74" t="s">
+      <c r="E4" s="72" t="s">
         <v>1386</v>
       </c>
       <c r="F4" s="63" t="s">
@@ -20351,7 +20362,7 @@
       <c r="D5" s="23" t="s">
         <v>1191</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="73" t="s">
         <v>1388</v>
       </c>
       <c r="F5" s="23" t="s">
@@ -20405,7 +20416,7 @@
       <c r="D7" s="23" t="s">
         <v>1191</v>
       </c>
-      <c r="E7" s="75" t="s">
+      <c r="E7" s="73" t="s">
         <v>1391</v>
       </c>
       <c r="F7" s="23" t="s">
@@ -20432,7 +20443,7 @@
       <c r="D8" s="23" t="s">
         <v>1191</v>
       </c>
-      <c r="E8" s="74" t="s">
+      <c r="E8" s="72" t="s">
         <v>1393</v>
       </c>
       <c r="F8" s="23" t="s">
@@ -20467,7 +20478,7 @@
       <c r="D9" s="23" t="s">
         <v>1191</v>
       </c>
-      <c r="E9" s="74" t="s">
+      <c r="E9" s="72" t="s">
         <v>1395</v>
       </c>
       <c r="F9" s="23" t="s">
@@ -20500,7 +20511,7 @@
       <c r="D10" s="23" t="s">
         <v>1191</v>
       </c>
-      <c r="E10" s="74" t="s">
+      <c r="E10" s="72" t="s">
         <v>1396</v>
       </c>
       <c r="F10" s="23" t="s">
@@ -20535,7 +20546,7 @@
       <c r="D11" s="23" t="s">
         <v>1191</v>
       </c>
-      <c r="E11" s="74" t="s">
+      <c r="E11" s="72" t="s">
         <v>1397</v>
       </c>
       <c r="F11" s="23" t="s">
@@ -20570,7 +20581,7 @@
       <c r="D12" s="23" t="s">
         <v>1191</v>
       </c>
-      <c r="E12" s="74" t="s">
+      <c r="E12" s="72" t="s">
         <v>1400</v>
       </c>
       <c r="F12" s="23" t="s">
@@ -20603,13 +20614,13 @@
       <c r="D13" s="23" t="s">
         <v>1191</v>
       </c>
-      <c r="E13" s="74" t="s">
+      <c r="E13" s="72" t="s">
         <v>1404</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>967</v>
       </c>
-      <c r="G13" s="76" t="s">
+      <c r="G13" s="74" t="s">
         <v>1405</v>
       </c>
       <c r="H13" s="63" t="s">
@@ -20636,13 +20647,13 @@
       <c r="D14" s="23" t="s">
         <v>1191</v>
       </c>
-      <c r="E14" s="74" t="s">
+      <c r="E14" s="72" t="s">
         <v>1408</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>967</v>
       </c>
-      <c r="G14" s="76" t="s">
+      <c r="G14" s="74" t="s">
         <v>1409</v>
       </c>
       <c r="H14" s="63" t="s">
@@ -20656,655 +20667,683 @@
         <v>996</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="112.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>1574</v>
-      </c>
-      <c r="B15" s="77" t="s">
-        <v>708</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="78" t="s">
-        <v>1191</v>
-      </c>
-      <c r="E15" s="77" t="s">
-        <v>1192</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>1412</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>713</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="I15" s="79"/>
-      <c r="J15" s="15" t="s">
-        <v>1413</v>
-      </c>
-      <c r="K15" s="16" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="D15" s="88" t="s">
+        <v>984</v>
+      </c>
+      <c r="E15" s="72" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G15" s="89" t="s">
+        <v>253</v>
+      </c>
+      <c r="H15" s="89" t="s">
+        <v>254</v>
+      </c>
+      <c r="I15" s="89"/>
+      <c r="J15" s="89" t="s">
+        <v>1577</v>
+      </c>
+      <c r="K15" s="89" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="D16" s="88" t="s">
+        <v>984</v>
+      </c>
+      <c r="E16" s="72" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G16" s="89" t="s">
+        <v>971</v>
+      </c>
+      <c r="H16" s="90" t="s">
+        <v>1165</v>
+      </c>
+      <c r="I16" s="91"/>
+      <c r="J16" s="89" t="s">
+        <v>1166</v>
+      </c>
+      <c r="K16" s="90" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="D17" s="88" t="s">
+        <v>984</v>
+      </c>
+      <c r="E17" s="72" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G17" s="89" t="s">
+        <v>971</v>
+      </c>
+      <c r="H17" s="91" t="s">
+        <v>1256</v>
+      </c>
+      <c r="I17" s="91"/>
+      <c r="J17" s="91" t="s">
+        <v>1280</v>
+      </c>
+      <c r="K17" s="91" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="88" t="s">
+        <v>985</v>
+      </c>
+      <c r="E18" s="72" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G18" s="89" t="s">
+        <v>115</v>
+      </c>
+      <c r="H18" s="90" t="s">
+        <v>116</v>
+      </c>
+      <c r="I18" s="90"/>
+      <c r="J18" s="89" t="s">
+        <v>1578</v>
+      </c>
+      <c r="K18" s="90" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="88" t="s">
+        <v>985</v>
+      </c>
+      <c r="E19" s="72" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G19" s="89" t="s">
+        <v>971</v>
+      </c>
+      <c r="H19" s="90" t="s">
+        <v>1333</v>
+      </c>
+      <c r="I19" s="91"/>
+      <c r="J19" s="90" t="s">
+        <v>1334</v>
+      </c>
+      <c r="K19" s="90" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="88" t="s">
+        <v>985</v>
+      </c>
+      <c r="E20" s="72" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G20" s="89" t="s">
+        <v>971</v>
+      </c>
+      <c r="H20" s="90" t="s">
+        <v>1335</v>
+      </c>
+      <c r="I20" s="91"/>
+      <c r="J20" s="90" t="s">
+        <v>1336</v>
+      </c>
+      <c r="K20" s="90" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>971</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D21" s="87" t="s">
+        <v>1301</v>
+      </c>
+      <c r="E21" s="72" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G21" s="92" t="s">
+        <v>971</v>
+      </c>
+      <c r="H21" s="91" t="s">
+        <v>1305</v>
+      </c>
+      <c r="I21" s="91"/>
+      <c r="J21" s="90" t="s">
+        <v>1306</v>
+      </c>
+      <c r="K21" s="90" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>971</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D22" s="87" t="s">
+        <v>1301</v>
+      </c>
+      <c r="E22" s="72" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G22" s="92" t="s">
+        <v>971</v>
+      </c>
+      <c r="H22" s="91" t="s">
+        <v>1307</v>
+      </c>
+      <c r="I22" s="91"/>
+      <c r="J22" s="91" t="s">
+        <v>1308</v>
+      </c>
+      <c r="K22" s="90" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>971</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D23" s="87" t="s">
+        <v>1301</v>
+      </c>
+      <c r="E23" s="72" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G23" s="92" t="s">
+        <v>971</v>
+      </c>
+      <c r="H23" s="91" t="s">
+        <v>1309</v>
+      </c>
+      <c r="I23" s="91"/>
+      <c r="J23" s="91" t="s">
+        <v>1310</v>
+      </c>
+      <c r="K23" s="90" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>997</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>1574</v>
-      </c>
-      <c r="B16" s="77" t="s">
-        <v>708</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="78" t="s">
-        <v>1191</v>
-      </c>
-      <c r="E16" s="77" t="s">
-        <v>1192</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>1412</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>718</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>719</v>
-      </c>
-      <c r="I16" s="79"/>
-      <c r="J16" s="15" t="s">
-        <v>720</v>
-      </c>
-      <c r="K16" s="13"/>
-    </row>
-    <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>1574</v>
-      </c>
-      <c r="B17" s="77" t="s">
-        <v>708</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="78" t="s">
-        <v>1191</v>
-      </c>
-      <c r="E17" s="77" t="s">
-        <v>1192</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>1412</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>722</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>723</v>
-      </c>
-      <c r="I17" s="79"/>
-      <c r="J17" s="15" t="s">
-        <v>724</v>
-      </c>
-      <c r="K17" s="13"/>
-    </row>
-    <row r="18" spans="1:11" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>1574</v>
-      </c>
-      <c r="B18" s="77" t="s">
-        <v>708</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="78" t="s">
-        <v>1191</v>
-      </c>
-      <c r="E18" s="77" t="s">
-        <v>1192</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>1412</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>726</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>727</v>
-      </c>
-      <c r="I18" s="79"/>
-      <c r="J18" s="15" t="s">
-        <v>728</v>
-      </c>
-      <c r="K18" s="13"/>
-    </row>
-    <row r="19" spans="1:11" ht="50" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>1575</v>
-      </c>
-      <c r="B19" s="77" t="s">
-        <v>667</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="80" t="s">
-        <v>1382</v>
-      </c>
-      <c r="E19" s="77" t="s">
-        <v>1414</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>1412</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>675</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>676</v>
-      </c>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15" t="s">
-        <v>677</v>
-      </c>
-      <c r="K19" s="13"/>
-    </row>
-    <row r="20" spans="1:11" ht="50" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
-        <v>1575</v>
-      </c>
-      <c r="B20" s="77" t="s">
-        <v>667</v>
-      </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="80" t="s">
-        <v>1382</v>
-      </c>
-      <c r="E20" s="77" t="s">
-        <v>1414</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>1412</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>684</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>685</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>686</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>687</v>
-      </c>
-      <c r="K20" s="13"/>
-    </row>
-    <row r="21" spans="1:11" ht="50" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
-        <v>1575</v>
-      </c>
-      <c r="B21" s="77" t="s">
-        <v>667</v>
-      </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="80" t="s">
-        <v>1382</v>
-      </c>
-      <c r="E21" s="77" t="s">
-        <v>1414</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>1412</v>
-      </c>
-      <c r="G21" s="15" t="s">
-        <v>671</v>
-      </c>
-      <c r="H21" s="15" t="s">
-        <v>672</v>
-      </c>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15" t="s">
-        <v>673</v>
-      </c>
-      <c r="K21" s="13"/>
-    </row>
-    <row r="22" spans="1:11" ht="50" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
-        <v>1575</v>
-      </c>
-      <c r="B22" s="77" t="s">
-        <v>667</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="80" t="s">
-        <v>1382</v>
-      </c>
-      <c r="E22" s="77" t="s">
-        <v>1414</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>1412</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>678</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>679</v>
-      </c>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15" t="s">
-        <v>680</v>
-      </c>
-      <c r="K22" s="13"/>
-    </row>
-    <row r="23" spans="1:11" ht="50" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
-        <v>1575</v>
-      </c>
-      <c r="B23" s="77" t="s">
-        <v>667</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="80" t="s">
-        <v>1382</v>
-      </c>
-      <c r="E23" s="77" t="s">
-        <v>1414</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>1412</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>681</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>682</v>
-      </c>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15" t="s">
-        <v>683</v>
-      </c>
-      <c r="K23" s="13"/>
-    </row>
-    <row r="24" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
-        <v>1574</v>
-      </c>
-      <c r="B24" s="77" t="s">
-        <v>652</v>
-      </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="78" t="s">
-        <v>149</v>
-      </c>
-      <c r="E24" s="77" t="s">
-        <v>1195</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>1412</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>660</v>
-      </c>
-      <c r="H24" s="57" t="s">
-        <v>661</v>
-      </c>
-      <c r="I24" s="15" t="s">
-        <v>662</v>
-      </c>
-      <c r="J24" s="15" t="s">
-        <v>995</v>
-      </c>
-      <c r="K24" s="13"/>
-    </row>
-    <row r="25" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="C24" s="16" t="s">
+        <v>997</v>
+      </c>
+      <c r="D24" s="87" t="s">
+        <v>972</v>
+      </c>
+      <c r="E24" s="72" t="s">
+        <v>1501</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>978</v>
+      </c>
+      <c r="G24" s="74"/>
+      <c r="H24" s="63"/>
+      <c r="I24" s="63"/>
+      <c r="J24" s="63"/>
+      <c r="K24" s="16" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B25" s="77" t="s">
-        <v>652</v>
+      <c r="B25" s="75" t="s">
+        <v>708</v>
       </c>
       <c r="C25" s="13"/>
-      <c r="D25" s="78" t="s">
-        <v>149</v>
-      </c>
-      <c r="E25" s="77" t="s">
-        <v>1195</v>
+      <c r="D25" s="76" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E25" s="75" t="s">
+        <v>1192</v>
       </c>
       <c r="F25" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>656</v>
+        <v>713</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>657</v>
-      </c>
-      <c r="I25" s="15"/>
+        <v>714</v>
+      </c>
+      <c r="I25" s="77"/>
       <c r="J25" s="15" t="s">
-        <v>658</v>
-      </c>
-      <c r="K25" s="13"/>
-    </row>
-    <row r="26" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
+        <v>1413</v>
+      </c>
+      <c r="K25" s="16" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B26" s="77" t="s">
-        <v>652</v>
+      <c r="B26" s="75" t="s">
+        <v>708</v>
       </c>
       <c r="C26" s="13"/>
-      <c r="D26" s="78" t="s">
-        <v>149</v>
-      </c>
-      <c r="E26" s="77" t="s">
-        <v>1195</v>
+      <c r="D26" s="76" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E26" s="75" t="s">
+        <v>1192</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>663</v>
+        <v>718</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>664</v>
-      </c>
-      <c r="I26" s="15" t="s">
-        <v>1415</v>
-      </c>
+        <v>719</v>
+      </c>
+      <c r="I26" s="77"/>
       <c r="J26" s="15" t="s">
-        <v>1416</v>
+        <v>720</v>
       </c>
       <c r="K26" s="13"/>
     </row>
-    <row r="27" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B27" s="77" t="s">
-        <v>638</v>
+      <c r="B27" s="75" t="s">
+        <v>708</v>
       </c>
       <c r="C27" s="13"/>
-      <c r="D27" s="78" t="s">
-        <v>984</v>
-      </c>
-      <c r="E27" s="77" t="s">
-        <v>1347</v>
+      <c r="D27" s="76" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E27" s="75" t="s">
+        <v>1192</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>642</v>
+        <v>722</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>643</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>1417</v>
-      </c>
+        <v>723</v>
+      </c>
+      <c r="I27" s="77"/>
       <c r="J27" s="15" t="s">
-        <v>645</v>
+        <v>724</v>
       </c>
       <c r="K27" s="13"/>
     </row>
-    <row r="28" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="137.5" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B28" s="77" t="s">
-        <v>638</v>
+      <c r="B28" s="75" t="s">
+        <v>708</v>
       </c>
       <c r="C28" s="13"/>
-      <c r="D28" s="78" t="s">
-        <v>984</v>
-      </c>
-      <c r="E28" s="77" t="s">
-        <v>1347</v>
+      <c r="D28" s="76" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E28" s="75" t="s">
+        <v>1192</v>
       </c>
       <c r="F28" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>647</v>
+        <v>726</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>648</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>1418</v>
-      </c>
+        <v>727</v>
+      </c>
+      <c r="I28" s="77"/>
       <c r="J28" s="15" t="s">
-        <v>650</v>
+        <v>728</v>
       </c>
       <c r="K28" s="13"/>
     </row>
-    <row r="29" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>1574</v>
-      </c>
-      <c r="B29" s="77" t="s">
-        <v>638</v>
+        <v>1575</v>
+      </c>
+      <c r="B29" s="75" t="s">
+        <v>667</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="78" t="s">
-        <v>984</v>
-      </c>
-      <c r="E29" s="77" t="s">
-        <v>1347</v>
+        <v>1382</v>
+      </c>
+      <c r="E29" s="75" t="s">
+        <v>1414</v>
       </c>
       <c r="F29" s="16" t="s">
         <v>1412</v>
       </c>
-      <c r="G29" s="57" t="s">
-        <v>1376</v>
-      </c>
-      <c r="H29" s="57" t="s">
-        <v>1374</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>1378</v>
-      </c>
+      <c r="G29" s="15" t="s">
+        <v>675</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>676</v>
+      </c>
+      <c r="I29" s="15"/>
       <c r="J29" s="15" t="s">
-        <v>1377</v>
+        <v>677</v>
       </c>
       <c r="K29" s="13"/>
     </row>
-    <row r="30" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>1574</v>
-      </c>
-      <c r="B30" s="77" t="s">
-        <v>440</v>
+        <v>1575</v>
+      </c>
+      <c r="B30" s="75" t="s">
+        <v>667</v>
       </c>
       <c r="C30" s="13"/>
       <c r="D30" s="78" t="s">
-        <v>985</v>
-      </c>
-      <c r="E30" s="77" t="s">
-        <v>1419</v>
+        <v>1382</v>
+      </c>
+      <c r="E30" s="75" t="s">
+        <v>1414</v>
       </c>
       <c r="F30" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>447</v>
+        <v>684</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>448</v>
-      </c>
-      <c r="I30" s="15"/>
+        <v>685</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>686</v>
+      </c>
       <c r="J30" s="15" t="s">
-        <v>449</v>
+        <v>687</v>
       </c>
       <c r="K30" s="13"/>
     </row>
-    <row r="31" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>1574</v>
-      </c>
-      <c r="B31" s="77" t="s">
-        <v>440</v>
+        <v>1575</v>
+      </c>
+      <c r="B31" s="75" t="s">
+        <v>667</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="78" t="s">
-        <v>985</v>
-      </c>
-      <c r="E31" s="77" t="s">
-        <v>1419</v>
+        <v>1382</v>
+      </c>
+      <c r="E31" s="75" t="s">
+        <v>1414</v>
       </c>
       <c r="F31" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>450</v>
+        <v>671</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>451</v>
+        <v>672</v>
       </c>
       <c r="I31" s="15"/>
       <c r="J31" s="15" t="s">
-        <v>452</v>
+        <v>673</v>
       </c>
       <c r="K31" s="13"/>
     </row>
-    <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>1574</v>
-      </c>
-      <c r="B32" s="77" t="s">
-        <v>440</v>
+        <v>1575</v>
+      </c>
+      <c r="B32" s="75" t="s">
+        <v>667</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="78" t="s">
-        <v>985</v>
-      </c>
-      <c r="E32" s="77" t="s">
-        <v>1419</v>
+        <v>1382</v>
+      </c>
+      <c r="E32" s="75" t="s">
+        <v>1414</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>444</v>
+        <v>678</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>445</v>
+        <v>679</v>
       </c>
       <c r="I32" s="15"/>
       <c r="J32" s="15" t="s">
-        <v>446</v>
+        <v>680</v>
       </c>
       <c r="K32" s="13"/>
     </row>
-    <row r="33" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>1574</v>
-      </c>
-      <c r="B33" s="77" t="s">
-        <v>688</v>
+        <v>1575</v>
+      </c>
+      <c r="B33" s="75" t="s">
+        <v>667</v>
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="78" t="s">
-        <v>986</v>
-      </c>
-      <c r="E33" s="77" t="s">
-        <v>1203</v>
+        <v>1382</v>
+      </c>
+      <c r="E33" s="75" t="s">
+        <v>1414</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>695</v>
+        <v>681</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="I33" s="15"/>
       <c r="J33" s="15" t="s">
-        <v>697</v>
+        <v>683</v>
       </c>
       <c r="K33" s="13"/>
     </row>
-    <row r="34" spans="1:11" ht="162.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B34" s="77" t="s">
-        <v>688</v>
+      <c r="B34" s="75" t="s">
+        <v>652</v>
       </c>
       <c r="C34" s="13"/>
-      <c r="D34" s="78" t="s">
-        <v>986</v>
-      </c>
-      <c r="E34" s="77" t="s">
-        <v>1203</v>
+      <c r="D34" s="76" t="s">
+        <v>149</v>
+      </c>
+      <c r="E34" s="75" t="s">
+        <v>1195</v>
       </c>
       <c r="F34" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>698</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>699</v>
-      </c>
-      <c r="I34" s="15"/>
+        <v>660</v>
+      </c>
+      <c r="H34" s="57" t="s">
+        <v>661</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>662</v>
+      </c>
       <c r="J34" s="15" t="s">
-        <v>700</v>
+        <v>995</v>
       </c>
       <c r="K34" s="13"/>
     </row>
-    <row r="35" spans="1:11" ht="100" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B35" s="77" t="s">
-        <v>688</v>
+      <c r="B35" s="75" t="s">
+        <v>652</v>
       </c>
       <c r="C35" s="13"/>
-      <c r="D35" s="78" t="s">
-        <v>986</v>
-      </c>
-      <c r="E35" s="77" t="s">
-        <v>1203</v>
+      <c r="D35" s="76" t="s">
+        <v>149</v>
+      </c>
+      <c r="E35" s="75" t="s">
+        <v>1195</v>
       </c>
       <c r="F35" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>702</v>
+        <v>656</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>703</v>
+        <v>657</v>
       </c>
       <c r="I35" s="15"/>
       <c r="J35" s="15" t="s">
-        <v>704</v>
+        <v>658</v>
       </c>
       <c r="K35" s="13"/>
     </row>
-    <row r="36" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B36" s="77" t="s">
-        <v>688</v>
+      <c r="B36" s="75" t="s">
+        <v>652</v>
       </c>
       <c r="C36" s="13"/>
-      <c r="D36" s="78" t="s">
-        <v>986</v>
-      </c>
-      <c r="E36" s="77" t="s">
-        <v>1203</v>
+      <c r="D36" s="76" t="s">
+        <v>149</v>
+      </c>
+      <c r="E36" s="75" t="s">
+        <v>1195</v>
       </c>
       <c r="F36" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>705</v>
+        <v>663</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>706</v>
-      </c>
-      <c r="I36" s="15"/>
+        <v>664</v>
+      </c>
+      <c r="I36" s="15" t="s">
+        <v>1415</v>
+      </c>
       <c r="J36" s="15" t="s">
-        <v>707</v>
+        <v>1416</v>
       </c>
       <c r="K36" s="13"/>
     </row>
@@ -21312,28 +21351,30 @@
       <c r="A37" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B37" s="77" t="s">
-        <v>688</v>
+      <c r="B37" s="75" t="s">
+        <v>638</v>
       </c>
       <c r="C37" s="13"/>
-      <c r="D37" s="78" t="s">
-        <v>986</v>
-      </c>
-      <c r="E37" s="77" t="s">
-        <v>1203</v>
+      <c r="D37" s="76" t="s">
+        <v>984</v>
+      </c>
+      <c r="E37" s="75" t="s">
+        <v>1347</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>692</v>
+        <v>642</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>693</v>
-      </c>
-      <c r="I37" s="15"/>
+        <v>643</v>
+      </c>
+      <c r="I37" s="15" t="s">
+        <v>1417</v>
+      </c>
       <c r="J37" s="15" t="s">
-        <v>694</v>
+        <v>645</v>
       </c>
       <c r="K37" s="13"/>
     </row>
@@ -21341,28 +21382,30 @@
       <c r="A38" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B38" s="77" t="s">
-        <v>529</v>
+      <c r="B38" s="75" t="s">
+        <v>638</v>
       </c>
       <c r="C38" s="13"/>
-      <c r="D38" s="78" t="s">
-        <v>987</v>
-      </c>
-      <c r="E38" s="77" t="s">
-        <v>1206</v>
+      <c r="D38" s="76" t="s">
+        <v>984</v>
+      </c>
+      <c r="E38" s="75" t="s">
+        <v>1347</v>
       </c>
       <c r="F38" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>534</v>
+        <v>647</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>535</v>
-      </c>
-      <c r="I38" s="15"/>
+        <v>648</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>1418</v>
+      </c>
       <c r="J38" s="15" t="s">
-        <v>536</v>
+        <v>650</v>
       </c>
       <c r="K38" s="13"/>
     </row>
@@ -21370,119 +21413,117 @@
       <c r="A39" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B39" s="77" t="s">
-        <v>529</v>
+      <c r="B39" s="75" t="s">
+        <v>638</v>
       </c>
       <c r="C39" s="13"/>
-      <c r="D39" s="78" t="s">
-        <v>987</v>
-      </c>
-      <c r="E39" s="77" t="s">
-        <v>1206</v>
+      <c r="D39" s="76" t="s">
+        <v>984</v>
+      </c>
+      <c r="E39" s="75" t="s">
+        <v>1347</v>
       </c>
       <c r="F39" s="16" t="s">
         <v>1412</v>
       </c>
-      <c r="G39" s="15" t="s">
-        <v>538</v>
-      </c>
-      <c r="H39" s="15" t="s">
-        <v>539</v>
-      </c>
-      <c r="I39" s="15"/>
+      <c r="G39" s="57" t="s">
+        <v>1376</v>
+      </c>
+      <c r="H39" s="57" t="s">
+        <v>1374</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>1378</v>
+      </c>
       <c r="J39" s="15" t="s">
-        <v>540</v>
+        <v>1377</v>
       </c>
       <c r="K39" s="13"/>
     </row>
-    <row r="40" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B40" s="77" t="s">
-        <v>529</v>
+      <c r="B40" s="75" t="s">
+        <v>440</v>
       </c>
       <c r="C40" s="13"/>
-      <c r="D40" s="78" t="s">
-        <v>987</v>
-      </c>
-      <c r="E40" s="77" t="s">
-        <v>1206</v>
+      <c r="D40" s="76" t="s">
+        <v>985</v>
+      </c>
+      <c r="E40" s="75" t="s">
+        <v>1419</v>
       </c>
       <c r="F40" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>542</v>
+        <v>447</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>543</v>
-      </c>
-      <c r="I40" s="15" t="s">
-        <v>544</v>
-      </c>
+        <v>448</v>
+      </c>
+      <c r="I40" s="15"/>
       <c r="J40" s="15" t="s">
-        <v>545</v>
+        <v>449</v>
       </c>
       <c r="K40" s="13"/>
     </row>
-    <row r="41" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B41" s="77" t="s">
-        <v>529</v>
+      <c r="B41" s="75" t="s">
+        <v>440</v>
       </c>
       <c r="C41" s="13"/>
-      <c r="D41" s="78" t="s">
-        <v>987</v>
-      </c>
-      <c r="E41" s="77" t="s">
-        <v>1206</v>
+      <c r="D41" s="76" t="s">
+        <v>985</v>
+      </c>
+      <c r="E41" s="75" t="s">
+        <v>1419</v>
       </c>
       <c r="F41" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>547</v>
+        <v>450</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>548</v>
+        <v>451</v>
       </c>
       <c r="I41" s="15"/>
       <c r="J41" s="15" t="s">
-        <v>549</v>
+        <v>452</v>
       </c>
       <c r="K41" s="13"/>
     </row>
-    <row r="42" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B42" s="77" t="s">
-        <v>529</v>
+      <c r="B42" s="75" t="s">
+        <v>440</v>
       </c>
       <c r="C42" s="13"/>
-      <c r="D42" s="78" t="s">
-        <v>987</v>
-      </c>
-      <c r="E42" s="77" t="s">
-        <v>1206</v>
+      <c r="D42" s="76" t="s">
+        <v>985</v>
+      </c>
+      <c r="E42" s="75" t="s">
+        <v>1419</v>
       </c>
       <c r="F42" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>551</v>
+        <v>444</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>552</v>
-      </c>
-      <c r="I42" s="15" t="s">
-        <v>553</v>
-      </c>
+        <v>445</v>
+      </c>
+      <c r="I42" s="15"/>
       <c r="J42" s="15" t="s">
-        <v>554</v>
+        <v>446</v>
       </c>
       <c r="K42" s="13"/>
     </row>
@@ -21490,115 +21531,115 @@
       <c r="A43" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B43" s="77" t="s">
-        <v>529</v>
+      <c r="B43" s="75" t="s">
+        <v>688</v>
       </c>
       <c r="C43" s="13"/>
-      <c r="D43" s="78" t="s">
-        <v>987</v>
-      </c>
-      <c r="E43" s="77" t="s">
-        <v>1206</v>
+      <c r="D43" s="76" t="s">
+        <v>986</v>
+      </c>
+      <c r="E43" s="75" t="s">
+        <v>1203</v>
       </c>
       <c r="F43" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>556</v>
+        <v>695</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>557</v>
+        <v>696</v>
       </c>
       <c r="I43" s="15"/>
       <c r="J43" s="15" t="s">
-        <v>558</v>
+        <v>697</v>
       </c>
       <c r="K43" s="13"/>
     </row>
-    <row r="44" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="162.5" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B44" s="77" t="s">
-        <v>529</v>
+      <c r="B44" s="75" t="s">
+        <v>688</v>
       </c>
       <c r="C44" s="13"/>
-      <c r="D44" s="78" t="s">
-        <v>987</v>
-      </c>
-      <c r="E44" s="77" t="s">
-        <v>1206</v>
+      <c r="D44" s="76" t="s">
+        <v>986</v>
+      </c>
+      <c r="E44" s="75" t="s">
+        <v>1203</v>
       </c>
       <c r="F44" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>560</v>
+        <v>698</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>561</v>
+        <v>699</v>
       </c>
       <c r="I44" s="15"/>
       <c r="J44" s="15" t="s">
-        <v>562</v>
+        <v>700</v>
       </c>
       <c r="K44" s="13"/>
     </row>
-    <row r="45" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="100" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B45" s="77" t="s">
-        <v>529</v>
+      <c r="B45" s="75" t="s">
+        <v>688</v>
       </c>
       <c r="C45" s="13"/>
-      <c r="D45" s="78" t="s">
-        <v>987</v>
-      </c>
-      <c r="E45" s="77" t="s">
-        <v>1206</v>
+      <c r="D45" s="76" t="s">
+        <v>986</v>
+      </c>
+      <c r="E45" s="75" t="s">
+        <v>1203</v>
       </c>
       <c r="F45" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>564</v>
+        <v>702</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>565</v>
+        <v>703</v>
       </c>
       <c r="I45" s="15"/>
       <c r="J45" s="15" t="s">
-        <v>566</v>
+        <v>704</v>
       </c>
       <c r="K45" s="13"/>
     </row>
-    <row r="46" spans="1:11" ht="87.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B46" s="77" t="s">
-        <v>529</v>
+      <c r="B46" s="75" t="s">
+        <v>688</v>
       </c>
       <c r="C46" s="13"/>
-      <c r="D46" s="78" t="s">
-        <v>987</v>
-      </c>
-      <c r="E46" s="77" t="s">
-        <v>1206</v>
+      <c r="D46" s="76" t="s">
+        <v>986</v>
+      </c>
+      <c r="E46" s="75" t="s">
+        <v>1203</v>
       </c>
       <c r="F46" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>568</v>
+        <v>705</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>569</v>
+        <v>706</v>
       </c>
       <c r="I46" s="15"/>
       <c r="J46" s="15" t="s">
-        <v>1420</v>
+        <v>707</v>
       </c>
       <c r="K46" s="13"/>
     </row>
@@ -21606,28 +21647,28 @@
       <c r="A47" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B47" s="77" t="s">
-        <v>529</v>
+      <c r="B47" s="75" t="s">
+        <v>688</v>
       </c>
       <c r="C47" s="13"/>
-      <c r="D47" s="78" t="s">
-        <v>987</v>
-      </c>
-      <c r="E47" s="77" t="s">
-        <v>1206</v>
+      <c r="D47" s="76" t="s">
+        <v>986</v>
+      </c>
+      <c r="E47" s="75" t="s">
+        <v>1203</v>
       </c>
       <c r="F47" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>571</v>
+        <v>692</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>572</v>
+        <v>693</v>
       </c>
       <c r="I47" s="15"/>
       <c r="J47" s="15" t="s">
-        <v>573</v>
+        <v>694</v>
       </c>
       <c r="K47" s="13"/>
     </row>
@@ -21635,57 +21676,57 @@
       <c r="A48" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B48" s="77" t="s">
+      <c r="B48" s="75" t="s">
         <v>529</v>
       </c>
       <c r="C48" s="13"/>
-      <c r="D48" s="78" t="s">
+      <c r="D48" s="76" t="s">
         <v>987</v>
       </c>
-      <c r="E48" s="77" t="s">
+      <c r="E48" s="75" t="s">
         <v>1206</v>
       </c>
       <c r="F48" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>575</v>
+        <v>534</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>576</v>
+        <v>535</v>
       </c>
       <c r="I48" s="15"/>
       <c r="J48" s="15" t="s">
-        <v>577</v>
+        <v>536</v>
       </c>
       <c r="K48" s="13"/>
     </row>
-    <row r="49" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B49" s="77" t="s">
+      <c r="B49" s="75" t="s">
         <v>529</v>
       </c>
       <c r="C49" s="13"/>
-      <c r="D49" s="78" t="s">
+      <c r="D49" s="76" t="s">
         <v>987</v>
       </c>
-      <c r="E49" s="77" t="s">
+      <c r="E49" s="75" t="s">
         <v>1206</v>
       </c>
       <c r="F49" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>579</v>
+        <v>538</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>580</v>
+        <v>539</v>
       </c>
       <c r="I49" s="15"/>
       <c r="J49" s="15" t="s">
-        <v>581</v>
+        <v>540</v>
       </c>
       <c r="K49" s="13"/>
     </row>
@@ -21693,57 +21734,59 @@
       <c r="A50" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B50" s="77" t="s">
-        <v>433</v>
-      </c>
-      <c r="C50" s="16"/>
-      <c r="D50" s="78" t="s">
-        <v>976</v>
-      </c>
-      <c r="E50" s="77" t="s">
-        <v>1209</v>
+      <c r="B50" s="75" t="s">
+        <v>529</v>
+      </c>
+      <c r="C50" s="13"/>
+      <c r="D50" s="76" t="s">
+        <v>987</v>
+      </c>
+      <c r="E50" s="75" t="s">
+        <v>1206</v>
       </c>
       <c r="F50" s="16" t="s">
         <v>1412</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>437</v>
+        <v>542</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>438</v>
-      </c>
-      <c r="I50" s="15"/>
+        <v>543</v>
+      </c>
+      <c r="I50" s="15" t="s">
+        <v>544</v>
+      </c>
       <c r="J50" s="15" t="s">
-        <v>439</v>
-      </c>
-      <c r="K50" s="16"/>
+        <v>545</v>
+      </c>
+      <c r="K50" s="13"/>
     </row>
     <row r="51" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B51" s="81" t="s">
-        <v>971</v>
+      <c r="B51" s="75" t="s">
+        <v>529</v>
       </c>
       <c r="C51" s="13"/>
-      <c r="D51" s="82" t="s">
-        <v>1019</v>
-      </c>
-      <c r="E51" s="77" t="s">
-        <v>1421</v>
+      <c r="D51" s="76" t="s">
+        <v>987</v>
+      </c>
+      <c r="E51" s="75" t="s">
+        <v>1206</v>
       </c>
       <c r="F51" s="16" t="s">
         <v>1412</v>
       </c>
-      <c r="G51" s="57" t="s">
-        <v>971</v>
+      <c r="G51" s="15" t="s">
+        <v>547</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>1422</v>
-      </c>
-      <c r="I51" s="57"/>
+        <v>548</v>
+      </c>
+      <c r="I51" s="15"/>
       <c r="J51" s="15" t="s">
-        <v>1423</v>
+        <v>549</v>
       </c>
       <c r="K51" s="13"/>
     </row>
@@ -21751,28 +21794,30 @@
       <c r="A52" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B52" s="81" t="s">
-        <v>971</v>
+      <c r="B52" s="75" t="s">
+        <v>529</v>
       </c>
       <c r="C52" s="13"/>
-      <c r="D52" s="82" t="s">
-        <v>1019</v>
-      </c>
-      <c r="E52" s="77" t="s">
-        <v>1421</v>
+      <c r="D52" s="76" t="s">
+        <v>987</v>
+      </c>
+      <c r="E52" s="75" t="s">
+        <v>1206</v>
       </c>
       <c r="F52" s="16" t="s">
         <v>1412</v>
       </c>
-      <c r="G52" s="57" t="s">
-        <v>971</v>
+      <c r="G52" s="15" t="s">
+        <v>551</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>1424</v>
-      </c>
-      <c r="I52" s="57"/>
+        <v>552</v>
+      </c>
+      <c r="I52" s="15" t="s">
+        <v>553</v>
+      </c>
       <c r="J52" s="15" t="s">
-        <v>1425</v>
+        <v>554</v>
       </c>
       <c r="K52" s="13"/>
     </row>
@@ -21780,28 +21825,28 @@
       <c r="A53" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B53" s="81" t="s">
-        <v>971</v>
+      <c r="B53" s="75" t="s">
+        <v>529</v>
       </c>
       <c r="C53" s="13"/>
-      <c r="D53" s="82" t="s">
-        <v>1019</v>
-      </c>
-      <c r="E53" s="77" t="s">
-        <v>1421</v>
+      <c r="D53" s="76" t="s">
+        <v>987</v>
+      </c>
+      <c r="E53" s="75" t="s">
+        <v>1206</v>
       </c>
       <c r="F53" s="16" t="s">
         <v>1412</v>
       </c>
-      <c r="G53" s="57" t="s">
-        <v>971</v>
+      <c r="G53" s="15" t="s">
+        <v>556</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>1426</v>
+        <v>557</v>
       </c>
       <c r="I53" s="15"/>
       <c r="J53" s="15" t="s">
-        <v>1427</v>
+        <v>558</v>
       </c>
       <c r="K53" s="13"/>
     </row>
@@ -21809,88 +21854,86 @@
       <c r="A54" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B54" s="83" t="s">
-        <v>1428</v>
+      <c r="B54" s="75" t="s">
+        <v>529</v>
       </c>
       <c r="C54" s="13"/>
-      <c r="D54" s="82" t="s">
-        <v>986</v>
-      </c>
-      <c r="E54" s="77" t="s">
-        <v>1199</v>
+      <c r="D54" s="76" t="s">
+        <v>987</v>
+      </c>
+      <c r="E54" s="75" t="s">
+        <v>1206</v>
       </c>
       <c r="F54" s="16" t="s">
         <v>1412</v>
       </c>
-      <c r="G54" s="57" t="s">
-        <v>1429</v>
-      </c>
-      <c r="H54" s="57" t="s">
-        <v>1430</v>
-      </c>
-      <c r="I54" s="84"/>
-      <c r="J54" s="84" t="s">
-        <v>1431</v>
+      <c r="G54" s="15" t="s">
+        <v>560</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15" t="s">
+        <v>562</v>
       </c>
       <c r="K54" s="13"/>
     </row>
-    <row r="55" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B55" s="83" t="s">
-        <v>1428</v>
+      <c r="B55" s="75" t="s">
+        <v>529</v>
       </c>
       <c r="C55" s="13"/>
-      <c r="D55" s="82" t="s">
-        <v>986</v>
-      </c>
-      <c r="E55" s="77" t="s">
-        <v>1199</v>
+      <c r="D55" s="76" t="s">
+        <v>987</v>
+      </c>
+      <c r="E55" s="75" t="s">
+        <v>1206</v>
       </c>
       <c r="F55" s="16" t="s">
         <v>1412</v>
       </c>
-      <c r="G55" s="57" t="s">
-        <v>1432</v>
-      </c>
-      <c r="H55" s="57" t="s">
-        <v>1433</v>
-      </c>
-      <c r="I55" s="57"/>
-      <c r="J55" s="57" t="s">
-        <v>1434</v>
+      <c r="G55" s="15" t="s">
+        <v>564</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>565</v>
+      </c>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15" t="s">
+        <v>566</v>
       </c>
       <c r="K55" s="13"/>
     </row>
-    <row r="56" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B56" s="83" t="s">
-        <v>1428</v>
+      <c r="B56" s="75" t="s">
+        <v>529</v>
       </c>
       <c r="C56" s="13"/>
-      <c r="D56" s="82" t="s">
-        <v>986</v>
-      </c>
-      <c r="E56" s="77" t="s">
-        <v>1199</v>
+      <c r="D56" s="76" t="s">
+        <v>987</v>
+      </c>
+      <c r="E56" s="75" t="s">
+        <v>1206</v>
       </c>
       <c r="F56" s="16" t="s">
         <v>1412</v>
       </c>
-      <c r="G56" s="57" t="s">
-        <v>1435</v>
-      </c>
-      <c r="H56" s="57" t="s">
-        <v>1436</v>
-      </c>
-      <c r="I56" s="57" t="s">
-        <v>1437</v>
-      </c>
-      <c r="J56" s="57" t="s">
-        <v>1438</v>
+      <c r="G56" s="15" t="s">
+        <v>568</v>
+      </c>
+      <c r="H56" s="15" t="s">
+        <v>569</v>
+      </c>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15" t="s">
+        <v>1420</v>
       </c>
       <c r="K56" s="13"/>
     </row>
@@ -21898,28 +21941,28 @@
       <c r="A57" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B57" s="83" t="s">
-        <v>1428</v>
+      <c r="B57" s="75" t="s">
+        <v>529</v>
       </c>
       <c r="C57" s="13"/>
-      <c r="D57" s="82" t="s">
-        <v>986</v>
-      </c>
-      <c r="E57" s="77" t="s">
-        <v>1199</v>
+      <c r="D57" s="76" t="s">
+        <v>987</v>
+      </c>
+      <c r="E57" s="75" t="s">
+        <v>1206</v>
       </c>
       <c r="F57" s="16" t="s">
         <v>1412</v>
       </c>
-      <c r="G57" s="57" t="s">
-        <v>1439</v>
-      </c>
-      <c r="H57" s="57" t="s">
-        <v>1440</v>
-      </c>
-      <c r="I57" s="57"/>
-      <c r="J57" s="57" t="s">
-        <v>1441</v>
+      <c r="G57" s="15" t="s">
+        <v>571</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>572</v>
+      </c>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15" t="s">
+        <v>573</v>
       </c>
       <c r="K57" s="13"/>
     </row>
@@ -21927,110 +21970,402 @@
       <c r="A58" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B58" s="83" t="s">
-        <v>1428</v>
+      <c r="B58" s="75" t="s">
+        <v>529</v>
       </c>
       <c r="C58" s="13"/>
-      <c r="D58" s="82" t="s">
-        <v>986</v>
-      </c>
-      <c r="E58" s="77" t="s">
-        <v>1199</v>
+      <c r="D58" s="76" t="s">
+        <v>987</v>
+      </c>
+      <c r="E58" s="75" t="s">
+        <v>1206</v>
       </c>
       <c r="F58" s="16" t="s">
         <v>1412</v>
       </c>
-      <c r="G58" s="57" t="s">
-        <v>1442</v>
-      </c>
-      <c r="H58" s="57" t="s">
-        <v>1443</v>
-      </c>
-      <c r="I58" s="57" t="s">
-        <v>1444</v>
-      </c>
-      <c r="J58" s="57" t="s">
-        <v>1445</v>
+      <c r="G58" s="15" t="s">
+        <v>575</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>576</v>
+      </c>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15" t="s">
+        <v>577</v>
       </c>
       <c r="K58" s="13"/>
     </row>
-    <row r="59" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B59" s="83" t="s">
-        <v>1428</v>
+      <c r="B59" s="75" t="s">
+        <v>529</v>
       </c>
       <c r="C59" s="13"/>
-      <c r="D59" s="82" t="s">
-        <v>986</v>
-      </c>
-      <c r="E59" s="77" t="s">
-        <v>1199</v>
+      <c r="D59" s="76" t="s">
+        <v>987</v>
+      </c>
+      <c r="E59" s="75" t="s">
+        <v>1206</v>
       </c>
       <c r="F59" s="16" t="s">
         <v>1412</v>
       </c>
-      <c r="G59" s="57" t="s">
-        <v>1446</v>
-      </c>
-      <c r="H59" s="57" t="s">
-        <v>1447</v>
-      </c>
-      <c r="I59" s="57" t="s">
-        <v>1448</v>
-      </c>
-      <c r="J59" s="57" t="s">
-        <v>1449</v>
+      <c r="G59" s="15" t="s">
+        <v>579</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>580</v>
+      </c>
+      <c r="I59" s="15"/>
+      <c r="J59" s="15" t="s">
+        <v>581</v>
       </c>
       <c r="K59" s="13"/>
     </row>
-    <row r="60" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="B60" s="83" t="s">
-        <v>1428</v>
-      </c>
-      <c r="C60" s="13"/>
-      <c r="D60" s="82" t="s">
-        <v>986</v>
-      </c>
-      <c r="E60" s="77" t="s">
-        <v>1199</v>
+      <c r="B60" s="75" t="s">
+        <v>433</v>
+      </c>
+      <c r="C60" s="16"/>
+      <c r="D60" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E60" s="75" t="s">
+        <v>1209</v>
       </c>
       <c r="F60" s="16" t="s">
         <v>1412</v>
       </c>
-      <c r="G60" s="57" t="s">
+      <c r="G60" s="15" t="s">
+        <v>437</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>438</v>
+      </c>
+      <c r="I60" s="15"/>
+      <c r="J60" s="15" t="s">
+        <v>439</v>
+      </c>
+      <c r="K60" s="16"/>
+    </row>
+    <row r="61" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="16" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B61" s="79" t="s">
+        <v>971</v>
+      </c>
+      <c r="C61" s="13"/>
+      <c r="D61" s="80" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E61" s="75" t="s">
+        <v>1421</v>
+      </c>
+      <c r="F61" s="16" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G61" s="57" t="s">
+        <v>971</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>1422</v>
+      </c>
+      <c r="I61" s="57"/>
+      <c r="J61" s="15" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K61" s="13"/>
+    </row>
+    <row r="62" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B62" s="79" t="s">
+        <v>971</v>
+      </c>
+      <c r="C62" s="13"/>
+      <c r="D62" s="80" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E62" s="75" t="s">
+        <v>1421</v>
+      </c>
+      <c r="F62" s="16" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G62" s="57" t="s">
+        <v>971</v>
+      </c>
+      <c r="H62" s="15" t="s">
+        <v>1424</v>
+      </c>
+      <c r="I62" s="57"/>
+      <c r="J62" s="15" t="s">
+        <v>1425</v>
+      </c>
+      <c r="K62" s="13"/>
+    </row>
+    <row r="63" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B63" s="79" t="s">
+        <v>971</v>
+      </c>
+      <c r="C63" s="13"/>
+      <c r="D63" s="80" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E63" s="75" t="s">
+        <v>1421</v>
+      </c>
+      <c r="F63" s="16" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G63" s="57" t="s">
+        <v>971</v>
+      </c>
+      <c r="H63" s="15" t="s">
+        <v>1426</v>
+      </c>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15" t="s">
+        <v>1427</v>
+      </c>
+      <c r="K63" s="13"/>
+    </row>
+    <row r="64" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B64" s="81" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C64" s="13"/>
+      <c r="D64" s="80" t="s">
+        <v>986</v>
+      </c>
+      <c r="E64" s="75" t="s">
+        <v>1199</v>
+      </c>
+      <c r="F64" s="16" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G64" s="57" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H64" s="57" t="s">
+        <v>1430</v>
+      </c>
+      <c r="I64" s="82"/>
+      <c r="J64" s="82" t="s">
+        <v>1431</v>
+      </c>
+      <c r="K64" s="13"/>
+    </row>
+    <row r="65" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="16" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B65" s="81" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C65" s="13"/>
+      <c r="D65" s="80" t="s">
+        <v>986</v>
+      </c>
+      <c r="E65" s="75" t="s">
+        <v>1199</v>
+      </c>
+      <c r="F65" s="16" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G65" s="57" t="s">
+        <v>1432</v>
+      </c>
+      <c r="H65" s="57" t="s">
+        <v>1433</v>
+      </c>
+      <c r="I65" s="57"/>
+      <c r="J65" s="57" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K65" s="13"/>
+    </row>
+    <row r="66" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="16" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B66" s="81" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C66" s="13"/>
+      <c r="D66" s="80" t="s">
+        <v>986</v>
+      </c>
+      <c r="E66" s="75" t="s">
+        <v>1199</v>
+      </c>
+      <c r="F66" s="16" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G66" s="57" t="s">
+        <v>1435</v>
+      </c>
+      <c r="H66" s="57" t="s">
+        <v>1436</v>
+      </c>
+      <c r="I66" s="57" t="s">
+        <v>1437</v>
+      </c>
+      <c r="J66" s="57" t="s">
+        <v>1438</v>
+      </c>
+      <c r="K66" s="13"/>
+    </row>
+    <row r="67" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="16" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B67" s="81" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C67" s="13"/>
+      <c r="D67" s="80" t="s">
+        <v>986</v>
+      </c>
+      <c r="E67" s="75" t="s">
+        <v>1199</v>
+      </c>
+      <c r="F67" s="16" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G67" s="57" t="s">
+        <v>1439</v>
+      </c>
+      <c r="H67" s="57" t="s">
+        <v>1440</v>
+      </c>
+      <c r="I67" s="57"/>
+      <c r="J67" s="57" t="s">
+        <v>1441</v>
+      </c>
+      <c r="K67" s="13"/>
+    </row>
+    <row r="68" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A68" s="16" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B68" s="81" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C68" s="13"/>
+      <c r="D68" s="80" t="s">
+        <v>986</v>
+      </c>
+      <c r="E68" s="75" t="s">
+        <v>1199</v>
+      </c>
+      <c r="F68" s="16" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G68" s="57" t="s">
+        <v>1442</v>
+      </c>
+      <c r="H68" s="57" t="s">
+        <v>1443</v>
+      </c>
+      <c r="I68" s="57" t="s">
+        <v>1444</v>
+      </c>
+      <c r="J68" s="57" t="s">
+        <v>1445</v>
+      </c>
+      <c r="K68" s="13"/>
+    </row>
+    <row r="69" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="16" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B69" s="81" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C69" s="13"/>
+      <c r="D69" s="80" t="s">
+        <v>986</v>
+      </c>
+      <c r="E69" s="75" t="s">
+        <v>1199</v>
+      </c>
+      <c r="F69" s="16" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G69" s="57" t="s">
+        <v>1446</v>
+      </c>
+      <c r="H69" s="57" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I69" s="57" t="s">
+        <v>1448</v>
+      </c>
+      <c r="J69" s="57" t="s">
+        <v>1449</v>
+      </c>
+      <c r="K69" s="13"/>
+    </row>
+    <row r="70" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+      <c r="A70" s="16" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B70" s="81" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C70" s="13"/>
+      <c r="D70" s="80" t="s">
+        <v>986</v>
+      </c>
+      <c r="E70" s="75" t="s">
+        <v>1199</v>
+      </c>
+      <c r="F70" s="16" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G70" s="57" t="s">
         <v>1450</v>
       </c>
-      <c r="H60" s="57" t="s">
+      <c r="H70" s="57" t="s">
         <v>1451</v>
       </c>
-      <c r="I60" s="57"/>
-      <c r="J60" s="57" t="s">
+      <c r="I70" s="57"/>
+      <c r="J70" s="57" t="s">
         <v>1452</v>
       </c>
-      <c r="K60" s="13"/>
-    </row>
-    <row r="61" spans="1:11" ht="175" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
+      <c r="K70" s="13"/>
+    </row>
+    <row r="71" spans="1:11" ht="175" x14ac:dyDescent="0.25">
+      <c r="A71" s="16" t="s">
         <v>1453</v>
       </c>
-      <c r="B61" s="13"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="13"/>
-      <c r="I61" s="13"/>
-      <c r="J61" s="13"/>
-      <c r="K61" s="13"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H29">
+  <conditionalFormatting sqref="H39">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added relationship to Procedure class
studyIntervention
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95434A5C-2ABA-41C8-886A-6601FE11CB30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B194EC7-05C3-411C-AE7B-1D086BD01259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="680" windowWidth="15280" windowHeight="9390" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="16270" windowHeight="9270" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5712" uniqueCount="1823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5719" uniqueCount="1824">
   <si>
     <t>Code</t>
   </si>
@@ -10798,6 +10798,9 @@
   </si>
   <si>
     <t>Update Attribute name in DDF Valid Value Sets tab</t>
+  </si>
+  <si>
+    <t>studyIntervention</t>
   </si>
 </sst>
 </file>
@@ -22532,7 +22535,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -23660,65 +23663,59 @@
     </row>
     <row r="35" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>1454</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>1654</v>
-      </c>
-      <c r="E35" s="51" t="s">
-        <v>1654</v>
+        <v>1470</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>997</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>997</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E35" s="44" t="s">
+        <v>1823</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>1012</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>1655</v>
-      </c>
-      <c r="H35" s="16" t="s">
-        <v>1654</v>
-      </c>
+        <v>978</v>
+      </c>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
       <c r="I35" s="13"/>
-      <c r="J35" s="16" t="s">
-        <v>1656</v>
-      </c>
-      <c r="K35" s="13" t="s">
-        <v>996</v>
+      <c r="J35" s="13"/>
+      <c r="K35" s="16" t="s">
+        <v>997</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>1458</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>971</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>1657</v>
+        <v>1454</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>125</v>
       </c>
       <c r="D36" s="16" t="s">
         <v>1654</v>
       </c>
-      <c r="E36" s="52" t="s">
-        <v>1658</v>
+      <c r="E36" s="51" t="s">
+        <v>1654</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>967</v>
+        <v>1012</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>1659</v>
+        <v>1655</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>1660</v>
+        <v>1654</v>
       </c>
       <c r="I36" s="13"/>
       <c r="J36" s="16" t="s">
-        <v>1661</v>
+        <v>1656</v>
       </c>
       <c r="K36" s="13" t="s">
         <v>996</v>
@@ -23738,49 +23735,82 @@
         <v>1654</v>
       </c>
       <c r="E37" s="52" t="s">
-        <v>1662</v>
+        <v>1658</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>967</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>1663</v>
+        <v>1659</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>1664</v>
+        <v>1660</v>
       </c>
       <c r="I37" s="13"/>
       <c r="J37" s="16" t="s">
-        <v>1665</v>
-      </c>
-      <c r="K37" s="16" t="s">
-        <v>1666</v>
+        <v>1661</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>996</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
+        <v>1458</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>971</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>1657</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>1654</v>
+      </c>
+      <c r="E38" s="52" t="s">
+        <v>1662</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>967</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>1663</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>1664</v>
+      </c>
+      <c r="I38" s="13"/>
+      <c r="J38" s="16" t="s">
+        <v>1665</v>
+      </c>
+      <c r="K38" s="16" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
         <v>1470</v>
       </c>
-      <c r="B38" s="16" t="s">
-        <v>997</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>997</v>
-      </c>
-      <c r="D38" s="15" t="s">
+      <c r="B39" s="16" t="s">
+        <v>997</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>997</v>
+      </c>
+      <c r="D39" s="15" t="s">
         <v>988</v>
       </c>
-      <c r="E38" s="44" t="s">
+      <c r="E39" s="44" t="s">
         <v>1667</v>
       </c>
-      <c r="F38" s="16" t="s">
+      <c r="F39" s="16" t="s">
         <v>978</v>
       </c>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="16" t="s">
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="16" t="s">
         <v>997</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final fixes for 2-6 take 2
With Berber QC comments resolved - value set attribute name updates for four values sets.
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF799FF8-E41E-49D0-A817-2987067002BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CCEE07-36D0-46C1-93B2-87163878B53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="0" windowWidth="17790" windowHeight="9970" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1060" yWindow="120" windowWidth="17790" windowHeight="9970" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6118" uniqueCount="1902">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6452" uniqueCount="1936">
   <si>
     <t>Code</t>
   </si>
@@ -11512,6 +11512,134 @@
       </rPr>
       <t>exits</t>
     </r>
+  </si>
+  <si>
+    <t>C66735</t>
+  </si>
+  <si>
+    <t>C201265</t>
+  </si>
+  <si>
+    <t>C15228</t>
+  </si>
+  <si>
+    <t>DOUBLE BLIND</t>
+  </si>
+  <si>
+    <t>Double Masked; Double-Masked</t>
+  </si>
+  <si>
+    <t>A study in which neither the subject nor the study personnel interacting with the subject or data during the study knows what intervention a subject is receiving.</t>
+  </si>
+  <si>
+    <t>C187674</t>
+  </si>
+  <si>
+    <t>OBSERVER BLIND</t>
+  </si>
+  <si>
+    <t>A study in which the study personnel who measure, record, or assess the subject do not know which intervention the subject is receiving or, in the context of observational studies, do not know the external factors to which a subject has been exposed.</t>
+  </si>
+  <si>
+    <t>C156592</t>
+  </si>
+  <si>
+    <t>OPEN LABEL TO TREATMENT AND DOUBLE BLIND TO IMP DOSE</t>
+  </si>
+  <si>
+    <t>A study in which the therapeutic treatment is open label but the dosing information of the investigational medicinal product (IMP) is double-blinded.</t>
+  </si>
+  <si>
+    <t>C49659</t>
+  </si>
+  <si>
+    <t>OPEN LABEL</t>
+  </si>
+  <si>
+    <t>A study in which subjects and study personnel know which intervention each subject is receiving.</t>
+  </si>
+  <si>
+    <t>C28233</t>
+  </si>
+  <si>
+    <t>SINGLE BLIND</t>
+  </si>
+  <si>
+    <t>Single Masked; Single-Masked</t>
+  </si>
+  <si>
+    <t>A study in which one party, either the subject or study personnel, does not know which intervention is administered to the subject.</t>
+  </si>
+  <si>
+    <t>C201352</t>
+  </si>
+  <si>
+    <t>End to End</t>
+  </si>
+  <si>
+    <t>A timing relationship defined as the end of one event to the end of another event.</t>
+  </si>
+  <si>
+    <t>C201353</t>
+  </si>
+  <si>
+    <t>End to Start</t>
+  </si>
+  <si>
+    <t>A timing relationship defined as the end of one event to the start of another event.</t>
+  </si>
+  <si>
+    <t>C201354</t>
+  </si>
+  <si>
+    <t>Start to End</t>
+  </si>
+  <si>
+    <t>A timing relationship defined as the start of one event to the end of another event.</t>
+  </si>
+  <si>
+    <t>C201355</t>
+  </si>
+  <si>
+    <t>Start to Start</t>
+  </si>
+  <si>
+    <t>A timing relationship defined as the start of one event to the start of another event.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>timingRelativeToFrom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>relativeToFrom</t>
+    </r>
+  </si>
+  <si>
+    <t>Timing Relative To From Value Set Terminolog</t>
+  </si>
+  <si>
+    <t>Trial Blinding Schema Response</t>
   </si>
 </sst>
 </file>
@@ -24234,7 +24362,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -25224,6 +25352,1136 @@
         <v>997</v>
       </c>
       <c r="L27" s="13"/>
+    </row>
+    <row r="28" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B28" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C28" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E28" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F28" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G28" s="75" t="s">
+        <v>457</v>
+      </c>
+      <c r="H28" s="75" t="s">
+        <v>458</v>
+      </c>
+      <c r="I28" s="75"/>
+      <c r="J28" s="75" t="s">
+        <v>459</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L28" s="13"/>
+    </row>
+    <row r="29" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B29" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C29" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E29" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F29" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G29" s="75" t="s">
+        <v>461</v>
+      </c>
+      <c r="H29" s="75" t="s">
+        <v>462</v>
+      </c>
+      <c r="I29" s="75"/>
+      <c r="J29" s="75" t="s">
+        <v>463</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L29" s="13"/>
+    </row>
+    <row r="30" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B30" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C30" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E30" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F30" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G30" s="75" t="s">
+        <v>465</v>
+      </c>
+      <c r="H30" s="75" t="s">
+        <v>466</v>
+      </c>
+      <c r="I30" s="75"/>
+      <c r="J30" s="75" t="s">
+        <v>467</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L30" s="13"/>
+    </row>
+    <row r="31" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B31" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C31" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E31" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F31" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G31" s="75" t="s">
+        <v>469</v>
+      </c>
+      <c r="H31" s="75" t="s">
+        <v>470</v>
+      </c>
+      <c r="I31" s="75"/>
+      <c r="J31" s="75" t="s">
+        <v>471</v>
+      </c>
+      <c r="K31" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L31" s="13"/>
+    </row>
+    <row r="32" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B32" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C32" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E32" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F32" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G32" s="75" t="s">
+        <v>473</v>
+      </c>
+      <c r="H32" s="75" t="s">
+        <v>474</v>
+      </c>
+      <c r="I32" s="75"/>
+      <c r="J32" s="75" t="s">
+        <v>475</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L32" s="13"/>
+    </row>
+    <row r="33" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B33" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C33" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E33" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F33" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G33" s="75" t="s">
+        <v>477</v>
+      </c>
+      <c r="H33" s="75" t="s">
+        <v>478</v>
+      </c>
+      <c r="I33" s="75"/>
+      <c r="J33" s="75" t="s">
+        <v>479</v>
+      </c>
+      <c r="K33" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L33" s="13"/>
+    </row>
+    <row r="34" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B34" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C34" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E34" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F34" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G34" s="75" t="s">
+        <v>481</v>
+      </c>
+      <c r="H34" s="75" t="s">
+        <v>482</v>
+      </c>
+      <c r="I34" s="75"/>
+      <c r="J34" s="75" t="s">
+        <v>483</v>
+      </c>
+      <c r="K34" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L34" s="13"/>
+    </row>
+    <row r="35" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B35" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C35" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E35" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F35" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G35" s="75" t="s">
+        <v>485</v>
+      </c>
+      <c r="H35" s="75" t="s">
+        <v>486</v>
+      </c>
+      <c r="I35" s="75"/>
+      <c r="J35" s="75" t="s">
+        <v>487</v>
+      </c>
+      <c r="K35" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L35" s="13"/>
+    </row>
+    <row r="36" spans="1:12" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B36" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C36" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E36" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F36" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G36" s="75" t="s">
+        <v>489</v>
+      </c>
+      <c r="H36" s="75" t="s">
+        <v>490</v>
+      </c>
+      <c r="I36" s="75"/>
+      <c r="J36" s="75" t="s">
+        <v>491</v>
+      </c>
+      <c r="K36" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L36" s="13"/>
+    </row>
+    <row r="37" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B37" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C37" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E37" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F37" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G37" s="75" t="s">
+        <v>493</v>
+      </c>
+      <c r="H37" s="75" t="s">
+        <v>494</v>
+      </c>
+      <c r="I37" s="75"/>
+      <c r="J37" s="75" t="s">
+        <v>495</v>
+      </c>
+      <c r="K37" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L37" s="13"/>
+    </row>
+    <row r="38" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B38" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C38" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E38" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F38" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G38" s="75" t="s">
+        <v>497</v>
+      </c>
+      <c r="H38" s="75" t="s">
+        <v>498</v>
+      </c>
+      <c r="I38" s="75"/>
+      <c r="J38" s="75" t="s">
+        <v>499</v>
+      </c>
+      <c r="K38" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L38" s="13"/>
+    </row>
+    <row r="39" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B39" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C39" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E39" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F39" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G39" s="75" t="s">
+        <v>501</v>
+      </c>
+      <c r="H39" s="75" t="s">
+        <v>502</v>
+      </c>
+      <c r="I39" s="75"/>
+      <c r="J39" s="75" t="s">
+        <v>503</v>
+      </c>
+      <c r="K39" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L39" s="13"/>
+    </row>
+    <row r="40" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B40" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C40" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E40" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F40" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G40" s="75" t="s">
+        <v>505</v>
+      </c>
+      <c r="H40" s="75" t="s">
+        <v>506</v>
+      </c>
+      <c r="I40" s="75"/>
+      <c r="J40" s="75" t="s">
+        <v>507</v>
+      </c>
+      <c r="K40" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L40" s="13"/>
+    </row>
+    <row r="41" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B41" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C41" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E41" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F41" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G41" s="75" t="s">
+        <v>509</v>
+      </c>
+      <c r="H41" s="75" t="s">
+        <v>510</v>
+      </c>
+      <c r="I41" s="75"/>
+      <c r="J41" s="75" t="s">
+        <v>511</v>
+      </c>
+      <c r="K41" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L41" s="13"/>
+    </row>
+    <row r="42" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B42" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C42" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E42" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F42" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G42" s="75" t="s">
+        <v>513</v>
+      </c>
+      <c r="H42" s="75" t="s">
+        <v>514</v>
+      </c>
+      <c r="I42" s="75"/>
+      <c r="J42" s="75" t="s">
+        <v>515</v>
+      </c>
+      <c r="K42" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L42" s="13"/>
+    </row>
+    <row r="43" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B43" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C43" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E43" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F43" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G43" s="75" t="s">
+        <v>517</v>
+      </c>
+      <c r="H43" s="75" t="s">
+        <v>518</v>
+      </c>
+      <c r="I43" s="75"/>
+      <c r="J43" s="75" t="s">
+        <v>519</v>
+      </c>
+      <c r="K43" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L43" s="13"/>
+    </row>
+    <row r="44" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B44" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C44" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E44" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F44" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G44" s="75" t="s">
+        <v>521</v>
+      </c>
+      <c r="H44" s="75" t="s">
+        <v>522</v>
+      </c>
+      <c r="I44" s="75"/>
+      <c r="J44" s="75" t="s">
+        <v>523</v>
+      </c>
+      <c r="K44" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L44" s="13"/>
+    </row>
+    <row r="45" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B45" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="C45" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E45" s="75" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F45" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G45" s="75" t="s">
+        <v>525</v>
+      </c>
+      <c r="H45" s="75" t="s">
+        <v>526</v>
+      </c>
+      <c r="I45" s="75"/>
+      <c r="J45" s="75" t="s">
+        <v>527</v>
+      </c>
+      <c r="K45" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L45" s="13"/>
+    </row>
+    <row r="46" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B46" s="75" t="s">
+        <v>608</v>
+      </c>
+      <c r="C46" s="75" t="s">
+        <v>609</v>
+      </c>
+      <c r="D46" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E46" s="75" t="s">
+        <v>1715</v>
+      </c>
+      <c r="F46" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G46" s="75" t="s">
+        <v>613</v>
+      </c>
+      <c r="H46" s="75" t="s">
+        <v>614</v>
+      </c>
+      <c r="I46" s="75" t="s">
+        <v>615</v>
+      </c>
+      <c r="J46" s="75" t="s">
+        <v>616</v>
+      </c>
+      <c r="K46" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L46" s="13"/>
+    </row>
+    <row r="47" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B47" s="75" t="s">
+        <v>608</v>
+      </c>
+      <c r="C47" s="75" t="s">
+        <v>609</v>
+      </c>
+      <c r="D47" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E47" s="75" t="s">
+        <v>1715</v>
+      </c>
+      <c r="F47" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G47" s="75" t="s">
+        <v>618</v>
+      </c>
+      <c r="H47" s="75" t="s">
+        <v>619</v>
+      </c>
+      <c r="I47" s="75" t="s">
+        <v>620</v>
+      </c>
+      <c r="J47" s="75" t="s">
+        <v>621</v>
+      </c>
+      <c r="K47" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L47" s="13"/>
+    </row>
+    <row r="48" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B48" s="75" t="s">
+        <v>608</v>
+      </c>
+      <c r="C48" s="75" t="s">
+        <v>609</v>
+      </c>
+      <c r="D48" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E48" s="75" t="s">
+        <v>1715</v>
+      </c>
+      <c r="F48" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G48" s="75" t="s">
+        <v>622</v>
+      </c>
+      <c r="H48" s="75" t="s">
+        <v>623</v>
+      </c>
+      <c r="I48" s="75"/>
+      <c r="J48" s="75" t="s">
+        <v>624</v>
+      </c>
+      <c r="K48" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L48" s="13"/>
+    </row>
+    <row r="49" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B49" s="75" t="s">
+        <v>608</v>
+      </c>
+      <c r="C49" s="75" t="s">
+        <v>609</v>
+      </c>
+      <c r="D49" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E49" s="75" t="s">
+        <v>1715</v>
+      </c>
+      <c r="F49" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G49" s="75" t="s">
+        <v>626</v>
+      </c>
+      <c r="H49" s="75" t="s">
+        <v>627</v>
+      </c>
+      <c r="I49" s="75"/>
+      <c r="J49" s="75" t="s">
+        <v>628</v>
+      </c>
+      <c r="K49" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L49" s="13"/>
+    </row>
+    <row r="50" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B50" s="75" t="s">
+        <v>608</v>
+      </c>
+      <c r="C50" s="75" t="s">
+        <v>609</v>
+      </c>
+      <c r="D50" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E50" s="75" t="s">
+        <v>1715</v>
+      </c>
+      <c r="F50" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G50" s="75" t="s">
+        <v>630</v>
+      </c>
+      <c r="H50" s="75" t="s">
+        <v>631</v>
+      </c>
+      <c r="I50" s="75"/>
+      <c r="J50" s="75" t="s">
+        <v>632</v>
+      </c>
+      <c r="K50" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L50" s="13"/>
+    </row>
+    <row r="51" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B51" s="75" t="s">
+        <v>608</v>
+      </c>
+      <c r="C51" s="75" t="s">
+        <v>609</v>
+      </c>
+      <c r="D51" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="E51" s="75" t="s">
+        <v>1715</v>
+      </c>
+      <c r="F51" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G51" s="75" t="s">
+        <v>634</v>
+      </c>
+      <c r="H51" s="75" t="s">
+        <v>635</v>
+      </c>
+      <c r="I51" s="75"/>
+      <c r="J51" s="75" t="s">
+        <v>636</v>
+      </c>
+      <c r="K51" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L51" s="13"/>
+    </row>
+    <row r="52" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B52" s="75" t="s">
+        <v>1902</v>
+      </c>
+      <c r="C52" s="75" t="s">
+        <v>1935</v>
+      </c>
+      <c r="D52" s="76" t="s">
+        <v>972</v>
+      </c>
+      <c r="E52" s="75" t="s">
+        <v>1770</v>
+      </c>
+      <c r="F52" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G52" s="75" t="s">
+        <v>1904</v>
+      </c>
+      <c r="H52" s="75" t="s">
+        <v>1905</v>
+      </c>
+      <c r="I52" s="75" t="s">
+        <v>1906</v>
+      </c>
+      <c r="J52" s="75" t="s">
+        <v>1907</v>
+      </c>
+      <c r="K52" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L52" s="13"/>
+    </row>
+    <row r="53" spans="1:12" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B53" s="75" t="s">
+        <v>1902</v>
+      </c>
+      <c r="C53" s="75" t="s">
+        <v>1935</v>
+      </c>
+      <c r="D53" s="76" t="s">
+        <v>972</v>
+      </c>
+      <c r="E53" s="75" t="s">
+        <v>1770</v>
+      </c>
+      <c r="F53" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G53" s="75" t="s">
+        <v>1908</v>
+      </c>
+      <c r="H53" s="75" t="s">
+        <v>1909</v>
+      </c>
+      <c r="I53" s="75"/>
+      <c r="J53" s="75" t="s">
+        <v>1910</v>
+      </c>
+      <c r="K53" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L53" s="13"/>
+    </row>
+    <row r="54" spans="1:12" ht="50" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B54" s="75" t="s">
+        <v>1902</v>
+      </c>
+      <c r="C54" s="75" t="s">
+        <v>1935</v>
+      </c>
+      <c r="D54" s="76" t="s">
+        <v>972</v>
+      </c>
+      <c r="E54" s="75" t="s">
+        <v>1770</v>
+      </c>
+      <c r="F54" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G54" s="75" t="s">
+        <v>1911</v>
+      </c>
+      <c r="H54" s="75" t="s">
+        <v>1912</v>
+      </c>
+      <c r="I54" s="75"/>
+      <c r="J54" s="75" t="s">
+        <v>1913</v>
+      </c>
+      <c r="K54" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L54" s="13"/>
+    </row>
+    <row r="55" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B55" s="75" t="s">
+        <v>1902</v>
+      </c>
+      <c r="C55" s="75" t="s">
+        <v>1935</v>
+      </c>
+      <c r="D55" s="76" t="s">
+        <v>972</v>
+      </c>
+      <c r="E55" s="75" t="s">
+        <v>1770</v>
+      </c>
+      <c r="F55" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G55" s="75" t="s">
+        <v>1914</v>
+      </c>
+      <c r="H55" s="75" t="s">
+        <v>1915</v>
+      </c>
+      <c r="I55" s="75"/>
+      <c r="J55" s="75" t="s">
+        <v>1916</v>
+      </c>
+      <c r="K55" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L55" s="13"/>
+    </row>
+    <row r="56" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B56" s="75" t="s">
+        <v>1902</v>
+      </c>
+      <c r="C56" s="75" t="s">
+        <v>1935</v>
+      </c>
+      <c r="D56" s="76" t="s">
+        <v>972</v>
+      </c>
+      <c r="E56" s="75" t="s">
+        <v>1770</v>
+      </c>
+      <c r="F56" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G56" s="75" t="s">
+        <v>1917</v>
+      </c>
+      <c r="H56" s="75" t="s">
+        <v>1918</v>
+      </c>
+      <c r="I56" s="75" t="s">
+        <v>1919</v>
+      </c>
+      <c r="J56" s="75" t="s">
+        <v>1920</v>
+      </c>
+      <c r="K56" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L56" s="13"/>
+    </row>
+    <row r="57" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B57" s="79" t="s">
+        <v>1903</v>
+      </c>
+      <c r="C57" s="75" t="s">
+        <v>1934</v>
+      </c>
+      <c r="D57" s="80" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E57" s="75" t="s">
+        <v>1933</v>
+      </c>
+      <c r="F57" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G57" s="79" t="s">
+        <v>1921</v>
+      </c>
+      <c r="H57" s="79" t="s">
+        <v>1922</v>
+      </c>
+      <c r="I57" s="79"/>
+      <c r="J57" s="79" t="s">
+        <v>1923</v>
+      </c>
+      <c r="K57" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L57" s="13"/>
+    </row>
+    <row r="58" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B58" s="79" t="s">
+        <v>1903</v>
+      </c>
+      <c r="C58" s="75" t="s">
+        <v>1934</v>
+      </c>
+      <c r="D58" s="80" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E58" s="75" t="s">
+        <v>1933</v>
+      </c>
+      <c r="F58" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G58" s="79" t="s">
+        <v>1924</v>
+      </c>
+      <c r="H58" s="79" t="s">
+        <v>1925</v>
+      </c>
+      <c r="I58" s="79"/>
+      <c r="J58" s="79" t="s">
+        <v>1926</v>
+      </c>
+      <c r="K58" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L58" s="13"/>
+    </row>
+    <row r="59" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B59" s="79" t="s">
+        <v>1903</v>
+      </c>
+      <c r="C59" s="75" t="s">
+        <v>1934</v>
+      </c>
+      <c r="D59" s="80" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E59" s="75" t="s">
+        <v>1933</v>
+      </c>
+      <c r="F59" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G59" s="79" t="s">
+        <v>1927</v>
+      </c>
+      <c r="H59" s="79" t="s">
+        <v>1928</v>
+      </c>
+      <c r="I59" s="79"/>
+      <c r="J59" s="79" t="s">
+        <v>1929</v>
+      </c>
+      <c r="K59" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L59" s="13"/>
+    </row>
+    <row r="60" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="15" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B60" s="79" t="s">
+        <v>1903</v>
+      </c>
+      <c r="C60" s="75" t="s">
+        <v>1934</v>
+      </c>
+      <c r="D60" s="80" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E60" s="75" t="s">
+        <v>1933</v>
+      </c>
+      <c r="F60" s="75" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G60" s="79" t="s">
+        <v>1930</v>
+      </c>
+      <c r="H60" s="79" t="s">
+        <v>1931</v>
+      </c>
+      <c r="I60" s="79"/>
+      <c r="J60" s="79" t="s">
+        <v>1932</v>
+      </c>
+      <c r="K60" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="L60" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -26544,8 +27802,8 @@
   <dimension ref="A1:K117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Sprint 11 draft updates
CT and changes files updated
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69053149-E133-4AD6-B528-ED558D5622B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DD0418-5667-408A-A6F6-B77F423BBD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="410" yWindow="230" windowWidth="17820" windowHeight="9660" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="20" windowWidth="18970" windowHeight="8990" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8403" uniqueCount="2275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8392" uniqueCount="2274">
   <si>
     <t>Code</t>
   </si>
@@ -12584,46 +12584,7 @@
     <t>Add new relationship to StudyVersion class</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>study</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Titles</t>
-    </r>
-  </si>
-  <si>
     <t>Add new class</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Study</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Title</t>
-    </r>
   </si>
   <si>
     <t>DDF Study Title Attribute Terminology</t>
@@ -12814,9 +12775,6 @@
     </r>
   </si>
   <si>
-    <t>Y (Point out to external dictionaries ISO-3166, GENC, UN Region Codes, etc.)</t>
-  </si>
-  <si>
     <t>Y (Point out to multiple Biomedical coding dictionaries such as SNOMEDCT (for FDA), MedDRA, NCIt, ICD's, etc.)</t>
   </si>
   <si>
@@ -13015,6 +12973,12 @@
   </si>
   <si>
     <t>Move 'inheritance' information out of Role column and into a new/separate column called 'Inherited From' and then put the name of the class in as the value.</t>
+  </si>
+  <si>
+    <t>StudyTitle</t>
+  </si>
+  <si>
+    <t>studyTitles</t>
   </si>
 </sst>
 </file>
@@ -13428,7 +13392,7 @@
     <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -13743,12 +13707,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -13776,13 +13734,22 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -14112,10 +14079,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="118" t="s">
         <v>914</v>
       </c>
-      <c r="B1" s="107"/>
+      <c r="B1" s="119"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -35549,7 +35516,7 @@
     <col min="4" max="4" width="16.1796875" customWidth="1"/>
     <col min="5" max="5" width="23.1796875" customWidth="1"/>
     <col min="6" max="6" width="17.81640625" customWidth="1"/>
-    <col min="7" max="7" width="17.81640625" style="119" customWidth="1"/>
+    <col min="7" max="7" width="17.81640625" style="117" customWidth="1"/>
     <col min="8" max="8" width="12.6328125" customWidth="1"/>
     <col min="9" max="9" width="22.453125" customWidth="1"/>
     <col min="10" max="10" width="14.36328125" customWidth="1"/>
@@ -35577,8 +35544,8 @@
       <c r="F1" s="32" t="s">
         <v>923</v>
       </c>
-      <c r="G1" s="112" t="s">
-        <v>2212</v>
+      <c r="G1" s="110" t="s">
+        <v>2210</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>916</v>
@@ -35705,13 +35672,13 @@
       <c r="D5" s="88" t="s">
         <v>1473</v>
       </c>
-      <c r="E5" s="108" t="s">
-        <v>2190</v>
+      <c r="E5" s="120" t="s">
+        <v>2273</v>
       </c>
       <c r="F5" s="85" t="s">
         <v>926</v>
       </c>
-      <c r="G5" s="118"/>
+      <c r="G5" s="116"/>
       <c r="H5" s="87"/>
       <c r="I5" s="87"/>
       <c r="J5" s="87"/>
@@ -35723,7 +35690,7 @@
     </row>
     <row r="6" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>118</v>
@@ -35732,10 +35699,10 @@
         <v>119</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>2192</v>
+        <v>2272</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>2192</v>
+        <v>2272</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>960</v>
@@ -35766,10 +35733,10 @@
         <v>919</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>2193</v>
+        <v>2191</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>2192</v>
+        <v>2272</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>1103</v>
@@ -35782,11 +35749,11 @@
         <v>919</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>2194</v>
+        <v>2192</v>
       </c>
       <c r="J7" s="13"/>
       <c r="K7" s="16" t="s">
-        <v>2195</v>
+        <v>2193</v>
       </c>
       <c r="L7" s="16" t="s">
         <v>944</v>
@@ -35801,10 +35768,10 @@
         <v>919</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>2193</v>
+        <v>2191</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>2192</v>
+        <v>2272</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>1344</v>
@@ -35817,29 +35784,29 @@
         <v>919</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>2196</v>
+        <v>2194</v>
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="16" t="s">
-        <v>2197</v>
+        <v>2195</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>2198</v>
+        <v>2196</v>
       </c>
       <c r="M8" s="13"/>
     </row>
     <row r="9" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>2199</v>
+        <v>2197</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>919</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>2200</v>
+        <v>2198</v>
       </c>
       <c r="D9" s="75" t="s">
-        <v>2192</v>
+        <v>2272</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>1344</v>
@@ -35852,13 +35819,13 @@
         <v>919</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>2201</v>
+        <v>2199</v>
       </c>
       <c r="J9" s="16" t="s">
         <v>354</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>2202</v>
+        <v>2200</v>
       </c>
       <c r="L9" s="16" t="s">
         <v>945</v>
@@ -35867,16 +35834,16 @@
     </row>
     <row r="10" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>2199</v>
+        <v>2197</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>919</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>2200</v>
+        <v>2198</v>
       </c>
       <c r="D10" s="75" t="s">
-        <v>2192</v>
+        <v>2272</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>1344</v>
@@ -35889,11 +35856,11 @@
         <v>919</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>2203</v>
+        <v>2201</v>
       </c>
       <c r="J10" s="16"/>
       <c r="K10" s="16" t="s">
-        <v>2204</v>
+        <v>2202</v>
       </c>
       <c r="L10" s="16" t="s">
         <v>945</v>
@@ -35902,16 +35869,16 @@
     </row>
     <row r="11" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>2199</v>
+        <v>2197</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>919</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>2200</v>
+        <v>2198</v>
       </c>
       <c r="D11" s="75" t="s">
-        <v>2192</v>
+        <v>2272</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>1344</v>
@@ -35924,11 +35891,11 @@
         <v>919</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>2205</v>
+        <v>2203</v>
       </c>
       <c r="J11" s="16"/>
       <c r="K11" s="16" t="s">
-        <v>2206</v>
+        <v>2204</v>
       </c>
       <c r="L11" s="16" t="s">
         <v>945</v>
@@ -35937,16 +35904,16 @@
     </row>
     <row r="12" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>2199</v>
+        <v>2197</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>919</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>2200</v>
+        <v>2198</v>
       </c>
       <c r="D12" s="75" t="s">
-        <v>2192</v>
+        <v>2272</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>1344</v>
@@ -35959,11 +35926,11 @@
         <v>919</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>2207</v>
+        <v>2205</v>
       </c>
       <c r="J12" s="16"/>
       <c r="K12" s="16" t="s">
-        <v>2208</v>
+        <v>2206</v>
       </c>
       <c r="L12" s="16" t="s">
         <v>945</v>
@@ -35972,16 +35939,16 @@
     </row>
     <row r="13" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>2199</v>
+        <v>2197</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>919</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>2200</v>
+        <v>2198</v>
       </c>
       <c r="D13" s="75" t="s">
-        <v>2192</v>
+        <v>2272</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>1344</v>
@@ -36007,7 +35974,7 @@
     </row>
     <row r="14" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>2209</v>
+        <v>2207</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>945</v>
@@ -36018,24 +35985,22 @@
       <c r="D14" s="16" t="s">
         <v>2156</v>
       </c>
-      <c r="E14" s="108" t="s">
-        <v>2213</v>
+      <c r="E14" s="106" t="s">
+        <v>2211</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>2214</v>
-      </c>
-      <c r="G14" s="89" t="s">
-        <v>2156</v>
-      </c>
+        <v>2212</v>
+      </c>
+      <c r="G14" s="89"/>
       <c r="H14" s="16" t="s">
         <v>919</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>2210</v>
+        <v>2208</v>
       </c>
       <c r="J14" s="16"/>
       <c r="K14" s="16" t="s">
-        <v>2211</v>
+        <v>2209</v>
       </c>
       <c r="L14" s="16" t="s">
         <v>944</v>
@@ -36044,7 +36009,7 @@
     </row>
     <row r="15" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>2209</v>
+        <v>2207</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>945</v>
@@ -36055,8 +36020,8 @@
       <c r="D15" s="16" t="s">
         <v>931</v>
       </c>
-      <c r="E15" s="108" t="s">
-        <v>2213</v>
+      <c r="E15" s="106" t="s">
+        <v>2211</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>926</v>
@@ -36075,7 +36040,7 @@
     </row>
     <row r="16" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>2209</v>
+        <v>2207</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>945</v>
@@ -36083,11 +36048,11 @@
       <c r="C16" s="16" t="s">
         <v>945</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="16" t="s">
         <v>2126</v>
       </c>
       <c r="E16" s="83" t="s">
-        <v>2213</v>
+        <v>2211</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>926</v>
@@ -36114,7 +36079,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:M79"/>
+  <dimension ref="A1:M78"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
@@ -36150,8 +36115,8 @@
       <c r="F1" s="32" t="s">
         <v>923</v>
       </c>
-      <c r="G1" s="112" t="s">
-        <v>2212</v>
+      <c r="G1" s="110" t="s">
+        <v>2210</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>916</v>
@@ -36174,7 +36139,7 @@
     </row>
     <row r="2" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>1892</v>
@@ -36186,10 +36151,10 @@
         <v>1938</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>2216</v>
+        <v>2214</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G2" s="92"/>
       <c r="H2" s="58" t="s">
@@ -36203,13 +36168,13 @@
         <v>1519</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>2218</v>
-      </c>
-      <c r="M2" s="109"/>
+        <v>2216</v>
+      </c>
+      <c r="M2" s="107"/>
     </row>
     <row r="3" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>2219</v>
+        <v>2217</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>919</v>
@@ -36224,18 +36189,18 @@
         <v>1487</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>2220</v>
+        <v>2218</v>
       </c>
       <c r="G3" s="89"/>
-      <c r="H3" s="109" t="s">
+      <c r="H3" s="107" t="s">
         <v>919</v>
       </c>
       <c r="I3" s="89" t="s">
-        <v>2221</v>
+        <v>2219</v>
       </c>
       <c r="J3" s="89"/>
       <c r="K3" s="89" t="s">
-        <v>2222</v>
+        <v>2220</v>
       </c>
       <c r="L3" s="89" t="s">
         <v>944</v>
@@ -36244,7 +36209,7 @@
     </row>
     <row r="4" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>2219</v>
+        <v>2217</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>919</v>
@@ -36259,18 +36224,18 @@
         <v>1565</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>2220</v>
+        <v>2218</v>
       </c>
       <c r="G4" s="89"/>
-      <c r="H4" s="109" t="s">
+      <c r="H4" s="107" t="s">
         <v>919</v>
       </c>
       <c r="I4" s="89" t="s">
-        <v>2223</v>
+        <v>2221</v>
       </c>
       <c r="J4" s="89"/>
       <c r="K4" s="89" t="s">
-        <v>2224</v>
+        <v>2222</v>
       </c>
       <c r="L4" s="89" t="s">
         <v>944</v>
@@ -36279,7 +36244,7 @@
     </row>
     <row r="5" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>919</v>
@@ -36294,7 +36259,7 @@
         <v>1554</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G5" s="92"/>
       <c r="H5" s="15" t="s">
@@ -36310,7 +36275,7 @@
         <v>1557</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>2225</v>
+        <v>2223</v>
       </c>
       <c r="M5" s="96" t="s">
         <v>1822</v>
@@ -36318,7 +36283,7 @@
     </row>
     <row r="6" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>919</v>
@@ -36333,7 +36298,7 @@
         <v>1559</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G6" s="92"/>
       <c r="H6" s="15" t="s">
@@ -36349,7 +36314,7 @@
         <v>1562</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>2226</v>
+        <v>2224</v>
       </c>
       <c r="M6" s="16" t="s">
         <v>1823</v>
@@ -36357,7 +36322,7 @@
     </row>
     <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>919</v>
@@ -36372,7 +36337,7 @@
         <v>1259</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G7" s="92"/>
       <c r="H7" s="55" t="s">
@@ -36386,7 +36351,7 @@
         <v>1262</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>2227</v>
+        <v>2225</v>
       </c>
       <c r="M7" s="96" t="s">
         <v>1824</v>
@@ -36394,7 +36359,7 @@
     </row>
     <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>78</v>
@@ -36409,7 +36374,7 @@
         <v>1344</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G8" s="92"/>
       <c r="H8" s="15" t="s">
@@ -36431,7 +36396,7 @@
     </row>
     <row r="9" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>78</v>
@@ -36446,7 +36411,7 @@
         <v>1789</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G9" s="92"/>
       <c r="H9" s="15" t="s">
@@ -36460,7 +36425,7 @@
         <v>96</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>2228</v>
+        <v>2226</v>
       </c>
       <c r="M9" s="97" t="s">
         <v>1825</v>
@@ -36468,7 +36433,7 @@
     </row>
     <row r="10" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>78</v>
@@ -36483,7 +36448,7 @@
         <v>1791</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G10" s="92"/>
       <c r="H10" s="15" t="s">
@@ -36497,7 +36462,7 @@
         <v>93</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>2229</v>
+        <v>2227</v>
       </c>
       <c r="M10" s="97" t="s">
         <v>1826</v>
@@ -36505,7 +36470,7 @@
     </row>
     <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>105</v>
@@ -36520,7 +36485,7 @@
         <v>1793</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G11" s="92"/>
       <c r="H11" s="15" t="s">
@@ -36542,7 +36507,7 @@
     </row>
     <row r="12" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>2230</v>
+        <v>2228</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>919</v>
@@ -36556,8 +36521,8 @@
       <c r="E12" s="18" t="s">
         <v>1424</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>915</v>
+      <c r="F12" s="15" t="s">
+        <v>2215</v>
       </c>
       <c r="G12" s="89"/>
       <c r="H12" s="15" t="s">
@@ -36571,13 +36536,13 @@
         <v>1481</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>2231</v>
+        <v>2229</v>
       </c>
       <c r="M12" s="13"/>
     </row>
     <row r="13" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>919</v>
@@ -36592,7 +36557,7 @@
         <v>1344</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G13" s="92"/>
       <c r="H13" s="15" t="s">
@@ -36610,184 +36575,184 @@
       </c>
       <c r="M13" s="58"/>
     </row>
-    <row r="14" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>919</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>1495</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>1476</v>
+        <v>1490</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>1403</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>1424</v>
+        <v>1344</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G14" s="92"/>
       <c r="H14" s="15" t="s">
         <v>919</v>
       </c>
-      <c r="I14" s="54" t="s">
-        <v>1480</v>
+      <c r="I14" s="16" t="s">
+        <v>1416</v>
       </c>
       <c r="J14" s="54"/>
       <c r="K14" s="16" t="s">
-        <v>1481</v>
+        <v>1417</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>2232</v>
+        <v>1508</v>
       </c>
       <c r="M14" s="58"/>
     </row>
-    <row r="15" spans="1:13" ht="50" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
+        <v>2213</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>930</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>1677</v>
+      </c>
+      <c r="F15" s="15" t="s">
         <v>2215</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>919</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>1490</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>1403</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>1344</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>2217</v>
       </c>
       <c r="G15" s="92"/>
       <c r="H15" s="15" t="s">
-        <v>919</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>1416</v>
-      </c>
-      <c r="J15" s="54"/>
-      <c r="K15" s="16" t="s">
-        <v>1417</v>
-      </c>
-      <c r="L15" s="16" t="s">
-        <v>1508</v>
+        <v>208</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>2230</v>
       </c>
       <c r="M15" s="58"/>
     </row>
     <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
+        <v>2213</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>932</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>1793</v>
+      </c>
+      <c r="F16" s="15" t="s">
         <v>2215</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>930</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>1677</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>2217</v>
       </c>
       <c r="G16" s="92"/>
       <c r="H16" s="15" t="s">
-        <v>208</v>
+        <v>241</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>209</v>
+        <v>242</v>
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15" t="s">
-        <v>210</v>
+        <v>1296</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>2233</v>
-      </c>
-      <c r="M16" s="58"/>
+        <v>1297</v>
+      </c>
+      <c r="M16" s="13" t="s">
+        <v>1829</v>
+      </c>
     </row>
     <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
+        <v>2213</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>2215</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>932</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>1793</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>2217</v>
       </c>
       <c r="G17" s="92"/>
       <c r="H17" s="15" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="15" t="s">
-        <v>1296</v>
+        <v>258</v>
       </c>
       <c r="L17" s="15" t="s">
-        <v>1297</v>
+        <v>1144</v>
       </c>
       <c r="M17" s="13" t="s">
-        <v>1829</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>2215</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>244</v>
+        <v>1532</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>919</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>2159</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>1344</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>2217</v>
-      </c>
-      <c r="G18" s="92"/>
-      <c r="H18" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15" t="s">
-        <v>258</v>
-      </c>
-      <c r="L18" s="15" t="s">
-        <v>1144</v>
-      </c>
-      <c r="M18" s="13" t="s">
-        <v>1830</v>
-      </c>
+        <v>2156</v>
+      </c>
+      <c r="E18" s="65" t="s">
+        <v>1108</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>2231</v>
+      </c>
+      <c r="G18" s="89"/>
+      <c r="H18" s="16" t="s">
+        <v>919</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>2161</v>
+      </c>
+      <c r="J18" s="13"/>
+      <c r="K18" s="16" t="s">
+        <v>2162</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>944</v>
+      </c>
+      <c r="M18" s="13"/>
     </row>
     <row r="19" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
@@ -36803,21 +36768,21 @@
         <v>2156</v>
       </c>
       <c r="E19" s="65" t="s">
-        <v>1108</v>
+        <v>1185</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>2234</v>
+        <v>2231</v>
       </c>
       <c r="G19" s="89"/>
       <c r="H19" s="16" t="s">
         <v>919</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>2161</v>
+        <v>2163</v>
       </c>
       <c r="J19" s="13"/>
       <c r="K19" s="16" t="s">
-        <v>2162</v>
+        <v>2164</v>
       </c>
       <c r="L19" s="16" t="s">
         <v>944</v>
@@ -36838,65 +36803,59 @@
         <v>2156</v>
       </c>
       <c r="E20" s="65" t="s">
-        <v>1185</v>
+        <v>1116</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>2234</v>
+        <v>2231</v>
       </c>
       <c r="G20" s="89"/>
       <c r="H20" s="16" t="s">
         <v>919</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>2163</v>
+        <v>2165</v>
       </c>
       <c r="J20" s="13"/>
       <c r="K20" s="16" t="s">
-        <v>2164</v>
+        <v>2166</v>
       </c>
       <c r="L20" s="16" t="s">
         <v>944</v>
       </c>
       <c r="M20" s="13"/>
     </row>
-    <row r="21" spans="1:13" ht="50" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>1532</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>919</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>2159</v>
-      </c>
-      <c r="D21" s="15" t="s">
+        <v>2232</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>945</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>945</v>
+      </c>
+      <c r="D21" s="23" t="s">
         <v>2156</v>
       </c>
-      <c r="E21" s="65" t="s">
-        <v>1116</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>2234</v>
-      </c>
-      <c r="G21" s="89"/>
-      <c r="H21" s="16" t="s">
-        <v>919</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>2165</v>
-      </c>
-      <c r="J21" s="13"/>
-      <c r="K21" s="16" t="s">
-        <v>2166</v>
-      </c>
-      <c r="L21" s="16" t="s">
-        <v>944</v>
+      <c r="E21" s="25" t="s">
+        <v>2140</v>
+      </c>
+      <c r="F21" s="61" t="s">
+        <v>926</v>
+      </c>
+      <c r="G21" s="111"/>
+      <c r="H21" s="108"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="61"/>
+      <c r="K21" s="61"/>
+      <c r="L21" s="61" t="s">
+        <v>945</v>
       </c>
       <c r="M21" s="13"/>
     </row>
     <row r="22" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>2235</v>
+        <v>2232</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>945</v>
@@ -36908,13 +36867,13 @@
         <v>2156</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>2140</v>
+        <v>2141</v>
       </c>
       <c r="F22" s="61" t="s">
         <v>926</v>
       </c>
-      <c r="G22" s="113"/>
-      <c r="H22" s="110"/>
+      <c r="G22" s="111"/>
+      <c r="H22" s="108"/>
       <c r="I22" s="61"/>
       <c r="J22" s="61"/>
       <c r="K22" s="61"/>
@@ -36923,9 +36882,9 @@
       </c>
       <c r="M22" s="13"/>
     </row>
-    <row r="23" spans="1:13" ht="25" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
-        <v>2235</v>
+    <row r="23" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>2233</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>945</v>
@@ -36933,17 +36892,17 @@
       <c r="C23" s="13" t="s">
         <v>945</v>
       </c>
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="15" t="s">
         <v>2156</v>
       </c>
-      <c r="E23" s="25" t="s">
-        <v>2141</v>
-      </c>
-      <c r="F23" s="61" t="s">
-        <v>926</v>
-      </c>
-      <c r="G23" s="113"/>
-      <c r="H23" s="110"/>
+      <c r="E23" s="83" t="s">
+        <v>2123</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>2234</v>
+      </c>
+      <c r="G23" s="89"/>
+      <c r="H23" s="108"/>
       <c r="I23" s="61"/>
       <c r="J23" s="61"/>
       <c r="K23" s="61"/>
@@ -36952,38 +36911,44 @@
       </c>
       <c r="M23" s="13"/>
     </row>
-    <row r="24" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>2236</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>945</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>945</v>
+    <row r="24" spans="1:13" ht="50" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>2217</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>919</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>2159</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>2156</v>
       </c>
-      <c r="E24" s="83" t="s">
-        <v>2123</v>
+      <c r="E24" s="18" t="s">
+        <v>2120</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>2237</v>
+        <v>2218</v>
       </c>
       <c r="G24" s="89"/>
-      <c r="H24" s="110"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="61"/>
-      <c r="L24" s="61" t="s">
-        <v>945</v>
+      <c r="H24" s="107" t="s">
+        <v>919</v>
+      </c>
+      <c r="I24" s="89" t="s">
+        <v>2235</v>
+      </c>
+      <c r="J24" s="89"/>
+      <c r="K24" s="89" t="s">
+        <v>2236</v>
+      </c>
+      <c r="L24" s="89" t="s">
+        <v>944</v>
       </c>
       <c r="M24" s="13"/>
     </row>
     <row r="25" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>2219</v>
+        <v>2217</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>919</v>
@@ -36995,21 +36960,21 @@
         <v>2156</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>2120</v>
+        <v>2139</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>2220</v>
+        <v>2218</v>
       </c>
       <c r="G25" s="89"/>
-      <c r="H25" s="109" t="s">
+      <c r="H25" s="107" t="s">
         <v>919</v>
       </c>
       <c r="I25" s="89" t="s">
-        <v>2238</v>
+        <v>2237</v>
       </c>
       <c r="J25" s="89"/>
       <c r="K25" s="89" t="s">
-        <v>2239</v>
+        <v>2238</v>
       </c>
       <c r="L25" s="89" t="s">
         <v>944</v>
@@ -37018,114 +36983,110 @@
     </row>
     <row r="26" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>2219</v>
+        <v>2213</v>
       </c>
       <c r="B26" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>1424</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>2215</v>
+      </c>
+      <c r="G26" s="92"/>
+      <c r="H26" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="L26" s="15" t="s">
+        <v>1166</v>
+      </c>
+      <c r="M26" s="58"/>
+    </row>
+    <row r="27" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>2213</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>919</v>
       </c>
-      <c r="C26" s="16" t="s">
-        <v>2159</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>2156</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>2139</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>2220</v>
-      </c>
-      <c r="G26" s="89"/>
-      <c r="H26" s="109" t="s">
-        <v>919</v>
-      </c>
-      <c r="I26" s="89" t="s">
-        <v>2240</v>
-      </c>
-      <c r="J26" s="89"/>
-      <c r="K26" s="89" t="s">
-        <v>2241</v>
-      </c>
-      <c r="L26" s="89" t="s">
-        <v>944</v>
-      </c>
-      <c r="M26" s="13"/>
-    </row>
-    <row r="27" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
+      <c r="C27" s="16" t="s">
+        <v>1605</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>1602</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>1610</v>
+      </c>
+      <c r="F27" s="15" t="s">
         <v>2215</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>259</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>1424</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>2217</v>
       </c>
       <c r="G27" s="92"/>
       <c r="H27" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>264</v>
-      </c>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="L27" s="15" t="s">
-        <v>1166</v>
-      </c>
-      <c r="M27" s="58"/>
-    </row>
-    <row r="28" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>1611</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>1612</v>
+      </c>
+      <c r="J27" s="13"/>
+      <c r="K27" s="16" t="s">
+        <v>1613</v>
+      </c>
+      <c r="L27" s="16" t="s">
+        <v>2239</v>
+      </c>
+      <c r="M27" s="16" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>2215</v>
+        <v>2240</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>919</v>
+        <v>945</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>1605</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>1602</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>1610</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>2217</v>
-      </c>
-      <c r="G28" s="92"/>
-      <c r="H28" s="15" t="s">
-        <v>1611</v>
-      </c>
-      <c r="I28" s="16" t="s">
-        <v>1612</v>
-      </c>
+        <v>945</v>
+      </c>
+      <c r="D28" s="55" t="s">
+        <v>959</v>
+      </c>
+      <c r="E28" s="83" t="s">
+        <v>1779</v>
+      </c>
+      <c r="F28" s="55" t="s">
+        <v>926</v>
+      </c>
+      <c r="G28" s="92" t="s">
+        <v>961</v>
+      </c>
+      <c r="H28" s="55"/>
+      <c r="I28" s="13"/>
       <c r="J28" s="13"/>
-      <c r="K28" s="16" t="s">
-        <v>1613</v>
-      </c>
+      <c r="K28" s="13"/>
       <c r="L28" s="16" t="s">
-        <v>2242</v>
-      </c>
-      <c r="M28" s="16" t="s">
-        <v>1831</v>
-      </c>
+        <v>945</v>
+      </c>
+      <c r="M28" s="13"/>
     </row>
     <row r="29" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>2243</v>
+        <v>2240</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>945</v>
@@ -37137,7 +37098,7 @@
         <v>959</v>
       </c>
       <c r="E29" s="83" t="s">
-        <v>1779</v>
+        <v>1781</v>
       </c>
       <c r="F29" s="55" t="s">
         <v>926</v>
@@ -37156,7 +37117,7 @@
     </row>
     <row r="30" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>2243</v>
+        <v>2240</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>945</v>
@@ -37168,7 +37129,7 @@
         <v>959</v>
       </c>
       <c r="E30" s="83" t="s">
-        <v>1781</v>
+        <v>1782</v>
       </c>
       <c r="F30" s="55" t="s">
         <v>926</v>
@@ -37187,7 +37148,7 @@
     </row>
     <row r="31" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>2243</v>
+        <v>2240</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>945</v>
@@ -37199,7 +37160,7 @@
         <v>959</v>
       </c>
       <c r="E31" s="83" t="s">
-        <v>1782</v>
+        <v>1783</v>
       </c>
       <c r="F31" s="55" t="s">
         <v>926</v>
@@ -37217,20 +37178,20 @@
       <c r="M31" s="13"/>
     </row>
     <row r="32" spans="1:13" ht="25" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
-        <v>2243</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>945</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>945</v>
-      </c>
-      <c r="D32" s="55" t="s">
+      <c r="A32" s="85" t="s">
+        <v>2240</v>
+      </c>
+      <c r="B32" s="85" t="s">
+        <v>945</v>
+      </c>
+      <c r="C32" s="85" t="s">
+        <v>945</v>
+      </c>
+      <c r="D32" s="84" t="s">
         <v>959</v>
       </c>
-      <c r="E32" s="83" t="s">
-        <v>1783</v>
+      <c r="E32" s="106" t="s">
+        <v>1784</v>
       </c>
       <c r="F32" s="55" t="s">
         <v>926</v>
@@ -37238,30 +37199,30 @@
       <c r="G32" s="92" t="s">
         <v>961</v>
       </c>
-      <c r="H32" s="55"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="16" t="s">
-        <v>945</v>
-      </c>
-      <c r="M32" s="13"/>
+      <c r="H32" s="84"/>
+      <c r="I32" s="87"/>
+      <c r="J32" s="87"/>
+      <c r="K32" s="87"/>
+      <c r="L32" s="85" t="s">
+        <v>945</v>
+      </c>
+      <c r="M32" s="87"/>
     </row>
     <row r="33" spans="1:13" ht="25" x14ac:dyDescent="0.25">
-      <c r="A33" s="85" t="s">
-        <v>2243</v>
-      </c>
-      <c r="B33" s="85" t="s">
-        <v>945</v>
-      </c>
-      <c r="C33" s="85" t="s">
-        <v>945</v>
-      </c>
-      <c r="D33" s="84" t="s">
-        <v>959</v>
-      </c>
-      <c r="E33" s="108" t="s">
-        <v>1784</v>
+      <c r="A33" s="16" t="s">
+        <v>2240</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>945</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>945</v>
+      </c>
+      <c r="D33" s="55" t="s">
+        <v>1785</v>
+      </c>
+      <c r="E33" s="83" t="s">
+        <v>1779</v>
       </c>
       <c r="F33" s="55" t="s">
         <v>926</v>
@@ -37269,18 +37230,18 @@
       <c r="G33" s="92" t="s">
         <v>961</v>
       </c>
-      <c r="H33" s="84"/>
-      <c r="I33" s="87"/>
-      <c r="J33" s="87"/>
-      <c r="K33" s="87"/>
-      <c r="L33" s="85" t="s">
-        <v>945</v>
-      </c>
-      <c r="M33" s="87"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="16" t="s">
+        <v>945</v>
+      </c>
+      <c r="M33" s="13"/>
     </row>
     <row r="34" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>2243</v>
+        <v>2240</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>945</v>
@@ -37292,7 +37253,7 @@
         <v>1785</v>
       </c>
       <c r="E34" s="83" t="s">
-        <v>1779</v>
+        <v>1781</v>
       </c>
       <c r="F34" s="55" t="s">
         <v>926</v>
@@ -37311,7 +37272,7 @@
     </row>
     <row r="35" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>2243</v>
+        <v>2240</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>945</v>
@@ -37323,7 +37284,7 @@
         <v>1785</v>
       </c>
       <c r="E35" s="83" t="s">
-        <v>1781</v>
+        <v>1782</v>
       </c>
       <c r="F35" s="55" t="s">
         <v>926</v>
@@ -37342,7 +37303,7 @@
     </row>
     <row r="36" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>2243</v>
+        <v>2240</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>945</v>
@@ -37354,7 +37315,7 @@
         <v>1785</v>
       </c>
       <c r="E36" s="83" t="s">
-        <v>1782</v>
+        <v>1783</v>
       </c>
       <c r="F36" s="55" t="s">
         <v>926</v>
@@ -37373,7 +37334,7 @@
     </row>
     <row r="37" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>2243</v>
+        <v>2240</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>945</v>
@@ -37385,7 +37346,7 @@
         <v>1785</v>
       </c>
       <c r="E37" s="83" t="s">
-        <v>1783</v>
+        <v>1784</v>
       </c>
       <c r="F37" s="55" t="s">
         <v>926</v>
@@ -37402,77 +37363,83 @@
       </c>
       <c r="M37" s="13"/>
     </row>
-    <row r="38" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>2243</v>
+        <v>2213</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>945</v>
+        <v>919</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>945</v>
-      </c>
-      <c r="D38" s="55" t="s">
-        <v>1785</v>
-      </c>
-      <c r="E38" s="83" t="s">
-        <v>1784</v>
-      </c>
-      <c r="F38" s="55" t="s">
-        <v>926</v>
-      </c>
-      <c r="G38" s="92" t="s">
-        <v>961</v>
-      </c>
-      <c r="H38" s="55"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
+        <v>1491</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>1420</v>
+      </c>
+      <c r="E38" s="65" t="s">
+        <v>1424</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>2215</v>
+      </c>
+      <c r="G38" s="92"/>
+      <c r="H38" s="55" t="s">
+        <v>919</v>
+      </c>
+      <c r="I38" s="16" t="s">
+        <v>1425</v>
+      </c>
+      <c r="J38" s="16" t="s">
+        <v>1425</v>
+      </c>
+      <c r="K38" s="16" t="s">
+        <v>1426</v>
+      </c>
       <c r="L38" s="16" t="s">
-        <v>945</v>
-      </c>
-      <c r="M38" s="13"/>
-    </row>
-    <row r="39" spans="1:13" ht="50" x14ac:dyDescent="0.25">
+        <v>2241</v>
+      </c>
+      <c r="M38" s="58"/>
+    </row>
+    <row r="39" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
+        <v>2213</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>934</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F39" s="15" t="s">
         <v>2215</v>
       </c>
-      <c r="B39" s="16" t="s">
-        <v>919</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>1491</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>1420</v>
-      </c>
-      <c r="E39" s="65" t="s">
-        <v>1424</v>
-      </c>
-      <c r="F39" s="15" t="s">
-        <v>2217</v>
-      </c>
       <c r="G39" s="92"/>
-      <c r="H39" s="55" t="s">
-        <v>919</v>
-      </c>
-      <c r="I39" s="16" t="s">
-        <v>1425</v>
-      </c>
-      <c r="J39" s="16" t="s">
-        <v>1425</v>
-      </c>
-      <c r="K39" s="16" t="s">
-        <v>1426</v>
-      </c>
-      <c r="L39" s="16" t="s">
-        <v>2244</v>
-      </c>
-      <c r="M39" s="58"/>
+      <c r="H39" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>1148</v>
+      </c>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15" t="s">
+        <v>1149</v>
+      </c>
+      <c r="L39" s="15" t="s">
+        <v>2242</v>
+      </c>
+      <c r="M39" s="97" t="s">
+        <v>1832</v>
+      </c>
     </row>
     <row r="40" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>270</v>
@@ -37484,69 +37451,61 @@
         <v>934</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>1344</v>
+        <v>1796</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G40" s="92"/>
       <c r="H40" s="15" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>1148</v>
+        <v>278</v>
       </c>
       <c r="J40" s="15"/>
-      <c r="K40" s="15" t="s">
-        <v>1149</v>
+      <c r="K40" s="16" t="s">
+        <v>1152</v>
       </c>
       <c r="L40" s="15" t="s">
-        <v>2245</v>
-      </c>
-      <c r="M40" s="97" t="s">
-        <v>1832</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>1153</v>
+      </c>
+      <c r="M40" s="13" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>2215</v>
+        <v>2232</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>270</v>
+        <v>945</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>271</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>934</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>1796</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>2217</v>
-      </c>
-      <c r="G41" s="92"/>
-      <c r="H41" s="15" t="s">
-        <v>277</v>
-      </c>
-      <c r="I41" s="15" t="s">
-        <v>278</v>
-      </c>
-      <c r="J41" s="15"/>
-      <c r="K41" s="16" t="s">
-        <v>1152</v>
-      </c>
-      <c r="L41" s="15" t="s">
-        <v>1153</v>
-      </c>
-      <c r="M41" s="13" t="s">
-        <v>1833</v>
-      </c>
+        <v>945</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>2126</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>2140</v>
+      </c>
+      <c r="F41" s="61" t="s">
+        <v>2121</v>
+      </c>
+      <c r="G41" s="111"/>
+      <c r="H41" s="61"/>
+      <c r="I41" s="61"/>
+      <c r="J41" s="61"/>
+      <c r="K41" s="61"/>
+      <c r="L41" s="61" t="s">
+        <v>945</v>
+      </c>
+      <c r="M41" s="13"/>
     </row>
     <row r="42" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>2235</v>
+        <v>2232</v>
       </c>
       <c r="B42" s="16" t="s">
         <v>945</v>
@@ -37558,12 +37517,12 @@
         <v>2126</v>
       </c>
       <c r="E42" s="25" t="s">
-        <v>2140</v>
+        <v>2141</v>
       </c>
       <c r="F42" s="61" t="s">
         <v>2121</v>
       </c>
-      <c r="G42" s="113"/>
+      <c r="G42" s="111"/>
       <c r="H42" s="61"/>
       <c r="I42" s="61"/>
       <c r="J42" s="61"/>
@@ -37573,38 +37532,48 @@
       </c>
       <c r="M42" s="13"/>
     </row>
-    <row r="43" spans="1:13" ht="50" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
-        <v>2235</v>
+        <v>2213</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>945</v>
+        <v>289</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>945</v>
-      </c>
-      <c r="D43" s="23" t="s">
-        <v>2126</v>
-      </c>
-      <c r="E43" s="25" t="s">
-        <v>2141</v>
-      </c>
-      <c r="F43" s="61" t="s">
-        <v>2121</v>
-      </c>
-      <c r="G43" s="113"/>
-      <c r="H43" s="61"/>
-      <c r="I43" s="61"/>
-      <c r="J43" s="61"/>
-      <c r="K43" s="61"/>
-      <c r="L43" s="61" t="s">
-        <v>945</v>
-      </c>
-      <c r="M43" s="13"/>
+        <v>290</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>920</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>1797</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>2215</v>
+      </c>
+      <c r="G43" s="112"/>
+      <c r="H43" s="88" t="s">
+        <v>297</v>
+      </c>
+      <c r="I43" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="J43" s="85" t="s">
+        <v>298</v>
+      </c>
+      <c r="K43" s="85" t="s">
+        <v>299</v>
+      </c>
+      <c r="L43" s="88" t="s">
+        <v>2243</v>
+      </c>
+      <c r="M43" s="97" t="s">
+        <v>1834</v>
+      </c>
     </row>
     <row r="44" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B44" s="16" t="s">
         <v>289</v>
@@ -37616,34 +37585,34 @@
         <v>920</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>1797</v>
+        <v>1799</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>2217</v>
-      </c>
-      <c r="G44" s="114"/>
+        <v>2215</v>
+      </c>
+      <c r="G44" s="112"/>
       <c r="H44" s="88" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="I44" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="J44" s="85" t="s">
-        <v>298</v>
-      </c>
-      <c r="K44" s="85" t="s">
-        <v>299</v>
-      </c>
-      <c r="L44" s="88" t="s">
-        <v>2246</v>
+        <v>302</v>
+      </c>
+      <c r="J44" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="K44" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="L44" s="15" t="s">
+        <v>2244</v>
       </c>
       <c r="M44" s="97" t="s">
-        <v>1834</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B45" s="16" t="s">
         <v>289</v>
@@ -37655,34 +37624,32 @@
         <v>920</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>1799</v>
+        <v>1801</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>2217</v>
-      </c>
-      <c r="G45" s="114"/>
-      <c r="H45" s="88" t="s">
-        <v>301</v>
+        <v>2215</v>
+      </c>
+      <c r="G45" s="92"/>
+      <c r="H45" s="15" t="s">
+        <v>293</v>
       </c>
       <c r="I45" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="J45" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="K45" s="16" t="s">
-        <v>304</v>
+        <v>294</v>
+      </c>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15" t="s">
+        <v>296</v>
       </c>
       <c r="L45" s="15" t="s">
-        <v>2247</v>
+        <v>2245</v>
       </c>
       <c r="M45" s="97" t="s">
-        <v>1835</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B46" s="16" t="s">
         <v>289</v>
@@ -37694,32 +37661,32 @@
         <v>920</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>1801</v>
+        <v>2246</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G46" s="92"/>
       <c r="H46" s="15" t="s">
-        <v>293</v>
+        <v>2018</v>
       </c>
       <c r="I46" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15" t="s">
-        <v>296</v>
+        <v>2019</v>
+      </c>
+      <c r="J46" s="15" t="s">
+        <v>2020</v>
+      </c>
+      <c r="K46" s="55" t="s">
+        <v>2021</v>
       </c>
       <c r="L46" s="15" t="s">
-        <v>2248</v>
-      </c>
-      <c r="M46" s="97" t="s">
-        <v>1836</v>
-      </c>
+        <v>2247</v>
+      </c>
+      <c r="M46" s="58"/>
     </row>
     <row r="47" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B47" s="16" t="s">
         <v>289</v>
@@ -37731,102 +37698,100 @@
         <v>920</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>2249</v>
+        <v>1803</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G47" s="92"/>
       <c r="H47" s="15" t="s">
-        <v>2018</v>
-      </c>
-      <c r="I47" s="15" t="s">
-        <v>2019</v>
-      </c>
-      <c r="J47" s="15" t="s">
-        <v>2020</v>
-      </c>
-      <c r="K47" s="55" t="s">
-        <v>2021</v>
-      </c>
-      <c r="L47" s="15" t="s">
+        <v>1719</v>
+      </c>
+      <c r="I47" s="16" t="s">
+        <v>1720</v>
+      </c>
+      <c r="J47" s="16" t="s">
+        <v>1721</v>
+      </c>
+      <c r="K47" s="16" t="s">
+        <v>1722</v>
+      </c>
+      <c r="L47" s="16" t="s">
+        <v>2248</v>
+      </c>
+      <c r="M47" s="96" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>2240</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>945</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>945</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>931</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>2120</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>926</v>
+      </c>
+      <c r="G48" s="89" t="s">
+        <v>2156</v>
+      </c>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="16" t="s">
+        <v>945</v>
+      </c>
+      <c r="M48" s="13"/>
+    </row>
+    <row r="49" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
+        <v>2249</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>2061</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>2062</v>
+      </c>
+      <c r="D49" s="73" t="s">
+        <v>931</v>
+      </c>
+      <c r="E49" s="72" t="s">
         <v>2250</v>
       </c>
-      <c r="M47" s="58"/>
-    </row>
-    <row r="48" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
-        <v>2215</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>289</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>290</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>920</v>
-      </c>
-      <c r="E48" s="17" t="s">
-        <v>1803</v>
-      </c>
-      <c r="F48" s="15" t="s">
-        <v>2217</v>
-      </c>
-      <c r="G48" s="92"/>
-      <c r="H48" s="15" t="s">
-        <v>1719</v>
-      </c>
-      <c r="I48" s="16" t="s">
-        <v>1720</v>
-      </c>
-      <c r="J48" s="16" t="s">
-        <v>1721</v>
-      </c>
-      <c r="K48" s="16" t="s">
-        <v>1722</v>
-      </c>
-      <c r="L48" s="16" t="s">
-        <v>2251</v>
-      </c>
-      <c r="M48" s="96" t="s">
-        <v>1837</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="25" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="s">
-        <v>2243</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>945</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>945</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>931</v>
-      </c>
-      <c r="E49" s="22" t="s">
-        <v>2120</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>926</v>
-      </c>
-      <c r="G49" s="89" t="s">
-        <v>2156</v>
-      </c>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-      <c r="J49" s="13"/>
-      <c r="K49" s="13"/>
+      <c r="F49" s="72" t="s">
+        <v>1805</v>
+      </c>
+      <c r="G49" s="113"/>
+      <c r="H49" s="72" t="s">
+        <v>2066</v>
+      </c>
+      <c r="I49" s="72" t="s">
+        <v>2067</v>
+      </c>
+      <c r="J49" s="72"/>
+      <c r="K49" s="72" t="s">
+        <v>2068</v>
+      </c>
       <c r="L49" s="16" t="s">
         <v>945</v>
       </c>
       <c r="M49" s="13"/>
     </row>
-    <row r="50" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
-        <v>2252</v>
+        <v>2249</v>
       </c>
       <c r="B50" s="15" t="s">
         <v>2061</v>
@@ -37838,21 +37803,23 @@
         <v>931</v>
       </c>
       <c r="E50" s="72" t="s">
-        <v>2253</v>
+        <v>2250</v>
       </c>
       <c r="F50" s="72" t="s">
         <v>1805</v>
       </c>
-      <c r="G50" s="115"/>
+      <c r="G50" s="113"/>
       <c r="H50" s="72" t="s">
-        <v>2066</v>
+        <v>2070</v>
       </c>
       <c r="I50" s="72" t="s">
-        <v>2067</v>
-      </c>
-      <c r="J50" s="72"/>
+        <v>2071</v>
+      </c>
+      <c r="J50" s="72" t="s">
+        <v>2072</v>
+      </c>
       <c r="K50" s="72" t="s">
-        <v>2068</v>
+        <v>2073</v>
       </c>
       <c r="L50" s="16" t="s">
         <v>945</v>
@@ -37861,7 +37828,7 @@
     </row>
     <row r="51" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>2252</v>
+        <v>2249</v>
       </c>
       <c r="B51" s="15" t="s">
         <v>2061</v>
@@ -37873,23 +37840,23 @@
         <v>931</v>
       </c>
       <c r="E51" s="72" t="s">
-        <v>2253</v>
+        <v>2250</v>
       </c>
       <c r="F51" s="72" t="s">
         <v>1805</v>
       </c>
-      <c r="G51" s="115"/>
+      <c r="G51" s="113"/>
       <c r="H51" s="72" t="s">
-        <v>2070</v>
+        <v>2074</v>
       </c>
       <c r="I51" s="72" t="s">
-        <v>2071</v>
+        <v>2075</v>
       </c>
       <c r="J51" s="72" t="s">
-        <v>2072</v>
+        <v>2076</v>
       </c>
       <c r="K51" s="72" t="s">
-        <v>2073</v>
+        <v>2077</v>
       </c>
       <c r="L51" s="16" t="s">
         <v>945</v>
@@ -37898,44 +37865,42 @@
     </row>
     <row r="52" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>2252</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>2061</v>
+        <v>2232</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>945</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>2062</v>
-      </c>
-      <c r="D52" s="73" t="s">
+        <v>945</v>
+      </c>
+      <c r="D52" s="23" t="s">
         <v>931</v>
       </c>
-      <c r="E52" s="72" t="s">
-        <v>2253</v>
-      </c>
-      <c r="F52" s="72" t="s">
-        <v>1805</v>
-      </c>
-      <c r="G52" s="115"/>
-      <c r="H52" s="72" t="s">
-        <v>2074</v>
-      </c>
-      <c r="I52" s="72" t="s">
-        <v>2075</v>
-      </c>
-      <c r="J52" s="72" t="s">
-        <v>2076</v>
-      </c>
-      <c r="K52" s="72" t="s">
-        <v>2077</v>
-      </c>
-      <c r="L52" s="16" t="s">
-        <v>945</v>
+      <c r="E52" s="28" t="s">
+        <v>2140</v>
+      </c>
+      <c r="F52" s="23" t="s">
+        <v>2121</v>
+      </c>
+      <c r="G52" s="114"/>
+      <c r="H52" s="108" t="s">
+        <v>2022</v>
+      </c>
+      <c r="I52" s="61" t="s">
+        <v>2023</v>
+      </c>
+      <c r="J52" s="61"/>
+      <c r="K52" s="61" t="s">
+        <v>2024</v>
+      </c>
+      <c r="L52" s="61" t="s">
+        <v>944</v>
       </c>
       <c r="M52" s="13"/>
     </row>
     <row r="53" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
-        <v>2235</v>
+        <v>2232</v>
       </c>
       <c r="B53" s="16" t="s">
         <v>945</v>
@@ -37947,30 +37912,30 @@
         <v>931</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>2140</v>
+        <v>2141</v>
       </c>
       <c r="F53" s="23" t="s">
         <v>2121</v>
       </c>
-      <c r="G53" s="116"/>
-      <c r="H53" s="110" t="s">
-        <v>2022</v>
+      <c r="G53" s="114"/>
+      <c r="H53" s="108" t="s">
+        <v>2025</v>
       </c>
       <c r="I53" s="61" t="s">
-        <v>2023</v>
+        <v>2026</v>
       </c>
       <c r="J53" s="61"/>
       <c r="K53" s="61" t="s">
-        <v>2024</v>
+        <v>2027</v>
       </c>
       <c r="L53" s="61" t="s">
         <v>944</v>
       </c>
       <c r="M53" s="13"/>
     </row>
-    <row r="54" spans="1:13" ht="50" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
-        <v>2235</v>
+        <v>2251</v>
       </c>
       <c r="B54" s="16" t="s">
         <v>945</v>
@@ -37978,387 +37943,387 @@
       <c r="C54" s="16" t="s">
         <v>945</v>
       </c>
-      <c r="D54" s="23" t="s">
+      <c r="D54" s="15" t="s">
         <v>931</v>
       </c>
-      <c r="E54" s="28" t="s">
-        <v>2141</v>
-      </c>
-      <c r="F54" s="23" t="s">
-        <v>2121</v>
-      </c>
-      <c r="G54" s="116"/>
-      <c r="H54" s="110" t="s">
-        <v>2025</v>
-      </c>
-      <c r="I54" s="61" t="s">
-        <v>2026</v>
-      </c>
+      <c r="E54" s="83" t="s">
+        <v>2123</v>
+      </c>
+      <c r="F54" s="15" t="s">
+        <v>926</v>
+      </c>
+      <c r="G54" s="89" t="s">
+        <v>2156</v>
+      </c>
+      <c r="H54" s="108"/>
+      <c r="I54" s="61"/>
       <c r="J54" s="61"/>
-      <c r="K54" s="61" t="s">
-        <v>2027</v>
-      </c>
-      <c r="L54" s="61" t="s">
-        <v>944</v>
+      <c r="K54" s="61"/>
+      <c r="L54" s="16" t="s">
+        <v>945</v>
       </c>
       <c r="M54" s="13"/>
     </row>
-    <row r="55" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
-        <v>2254</v>
+        <v>2213</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>945</v>
+        <v>305</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>945</v>
+        <v>306</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>931</v>
       </c>
-      <c r="E55" s="83" t="s">
-        <v>2123</v>
+      <c r="E55" s="65" t="s">
+        <v>2142</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>926</v>
+        <v>2215</v>
       </c>
       <c r="G55" s="89" t="s">
         <v>2156</v>
       </c>
-      <c r="H55" s="110"/>
-      <c r="I55" s="61"/>
-      <c r="J55" s="61"/>
-      <c r="K55" s="61"/>
+      <c r="H55" s="58" t="s">
+        <v>1806</v>
+      </c>
+      <c r="I55" s="16" t="s">
+        <v>1807</v>
+      </c>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16" t="s">
+        <v>1808</v>
+      </c>
       <c r="L55" s="16" t="s">
-        <v>945</v>
-      </c>
-      <c r="M55" s="13"/>
+        <v>2118</v>
+      </c>
+      <c r="M55" s="96" t="s">
+        <v>1838</v>
+      </c>
     </row>
     <row r="56" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
+        <v>2213</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>935</v>
+      </c>
+      <c r="E56" s="17" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F56" s="15" t="s">
         <v>2215</v>
       </c>
-      <c r="B56" s="16" t="s">
-        <v>305</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>306</v>
-      </c>
-      <c r="D56" s="15" t="s">
-        <v>931</v>
-      </c>
-      <c r="E56" s="65" t="s">
-        <v>2142</v>
-      </c>
-      <c r="F56" s="15" t="s">
+      <c r="G56" s="92"/>
+      <c r="H56" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="I56" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15" t="s">
+        <v>1155</v>
+      </c>
+      <c r="L56" s="15" t="s">
+        <v>2252</v>
+      </c>
+      <c r="M56" s="97" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="16" t="s">
         <v>2217</v>
       </c>
-      <c r="G56" s="89" t="s">
-        <v>2156</v>
-      </c>
-      <c r="H56" s="58" t="s">
-        <v>1806</v>
-      </c>
-      <c r="I56" s="16" t="s">
-        <v>1807</v>
-      </c>
-      <c r="J56" s="16"/>
-      <c r="K56" s="16" t="s">
-        <v>1808</v>
-      </c>
-      <c r="L56" s="16" t="s">
-        <v>2118</v>
-      </c>
-      <c r="M56" s="96" t="s">
-        <v>1838</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A57" s="16" t="s">
-        <v>2215</v>
-      </c>
       <c r="B57" s="16" t="s">
-        <v>323</v>
+        <v>224</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>324</v>
-      </c>
-      <c r="D57" s="15" t="s">
-        <v>935</v>
+        <v>2253</v>
+      </c>
+      <c r="D57" s="58" t="s">
+        <v>1811</v>
       </c>
       <c r="E57" s="17" t="s">
-        <v>1344</v>
-      </c>
-      <c r="F57" s="15" t="s">
-        <v>2217</v>
-      </c>
-      <c r="G57" s="92"/>
-      <c r="H57" s="15" t="s">
-        <v>341</v>
-      </c>
-      <c r="I57" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="J57" s="15"/>
-      <c r="K57" s="15" t="s">
-        <v>1155</v>
-      </c>
-      <c r="L57" s="15" t="s">
+        <v>1598</v>
+      </c>
+      <c r="F57" s="16" t="s">
+        <v>2218</v>
+      </c>
+      <c r="G57" s="89"/>
+      <c r="H57" s="107" t="s">
+        <v>919</v>
+      </c>
+      <c r="I57" s="89" t="s">
+        <v>2254</v>
+      </c>
+      <c r="J57" s="89"/>
+      <c r="K57" s="89" t="s">
         <v>2255</v>
       </c>
-      <c r="M57" s="97" t="s">
-        <v>1839</v>
-      </c>
+      <c r="L57" s="89" t="s">
+        <v>944</v>
+      </c>
+      <c r="M57" s="13"/>
     </row>
     <row r="58" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
-        <v>2219</v>
+        <v>2213</v>
       </c>
       <c r="B58" s="16" t="s">
         <v>224</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>2256</v>
+        <v>2253</v>
       </c>
       <c r="D58" s="58" t="s">
         <v>1811</v>
       </c>
       <c r="E58" s="17" t="s">
-        <v>1598</v>
-      </c>
-      <c r="F58" s="16" t="s">
-        <v>2220</v>
-      </c>
-      <c r="G58" s="89"/>
-      <c r="H58" s="109" t="s">
+        <v>1677</v>
+      </c>
+      <c r="F58" s="15" t="s">
+        <v>2215</v>
+      </c>
+      <c r="G58" s="92"/>
+      <c r="H58" s="15" t="s">
         <v>919</v>
       </c>
-      <c r="I58" s="89" t="s">
+      <c r="I58" s="15" t="s">
+        <v>2256</v>
+      </c>
+      <c r="J58" s="58"/>
+      <c r="K58" s="58" t="s">
         <v>2257</v>
       </c>
-      <c r="J58" s="89"/>
-      <c r="K58" s="89" t="s">
+      <c r="L58" s="15" t="s">
         <v>2258</v>
       </c>
-      <c r="L58" s="89" t="s">
-        <v>944</v>
-      </c>
-      <c r="M58" s="13"/>
+      <c r="M58" s="58"/>
     </row>
     <row r="59" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B59" s="16" t="s">
         <v>224</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>2256</v>
+        <v>2253</v>
       </c>
       <c r="D59" s="58" t="s">
         <v>1811</v>
       </c>
-      <c r="E59" s="17" t="s">
-        <v>1677</v>
+      <c r="E59" s="18" t="s">
+        <v>1579</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G59" s="92"/>
       <c r="H59" s="15" t="s">
         <v>919</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>2259</v>
-      </c>
-      <c r="J59" s="58"/>
-      <c r="K59" s="58" t="s">
-        <v>2260</v>
-      </c>
-      <c r="L59" s="15" t="s">
-        <v>2261</v>
+        <v>1580</v>
+      </c>
+      <c r="J59" s="16" t="s">
+        <v>1581</v>
+      </c>
+      <c r="K59" s="15" t="s">
+        <v>1582</v>
+      </c>
+      <c r="L59" s="16" t="s">
+        <v>1583</v>
       </c>
       <c r="M59" s="58"/>
     </row>
     <row r="60" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B60" s="16" t="s">
         <v>224</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>2256</v>
+        <v>2253</v>
       </c>
       <c r="D60" s="58" t="s">
         <v>1811</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>1579</v>
+        <v>1344</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G60" s="92"/>
       <c r="H60" s="15" t="s">
-        <v>919</v>
-      </c>
-      <c r="I60" s="15" t="s">
-        <v>1580</v>
+        <v>1584</v>
+      </c>
+      <c r="I60" s="16" t="s">
+        <v>1585</v>
       </c>
       <c r="J60" s="16" t="s">
-        <v>1581</v>
-      </c>
-      <c r="K60" s="15" t="s">
-        <v>1582</v>
+        <v>1586</v>
+      </c>
+      <c r="K60" s="13" t="s">
+        <v>1587</v>
       </c>
       <c r="L60" s="16" t="s">
-        <v>1583</v>
-      </c>
-      <c r="M60" s="58"/>
+        <v>2259</v>
+      </c>
+      <c r="M60" s="96" t="s">
+        <v>1840</v>
+      </c>
     </row>
     <row r="61" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B61" s="16" t="s">
         <v>224</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>2256</v>
+        <v>2253</v>
       </c>
       <c r="D61" s="58" t="s">
         <v>1811</v>
       </c>
-      <c r="E61" s="18" t="s">
-        <v>1344</v>
+      <c r="E61" s="65" t="s">
+        <v>1589</v>
       </c>
       <c r="F61" s="15" t="s">
-        <v>2217</v>
-      </c>
-      <c r="G61" s="92"/>
-      <c r="H61" s="15" t="s">
-        <v>1584</v>
+        <v>2215</v>
+      </c>
+      <c r="G61" s="115"/>
+      <c r="H61" s="90" t="s">
+        <v>919</v>
       </c>
       <c r="I61" s="16" t="s">
-        <v>1585</v>
-      </c>
-      <c r="J61" s="16" t="s">
-        <v>1586</v>
-      </c>
-      <c r="K61" s="13" t="s">
-        <v>1587</v>
+        <v>1590</v>
+      </c>
+      <c r="J61" s="13"/>
+      <c r="K61" s="15" t="s">
+        <v>1591</v>
       </c>
       <c r="L61" s="16" t="s">
-        <v>2262</v>
-      </c>
-      <c r="M61" s="96" t="s">
-        <v>1840</v>
-      </c>
+        <v>1592</v>
+      </c>
+      <c r="M61" s="58"/>
     </row>
     <row r="62" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B62" s="16" t="s">
         <v>224</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>2256</v>
+        <v>2253</v>
       </c>
       <c r="D62" s="58" t="s">
         <v>1811</v>
       </c>
-      <c r="E62" s="65" t="s">
-        <v>1589</v>
+      <c r="E62" s="18" t="s">
+        <v>1593</v>
       </c>
       <c r="F62" s="15" t="s">
-        <v>2217</v>
-      </c>
-      <c r="G62" s="117"/>
-      <c r="H62" s="90" t="s">
+        <v>2215</v>
+      </c>
+      <c r="G62" s="92"/>
+      <c r="H62" s="15" t="s">
+        <v>1594</v>
+      </c>
+      <c r="I62" s="16" t="s">
+        <v>1595</v>
+      </c>
+      <c r="J62" s="16" t="s">
+        <v>1595</v>
+      </c>
+      <c r="K62" s="13" t="s">
+        <v>1596</v>
+      </c>
+      <c r="L62" s="16" t="s">
+        <v>1597</v>
+      </c>
+      <c r="M62" s="58"/>
+    </row>
+    <row r="63" spans="1:13" ht="50" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B63" s="16" t="s">
         <v>919</v>
       </c>
-      <c r="I62" s="16" t="s">
-        <v>1590</v>
-      </c>
-      <c r="J62" s="13"/>
-      <c r="K62" s="15" t="s">
-        <v>1591</v>
-      </c>
-      <c r="L62" s="16" t="s">
-        <v>1592</v>
-      </c>
-      <c r="M62" s="58"/>
-    </row>
-    <row r="63" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
-        <v>2215</v>
-      </c>
-      <c r="B63" s="16" t="s">
-        <v>224</v>
-      </c>
       <c r="C63" s="16" t="s">
-        <v>2256</v>
-      </c>
-      <c r="D63" s="58" t="s">
-        <v>1811</v>
-      </c>
-      <c r="E63" s="18" t="s">
-        <v>1593</v>
-      </c>
-      <c r="F63" s="15" t="s">
-        <v>2217</v>
-      </c>
-      <c r="G63" s="92"/>
-      <c r="H63" s="15" t="s">
-        <v>1594</v>
-      </c>
-      <c r="I63" s="16" t="s">
-        <v>1595</v>
-      </c>
-      <c r="J63" s="16" t="s">
-        <v>1595</v>
-      </c>
-      <c r="K63" s="13" t="s">
-        <v>1596</v>
-      </c>
-      <c r="L63" s="16" t="s">
-        <v>1597</v>
-      </c>
-      <c r="M63" s="58"/>
+        <v>2261</v>
+      </c>
+      <c r="D63" s="23" t="s">
+        <v>1813</v>
+      </c>
+      <c r="E63" s="69" t="s">
+        <v>2262</v>
+      </c>
+      <c r="F63" s="23" t="s">
+        <v>915</v>
+      </c>
+      <c r="G63" s="114"/>
+      <c r="H63" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="I63" s="61" t="s">
+        <v>353</v>
+      </c>
+      <c r="J63" s="61" t="s">
+        <v>354</v>
+      </c>
+      <c r="K63" s="61" t="s">
+        <v>355</v>
+      </c>
+      <c r="L63" s="23" t="s">
+        <v>944</v>
+      </c>
+      <c r="M63" s="61"/>
     </row>
     <row r="64" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
-        <v>2263</v>
+        <v>2260</v>
       </c>
       <c r="B64" s="16" t="s">
         <v>919</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>2264</v>
+        <v>2261</v>
       </c>
       <c r="D64" s="23" t="s">
         <v>1813</v>
       </c>
       <c r="E64" s="69" t="s">
-        <v>2265</v>
+        <v>2263</v>
       </c>
       <c r="F64" s="23" t="s">
         <v>915</v>
       </c>
-      <c r="G64" s="116"/>
+      <c r="G64" s="114"/>
       <c r="H64" s="23" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="I64" s="61" t="s">
-        <v>353</v>
-      </c>
-      <c r="J64" s="61" t="s">
-        <v>354</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="J64" s="61"/>
       <c r="K64" s="61" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="L64" s="23" t="s">
         <v>944</v>
@@ -38367,33 +38332,33 @@
     </row>
     <row r="65" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
-        <v>2263</v>
+        <v>2260</v>
       </c>
       <c r="B65" s="16" t="s">
         <v>919</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>2264</v>
+        <v>2261</v>
       </c>
       <c r="D65" s="23" t="s">
         <v>1813</v>
       </c>
       <c r="E65" s="69" t="s">
-        <v>2266</v>
+        <v>2264</v>
       </c>
       <c r="F65" s="23" t="s">
         <v>915</v>
       </c>
-      <c r="G65" s="116"/>
+      <c r="G65" s="114"/>
       <c r="H65" s="23" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="I65" s="61" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="J65" s="61"/>
       <c r="K65" s="61" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="L65" s="23" t="s">
         <v>944</v>
@@ -38402,114 +38367,116 @@
     </row>
     <row r="66" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
-        <v>2263</v>
+        <v>2260</v>
       </c>
       <c r="B66" s="16" t="s">
         <v>919</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>2264</v>
+        <v>2261</v>
       </c>
       <c r="D66" s="23" t="s">
         <v>1813</v>
       </c>
       <c r="E66" s="69" t="s">
-        <v>2267</v>
+        <v>2265</v>
       </c>
       <c r="F66" s="23" t="s">
         <v>915</v>
       </c>
-      <c r="G66" s="116"/>
+      <c r="G66" s="114"/>
       <c r="H66" s="23" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="I66" s="61" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="J66" s="61"/>
       <c r="K66" s="61" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="L66" s="23" t="s">
         <v>944</v>
       </c>
       <c r="M66" s="61"/>
     </row>
-    <row r="67" spans="1:13" ht="50" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
-        <v>2263</v>
+        <v>2213</v>
       </c>
       <c r="B67" s="16" t="s">
         <v>919</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>2264</v>
-      </c>
-      <c r="D67" s="23" t="s">
+        <v>2261</v>
+      </c>
+      <c r="D67" s="15" t="s">
         <v>1813</v>
       </c>
-      <c r="E67" s="69" t="s">
-        <v>2268</v>
-      </c>
-      <c r="F67" s="23" t="s">
-        <v>915</v>
-      </c>
-      <c r="G67" s="116"/>
-      <c r="H67" s="23" t="s">
-        <v>367</v>
-      </c>
-      <c r="I67" s="61" t="s">
-        <v>368</v>
-      </c>
-      <c r="J67" s="61"/>
-      <c r="K67" s="61" t="s">
-        <v>369</v>
-      </c>
-      <c r="L67" s="23" t="s">
-        <v>944</v>
-      </c>
-      <c r="M67" s="61"/>
-    </row>
-    <row r="68" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="E67" s="17" t="s">
+        <v>1362</v>
+      </c>
+      <c r="F67" s="15" t="s">
+        <v>2215</v>
+      </c>
+      <c r="G67" s="92"/>
+      <c r="H67" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="I67" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="J67" s="15"/>
+      <c r="K67" s="15" t="s">
+        <v>361</v>
+      </c>
+      <c r="L67" s="15" t="s">
+        <v>1814</v>
+      </c>
+      <c r="M67" s="13" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
-        <v>2215</v>
+        <v>2266</v>
       </c>
       <c r="B68" s="16" t="s">
         <v>919</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>2264</v>
-      </c>
-      <c r="D68" s="15" t="s">
-        <v>1813</v>
-      </c>
-      <c r="E68" s="17" t="s">
-        <v>1362</v>
-      </c>
-      <c r="F68" s="15" t="s">
-        <v>2217</v>
-      </c>
-      <c r="G68" s="92"/>
-      <c r="H68" s="15" t="s">
-        <v>359</v>
-      </c>
-      <c r="I68" s="15" t="s">
-        <v>360</v>
-      </c>
-      <c r="J68" s="15"/>
-      <c r="K68" s="15" t="s">
-        <v>361</v>
-      </c>
-      <c r="L68" s="15" t="s">
-        <v>1814</v>
-      </c>
-      <c r="M68" s="13" t="s">
-        <v>1841</v>
-      </c>
+        <v>1494</v>
+      </c>
+      <c r="D68" s="23" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E68" s="109" t="s">
+        <v>1341</v>
+      </c>
+      <c r="F68" s="61" t="s">
+        <v>915</v>
+      </c>
+      <c r="G68" s="111"/>
+      <c r="H68" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I68" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J68" s="23" t="s">
+        <v>1342</v>
+      </c>
+      <c r="K68" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="L68" s="23" t="s">
+        <v>944</v>
+      </c>
+      <c r="M68" s="13"/>
     </row>
     <row r="69" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
-        <v>2269</v>
+        <v>2266</v>
       </c>
       <c r="B69" s="16" t="s">
         <v>919</v>
@@ -38520,33 +38487,31 @@
       <c r="D69" s="23" t="s">
         <v>1473</v>
       </c>
-      <c r="E69" s="111" t="s">
-        <v>1341</v>
+      <c r="E69" s="109" t="s">
+        <v>1352</v>
       </c>
       <c r="F69" s="61" t="s">
         <v>915</v>
       </c>
-      <c r="G69" s="113"/>
-      <c r="H69" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="I69" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="J69" s="23" t="s">
-        <v>1342</v>
-      </c>
-      <c r="K69" s="23" t="s">
-        <v>46</v>
+      <c r="G69" s="111"/>
+      <c r="H69" s="108" t="s">
+        <v>1353</v>
+      </c>
+      <c r="I69" s="61" t="s">
+        <v>1354</v>
+      </c>
+      <c r="J69" s="61"/>
+      <c r="K69" s="61" t="s">
+        <v>1355</v>
       </c>
       <c r="L69" s="23" t="s">
         <v>944</v>
       </c>
       <c r="M69" s="13"/>
     </row>
-    <row r="70" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
-        <v>2269</v>
+        <v>2213</v>
       </c>
       <c r="B70" s="16" t="s">
         <v>919</v>
@@ -38554,34 +38519,38 @@
       <c r="C70" s="16" t="s">
         <v>1494</v>
       </c>
-      <c r="D70" s="23" t="s">
+      <c r="D70" s="15" t="s">
         <v>1473</v>
       </c>
-      <c r="E70" s="111" t="s">
-        <v>1352</v>
-      </c>
-      <c r="F70" s="61" t="s">
-        <v>915</v>
-      </c>
-      <c r="G70" s="113"/>
-      <c r="H70" s="110" t="s">
-        <v>1353</v>
-      </c>
-      <c r="I70" s="61" t="s">
-        <v>1354</v>
-      </c>
-      <c r="J70" s="61"/>
-      <c r="K70" s="61" t="s">
-        <v>1355</v>
-      </c>
-      <c r="L70" s="23" t="s">
-        <v>944</v>
-      </c>
-      <c r="M70" s="13"/>
-    </row>
-    <row r="71" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="E70" s="18" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F70" s="15" t="s">
+        <v>2215</v>
+      </c>
+      <c r="G70" s="92"/>
+      <c r="H70" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I70" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="J70" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="K70" s="16" t="s">
+        <v>1141</v>
+      </c>
+      <c r="L70" s="15" t="s">
+        <v>2267</v>
+      </c>
+      <c r="M70" s="97" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B71" s="16" t="s">
         <v>919</v>
@@ -38593,34 +38562,30 @@
         <v>1473</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>1344</v>
+        <v>1348</v>
       </c>
       <c r="F71" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G71" s="92"/>
       <c r="H71" s="15" t="s">
-        <v>48</v>
+        <v>919</v>
       </c>
       <c r="I71" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="J71" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="K71" s="16" t="s">
-        <v>1141</v>
+        <v>1349</v>
+      </c>
+      <c r="J71" s="15"/>
+      <c r="K71" s="15" t="s">
+        <v>1350</v>
       </c>
       <c r="L71" s="15" t="s">
-        <v>2270</v>
-      </c>
-      <c r="M71" s="97" t="s">
-        <v>1842</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" ht="50" x14ac:dyDescent="0.25">
+        <v>2247</v>
+      </c>
+      <c r="M71" s="58"/>
+    </row>
+    <row r="72" spans="1:13" ht="137.5" x14ac:dyDescent="0.25">
       <c r="A72" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B72" s="16" t="s">
         <v>919</v>
@@ -38632,69 +38597,71 @@
         <v>1473</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>1348</v>
+        <v>1345</v>
       </c>
       <c r="F72" s="15" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="G72" s="92"/>
       <c r="H72" s="15" t="s">
-        <v>919</v>
+        <v>56</v>
       </c>
       <c r="I72" s="15" t="s">
-        <v>1349</v>
-      </c>
-      <c r="J72" s="15"/>
-      <c r="K72" s="15" t="s">
-        <v>1350</v>
+        <v>57</v>
+      </c>
+      <c r="J72" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K72" s="16" t="s">
+        <v>1346</v>
       </c>
       <c r="L72" s="15" t="s">
-        <v>2250</v>
-      </c>
-      <c r="M72" s="58"/>
-    </row>
-    <row r="73" spans="1:13" ht="137.5" x14ac:dyDescent="0.25">
+        <v>2268</v>
+      </c>
+      <c r="M72" s="97" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A73" s="16" t="s">
-        <v>2215</v>
+        <v>2240</v>
       </c>
       <c r="B73" s="16" t="s">
         <v>919</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>1494</v>
+        <v>1496</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>1473</v>
+        <v>1483</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>1345</v>
-      </c>
-      <c r="F73" s="15" t="s">
-        <v>2217</v>
-      </c>
-      <c r="G73" s="92"/>
+        <v>1344</v>
+      </c>
+      <c r="F73" s="16" t="s">
+        <v>915</v>
+      </c>
+      <c r="G73" s="89" t="s">
+        <v>1476</v>
+      </c>
       <c r="H73" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="I73" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="J73" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K73" s="16" t="s">
-        <v>1346</v>
-      </c>
-      <c r="L73" s="15" t="s">
-        <v>2271</v>
-      </c>
-      <c r="M73" s="97" t="s">
-        <v>1843</v>
-      </c>
+        <v>919</v>
+      </c>
+      <c r="I73" s="16" t="s">
+        <v>1775</v>
+      </c>
+      <c r="J73" s="13"/>
+      <c r="K73" s="54" t="s">
+        <v>1776</v>
+      </c>
+      <c r="L73" s="13" t="s">
+        <v>944</v>
+      </c>
+      <c r="M73" s="13"/>
     </row>
     <row r="74" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
-        <v>2243</v>
+        <v>2240</v>
       </c>
       <c r="B74" s="16" t="s">
         <v>919</v>
@@ -38706,7 +38673,7 @@
         <v>1483</v>
       </c>
       <c r="E74" s="18" t="s">
-        <v>1344</v>
+        <v>1424</v>
       </c>
       <c r="F74" s="16" t="s">
         <v>915</v>
@@ -38718,20 +38685,20 @@
         <v>919</v>
       </c>
       <c r="I74" s="16" t="s">
-        <v>1775</v>
+        <v>1777</v>
       </c>
       <c r="J74" s="13"/>
-      <c r="K74" s="54" t="s">
-        <v>1776</v>
+      <c r="K74" s="16" t="s">
+        <v>1778</v>
       </c>
       <c r="L74" s="13" t="s">
         <v>944</v>
       </c>
       <c r="M74" s="13"/>
     </row>
-    <row r="75" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A75" s="16" t="s">
-        <v>2243</v>
+        <v>2213</v>
       </c>
       <c r="B75" s="16" t="s">
         <v>919</v>
@@ -38743,67 +38710,67 @@
         <v>1483</v>
       </c>
       <c r="E75" s="18" t="s">
-        <v>1424</v>
+        <v>1487</v>
       </c>
       <c r="F75" s="16" t="s">
-        <v>915</v>
-      </c>
-      <c r="G75" s="89" t="s">
-        <v>1476</v>
-      </c>
-      <c r="H75" s="15" t="s">
+        <v>2218</v>
+      </c>
+      <c r="G75" s="89"/>
+      <c r="H75" s="92" t="s">
         <v>919</v>
       </c>
-      <c r="I75" s="16" t="s">
-        <v>1777</v>
-      </c>
-      <c r="J75" s="13"/>
-      <c r="K75" s="16" t="s">
-        <v>1778</v>
-      </c>
-      <c r="L75" s="13" t="s">
+      <c r="I75" s="89" t="s">
+        <v>2269</v>
+      </c>
+      <c r="J75" s="89"/>
+      <c r="K75" s="89" t="s">
+        <v>2270</v>
+      </c>
+      <c r="L75" s="89" t="s">
         <v>944</v>
       </c>
       <c r="M75" s="13"/>
     </row>
-    <row r="76" spans="1:13" ht="50" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" s="16" t="s">
+        <v>2213</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>1742</v>
+      </c>
+      <c r="C76" s="16" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D76" s="55" t="s">
+        <v>967</v>
+      </c>
+      <c r="E76" s="53" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F76" s="15" t="s">
         <v>2215</v>
       </c>
-      <c r="B76" s="16" t="s">
-        <v>919</v>
-      </c>
-      <c r="C76" s="16" t="s">
-        <v>1496</v>
-      </c>
-      <c r="D76" s="15" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E76" s="18" t="s">
-        <v>1487</v>
-      </c>
-      <c r="F76" s="16" t="s">
-        <v>2220</v>
-      </c>
-      <c r="G76" s="89"/>
-      <c r="H76" s="92" t="s">
-        <v>919</v>
-      </c>
-      <c r="I76" s="89" t="s">
-        <v>2272</v>
-      </c>
-      <c r="J76" s="89"/>
-      <c r="K76" s="89" t="s">
-        <v>2273</v>
-      </c>
-      <c r="L76" s="89" t="s">
-        <v>944</v>
-      </c>
-      <c r="M76" s="13"/>
+      <c r="G76" s="92"/>
+      <c r="H76" s="55" t="s">
+        <v>1817</v>
+      </c>
+      <c r="I76" s="55" t="s">
+        <v>1162</v>
+      </c>
+      <c r="J76" s="54"/>
+      <c r="K76" s="54" t="s">
+        <v>1163</v>
+      </c>
+      <c r="L76" s="16" t="s">
+        <v>1818</v>
+      </c>
+      <c r="M76" s="13" t="s">
+        <v>1844</v>
+      </c>
     </row>
     <row r="77" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="B77" s="16" t="s">
         <v>1742</v>
@@ -38815,99 +38782,62 @@
         <v>967</v>
       </c>
       <c r="E77" s="53" t="s">
-        <v>1344</v>
+        <v>1819</v>
       </c>
       <c r="F77" s="15" t="s">
-        <v>2217</v>
-      </c>
-      <c r="G77" s="92"/>
+        <v>2215</v>
+      </c>
+      <c r="G77" s="15"/>
       <c r="H77" s="55" t="s">
-        <v>1817</v>
+        <v>1748</v>
       </c>
       <c r="I77" s="55" t="s">
-        <v>1162</v>
+        <v>1749</v>
       </c>
       <c r="J77" s="54"/>
       <c r="K77" s="54" t="s">
-        <v>1163</v>
+        <v>1750</v>
       </c>
       <c r="L77" s="16" t="s">
-        <v>1818</v>
+        <v>1820</v>
       </c>
       <c r="M77" s="13" t="s">
-        <v>1844</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A78" s="16" t="s">
-        <v>2215</v>
-      </c>
-      <c r="B78" s="16" t="s">
-        <v>1742</v>
-      </c>
-      <c r="C78" s="16" t="s">
-        <v>1115</v>
-      </c>
-      <c r="D78" s="55" t="s">
-        <v>967</v>
-      </c>
-      <c r="E78" s="53" t="s">
-        <v>1819</v>
-      </c>
-      <c r="F78" s="15" t="s">
-        <v>2217</v>
-      </c>
-      <c r="G78" s="15"/>
-      <c r="H78" s="55" t="s">
-        <v>1748</v>
-      </c>
-      <c r="I78" s="55" t="s">
-        <v>1749</v>
-      </c>
-      <c r="J78" s="54"/>
-      <c r="K78" s="54" t="s">
-        <v>1750</v>
-      </c>
-      <c r="L78" s="16" t="s">
-        <v>1820</v>
-      </c>
-      <c r="M78" s="13" t="s">
         <v>1845</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="13" t="s">
-        <v>2274</v>
-      </c>
-      <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
-      <c r="D79" s="58"/>
-      <c r="E79" s="58"/>
-      <c r="F79" s="58"/>
-      <c r="G79" s="58"/>
-      <c r="H79" s="58"/>
-      <c r="I79" s="58"/>
-      <c r="J79" s="58"/>
-      <c r="K79" s="58"/>
-      <c r="L79" s="58"/>
-      <c r="M79" s="15"/>
+    <row r="78" spans="1:13" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="13" t="s">
+        <v>2271</v>
+      </c>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="58"/>
+      <c r="E78" s="58"/>
+      <c r="F78" s="58"/>
+      <c r="G78" s="58"/>
+      <c r="H78" s="58"/>
+      <c r="I78" s="58"/>
+      <c r="J78" s="58"/>
+      <c r="K78" s="58"/>
+      <c r="L78" s="58"/>
+      <c r="M78" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M44" r:id="rId1" xr:uid="{81AEBDD3-7320-405D-8B78-14570C2C38FE}"/>
-    <hyperlink ref="M45" r:id="rId2" xr:uid="{21A8DD5C-38A0-4EDA-8A4A-C0698E6FB314}"/>
-    <hyperlink ref="M46" r:id="rId3" xr:uid="{27BF3011-7740-461D-A31E-ABBE2DE546F0}"/>
-    <hyperlink ref="M48" r:id="rId4" xr:uid="{43FA0470-081B-4961-A234-7003F0EA2B18}"/>
-    <hyperlink ref="M56" r:id="rId5" xr:uid="{EF4EFDCF-C8B8-45F3-A145-F1AFE1F70DBA}"/>
-    <hyperlink ref="M40" r:id="rId6" xr:uid="{96C1A88A-2738-4DFC-88F4-68B802C4F512}"/>
-    <hyperlink ref="M57" r:id="rId7" xr:uid="{42DDF036-BF78-4EF5-AA30-A63CA3A7011E}"/>
+    <hyperlink ref="M43" r:id="rId1" xr:uid="{81AEBDD3-7320-405D-8B78-14570C2C38FE}"/>
+    <hyperlink ref="M44" r:id="rId2" xr:uid="{21A8DD5C-38A0-4EDA-8A4A-C0698E6FB314}"/>
+    <hyperlink ref="M45" r:id="rId3" xr:uid="{27BF3011-7740-461D-A31E-ABBE2DE546F0}"/>
+    <hyperlink ref="M47" r:id="rId4" xr:uid="{43FA0470-081B-4961-A234-7003F0EA2B18}"/>
+    <hyperlink ref="M55" r:id="rId5" xr:uid="{EF4EFDCF-C8B8-45F3-A145-F1AFE1F70DBA}"/>
+    <hyperlink ref="M39" r:id="rId6" xr:uid="{96C1A88A-2738-4DFC-88F4-68B802C4F512}"/>
+    <hyperlink ref="M56" r:id="rId7" xr:uid="{42DDF036-BF78-4EF5-AA30-A63CA3A7011E}"/>
     <hyperlink ref="M8" r:id="rId8" xr:uid="{4E878370-2CC6-4E6B-8F68-C99908210AB2}"/>
     <hyperlink ref="M9" r:id="rId9" xr:uid="{E7032EDC-4CE6-4743-9B11-5DF838053107}"/>
     <hyperlink ref="M10" r:id="rId10" xr:uid="{78D6F338-F604-4AC0-8095-E0AD1D806B19}"/>
     <hyperlink ref="M7" r:id="rId11" xr:uid="{C14B2D0E-2DA6-41D1-B606-9AC90467F693}"/>
-    <hyperlink ref="M71" r:id="rId12" xr:uid="{3ABB19BD-A690-41F8-B566-C97AA152FCF0}"/>
-    <hyperlink ref="M73" r:id="rId13" xr:uid="{425281AC-554A-4B3E-93C5-292424F86B3C}"/>
-    <hyperlink ref="M61" r:id="rId14" xr:uid="{644B6BBD-D398-47C0-B886-A54EF8638D5D}"/>
+    <hyperlink ref="M70" r:id="rId12" xr:uid="{3ABB19BD-A690-41F8-B566-C97AA152FCF0}"/>
+    <hyperlink ref="M72" r:id="rId13" xr:uid="{425281AC-554A-4B3E-93C5-292424F86B3C}"/>
+    <hyperlink ref="M60" r:id="rId14" xr:uid="{644B6BBD-D398-47C0-B886-A54EF8638D5D}"/>
     <hyperlink ref="M5" r:id="rId15" xr:uid="{1C45E8D4-7AF9-4028-B7F1-BCCC41301176}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removal of SDTM and Protocol codelists
Removal of SDTM and Protocol codelists from DDF valid value sets tab. We will instead point to these codelists using the URL from NCIt.
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965E7C2E-9B9D-4FFC-84BE-49E4978AA0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D28C77-63DC-48ED-A297-742020EEE352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2470" yWindow="1620" windowWidth="15320" windowHeight="8480" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="490" windowWidth="15320" windowHeight="8480" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8962" uniqueCount="2392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10083" uniqueCount="2395">
   <si>
     <t>Code</t>
   </si>
@@ -13379,6 +13379,41 @@
         <family val="2"/>
       </rPr>
       <t>titles</t>
+    </r>
+  </si>
+  <si>
+    <t>Remove codelist and valid values from DDF valid value sets tab. Instead refer to the codelist URL in the DDF Entities&amp;Attributes tab</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">List of characteristics in a protocol, any one of which may exclude a potential subject from participation in a study. (CDISC glossary)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>List of characteristics in a protocol, any one of which makes a potential subject ineligible to participate in a study.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The criteria in a protocol that prospective subjects must meet to be eligible for participation in a study. NOTE: Exclusion and inclusion criteria define the study population. See also exclusion criteria. (CDISC glossary)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The criteria in a protocol that prospective subjects must meet to be eligible to participate in a study.</t>
     </r>
   </si>
 </sst>
@@ -13386,7 +13421,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -13559,6 +13594,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -13657,7 +13706,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -13793,6 +13842,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -13801,7 +13859,7 @@
     <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -14194,6 +14252,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -40727,7 +40809,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -40788,12 +40870,14 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>2386</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16" t="s">
+        <v>23</v>
+      </c>
       <c r="D2" s="61" t="s">
         <v>2387</v>
       </c>
@@ -40819,12 +40903,14 @@
       </c>
       <c r="M2" s="13"/>
     </row>
-    <row r="3" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>2386</v>
       </c>
       <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+      <c r="C3" s="16" t="s">
+        <v>23</v>
+      </c>
       <c r="D3" s="61" t="s">
         <v>2387</v>
       </c>
@@ -40850,12 +40936,14 @@
       </c>
       <c r="M3" s="13"/>
     </row>
-    <row r="4" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>2390</v>
       </c>
       <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
+      <c r="C4" s="16" t="s">
+        <v>260</v>
+      </c>
       <c r="D4" s="61" t="s">
         <v>144</v>
       </c>
@@ -40881,12 +40969,14 @@
       </c>
       <c r="M4" s="13"/>
     </row>
-    <row r="5" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>2390</v>
       </c>
       <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="C5" s="16" t="s">
+        <v>260</v>
+      </c>
       <c r="D5" s="61" t="s">
         <v>144</v>
       </c>
@@ -40916,8 +41006,12 @@
       <c r="A6" s="16" t="s">
         <v>1627</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
+      <c r="B6" s="16" t="s">
+        <v>945</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>945</v>
+      </c>
       <c r="D6" s="15" t="s">
         <v>1473</v>
       </c>
@@ -40936,6 +41030,3916 @@
         <v>945</v>
       </c>
       <c r="M6" s="13"/>
+    </row>
+    <row r="7" spans="1:13" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>659</v>
+      </c>
+      <c r="C7" s="61"/>
+      <c r="D7" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F7" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G7" s="61"/>
+      <c r="H7" s="44" t="s">
+        <v>664</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>665</v>
+      </c>
+      <c r="J7" s="133"/>
+      <c r="K7" s="23" t="s">
+        <v>1361</v>
+      </c>
+      <c r="L7" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="100" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>659</v>
+      </c>
+      <c r="C8" s="61"/>
+      <c r="D8" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F8" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G8" s="61"/>
+      <c r="H8" s="44" t="s">
+        <v>669</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>670</v>
+      </c>
+      <c r="J8" s="133"/>
+      <c r="K8" s="23" t="s">
+        <v>671</v>
+      </c>
+      <c r="L8" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="100" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>659</v>
+      </c>
+      <c r="C9" s="61"/>
+      <c r="D9" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G9" s="61"/>
+      <c r="H9" s="44" t="s">
+        <v>673</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>674</v>
+      </c>
+      <c r="J9" s="133"/>
+      <c r="K9" s="23" t="s">
+        <v>675</v>
+      </c>
+      <c r="L9" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="137.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>659</v>
+      </c>
+      <c r="C10" s="61"/>
+      <c r="D10" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F10" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G10" s="61"/>
+      <c r="H10" s="44" t="s">
+        <v>677</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>678</v>
+      </c>
+      <c r="J10" s="133"/>
+      <c r="K10" s="23" t="s">
+        <v>679</v>
+      </c>
+      <c r="L10" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="100" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C11" s="61"/>
+      <c r="D11" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F11" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G11" s="61"/>
+      <c r="H11" s="134" t="s">
+        <v>735</v>
+      </c>
+      <c r="I11" s="43" t="s">
+        <v>736</v>
+      </c>
+      <c r="J11" s="43" t="s">
+        <v>737</v>
+      </c>
+      <c r="K11" s="43" t="s">
+        <v>738</v>
+      </c>
+      <c r="L11" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="212.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C12" s="61"/>
+      <c r="D12" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F12" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G12" s="61"/>
+      <c r="H12" s="134" t="s">
+        <v>740</v>
+      </c>
+      <c r="I12" s="43" t="s">
+        <v>741</v>
+      </c>
+      <c r="J12" s="43" t="s">
+        <v>742</v>
+      </c>
+      <c r="K12" s="43" t="s">
+        <v>743</v>
+      </c>
+      <c r="L12" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="262.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C13" s="61"/>
+      <c r="D13" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F13" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G13" s="61"/>
+      <c r="H13" s="134" t="s">
+        <v>745</v>
+      </c>
+      <c r="I13" s="43" t="s">
+        <v>746</v>
+      </c>
+      <c r="J13" s="43" t="s">
+        <v>747</v>
+      </c>
+      <c r="K13" s="43" t="s">
+        <v>748</v>
+      </c>
+      <c r="L13" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="100" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C14" s="61"/>
+      <c r="D14" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F14" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G14" s="61"/>
+      <c r="H14" s="134" t="s">
+        <v>750</v>
+      </c>
+      <c r="I14" s="43" t="s">
+        <v>751</v>
+      </c>
+      <c r="J14" s="43" t="s">
+        <v>752</v>
+      </c>
+      <c r="K14" s="43" t="s">
+        <v>753</v>
+      </c>
+      <c r="L14" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="100" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C15" s="61"/>
+      <c r="D15" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F15" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G15" s="61"/>
+      <c r="H15" s="134" t="s">
+        <v>974</v>
+      </c>
+      <c r="I15" s="43" t="s">
+        <v>975</v>
+      </c>
+      <c r="J15" s="43" t="s">
+        <v>976</v>
+      </c>
+      <c r="K15" s="43" t="s">
+        <v>977</v>
+      </c>
+      <c r="L15" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="100" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C16" s="61"/>
+      <c r="D16" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F16" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G16" s="61"/>
+      <c r="H16" s="134" t="s">
+        <v>979</v>
+      </c>
+      <c r="I16" s="43" t="s">
+        <v>980</v>
+      </c>
+      <c r="J16" s="43" t="s">
+        <v>981</v>
+      </c>
+      <c r="K16" s="43" t="s">
+        <v>982</v>
+      </c>
+      <c r="L16" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C17" s="61"/>
+      <c r="D17" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F17" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G17" s="61"/>
+      <c r="H17" s="134" t="s">
+        <v>993</v>
+      </c>
+      <c r="I17" s="43" t="s">
+        <v>994</v>
+      </c>
+      <c r="J17" s="43" t="s">
+        <v>995</v>
+      </c>
+      <c r="K17" s="43" t="s">
+        <v>996</v>
+      </c>
+      <c r="L17" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C18" s="61"/>
+      <c r="D18" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F18" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G18" s="61"/>
+      <c r="H18" s="134" t="s">
+        <v>998</v>
+      </c>
+      <c r="I18" s="43" t="s">
+        <v>999</v>
+      </c>
+      <c r="J18" s="43" t="s">
+        <v>1000</v>
+      </c>
+      <c r="K18" s="43" t="s">
+        <v>1001</v>
+      </c>
+      <c r="L18" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C19" s="61"/>
+      <c r="D19" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F19" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G19" s="61"/>
+      <c r="H19" s="134" t="s">
+        <v>755</v>
+      </c>
+      <c r="I19" s="43" t="s">
+        <v>756</v>
+      </c>
+      <c r="J19" s="43" t="s">
+        <v>757</v>
+      </c>
+      <c r="K19" s="43" t="s">
+        <v>984</v>
+      </c>
+      <c r="L19" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C20" s="61"/>
+      <c r="D20" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F20" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G20" s="61"/>
+      <c r="H20" s="134" t="s">
+        <v>759</v>
+      </c>
+      <c r="I20" s="43" t="s">
+        <v>760</v>
+      </c>
+      <c r="J20" s="43" t="s">
+        <v>761</v>
+      </c>
+      <c r="K20" s="43" t="s">
+        <v>762</v>
+      </c>
+      <c r="L20" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C21" s="61"/>
+      <c r="D21" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F21" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G21" s="61"/>
+      <c r="H21" s="134" t="s">
+        <v>764</v>
+      </c>
+      <c r="I21" s="43" t="s">
+        <v>765</v>
+      </c>
+      <c r="J21" s="43" t="s">
+        <v>766</v>
+      </c>
+      <c r="K21" s="43" t="s">
+        <v>1767</v>
+      </c>
+      <c r="L21" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="125" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C22" s="61"/>
+      <c r="D22" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F22" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G22" s="61"/>
+      <c r="H22" s="134" t="s">
+        <v>768</v>
+      </c>
+      <c r="I22" s="43" t="s">
+        <v>769</v>
+      </c>
+      <c r="J22" s="43" t="s">
+        <v>770</v>
+      </c>
+      <c r="K22" s="43" t="s">
+        <v>1768</v>
+      </c>
+      <c r="L22" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="137.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C23" s="61"/>
+      <c r="D23" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F23" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G23" s="61"/>
+      <c r="H23" s="134" t="s">
+        <v>772</v>
+      </c>
+      <c r="I23" s="43" t="s">
+        <v>773</v>
+      </c>
+      <c r="J23" s="43" t="s">
+        <v>774</v>
+      </c>
+      <c r="K23" s="43" t="s">
+        <v>985</v>
+      </c>
+      <c r="L23" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C24" s="61"/>
+      <c r="D24" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F24" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G24" s="61"/>
+      <c r="H24" s="134" t="s">
+        <v>776</v>
+      </c>
+      <c r="I24" s="43" t="s">
+        <v>777</v>
+      </c>
+      <c r="J24" s="43" t="s">
+        <v>778</v>
+      </c>
+      <c r="K24" s="43" t="s">
+        <v>779</v>
+      </c>
+      <c r="L24" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C25" s="61"/>
+      <c r="D25" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F25" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G25" s="61"/>
+      <c r="H25" s="134" t="s">
+        <v>781</v>
+      </c>
+      <c r="I25" s="43" t="s">
+        <v>782</v>
+      </c>
+      <c r="J25" s="43" t="s">
+        <v>783</v>
+      </c>
+      <c r="K25" s="43" t="s">
+        <v>1769</v>
+      </c>
+      <c r="L25" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C26" s="61"/>
+      <c r="D26" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F26" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G26" s="61"/>
+      <c r="H26" s="134" t="s">
+        <v>785</v>
+      </c>
+      <c r="I26" s="43" t="s">
+        <v>786</v>
+      </c>
+      <c r="J26" s="43" t="s">
+        <v>787</v>
+      </c>
+      <c r="K26" s="43" t="s">
+        <v>986</v>
+      </c>
+      <c r="L26" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="C27" s="61"/>
+      <c r="D27" s="132" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F27" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G27" s="61"/>
+      <c r="H27" s="134" t="s">
+        <v>789</v>
+      </c>
+      <c r="I27" s="43" t="s">
+        <v>790</v>
+      </c>
+      <c r="J27" s="43" t="s">
+        <v>791</v>
+      </c>
+      <c r="K27" s="43" t="s">
+        <v>792</v>
+      </c>
+      <c r="L27" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>681</v>
+      </c>
+      <c r="C28" s="61"/>
+      <c r="D28" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>1797</v>
+      </c>
+      <c r="F28" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G28" s="61"/>
+      <c r="H28" s="44" t="s">
+        <v>686</v>
+      </c>
+      <c r="I28" s="23" t="s">
+        <v>687</v>
+      </c>
+      <c r="J28" s="23" t="s">
+        <v>688</v>
+      </c>
+      <c r="K28" s="23" t="s">
+        <v>689</v>
+      </c>
+      <c r="L28" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>681</v>
+      </c>
+      <c r="C29" s="61"/>
+      <c r="D29" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>1797</v>
+      </c>
+      <c r="F29" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G29" s="61"/>
+      <c r="H29" s="44" t="s">
+        <v>690</v>
+      </c>
+      <c r="I29" s="23" t="s">
+        <v>691</v>
+      </c>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23" t="s">
+        <v>692</v>
+      </c>
+      <c r="L29" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>681</v>
+      </c>
+      <c r="C30" s="61"/>
+      <c r="D30" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>1797</v>
+      </c>
+      <c r="F30" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G30" s="61"/>
+      <c r="H30" s="44" t="s">
+        <v>694</v>
+      </c>
+      <c r="I30" s="23" t="s">
+        <v>695</v>
+      </c>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23" t="s">
+        <v>696</v>
+      </c>
+      <c r="L30" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>681</v>
+      </c>
+      <c r="C31" s="61"/>
+      <c r="D31" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>1797</v>
+      </c>
+      <c r="F31" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G31" s="61"/>
+      <c r="H31" s="44" t="s">
+        <v>698</v>
+      </c>
+      <c r="I31" s="23" t="s">
+        <v>699</v>
+      </c>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23" t="s">
+        <v>700</v>
+      </c>
+      <c r="L31" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>681</v>
+      </c>
+      <c r="C32" s="61"/>
+      <c r="D32" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>1797</v>
+      </c>
+      <c r="F32" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G32" s="61"/>
+      <c r="H32" s="44" t="s">
+        <v>702</v>
+      </c>
+      <c r="I32" s="23" t="s">
+        <v>703</v>
+      </c>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23" t="s">
+        <v>704</v>
+      </c>
+      <c r="L32" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>681</v>
+      </c>
+      <c r="C33" s="61"/>
+      <c r="D33" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>1797</v>
+      </c>
+      <c r="F33" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G33" s="61"/>
+      <c r="H33" s="44" t="s">
+        <v>706</v>
+      </c>
+      <c r="I33" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23" t="s">
+        <v>708</v>
+      </c>
+      <c r="L33" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>681</v>
+      </c>
+      <c r="C34" s="61"/>
+      <c r="D34" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>1797</v>
+      </c>
+      <c r="F34" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G34" s="61"/>
+      <c r="H34" s="44" t="s">
+        <v>710</v>
+      </c>
+      <c r="I34" s="23" t="s">
+        <v>711</v>
+      </c>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23" t="s">
+        <v>712</v>
+      </c>
+      <c r="L34" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>681</v>
+      </c>
+      <c r="C35" s="61"/>
+      <c r="D35" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>1797</v>
+      </c>
+      <c r="F35" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G35" s="61"/>
+      <c r="H35" s="44" t="s">
+        <v>714</v>
+      </c>
+      <c r="I35" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="J35" s="23" t="s">
+        <v>716</v>
+      </c>
+      <c r="K35" s="23" t="s">
+        <v>717</v>
+      </c>
+      <c r="L35" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>681</v>
+      </c>
+      <c r="C36" s="61"/>
+      <c r="D36" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>1797</v>
+      </c>
+      <c r="F36" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G36" s="61"/>
+      <c r="H36" s="44" t="s">
+        <v>719</v>
+      </c>
+      <c r="I36" s="23" t="s">
+        <v>523</v>
+      </c>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="L36" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>681</v>
+      </c>
+      <c r="C37" s="61"/>
+      <c r="D37" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E37" s="23" t="s">
+        <v>1797</v>
+      </c>
+      <c r="F37" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G37" s="61"/>
+      <c r="H37" s="44" t="s">
+        <v>722</v>
+      </c>
+      <c r="I37" s="23" t="s">
+        <v>723</v>
+      </c>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23" t="s">
+        <v>724</v>
+      </c>
+      <c r="L37" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>681</v>
+      </c>
+      <c r="C38" s="61"/>
+      <c r="D38" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>1797</v>
+      </c>
+      <c r="F38" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G38" s="61"/>
+      <c r="H38" s="44" t="s">
+        <v>726</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>527</v>
+      </c>
+      <c r="J38" s="23" t="s">
+        <v>727</v>
+      </c>
+      <c r="K38" s="23" t="s">
+        <v>728</v>
+      </c>
+      <c r="L38" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C39" s="61"/>
+      <c r="D39" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F39" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G39" s="61"/>
+      <c r="H39" s="44" t="s">
+        <v>799</v>
+      </c>
+      <c r="I39" s="23" t="s">
+        <v>800</v>
+      </c>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23" t="s">
+        <v>801</v>
+      </c>
+      <c r="L39" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C40" s="61"/>
+      <c r="D40" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F40" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G40" s="61"/>
+      <c r="H40" s="44" t="s">
+        <v>803</v>
+      </c>
+      <c r="I40" s="23" t="s">
+        <v>804</v>
+      </c>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23" t="s">
+        <v>805</v>
+      </c>
+      <c r="L40" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C41" s="61"/>
+      <c r="D41" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E41" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F41" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G41" s="61"/>
+      <c r="H41" s="44" t="s">
+        <v>807</v>
+      </c>
+      <c r="I41" s="23" t="s">
+        <v>808</v>
+      </c>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23" t="s">
+        <v>809</v>
+      </c>
+      <c r="L41" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C42" s="61"/>
+      <c r="D42" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F42" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G42" s="61"/>
+      <c r="H42" s="44" t="s">
+        <v>811</v>
+      </c>
+      <c r="I42" s="23" t="s">
+        <v>812</v>
+      </c>
+      <c r="J42" s="23"/>
+      <c r="K42" s="23" t="s">
+        <v>813</v>
+      </c>
+      <c r="L42" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C43" s="61"/>
+      <c r="D43" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F43" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G43" s="61"/>
+      <c r="H43" s="44" t="s">
+        <v>815</v>
+      </c>
+      <c r="I43" s="23" t="s">
+        <v>816</v>
+      </c>
+      <c r="J43" s="23"/>
+      <c r="K43" s="23" t="s">
+        <v>817</v>
+      </c>
+      <c r="L43" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C44" s="61"/>
+      <c r="D44" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E44" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F44" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G44" s="61"/>
+      <c r="H44" s="44" t="s">
+        <v>819</v>
+      </c>
+      <c r="I44" s="23" t="s">
+        <v>820</v>
+      </c>
+      <c r="J44" s="23"/>
+      <c r="K44" s="23" t="s">
+        <v>821</v>
+      </c>
+      <c r="L44" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B45" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C45" s="61"/>
+      <c r="D45" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E45" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F45" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G45" s="61"/>
+      <c r="H45" s="44" t="s">
+        <v>698</v>
+      </c>
+      <c r="I45" s="23" t="s">
+        <v>699</v>
+      </c>
+      <c r="J45" s="23"/>
+      <c r="K45" s="23" t="s">
+        <v>700</v>
+      </c>
+      <c r="L45" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B46" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C46" s="61"/>
+      <c r="D46" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E46" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F46" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G46" s="61"/>
+      <c r="H46" s="44" t="s">
+        <v>823</v>
+      </c>
+      <c r="I46" s="23" t="s">
+        <v>824</v>
+      </c>
+      <c r="J46" s="23"/>
+      <c r="K46" s="23" t="s">
+        <v>825</v>
+      </c>
+      <c r="L46" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B47" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C47" s="61"/>
+      <c r="D47" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E47" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F47" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G47" s="61"/>
+      <c r="H47" s="44" t="s">
+        <v>827</v>
+      </c>
+      <c r="I47" s="23" t="s">
+        <v>828</v>
+      </c>
+      <c r="J47" s="23"/>
+      <c r="K47" s="23" t="s">
+        <v>829</v>
+      </c>
+      <c r="L47" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B48" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C48" s="61"/>
+      <c r="D48" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F48" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G48" s="61"/>
+      <c r="H48" s="44" t="s">
+        <v>831</v>
+      </c>
+      <c r="I48" s="23" t="s">
+        <v>832</v>
+      </c>
+      <c r="J48" s="23"/>
+      <c r="K48" s="23" t="s">
+        <v>833</v>
+      </c>
+      <c r="L48" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B49" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C49" s="61"/>
+      <c r="D49" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E49" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F49" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G49" s="61"/>
+      <c r="H49" s="44" t="s">
+        <v>835</v>
+      </c>
+      <c r="I49" s="23" t="s">
+        <v>836</v>
+      </c>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23" t="s">
+        <v>837</v>
+      </c>
+      <c r="L49" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B50" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C50" s="61"/>
+      <c r="D50" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E50" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F50" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G50" s="61"/>
+      <c r="H50" s="44" t="s">
+        <v>839</v>
+      </c>
+      <c r="I50" s="23" t="s">
+        <v>840</v>
+      </c>
+      <c r="J50" s="23" t="s">
+        <v>841</v>
+      </c>
+      <c r="K50" s="23" t="s">
+        <v>842</v>
+      </c>
+      <c r="L50" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B51" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C51" s="61"/>
+      <c r="D51" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F51" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G51" s="61"/>
+      <c r="H51" s="44" t="s">
+        <v>843</v>
+      </c>
+      <c r="I51" s="23" t="s">
+        <v>844</v>
+      </c>
+      <c r="J51" s="23"/>
+      <c r="K51" s="23" t="s">
+        <v>845</v>
+      </c>
+      <c r="L51" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B52" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C52" s="61"/>
+      <c r="D52" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E52" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F52" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G52" s="61"/>
+      <c r="H52" s="44" t="s">
+        <v>847</v>
+      </c>
+      <c r="I52" s="23" t="s">
+        <v>848</v>
+      </c>
+      <c r="J52" s="23"/>
+      <c r="K52" s="23" t="s">
+        <v>849</v>
+      </c>
+      <c r="L52" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B53" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C53" s="61"/>
+      <c r="D53" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F53" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G53" s="61"/>
+      <c r="H53" s="44" t="s">
+        <v>851</v>
+      </c>
+      <c r="I53" s="23" t="s">
+        <v>852</v>
+      </c>
+      <c r="J53" s="23"/>
+      <c r="K53" s="23" t="s">
+        <v>853</v>
+      </c>
+      <c r="L53" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B54" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C54" s="61"/>
+      <c r="D54" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F54" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G54" s="61"/>
+      <c r="H54" s="44" t="s">
+        <v>855</v>
+      </c>
+      <c r="I54" s="23" t="s">
+        <v>856</v>
+      </c>
+      <c r="J54" s="23"/>
+      <c r="K54" s="23" t="s">
+        <v>857</v>
+      </c>
+      <c r="L54" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C55" s="61"/>
+      <c r="D55" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E55" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F55" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G55" s="61"/>
+      <c r="H55" s="44" t="s">
+        <v>859</v>
+      </c>
+      <c r="I55" s="23" t="s">
+        <v>860</v>
+      </c>
+      <c r="J55" s="23"/>
+      <c r="K55" s="23" t="s">
+        <v>861</v>
+      </c>
+      <c r="L55" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A56" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B56" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C56" s="61"/>
+      <c r="D56" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E56" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F56" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G56" s="61"/>
+      <c r="H56" s="44" t="s">
+        <v>863</v>
+      </c>
+      <c r="I56" s="23" t="s">
+        <v>864</v>
+      </c>
+      <c r="J56" s="23"/>
+      <c r="K56" s="23" t="s">
+        <v>865</v>
+      </c>
+      <c r="L56" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A57" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C57" s="61"/>
+      <c r="D57" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E57" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F57" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G57" s="61"/>
+      <c r="H57" s="44" t="s">
+        <v>867</v>
+      </c>
+      <c r="I57" s="23" t="s">
+        <v>868</v>
+      </c>
+      <c r="J57" s="23"/>
+      <c r="K57" s="23" t="s">
+        <v>869</v>
+      </c>
+      <c r="L57" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B58" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C58" s="61"/>
+      <c r="D58" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E58" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F58" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G58" s="61"/>
+      <c r="H58" s="44" t="s">
+        <v>871</v>
+      </c>
+      <c r="I58" s="23" t="s">
+        <v>872</v>
+      </c>
+      <c r="J58" s="23"/>
+      <c r="K58" s="23" t="s">
+        <v>873</v>
+      </c>
+      <c r="L58" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A59" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B59" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C59" s="61"/>
+      <c r="D59" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E59" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F59" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G59" s="61"/>
+      <c r="H59" s="44" t="s">
+        <v>875</v>
+      </c>
+      <c r="I59" s="23" t="s">
+        <v>876</v>
+      </c>
+      <c r="J59" s="23"/>
+      <c r="K59" s="23" t="s">
+        <v>877</v>
+      </c>
+      <c r="L59" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B60" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C60" s="61"/>
+      <c r="D60" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E60" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F60" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G60" s="61"/>
+      <c r="H60" s="44" t="s">
+        <v>714</v>
+      </c>
+      <c r="I60" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="J60" s="23" t="s">
+        <v>716</v>
+      </c>
+      <c r="K60" s="23" t="s">
+        <v>717</v>
+      </c>
+      <c r="L60" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A61" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B61" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C61" s="61"/>
+      <c r="D61" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E61" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F61" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G61" s="61"/>
+      <c r="H61" s="44" t="s">
+        <v>879</v>
+      </c>
+      <c r="I61" s="23" t="s">
+        <v>880</v>
+      </c>
+      <c r="J61" s="23"/>
+      <c r="K61" s="23" t="s">
+        <v>881</v>
+      </c>
+      <c r="L61" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B62" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C62" s="61"/>
+      <c r="D62" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E62" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F62" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G62" s="61"/>
+      <c r="H62" s="44" t="s">
+        <v>883</v>
+      </c>
+      <c r="I62" s="23" t="s">
+        <v>884</v>
+      </c>
+      <c r="J62" s="23"/>
+      <c r="K62" s="23" t="s">
+        <v>885</v>
+      </c>
+      <c r="L62" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B63" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C63" s="61"/>
+      <c r="D63" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E63" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F63" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G63" s="61"/>
+      <c r="H63" s="44" t="s">
+        <v>887</v>
+      </c>
+      <c r="I63" s="23" t="s">
+        <v>888</v>
+      </c>
+      <c r="J63" s="23"/>
+      <c r="K63" s="23" t="s">
+        <v>889</v>
+      </c>
+      <c r="L63" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B64" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C64" s="61"/>
+      <c r="D64" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E64" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F64" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G64" s="61"/>
+      <c r="H64" s="44" t="s">
+        <v>891</v>
+      </c>
+      <c r="I64" s="23" t="s">
+        <v>892</v>
+      </c>
+      <c r="J64" s="23" t="s">
+        <v>893</v>
+      </c>
+      <c r="K64" s="23" t="s">
+        <v>894</v>
+      </c>
+      <c r="L64" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A65" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C65" s="61"/>
+      <c r="D65" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E65" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F65" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G65" s="61"/>
+      <c r="H65" s="44" t="s">
+        <v>896</v>
+      </c>
+      <c r="I65" s="23" t="s">
+        <v>897</v>
+      </c>
+      <c r="J65" s="23"/>
+      <c r="K65" s="23" t="s">
+        <v>898</v>
+      </c>
+      <c r="L65" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A66" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B66" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C66" s="61"/>
+      <c r="D66" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E66" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F66" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G66" s="61"/>
+      <c r="H66" s="44" t="s">
+        <v>726</v>
+      </c>
+      <c r="I66" s="23" t="s">
+        <v>527</v>
+      </c>
+      <c r="J66" s="23" t="s">
+        <v>727</v>
+      </c>
+      <c r="K66" s="23" t="s">
+        <v>728</v>
+      </c>
+      <c r="L66" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A67" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B67" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C67" s="61"/>
+      <c r="D67" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E67" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F67" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G67" s="61"/>
+      <c r="H67" s="44" t="s">
+        <v>900</v>
+      </c>
+      <c r="I67" s="23" t="s">
+        <v>901</v>
+      </c>
+      <c r="J67" s="23"/>
+      <c r="K67" s="23" t="s">
+        <v>902</v>
+      </c>
+      <c r="L67" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A68" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B68" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C68" s="61"/>
+      <c r="D68" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E68" s="23" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F68" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G68" s="61"/>
+      <c r="H68" s="44" t="s">
+        <v>904</v>
+      </c>
+      <c r="I68" s="23" t="s">
+        <v>905</v>
+      </c>
+      <c r="J68" s="23"/>
+      <c r="K68" s="23" t="s">
+        <v>906</v>
+      </c>
+      <c r="L68" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A69" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B69" s="23" t="s">
+        <v>534</v>
+      </c>
+      <c r="C69" s="61"/>
+      <c r="D69" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E69" s="23" t="s">
+        <v>1801</v>
+      </c>
+      <c r="F69" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G69" s="61"/>
+      <c r="H69" s="44" t="s">
+        <v>539</v>
+      </c>
+      <c r="I69" s="23" t="s">
+        <v>540</v>
+      </c>
+      <c r="J69" s="23"/>
+      <c r="K69" s="23" t="s">
+        <v>541</v>
+      </c>
+      <c r="L69" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A70" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B70" s="23" t="s">
+        <v>534</v>
+      </c>
+      <c r="C70" s="61"/>
+      <c r="D70" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E70" s="23" t="s">
+        <v>1801</v>
+      </c>
+      <c r="F70" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G70" s="61"/>
+      <c r="H70" s="44" t="s">
+        <v>543</v>
+      </c>
+      <c r="I70" s="23" t="s">
+        <v>544</v>
+      </c>
+      <c r="J70" s="23"/>
+      <c r="K70" s="23" t="s">
+        <v>545</v>
+      </c>
+      <c r="L70" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A71" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B71" s="23" t="s">
+        <v>534</v>
+      </c>
+      <c r="C71" s="61"/>
+      <c r="D71" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E71" s="23" t="s">
+        <v>1801</v>
+      </c>
+      <c r="F71" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G71" s="61"/>
+      <c r="H71" s="44" t="s">
+        <v>547</v>
+      </c>
+      <c r="I71" s="23" t="s">
+        <v>548</v>
+      </c>
+      <c r="J71" s="23"/>
+      <c r="K71" s="23" t="s">
+        <v>549</v>
+      </c>
+      <c r="L71" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A72" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B72" s="23" t="s">
+        <v>534</v>
+      </c>
+      <c r="C72" s="61"/>
+      <c r="D72" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E72" s="23" t="s">
+        <v>1801</v>
+      </c>
+      <c r="F72" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G72" s="61"/>
+      <c r="H72" s="44" t="s">
+        <v>551</v>
+      </c>
+      <c r="I72" s="23" t="s">
+        <v>552</v>
+      </c>
+      <c r="J72" s="23"/>
+      <c r="K72" s="23" t="s">
+        <v>553</v>
+      </c>
+      <c r="L72" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A73" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B73" s="23" t="s">
+        <v>534</v>
+      </c>
+      <c r="C73" s="61"/>
+      <c r="D73" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E73" s="23" t="s">
+        <v>1801</v>
+      </c>
+      <c r="F73" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G73" s="61"/>
+      <c r="H73" s="44" t="s">
+        <v>555</v>
+      </c>
+      <c r="I73" s="23" t="s">
+        <v>556</v>
+      </c>
+      <c r="J73" s="23"/>
+      <c r="K73" s="23" t="s">
+        <v>557</v>
+      </c>
+      <c r="L73" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A74" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B74" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="C74" s="61"/>
+      <c r="D74" s="132" t="s">
+        <v>935</v>
+      </c>
+      <c r="E74" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F74" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G74" s="61"/>
+      <c r="H74" s="44" t="s">
+        <v>485</v>
+      </c>
+      <c r="I74" s="23" t="s">
+        <v>486</v>
+      </c>
+      <c r="J74" s="23"/>
+      <c r="K74" s="23" t="s">
+        <v>487</v>
+      </c>
+      <c r="L74" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A75" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B75" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="C75" s="61"/>
+      <c r="D75" s="132" t="s">
+        <v>935</v>
+      </c>
+      <c r="E75" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F75" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G75" s="61"/>
+      <c r="H75" s="44" t="s">
+        <v>489</v>
+      </c>
+      <c r="I75" s="23" t="s">
+        <v>490</v>
+      </c>
+      <c r="J75" s="23"/>
+      <c r="K75" s="23" t="s">
+        <v>491</v>
+      </c>
+      <c r="L75" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A76" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B76" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="C76" s="61"/>
+      <c r="D76" s="132" t="s">
+        <v>935</v>
+      </c>
+      <c r="E76" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F76" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G76" s="61"/>
+      <c r="H76" s="44" t="s">
+        <v>493</v>
+      </c>
+      <c r="I76" s="23" t="s">
+        <v>494</v>
+      </c>
+      <c r="J76" s="23" t="s">
+        <v>495</v>
+      </c>
+      <c r="K76" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="L76" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A77" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B77" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="C77" s="61"/>
+      <c r="D77" s="132" t="s">
+        <v>935</v>
+      </c>
+      <c r="E77" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F77" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G77" s="61"/>
+      <c r="H77" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="I77" s="23" t="s">
+        <v>499</v>
+      </c>
+      <c r="J77" s="23"/>
+      <c r="K77" s="23" t="s">
+        <v>500</v>
+      </c>
+      <c r="L77" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A78" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B78" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="C78" s="61"/>
+      <c r="D78" s="132" t="s">
+        <v>935</v>
+      </c>
+      <c r="E78" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F78" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G78" s="61"/>
+      <c r="H78" s="44" t="s">
+        <v>502</v>
+      </c>
+      <c r="I78" s="23" t="s">
+        <v>503</v>
+      </c>
+      <c r="J78" s="23" t="s">
+        <v>504</v>
+      </c>
+      <c r="K78" s="23" t="s">
+        <v>505</v>
+      </c>
+      <c r="L78" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A79" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B79" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="C79" s="61"/>
+      <c r="D79" s="132" t="s">
+        <v>935</v>
+      </c>
+      <c r="E79" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F79" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G79" s="61"/>
+      <c r="H79" s="44" t="s">
+        <v>507</v>
+      </c>
+      <c r="I79" s="23" t="s">
+        <v>508</v>
+      </c>
+      <c r="J79" s="23"/>
+      <c r="K79" s="23" t="s">
+        <v>509</v>
+      </c>
+      <c r="L79" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A80" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B80" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="C80" s="61"/>
+      <c r="D80" s="132" t="s">
+        <v>935</v>
+      </c>
+      <c r="E80" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F80" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G80" s="61"/>
+      <c r="H80" s="44" t="s">
+        <v>511</v>
+      </c>
+      <c r="I80" s="23" t="s">
+        <v>512</v>
+      </c>
+      <c r="J80" s="23"/>
+      <c r="K80" s="23" t="s">
+        <v>513</v>
+      </c>
+      <c r="L80" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A81" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B81" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="C81" s="61"/>
+      <c r="D81" s="132" t="s">
+        <v>935</v>
+      </c>
+      <c r="E81" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F81" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G81" s="61"/>
+      <c r="H81" s="44" t="s">
+        <v>515</v>
+      </c>
+      <c r="I81" s="23" t="s">
+        <v>516</v>
+      </c>
+      <c r="J81" s="23"/>
+      <c r="K81" s="23" t="s">
+        <v>517</v>
+      </c>
+      <c r="L81" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A82" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B82" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="C82" s="61"/>
+      <c r="D82" s="132" t="s">
+        <v>935</v>
+      </c>
+      <c r="E82" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F82" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G82" s="61"/>
+      <c r="H82" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="I82" s="23" t="s">
+        <v>520</v>
+      </c>
+      <c r="J82" s="23"/>
+      <c r="K82" s="23" t="s">
+        <v>1368</v>
+      </c>
+      <c r="L82" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A83" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B83" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="C83" s="61"/>
+      <c r="D83" s="132" t="s">
+        <v>935</v>
+      </c>
+      <c r="E83" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F83" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G83" s="61"/>
+      <c r="H83" s="44" t="s">
+        <v>522</v>
+      </c>
+      <c r="I83" s="23" t="s">
+        <v>523</v>
+      </c>
+      <c r="J83" s="23"/>
+      <c r="K83" s="23" t="s">
+        <v>524</v>
+      </c>
+      <c r="L83" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A84" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B84" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="C84" s="61"/>
+      <c r="D84" s="132" t="s">
+        <v>935</v>
+      </c>
+      <c r="E84" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F84" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G84" s="61"/>
+      <c r="H84" s="44" t="s">
+        <v>526</v>
+      </c>
+      <c r="I84" s="23" t="s">
+        <v>527</v>
+      </c>
+      <c r="J84" s="23"/>
+      <c r="K84" s="23" t="s">
+        <v>528</v>
+      </c>
+      <c r="L84" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A85" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B85" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="C85" s="61"/>
+      <c r="D85" s="132" t="s">
+        <v>935</v>
+      </c>
+      <c r="E85" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F85" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G85" s="61"/>
+      <c r="H85" s="44" t="s">
+        <v>530</v>
+      </c>
+      <c r="I85" s="23" t="s">
+        <v>531</v>
+      </c>
+      <c r="J85" s="23"/>
+      <c r="K85" s="23" t="s">
+        <v>532</v>
+      </c>
+      <c r="L85" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A86" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B86" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C86" s="61"/>
+      <c r="D86" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E86" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F86" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G86" s="61"/>
+      <c r="H86" s="44" t="s">
+        <v>408</v>
+      </c>
+      <c r="I86" s="23" t="s">
+        <v>409</v>
+      </c>
+      <c r="J86" s="23"/>
+      <c r="K86" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="L86" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A87" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B87" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C87" s="61"/>
+      <c r="D87" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E87" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F87" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G87" s="61"/>
+      <c r="H87" s="44" t="s">
+        <v>412</v>
+      </c>
+      <c r="I87" s="23" t="s">
+        <v>413</v>
+      </c>
+      <c r="J87" s="23"/>
+      <c r="K87" s="23" t="s">
+        <v>414</v>
+      </c>
+      <c r="L87" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A88" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B88" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C88" s="61"/>
+      <c r="D88" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E88" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F88" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G88" s="61"/>
+      <c r="H88" s="44" t="s">
+        <v>416</v>
+      </c>
+      <c r="I88" s="23" t="s">
+        <v>417</v>
+      </c>
+      <c r="J88" s="23"/>
+      <c r="K88" s="23" t="s">
+        <v>418</v>
+      </c>
+      <c r="L88" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A89" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B89" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C89" s="61"/>
+      <c r="D89" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E89" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F89" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G89" s="61"/>
+      <c r="H89" s="44" t="s">
+        <v>420</v>
+      </c>
+      <c r="I89" s="23" t="s">
+        <v>421</v>
+      </c>
+      <c r="J89" s="23"/>
+      <c r="K89" s="23" t="s">
+        <v>422</v>
+      </c>
+      <c r="L89" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A90" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B90" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C90" s="61"/>
+      <c r="D90" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E90" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F90" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G90" s="61"/>
+      <c r="H90" s="44" t="s">
+        <v>424</v>
+      </c>
+      <c r="I90" s="23" t="s">
+        <v>425</v>
+      </c>
+      <c r="J90" s="23"/>
+      <c r="K90" s="23" t="s">
+        <v>426</v>
+      </c>
+      <c r="L90" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A91" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B91" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C91" s="61"/>
+      <c r="D91" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E91" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F91" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G91" s="61"/>
+      <c r="H91" s="44" t="s">
+        <v>428</v>
+      </c>
+      <c r="I91" s="23" t="s">
+        <v>429</v>
+      </c>
+      <c r="J91" s="23"/>
+      <c r="K91" s="23" t="s">
+        <v>430</v>
+      </c>
+      <c r="L91" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A92" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B92" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C92" s="61"/>
+      <c r="D92" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E92" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F92" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G92" s="61"/>
+      <c r="H92" s="44" t="s">
+        <v>432</v>
+      </c>
+      <c r="I92" s="23" t="s">
+        <v>433</v>
+      </c>
+      <c r="J92" s="23"/>
+      <c r="K92" s="23" t="s">
+        <v>434</v>
+      </c>
+      <c r="L92" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A93" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B93" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C93" s="61"/>
+      <c r="D93" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E93" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F93" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G93" s="61"/>
+      <c r="H93" s="44" t="s">
+        <v>436</v>
+      </c>
+      <c r="I93" s="23" t="s">
+        <v>437</v>
+      </c>
+      <c r="J93" s="23"/>
+      <c r="K93" s="23" t="s">
+        <v>438</v>
+      </c>
+      <c r="L93" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A94" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B94" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C94" s="61"/>
+      <c r="D94" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E94" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F94" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G94" s="61"/>
+      <c r="H94" s="44" t="s">
+        <v>440</v>
+      </c>
+      <c r="I94" s="23" t="s">
+        <v>441</v>
+      </c>
+      <c r="J94" s="23"/>
+      <c r="K94" s="23" t="s">
+        <v>442</v>
+      </c>
+      <c r="L94" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A95" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B95" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C95" s="61"/>
+      <c r="D95" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E95" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F95" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G95" s="61"/>
+      <c r="H95" s="44" t="s">
+        <v>444</v>
+      </c>
+      <c r="I95" s="23" t="s">
+        <v>445</v>
+      </c>
+      <c r="J95" s="23"/>
+      <c r="K95" s="23" t="s">
+        <v>446</v>
+      </c>
+      <c r="L95" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A96" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B96" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C96" s="61"/>
+      <c r="D96" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E96" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F96" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G96" s="61"/>
+      <c r="H96" s="44" t="s">
+        <v>448</v>
+      </c>
+      <c r="I96" s="23" t="s">
+        <v>449</v>
+      </c>
+      <c r="J96" s="23"/>
+      <c r="K96" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="L96" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A97" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B97" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C97" s="61"/>
+      <c r="D97" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E97" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F97" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G97" s="61"/>
+      <c r="H97" s="44" t="s">
+        <v>452</v>
+      </c>
+      <c r="I97" s="23" t="s">
+        <v>453</v>
+      </c>
+      <c r="J97" s="23"/>
+      <c r="K97" s="23" t="s">
+        <v>454</v>
+      </c>
+      <c r="L97" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A98" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B98" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C98" s="61"/>
+      <c r="D98" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E98" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F98" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G98" s="61"/>
+      <c r="H98" s="44" t="s">
+        <v>456</v>
+      </c>
+      <c r="I98" s="23" t="s">
+        <v>457</v>
+      </c>
+      <c r="J98" s="23"/>
+      <c r="K98" s="23" t="s">
+        <v>458</v>
+      </c>
+      <c r="L98" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A99" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B99" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C99" s="61"/>
+      <c r="D99" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E99" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F99" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G99" s="61"/>
+      <c r="H99" s="44" t="s">
+        <v>460</v>
+      </c>
+      <c r="I99" s="23" t="s">
+        <v>461</v>
+      </c>
+      <c r="J99" s="23"/>
+      <c r="K99" s="23" t="s">
+        <v>462</v>
+      </c>
+      <c r="L99" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A100" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B100" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C100" s="61"/>
+      <c r="D100" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E100" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F100" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G100" s="61"/>
+      <c r="H100" s="44" t="s">
+        <v>464</v>
+      </c>
+      <c r="I100" s="23" t="s">
+        <v>465</v>
+      </c>
+      <c r="J100" s="23"/>
+      <c r="K100" s="23" t="s">
+        <v>466</v>
+      </c>
+      <c r="L100" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A101" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B101" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C101" s="61"/>
+      <c r="D101" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E101" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F101" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G101" s="61"/>
+      <c r="H101" s="44" t="s">
+        <v>468</v>
+      </c>
+      <c r="I101" s="23" t="s">
+        <v>469</v>
+      </c>
+      <c r="J101" s="23"/>
+      <c r="K101" s="23" t="s">
+        <v>470</v>
+      </c>
+      <c r="L101" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A102" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B102" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C102" s="61"/>
+      <c r="D102" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E102" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F102" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G102" s="61"/>
+      <c r="H102" s="44" t="s">
+        <v>472</v>
+      </c>
+      <c r="I102" s="23" t="s">
+        <v>473</v>
+      </c>
+      <c r="J102" s="23"/>
+      <c r="K102" s="23" t="s">
+        <v>474</v>
+      </c>
+      <c r="L102" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A103" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B103" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C103" s="61"/>
+      <c r="D103" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E103" s="23" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F103" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G103" s="61"/>
+      <c r="H103" s="44" t="s">
+        <v>476</v>
+      </c>
+      <c r="I103" s="23" t="s">
+        <v>477</v>
+      </c>
+      <c r="J103" s="23"/>
+      <c r="K103" s="23" t="s">
+        <v>478</v>
+      </c>
+      <c r="L103" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A104" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B104" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="C104" s="61"/>
+      <c r="D104" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E104" s="23" t="s">
+        <v>1791</v>
+      </c>
+      <c r="F104" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G104" s="61"/>
+      <c r="H104" s="44" t="s">
+        <v>564</v>
+      </c>
+      <c r="I104" s="23" t="s">
+        <v>565</v>
+      </c>
+      <c r="J104" s="23" t="s">
+        <v>566</v>
+      </c>
+      <c r="K104" s="23" t="s">
+        <v>567</v>
+      </c>
+      <c r="L104" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A105" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B105" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="C105" s="61"/>
+      <c r="D105" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E105" s="23" t="s">
+        <v>1791</v>
+      </c>
+      <c r="F105" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G105" s="61"/>
+      <c r="H105" s="44" t="s">
+        <v>569</v>
+      </c>
+      <c r="I105" s="23" t="s">
+        <v>570</v>
+      </c>
+      <c r="J105" s="23" t="s">
+        <v>571</v>
+      </c>
+      <c r="K105" s="23" t="s">
+        <v>572</v>
+      </c>
+      <c r="L105" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A106" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B106" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="C106" s="61"/>
+      <c r="D106" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E106" s="23" t="s">
+        <v>1791</v>
+      </c>
+      <c r="F106" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G106" s="61"/>
+      <c r="H106" s="44" t="s">
+        <v>573</v>
+      </c>
+      <c r="I106" s="23" t="s">
+        <v>574</v>
+      </c>
+      <c r="J106" s="23"/>
+      <c r="K106" s="23" t="s">
+        <v>575</v>
+      </c>
+      <c r="L106" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A107" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B107" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="C107" s="61"/>
+      <c r="D107" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E107" s="23" t="s">
+        <v>1791</v>
+      </c>
+      <c r="F107" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G107" s="61"/>
+      <c r="H107" s="44" t="s">
+        <v>577</v>
+      </c>
+      <c r="I107" s="23" t="s">
+        <v>578</v>
+      </c>
+      <c r="J107" s="23"/>
+      <c r="K107" s="23" t="s">
+        <v>579</v>
+      </c>
+      <c r="L107" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A108" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B108" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="C108" s="61"/>
+      <c r="D108" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E108" s="23" t="s">
+        <v>1791</v>
+      </c>
+      <c r="F108" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G108" s="61"/>
+      <c r="H108" s="44" t="s">
+        <v>581</v>
+      </c>
+      <c r="I108" s="23" t="s">
+        <v>582</v>
+      </c>
+      <c r="J108" s="23"/>
+      <c r="K108" s="23" t="s">
+        <v>583</v>
+      </c>
+      <c r="L108" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A109" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B109" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="C109" s="61"/>
+      <c r="D109" s="132" t="s">
+        <v>924</v>
+      </c>
+      <c r="E109" s="23" t="s">
+        <v>1791</v>
+      </c>
+      <c r="F109" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G109" s="61"/>
+      <c r="H109" s="44" t="s">
+        <v>585</v>
+      </c>
+      <c r="I109" s="23" t="s">
+        <v>586</v>
+      </c>
+      <c r="J109" s="23"/>
+      <c r="K109" s="23" t="s">
+        <v>587</v>
+      </c>
+      <c r="L109" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A110" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B110" s="23" t="s">
+        <v>1850</v>
+      </c>
+      <c r="C110" s="61"/>
+      <c r="D110" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E110" s="23" t="s">
+        <v>1803</v>
+      </c>
+      <c r="F110" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G110" s="61"/>
+      <c r="H110" s="44" t="s">
+        <v>1852</v>
+      </c>
+      <c r="I110" s="23" t="s">
+        <v>1853</v>
+      </c>
+      <c r="J110" s="23" t="s">
+        <v>1854</v>
+      </c>
+      <c r="K110" s="23" t="s">
+        <v>1855</v>
+      </c>
+      <c r="L110" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A111" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B111" s="23" t="s">
+        <v>1850</v>
+      </c>
+      <c r="C111" s="61"/>
+      <c r="D111" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E111" s="23" t="s">
+        <v>1803</v>
+      </c>
+      <c r="F111" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G111" s="61"/>
+      <c r="H111" s="44" t="s">
+        <v>1856</v>
+      </c>
+      <c r="I111" s="23" t="s">
+        <v>1857</v>
+      </c>
+      <c r="J111" s="23"/>
+      <c r="K111" s="23" t="s">
+        <v>1858</v>
+      </c>
+      <c r="L111" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A112" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B112" s="23" t="s">
+        <v>1850</v>
+      </c>
+      <c r="C112" s="61"/>
+      <c r="D112" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E112" s="23" t="s">
+        <v>1803</v>
+      </c>
+      <c r="F112" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G112" s="61"/>
+      <c r="H112" s="44" t="s">
+        <v>1859</v>
+      </c>
+      <c r="I112" s="23" t="s">
+        <v>1860</v>
+      </c>
+      <c r="J112" s="23"/>
+      <c r="K112" s="23" t="s">
+        <v>1861</v>
+      </c>
+      <c r="L112" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A113" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B113" s="23" t="s">
+        <v>1850</v>
+      </c>
+      <c r="C113" s="61"/>
+      <c r="D113" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E113" s="23" t="s">
+        <v>1803</v>
+      </c>
+      <c r="F113" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G113" s="61"/>
+      <c r="H113" s="44" t="s">
+        <v>1862</v>
+      </c>
+      <c r="I113" s="23" t="s">
+        <v>1863</v>
+      </c>
+      <c r="J113" s="23"/>
+      <c r="K113" s="23" t="s">
+        <v>1864</v>
+      </c>
+      <c r="L113" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A114" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B114" s="23" t="s">
+        <v>1850</v>
+      </c>
+      <c r="C114" s="61"/>
+      <c r="D114" s="132" t="s">
+        <v>920</v>
+      </c>
+      <c r="E114" s="23" t="s">
+        <v>1803</v>
+      </c>
+      <c r="F114" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G114" s="61"/>
+      <c r="H114" s="44" t="s">
+        <v>1865</v>
+      </c>
+      <c r="I114" s="23" t="s">
+        <v>1866</v>
+      </c>
+      <c r="J114" s="23" t="s">
+        <v>1867</v>
+      </c>
+      <c r="K114" s="23" t="s">
+        <v>1868</v>
+      </c>
+      <c r="L114" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A115" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B115" s="23" t="s">
+        <v>2061</v>
+      </c>
+      <c r="C115" s="61"/>
+      <c r="D115" s="132" t="s">
+        <v>931</v>
+      </c>
+      <c r="E115" s="23" t="s">
+        <v>2142</v>
+      </c>
+      <c r="F115" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G115" s="61"/>
+      <c r="H115" s="44" t="s">
+        <v>2066</v>
+      </c>
+      <c r="I115" s="23" t="s">
+        <v>2067</v>
+      </c>
+      <c r="J115" s="23"/>
+      <c r="K115" s="23" t="s">
+        <v>2068</v>
+      </c>
+      <c r="L115" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A116" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B116" s="23" t="s">
+        <v>2061</v>
+      </c>
+      <c r="C116" s="61"/>
+      <c r="D116" s="132" t="s">
+        <v>931</v>
+      </c>
+      <c r="E116" s="23" t="s">
+        <v>2142</v>
+      </c>
+      <c r="F116" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G116" s="61"/>
+      <c r="H116" s="44" t="s">
+        <v>2070</v>
+      </c>
+      <c r="I116" s="23" t="s">
+        <v>2071</v>
+      </c>
+      <c r="J116" s="23" t="s">
+        <v>2072</v>
+      </c>
+      <c r="K116" s="23" t="s">
+        <v>2073</v>
+      </c>
+      <c r="L116" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A117" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B117" s="23" t="s">
+        <v>2061</v>
+      </c>
+      <c r="C117" s="61"/>
+      <c r="D117" s="132" t="s">
+        <v>931</v>
+      </c>
+      <c r="E117" s="23" t="s">
+        <v>2142</v>
+      </c>
+      <c r="F117" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G117" s="61"/>
+      <c r="H117" s="44" t="s">
+        <v>2074</v>
+      </c>
+      <c r="I117" s="23" t="s">
+        <v>2075</v>
+      </c>
+      <c r="J117" s="23" t="s">
+        <v>2076</v>
+      </c>
+      <c r="K117" s="23" t="s">
+        <v>2077</v>
+      </c>
+      <c r="L117" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A118" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B118" s="135" t="s">
+        <v>1376</v>
+      </c>
+      <c r="C118" s="61"/>
+      <c r="D118" s="136" t="s">
+        <v>934</v>
+      </c>
+      <c r="E118" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F118" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G118" s="61"/>
+      <c r="H118" s="137" t="s">
+        <v>1377</v>
+      </c>
+      <c r="I118" s="138" t="s">
+        <v>1378</v>
+      </c>
+      <c r="J118" s="139"/>
+      <c r="K118" s="139" t="s">
+        <v>1379</v>
+      </c>
+      <c r="L118" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A119" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B119" s="135" t="s">
+        <v>1376</v>
+      </c>
+      <c r="C119" s="61"/>
+      <c r="D119" s="136" t="s">
+        <v>934</v>
+      </c>
+      <c r="E119" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F119" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G119" s="61"/>
+      <c r="H119" s="134" t="s">
+        <v>1380</v>
+      </c>
+      <c r="I119" s="43" t="s">
+        <v>1381</v>
+      </c>
+      <c r="J119" s="43"/>
+      <c r="K119" s="43" t="s">
+        <v>1382</v>
+      </c>
+      <c r="L119" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A120" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B120" s="135" t="s">
+        <v>1376</v>
+      </c>
+      <c r="C120" s="61"/>
+      <c r="D120" s="136" t="s">
+        <v>934</v>
+      </c>
+      <c r="E120" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F120" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G120" s="61"/>
+      <c r="H120" s="134" t="s">
+        <v>1383</v>
+      </c>
+      <c r="I120" s="43" t="s">
+        <v>1384</v>
+      </c>
+      <c r="J120" s="43" t="s">
+        <v>1385</v>
+      </c>
+      <c r="K120" s="43" t="s">
+        <v>1386</v>
+      </c>
+      <c r="L120" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A121" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B121" s="135" t="s">
+        <v>1376</v>
+      </c>
+      <c r="C121" s="61"/>
+      <c r="D121" s="136" t="s">
+        <v>934</v>
+      </c>
+      <c r="E121" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F121" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G121" s="61"/>
+      <c r="H121" s="134" t="s">
+        <v>1387</v>
+      </c>
+      <c r="I121" s="43" t="s">
+        <v>1388</v>
+      </c>
+      <c r="J121" s="43"/>
+      <c r="K121" s="43" t="s">
+        <v>1389</v>
+      </c>
+      <c r="L121" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A122" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B122" s="135" t="s">
+        <v>1376</v>
+      </c>
+      <c r="C122" s="61"/>
+      <c r="D122" s="136" t="s">
+        <v>934</v>
+      </c>
+      <c r="E122" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F122" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G122" s="61"/>
+      <c r="H122" s="134" t="s">
+        <v>1390</v>
+      </c>
+      <c r="I122" s="43" t="s">
+        <v>1391</v>
+      </c>
+      <c r="J122" s="43" t="s">
+        <v>1392</v>
+      </c>
+      <c r="K122" s="43" t="s">
+        <v>1393</v>
+      </c>
+      <c r="L122" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A123" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B123" s="135" t="s">
+        <v>1376</v>
+      </c>
+      <c r="C123" s="61"/>
+      <c r="D123" s="136" t="s">
+        <v>934</v>
+      </c>
+      <c r="E123" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F123" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G123" s="61"/>
+      <c r="H123" s="134" t="s">
+        <v>1394</v>
+      </c>
+      <c r="I123" s="43" t="s">
+        <v>1395</v>
+      </c>
+      <c r="J123" s="43" t="s">
+        <v>1396</v>
+      </c>
+      <c r="K123" s="43" t="s">
+        <v>1397</v>
+      </c>
+      <c r="L123" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A124" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B124" s="135" t="s">
+        <v>1376</v>
+      </c>
+      <c r="C124" s="61"/>
+      <c r="D124" s="136" t="s">
+        <v>934</v>
+      </c>
+      <c r="E124" s="23" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F124" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G124" s="61"/>
+      <c r="H124" s="134" t="s">
+        <v>1398</v>
+      </c>
+      <c r="I124" s="43" t="s">
+        <v>1399</v>
+      </c>
+      <c r="J124" s="43"/>
+      <c r="K124" s="43" t="s">
+        <v>1400</v>
+      </c>
+      <c r="L124" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A125" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B125" s="135" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C125" s="61"/>
+      <c r="D125" s="136" t="s">
+        <v>1249</v>
+      </c>
+      <c r="E125" s="23" t="s">
+        <v>1259</v>
+      </c>
+      <c r="F125" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G125" s="61"/>
+      <c r="H125" s="44" t="s">
+        <v>1276</v>
+      </c>
+      <c r="I125" s="43" t="s">
+        <v>1273</v>
+      </c>
+      <c r="J125" s="43"/>
+      <c r="K125" s="23" t="s">
+        <v>2393</v>
+      </c>
+      <c r="L125" s="61" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" ht="100" x14ac:dyDescent="0.25">
+      <c r="A126" s="16" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B126" s="135" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C126" s="61"/>
+      <c r="D126" s="136" t="s">
+        <v>1249</v>
+      </c>
+      <c r="E126" s="23" t="s">
+        <v>1259</v>
+      </c>
+      <c r="F126" s="61" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G126" s="61"/>
+      <c r="H126" s="44" t="s">
+        <v>1278</v>
+      </c>
+      <c r="I126" s="43" t="s">
+        <v>1275</v>
+      </c>
+      <c r="J126" s="43"/>
+      <c r="K126" s="23" t="s">
+        <v>2394</v>
+      </c>
+      <c r="L126" s="61" t="s">
+        <v>945</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates to draft codelist names
For consistency across all CNEW draft codelists.
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2C2BED-2EC4-40EA-A4E1-1BF4B581FB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCCEBBC-80CA-48B4-955C-503700D4E3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3830" yWindow="0" windowWidth="15270" windowHeight="9980" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2490" yWindow="350" windowWidth="15270" windowHeight="9980" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10641" uniqueCount="2501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10681" uniqueCount="2509">
   <si>
     <t>Code</t>
   </si>
@@ -13979,7 +13979,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Y (CNEW) </t>
+      <t>Y (CNEW - Geographic Scope Type Value Set Terminology)</t>
     </r>
     <r>
       <rPr>
@@ -13997,7 +13997,135 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Y (CNEW - Study Design Characteristic Value Set Terminology)</t>
+      <t>Y (CNEW - Geographic Scope Type Response)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW - Study Design Characteristics Value Set Terminology)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW - Study Design Characteristics Response)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW - Governance Date Type Value Set Terminology)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW - Governance Date Type Response)</t>
+    </r>
+  </si>
+  <si>
+    <t>DDF Study Title Type Attribute Terminology</t>
+  </si>
+  <si>
+    <t>DDF Geographic Scope Type Attribute Terminology</t>
+  </si>
+  <si>
+    <t>DDF Study Design Characteristics Attribute Terminology</t>
+  </si>
+  <si>
+    <t>DDF Governance Date Type Attribute Terminology</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Y (CNEW) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW - Study Design Characteristic Response)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW-DDF Study Title Attribute Terminology)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW - Study Title Type Response)</t>
     </r>
   </si>
 </sst>
@@ -14441,7 +14569,7 @@
     <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -14849,12 +14977,6 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14870,8 +14992,11 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -15200,10 +15325,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="142" t="s">
         <v>908</v>
       </c>
-      <c r="B1" s="138"/>
+      <c r="B1" s="143"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -28404,50 +28529,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="47.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="137" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="139" t="s">
+      <c r="B1" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="139" t="s">
+      <c r="C1" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="139" t="s">
+      <c r="D1" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="139" t="s">
+      <c r="E1" s="137" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="139" t="s">
+      <c r="F1" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="139" t="s">
+      <c r="G1" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="139" t="s">
+      <c r="H1" s="137" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="140" t="s">
+      <c r="A2" s="138" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="140"/>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140" t="s">
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="140" t="s">
+      <c r="E2" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="140" t="s">
+      <c r="F2" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="140" t="s">
+      <c r="G2" s="138" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="140" t="s">
+      <c r="H2" s="138" t="s">
         <v>25</v>
       </c>
     </row>
@@ -28584,24 +28709,24 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A9" s="140" t="s">
+      <c r="A9" s="138" t="s">
         <v>1886</v>
       </c>
-      <c r="B9" s="140"/>
-      <c r="C9" s="140"/>
-      <c r="D9" s="140" t="s">
+      <c r="B9" s="138"/>
+      <c r="C9" s="138"/>
+      <c r="D9" s="138" t="s">
         <v>1887</v>
       </c>
-      <c r="E9" s="140" t="s">
+      <c r="E9" s="138" t="s">
         <v>1887</v>
       </c>
-      <c r="F9" s="140" t="s">
+      <c r="F9" s="138" t="s">
         <v>1887</v>
       </c>
-      <c r="G9" s="140" t="s">
+      <c r="G9" s="138" t="s">
         <v>1888</v>
       </c>
-      <c r="H9" s="140" t="s">
+      <c r="H9" s="138" t="s">
         <v>1889</v>
       </c>
     </row>
@@ -28760,24 +28885,24 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A17" s="140" t="s">
+      <c r="A17" s="138" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="140"/>
-      <c r="C17" s="140"/>
-      <c r="D17" s="140" t="s">
+      <c r="B17" s="138"/>
+      <c r="C17" s="138"/>
+      <c r="D17" s="138" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="140" t="s">
+      <c r="E17" s="138" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="140" t="s">
+      <c r="F17" s="138" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="140" t="s">
+      <c r="G17" s="138" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="140" t="s">
+      <c r="H17" s="138" t="s">
         <v>35</v>
       </c>
     </row>
@@ -28804,24 +28929,24 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A19" s="140" t="s">
+      <c r="A19" s="138" t="s">
         <v>1624</v>
       </c>
-      <c r="B19" s="140"/>
-      <c r="C19" s="140"/>
-      <c r="D19" s="140" t="s">
+      <c r="B19" s="138"/>
+      <c r="C19" s="138"/>
+      <c r="D19" s="138" t="s">
         <v>1116</v>
       </c>
-      <c r="E19" s="140" t="s">
+      <c r="E19" s="138" t="s">
         <v>1116</v>
       </c>
-      <c r="F19" s="140" t="s">
+      <c r="F19" s="138" t="s">
         <v>1116</v>
       </c>
-      <c r="G19" s="140" t="s">
+      <c r="G19" s="138" t="s">
         <v>1909</v>
       </c>
-      <c r="H19" s="140" t="s">
+      <c r="H19" s="138" t="s">
         <v>1910</v>
       </c>
     </row>
@@ -28892,24 +29017,24 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A23" s="140" t="s">
+      <c r="A23" s="138" t="s">
         <v>1912</v>
       </c>
-      <c r="B23" s="140"/>
-      <c r="C23" s="140"/>
-      <c r="D23" s="140" t="s">
+      <c r="B23" s="138"/>
+      <c r="C23" s="138"/>
+      <c r="D23" s="138" t="s">
         <v>946</v>
       </c>
-      <c r="E23" s="140" t="s">
+      <c r="E23" s="138" t="s">
         <v>946</v>
       </c>
-      <c r="F23" s="140" t="s">
+      <c r="F23" s="138" t="s">
         <v>946</v>
       </c>
-      <c r="G23" s="140" t="s">
+      <c r="G23" s="138" t="s">
         <v>1913</v>
       </c>
-      <c r="H23" s="140" t="s">
+      <c r="H23" s="138" t="s">
         <v>1914</v>
       </c>
     </row>
@@ -28980,24 +29105,24 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A27" s="140" t="s">
+      <c r="A27" s="138" t="s">
         <v>1636</v>
       </c>
-      <c r="B27" s="140"/>
-      <c r="C27" s="140"/>
-      <c r="D27" s="140" t="s">
+      <c r="B27" s="138"/>
+      <c r="C27" s="138"/>
+      <c r="D27" s="138" t="s">
         <v>1170</v>
       </c>
-      <c r="E27" s="140" t="s">
+      <c r="E27" s="138" t="s">
         <v>1170</v>
       </c>
-      <c r="F27" s="140" t="s">
+      <c r="F27" s="138" t="s">
         <v>1170</v>
       </c>
-      <c r="G27" s="140" t="s">
+      <c r="G27" s="138" t="s">
         <v>1919</v>
       </c>
-      <c r="H27" s="140" t="s">
+      <c r="H27" s="138" t="s">
         <v>1920</v>
       </c>
     </row>
@@ -29112,24 +29237,24 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A33" s="140" t="s">
+      <c r="A33" s="138" t="s">
         <v>1648</v>
       </c>
-      <c r="B33" s="140"/>
-      <c r="C33" s="140"/>
-      <c r="D33" s="140" t="s">
+      <c r="B33" s="138"/>
+      <c r="C33" s="138"/>
+      <c r="D33" s="138" t="s">
         <v>941</v>
       </c>
-      <c r="E33" s="140" t="s">
+      <c r="E33" s="138" t="s">
         <v>941</v>
       </c>
-      <c r="F33" s="140" t="s">
+      <c r="F33" s="138" t="s">
         <v>941</v>
       </c>
-      <c r="G33" s="140" t="s">
+      <c r="G33" s="138" t="s">
         <v>1922</v>
       </c>
-      <c r="H33" s="140" t="s">
+      <c r="H33" s="138" t="s">
         <v>1923</v>
       </c>
     </row>
@@ -29178,24 +29303,24 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A36" s="140" t="s">
+      <c r="A36" s="138" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="140"/>
-      <c r="C36" s="140"/>
-      <c r="D36" s="140" t="s">
+      <c r="B36" s="138"/>
+      <c r="C36" s="138"/>
+      <c r="D36" s="138" t="s">
         <v>40</v>
       </c>
-      <c r="E36" s="140" t="s">
+      <c r="E36" s="138" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="140" t="s">
+      <c r="F36" s="138" t="s">
         <v>40</v>
       </c>
-      <c r="G36" s="140" t="s">
+      <c r="G36" s="138" t="s">
         <v>41</v>
       </c>
-      <c r="H36" s="140" t="s">
+      <c r="H36" s="138" t="s">
         <v>42</v>
       </c>
     </row>
@@ -29364,24 +29489,24 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="140" t="s">
+      <c r="A44" s="138" t="s">
         <v>60</v>
       </c>
-      <c r="B44" s="140"/>
-      <c r="C44" s="140"/>
-      <c r="D44" s="140" t="s">
+      <c r="B44" s="138"/>
+      <c r="C44" s="138"/>
+      <c r="D44" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="140" t="s">
+      <c r="E44" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="F44" s="140" t="s">
+      <c r="F44" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="G44" s="140" t="s">
+      <c r="G44" s="138" t="s">
         <v>62</v>
       </c>
-      <c r="H44" s="140" t="s">
+      <c r="H44" s="138" t="s">
         <v>63</v>
       </c>
     </row>
@@ -29474,24 +29599,24 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A49" s="140" t="s">
+      <c r="A49" s="138" t="s">
         <v>78</v>
       </c>
-      <c r="B49" s="140"/>
-      <c r="C49" s="140"/>
-      <c r="D49" s="140" t="s">
+      <c r="B49" s="138"/>
+      <c r="C49" s="138"/>
+      <c r="D49" s="138" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="140" t="s">
+      <c r="E49" s="138" t="s">
         <v>79</v>
       </c>
-      <c r="F49" s="140" t="s">
+      <c r="F49" s="138" t="s">
         <v>79</v>
       </c>
-      <c r="G49" s="140" t="s">
+      <c r="G49" s="138" t="s">
         <v>80</v>
       </c>
-      <c r="H49" s="140" t="s">
+      <c r="H49" s="138" t="s">
         <v>81</v>
       </c>
     </row>
@@ -29650,24 +29775,24 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A57" s="140" t="s">
+      <c r="A57" s="138" t="s">
         <v>105</v>
       </c>
-      <c r="B57" s="140"/>
-      <c r="C57" s="140"/>
-      <c r="D57" s="140" t="s">
+      <c r="B57" s="138"/>
+      <c r="C57" s="138"/>
+      <c r="D57" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="E57" s="140" t="s">
+      <c r="E57" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="F57" s="140" t="s">
+      <c r="F57" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="G57" s="140" t="s">
+      <c r="G57" s="138" t="s">
         <v>107</v>
       </c>
-      <c r="H57" s="140" t="s">
+      <c r="H57" s="138" t="s">
         <v>108</v>
       </c>
     </row>
@@ -29738,24 +29863,24 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A61" s="140" t="s">
+      <c r="A61" s="138" t="s">
         <v>118</v>
       </c>
-      <c r="B61" s="140"/>
-      <c r="C61" s="140"/>
-      <c r="D61" s="140" t="s">
+      <c r="B61" s="138"/>
+      <c r="C61" s="138"/>
+      <c r="D61" s="138" t="s">
         <v>119</v>
       </c>
-      <c r="E61" s="140" t="s">
+      <c r="E61" s="138" t="s">
         <v>119</v>
       </c>
-      <c r="F61" s="140" t="s">
+      <c r="F61" s="138" t="s">
         <v>119</v>
       </c>
-      <c r="G61" s="140" t="s">
+      <c r="G61" s="138" t="s">
         <v>120</v>
       </c>
-      <c r="H61" s="140" t="s">
+      <c r="H61" s="138" t="s">
         <v>121</v>
       </c>
     </row>
@@ -30518,24 +30643,24 @@
       </c>
     </row>
     <row r="96" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A96" s="140" t="s">
+      <c r="A96" s="138" t="s">
         <v>194</v>
       </c>
-      <c r="B96" s="140"/>
-      <c r="C96" s="140"/>
-      <c r="D96" s="140" t="s">
+      <c r="B96" s="138"/>
+      <c r="C96" s="138"/>
+      <c r="D96" s="138" t="s">
         <v>195</v>
       </c>
-      <c r="E96" s="140" t="s">
+      <c r="E96" s="138" t="s">
         <v>195</v>
       </c>
-      <c r="F96" s="140" t="s">
+      <c r="F96" s="138" t="s">
         <v>195</v>
       </c>
-      <c r="G96" s="140" t="s">
+      <c r="G96" s="138" t="s">
         <v>196</v>
       </c>
-      <c r="H96" s="140" t="s">
+      <c r="H96" s="138" t="s">
         <v>197</v>
       </c>
     </row>
@@ -30584,24 +30709,24 @@
       </c>
     </row>
     <row r="99" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A99" s="140" t="s">
+      <c r="A99" s="138" t="s">
         <v>201</v>
       </c>
-      <c r="B99" s="140"/>
-      <c r="C99" s="140"/>
-      <c r="D99" s="140" t="s">
+      <c r="B99" s="138"/>
+      <c r="C99" s="138"/>
+      <c r="D99" s="138" t="s">
         <v>202</v>
       </c>
-      <c r="E99" s="140" t="s">
+      <c r="E99" s="138" t="s">
         <v>202</v>
       </c>
-      <c r="F99" s="140" t="s">
+      <c r="F99" s="138" t="s">
         <v>202</v>
       </c>
-      <c r="G99" s="140" t="s">
+      <c r="G99" s="138" t="s">
         <v>203</v>
       </c>
-      <c r="H99" s="140" t="s">
+      <c r="H99" s="138" t="s">
         <v>204</v>
       </c>
     </row>
@@ -30652,24 +30777,24 @@
       </c>
     </row>
     <row r="102" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A102" s="140" t="s">
+      <c r="A102" s="138" t="s">
         <v>208</v>
       </c>
-      <c r="B102" s="140"/>
-      <c r="C102" s="140"/>
-      <c r="D102" s="140" t="s">
+      <c r="B102" s="138"/>
+      <c r="C102" s="138"/>
+      <c r="D102" s="138" t="s">
         <v>209</v>
       </c>
-      <c r="E102" s="140" t="s">
+      <c r="E102" s="138" t="s">
         <v>209</v>
       </c>
-      <c r="F102" s="140" t="s">
+      <c r="F102" s="138" t="s">
         <v>209</v>
       </c>
-      <c r="G102" s="140" t="s">
+      <c r="G102" s="138" t="s">
         <v>210</v>
       </c>
-      <c r="H102" s="140" t="s">
+      <c r="H102" s="138" t="s">
         <v>211</v>
       </c>
     </row>
@@ -30740,24 +30865,24 @@
       </c>
     </row>
     <row r="106" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A106" s="140" t="s">
+      <c r="A106" s="138" t="s">
         <v>221</v>
       </c>
-      <c r="B106" s="140"/>
-      <c r="C106" s="140"/>
-      <c r="D106" s="140" t="s">
+      <c r="B106" s="138"/>
+      <c r="C106" s="138"/>
+      <c r="D106" s="138" t="s">
         <v>222</v>
       </c>
-      <c r="E106" s="140" t="s">
+      <c r="E106" s="138" t="s">
         <v>222</v>
       </c>
-      <c r="F106" s="140" t="s">
+      <c r="F106" s="138" t="s">
         <v>222</v>
       </c>
-      <c r="G106" s="140" t="s">
+      <c r="G106" s="138" t="s">
         <v>223</v>
       </c>
-      <c r="H106" s="140" t="s">
+      <c r="H106" s="138" t="s">
         <v>224</v>
       </c>
     </row>
@@ -30806,24 +30931,24 @@
       </c>
     </row>
     <row r="109" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A109" s="140" t="s">
+      <c r="A109" s="138" t="s">
         <v>231</v>
       </c>
-      <c r="B109" s="140"/>
-      <c r="C109" s="140"/>
-      <c r="D109" s="140" t="s">
+      <c r="B109" s="138"/>
+      <c r="C109" s="138"/>
+      <c r="D109" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="E109" s="140" t="s">
+      <c r="E109" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="F109" s="140" t="s">
+      <c r="F109" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="G109" s="140" t="s">
+      <c r="G109" s="138" t="s">
         <v>233</v>
       </c>
-      <c r="H109" s="140" t="s">
+      <c r="H109" s="138" t="s">
         <v>234</v>
       </c>
     </row>
@@ -30872,24 +30997,24 @@
       </c>
     </row>
     <row r="112" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A112" s="140" t="s">
+      <c r="A112" s="138" t="s">
         <v>240</v>
       </c>
-      <c r="B112" s="140"/>
-      <c r="C112" s="140"/>
-      <c r="D112" s="140" t="s">
+      <c r="B112" s="138"/>
+      <c r="C112" s="138"/>
+      <c r="D112" s="138" t="s">
         <v>241</v>
       </c>
-      <c r="E112" s="140" t="s">
+      <c r="E112" s="138" t="s">
         <v>241</v>
       </c>
-      <c r="F112" s="140" t="s">
+      <c r="F112" s="138" t="s">
         <v>241</v>
       </c>
-      <c r="G112" s="140" t="s">
+      <c r="G112" s="138" t="s">
         <v>242</v>
       </c>
-      <c r="H112" s="140" t="s">
+      <c r="H112" s="138" t="s">
         <v>243</v>
       </c>
     </row>
@@ -30982,24 +31107,24 @@
       </c>
     </row>
     <row r="117" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A117" s="140" t="s">
+      <c r="A117" s="138" t="s">
         <v>256</v>
       </c>
-      <c r="B117" s="140"/>
-      <c r="C117" s="140"/>
-      <c r="D117" s="140" t="s">
+      <c r="B117" s="138"/>
+      <c r="C117" s="138"/>
+      <c r="D117" s="138" t="s">
         <v>257</v>
       </c>
-      <c r="E117" s="140" t="s">
+      <c r="E117" s="138" t="s">
         <v>257</v>
       </c>
-      <c r="F117" s="140" t="s">
+      <c r="F117" s="138" t="s">
         <v>257</v>
       </c>
-      <c r="G117" s="140" t="s">
+      <c r="G117" s="138" t="s">
         <v>258</v>
       </c>
-      <c r="H117" s="140" t="s">
+      <c r="H117" s="138" t="s">
         <v>259</v>
       </c>
     </row>
@@ -31180,24 +31305,24 @@
       </c>
     </row>
     <row r="126" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A126" s="140" t="s">
+      <c r="A126" s="138" t="s">
         <v>1690</v>
       </c>
-      <c r="B126" s="140"/>
-      <c r="C126" s="140"/>
-      <c r="D126" s="140" t="s">
+      <c r="B126" s="138"/>
+      <c r="C126" s="138"/>
+      <c r="D126" s="138" t="s">
         <v>1691</v>
       </c>
-      <c r="E126" s="140" t="s">
+      <c r="E126" s="138" t="s">
         <v>1691</v>
       </c>
-      <c r="F126" s="140" t="s">
+      <c r="F126" s="138" t="s">
         <v>1691</v>
       </c>
-      <c r="G126" s="140" t="s">
+      <c r="G126" s="138" t="s">
         <v>1978</v>
       </c>
-      <c r="H126" s="140" t="s">
+      <c r="H126" s="138" t="s">
         <v>1979</v>
       </c>
     </row>
@@ -31246,24 +31371,24 @@
       </c>
     </row>
     <row r="129" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A129" s="140" t="s">
+      <c r="A129" s="138" t="s">
         <v>1980</v>
       </c>
-      <c r="B129" s="140"/>
-      <c r="C129" s="140"/>
-      <c r="D129" s="140" t="s">
+      <c r="B129" s="138"/>
+      <c r="C129" s="138"/>
+      <c r="D129" s="138" t="s">
         <v>981</v>
       </c>
-      <c r="E129" s="140" t="s">
+      <c r="E129" s="138" t="s">
         <v>981</v>
       </c>
-      <c r="F129" s="140" t="s">
+      <c r="F129" s="138" t="s">
         <v>981</v>
       </c>
-      <c r="G129" s="140" t="s">
+      <c r="G129" s="138" t="s">
         <v>1981</v>
       </c>
-      <c r="H129" s="140" t="s">
+      <c r="H129" s="138" t="s">
         <v>1982</v>
       </c>
     </row>
@@ -31356,24 +31481,24 @@
       </c>
     </row>
     <row r="134" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A134" s="140" t="s">
+      <c r="A134" s="138" t="s">
         <v>1992</v>
       </c>
-      <c r="B134" s="140"/>
-      <c r="C134" s="140"/>
-      <c r="D134" s="140" t="s">
+      <c r="B134" s="138"/>
+      <c r="C134" s="138"/>
+      <c r="D134" s="138" t="s">
         <v>1993</v>
       </c>
-      <c r="E134" s="140" t="s">
+      <c r="E134" s="138" t="s">
         <v>1993</v>
       </c>
-      <c r="F134" s="140" t="s">
+      <c r="F134" s="138" t="s">
         <v>1993</v>
       </c>
-      <c r="G134" s="140" t="s">
+      <c r="G134" s="138" t="s">
         <v>1994</v>
       </c>
-      <c r="H134" s="140" t="s">
+      <c r="H134" s="138" t="s">
         <v>1995</v>
       </c>
     </row>
@@ -31400,24 +31525,24 @@
       </c>
     </row>
     <row r="136" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A136" s="140" t="s">
+      <c r="A136" s="138" t="s">
         <v>1999</v>
       </c>
-      <c r="B136" s="140"/>
-      <c r="C136" s="140"/>
-      <c r="D136" s="140" t="s">
+      <c r="B136" s="138"/>
+      <c r="C136" s="138"/>
+      <c r="D136" s="138" t="s">
         <v>1171</v>
       </c>
-      <c r="E136" s="140" t="s">
+      <c r="E136" s="138" t="s">
         <v>1171</v>
       </c>
-      <c r="F136" s="140" t="s">
+      <c r="F136" s="138" t="s">
         <v>1171</v>
       </c>
-      <c r="G136" s="140" t="s">
+      <c r="G136" s="138" t="s">
         <v>2000</v>
       </c>
-      <c r="H136" s="140" t="s">
+      <c r="H136" s="138" t="s">
         <v>2001</v>
       </c>
     </row>
@@ -31466,24 +31591,24 @@
       </c>
     </row>
     <row r="139" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A139" s="140" t="s">
+      <c r="A139" s="138" t="s">
         <v>267</v>
       </c>
-      <c r="B139" s="140"/>
-      <c r="C139" s="140"/>
-      <c r="D139" s="140" t="s">
+      <c r="B139" s="138"/>
+      <c r="C139" s="138"/>
+      <c r="D139" s="138" t="s">
         <v>268</v>
       </c>
-      <c r="E139" s="140" t="s">
+      <c r="E139" s="138" t="s">
         <v>268</v>
       </c>
-      <c r="F139" s="140" t="s">
+      <c r="F139" s="138" t="s">
         <v>268</v>
       </c>
-      <c r="G139" s="140" t="s">
+      <c r="G139" s="138" t="s">
         <v>269</v>
       </c>
-      <c r="H139" s="140" t="s">
+      <c r="H139" s="138" t="s">
         <v>270</v>
       </c>
     </row>
@@ -31602,24 +31727,24 @@
       </c>
     </row>
     <row r="145" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A145" s="140" t="s">
+      <c r="A145" s="138" t="s">
         <v>286</v>
       </c>
-      <c r="B145" s="140"/>
-      <c r="C145" s="140"/>
-      <c r="D145" s="140" t="s">
+      <c r="B145" s="138"/>
+      <c r="C145" s="138"/>
+      <c r="D145" s="138" t="s">
         <v>287</v>
       </c>
-      <c r="E145" s="140" t="s">
+      <c r="E145" s="138" t="s">
         <v>287</v>
       </c>
-      <c r="F145" s="140" t="s">
+      <c r="F145" s="138" t="s">
         <v>287</v>
       </c>
-      <c r="G145" s="140" t="s">
+      <c r="G145" s="138" t="s">
         <v>288</v>
       </c>
-      <c r="H145" s="140" t="s">
+      <c r="H145" s="138" t="s">
         <v>289</v>
       </c>
     </row>
@@ -31812,24 +31937,24 @@
       </c>
     </row>
     <row r="154" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A154" s="140" t="s">
+      <c r="A154" s="138" t="s">
         <v>302</v>
       </c>
-      <c r="B154" s="140"/>
-      <c r="C154" s="140"/>
-      <c r="D154" s="140" t="s">
+      <c r="B154" s="138"/>
+      <c r="C154" s="138"/>
+      <c r="D154" s="138" t="s">
         <v>303</v>
       </c>
-      <c r="E154" s="140" t="s">
+      <c r="E154" s="138" t="s">
         <v>303</v>
       </c>
-      <c r="F154" s="140" t="s">
+      <c r="F154" s="138" t="s">
         <v>303</v>
       </c>
-      <c r="G154" s="140" t="s">
+      <c r="G154" s="138" t="s">
         <v>304</v>
       </c>
-      <c r="H154" s="140" t="s">
+      <c r="H154" s="138" t="s">
         <v>305</v>
       </c>
     </row>
@@ -31952,24 +32077,24 @@
       </c>
     </row>
     <row r="160" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A160" s="140" t="s">
+      <c r="A160" s="138" t="s">
         <v>310</v>
       </c>
-      <c r="B160" s="140"/>
-      <c r="C160" s="140"/>
-      <c r="D160" s="140" t="s">
+      <c r="B160" s="138"/>
+      <c r="C160" s="138"/>
+      <c r="D160" s="138" t="s">
         <v>311</v>
       </c>
-      <c r="E160" s="140" t="s">
+      <c r="E160" s="138" t="s">
         <v>311</v>
       </c>
-      <c r="F160" s="140" t="s">
+      <c r="F160" s="138" t="s">
         <v>311</v>
       </c>
-      <c r="G160" s="140" t="s">
+      <c r="G160" s="138" t="s">
         <v>312</v>
       </c>
-      <c r="H160" s="140" t="s">
+      <c r="H160" s="138" t="s">
         <v>313</v>
       </c>
     </row>
@@ -32062,24 +32187,24 @@
       </c>
     </row>
     <row r="165" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A165" s="140" t="s">
+      <c r="A165" s="138" t="s">
         <v>320</v>
       </c>
-      <c r="B165" s="140"/>
-      <c r="C165" s="140"/>
-      <c r="D165" s="140" t="s">
+      <c r="B165" s="138"/>
+      <c r="C165" s="138"/>
+      <c r="D165" s="138" t="s">
         <v>321</v>
       </c>
-      <c r="E165" s="140" t="s">
+      <c r="E165" s="138" t="s">
         <v>321</v>
       </c>
-      <c r="F165" s="140" t="s">
+      <c r="F165" s="138" t="s">
         <v>321</v>
       </c>
-      <c r="G165" s="140" t="s">
+      <c r="G165" s="138" t="s">
         <v>322</v>
       </c>
-      <c r="H165" s="140" t="s">
+      <c r="H165" s="138" t="s">
         <v>323</v>
       </c>
     </row>
@@ -32194,24 +32319,24 @@
       </c>
     </row>
     <row r="171" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A171" s="140" t="s">
+      <c r="A171" s="138" t="s">
         <v>341</v>
       </c>
-      <c r="B171" s="140"/>
-      <c r="C171" s="140"/>
-      <c r="D171" s="140" t="s">
+      <c r="B171" s="138"/>
+      <c r="C171" s="138"/>
+      <c r="D171" s="138" t="s">
         <v>342</v>
       </c>
-      <c r="E171" s="140" t="s">
+      <c r="E171" s="138" t="s">
         <v>342</v>
       </c>
-      <c r="F171" s="140" t="s">
+      <c r="F171" s="138" t="s">
         <v>342</v>
       </c>
-      <c r="G171" s="140" t="s">
+      <c r="G171" s="138" t="s">
         <v>343</v>
       </c>
-      <c r="H171" s="140" t="s">
+      <c r="H171" s="138" t="s">
         <v>344</v>
       </c>
     </row>
@@ -32238,24 +32363,24 @@
       </c>
     </row>
     <row r="173" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A173" s="140" t="s">
+      <c r="A173" s="138" t="s">
         <v>345</v>
       </c>
-      <c r="B173" s="140"/>
-      <c r="C173" s="140"/>
-      <c r="D173" s="140" t="s">
+      <c r="B173" s="138"/>
+      <c r="C173" s="138"/>
+      <c r="D173" s="138" t="s">
         <v>346</v>
       </c>
-      <c r="E173" s="140" t="s">
+      <c r="E173" s="138" t="s">
         <v>346</v>
       </c>
-      <c r="F173" s="140" t="s">
+      <c r="F173" s="138" t="s">
         <v>346</v>
       </c>
-      <c r="G173" s="140" t="s">
+      <c r="G173" s="138" t="s">
         <v>347</v>
       </c>
-      <c r="H173" s="140" t="s">
+      <c r="H173" s="138" t="s">
         <v>348</v>
       </c>
     </row>
@@ -32438,24 +32563,24 @@
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A182" s="140" t="s">
+      <c r="A182" s="138" t="s">
         <v>1736</v>
       </c>
-      <c r="B182" s="140"/>
-      <c r="C182" s="140"/>
-      <c r="D182" s="140" t="s">
+      <c r="B182" s="138"/>
+      <c r="C182" s="138"/>
+      <c r="D182" s="138" t="s">
         <v>1109</v>
       </c>
-      <c r="E182" s="140" t="s">
+      <c r="E182" s="138" t="s">
         <v>1109</v>
       </c>
-      <c r="F182" s="140" t="s">
+      <c r="F182" s="138" t="s">
         <v>1109</v>
       </c>
-      <c r="G182" s="140" t="s">
+      <c r="G182" s="138" t="s">
         <v>2034</v>
       </c>
-      <c r="H182" s="140" t="s">
+      <c r="H182" s="138" t="s">
         <v>2035</v>
       </c>
     </row>
@@ -32614,24 +32739,24 @@
       </c>
     </row>
     <row r="190" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A190" s="140" t="s">
+      <c r="A190" s="138" t="s">
         <v>374</v>
       </c>
-      <c r="B190" s="140"/>
-      <c r="C190" s="140"/>
-      <c r="D190" s="140" t="s">
+      <c r="B190" s="138"/>
+      <c r="C190" s="138"/>
+      <c r="D190" s="138" t="s">
         <v>375</v>
       </c>
-      <c r="E190" s="140" t="s">
+      <c r="E190" s="138" t="s">
         <v>375</v>
       </c>
-      <c r="F190" s="140" t="s">
+      <c r="F190" s="138" t="s">
         <v>375</v>
       </c>
-      <c r="G190" s="140" t="s">
+      <c r="G190" s="138" t="s">
         <v>376</v>
       </c>
-      <c r="H190" s="140" t="s">
+      <c r="H190" s="138" t="s">
         <v>377</v>
       </c>
     </row>
@@ -32658,24 +32783,24 @@
       </c>
     </row>
     <row r="192" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A192" s="140" t="s">
+      <c r="A192" s="138" t="s">
         <v>381</v>
       </c>
-      <c r="B192" s="140"/>
-      <c r="C192" s="140"/>
-      <c r="D192" s="140" t="s">
+      <c r="B192" s="138"/>
+      <c r="C192" s="138"/>
+      <c r="D192" s="138" t="s">
         <v>382</v>
       </c>
-      <c r="E192" s="140" t="s">
+      <c r="E192" s="138" t="s">
         <v>382</v>
       </c>
-      <c r="F192" s="140" t="s">
+      <c r="F192" s="138" t="s">
         <v>382</v>
       </c>
-      <c r="G192" s="140" t="s">
+      <c r="G192" s="138" t="s">
         <v>383</v>
       </c>
-      <c r="H192" s="140" t="s">
+      <c r="H192" s="138" t="s">
         <v>384</v>
       </c>
     </row>
@@ -32702,24 +32827,24 @@
       </c>
     </row>
     <row r="194" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A194" s="140" t="s">
+      <c r="A194" s="138" t="s">
         <v>388</v>
       </c>
-      <c r="B194" s="140"/>
-      <c r="C194" s="140"/>
-      <c r="D194" s="140" t="s">
+      <c r="B194" s="138"/>
+      <c r="C194" s="138"/>
+      <c r="D194" s="138" t="s">
         <v>389</v>
       </c>
-      <c r="E194" s="140" t="s">
+      <c r="E194" s="138" t="s">
         <v>389</v>
       </c>
-      <c r="F194" s="140" t="s">
+      <c r="F194" s="138" t="s">
         <v>389</v>
       </c>
-      <c r="G194" s="140" t="s">
+      <c r="G194" s="138" t="s">
         <v>390</v>
       </c>
-      <c r="H194" s="140" t="s">
+      <c r="H194" s="138" t="s">
         <v>391</v>
       </c>
     </row>
@@ -32790,26 +32915,26 @@
       </c>
     </row>
     <row r="198" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A198" s="140" t="s">
+      <c r="A198" s="138" t="s">
         <v>401</v>
       </c>
-      <c r="B198" s="140"/>
-      <c r="C198" s="140" t="s">
+      <c r="B198" s="138"/>
+      <c r="C198" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="D198" s="140" t="s">
+      <c r="D198" s="138" t="s">
         <v>95</v>
       </c>
-      <c r="E198" s="140" t="s">
+      <c r="E198" s="138" t="s">
         <v>402</v>
       </c>
-      <c r="F198" s="140" t="s">
+      <c r="F198" s="138" t="s">
         <v>95</v>
       </c>
-      <c r="G198" s="140" t="s">
+      <c r="G198" s="138" t="s">
         <v>403</v>
       </c>
-      <c r="H198" s="140" t="s">
+      <c r="H198" s="138" t="s">
         <v>404</v>
       </c>
     </row>
@@ -33210,26 +33335,26 @@
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A217" s="140" t="s">
+      <c r="A217" s="138" t="s">
         <v>477</v>
       </c>
-      <c r="B217" s="140"/>
-      <c r="C217" s="140" t="s">
+      <c r="B217" s="138"/>
+      <c r="C217" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="D217" s="140" t="s">
+      <c r="D217" s="138" t="s">
         <v>478</v>
       </c>
-      <c r="E217" s="140" t="s">
+      <c r="E217" s="138" t="s">
         <v>479</v>
       </c>
-      <c r="F217" s="140" t="s">
+      <c r="F217" s="138" t="s">
         <v>478</v>
       </c>
-      <c r="G217" s="140" t="s">
+      <c r="G217" s="138" t="s">
         <v>480</v>
       </c>
-      <c r="H217" s="140" t="s">
+      <c r="H217" s="138" t="s">
         <v>481</v>
       </c>
     </row>
@@ -33524,26 +33649,26 @@
       </c>
     </row>
     <row r="231" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A231" s="140" t="s">
+      <c r="A231" s="138" t="s">
         <v>528</v>
       </c>
-      <c r="B231" s="140"/>
-      <c r="C231" s="140" t="s">
+      <c r="B231" s="138"/>
+      <c r="C231" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="D231" s="140" t="s">
+      <c r="D231" s="138" t="s">
         <v>529</v>
       </c>
-      <c r="E231" s="140" t="s">
+      <c r="E231" s="138" t="s">
         <v>530</v>
       </c>
-      <c r="F231" s="140" t="s">
+      <c r="F231" s="138" t="s">
         <v>529</v>
       </c>
-      <c r="G231" s="140" t="s">
+      <c r="G231" s="138" t="s">
         <v>531</v>
       </c>
-      <c r="H231" s="140" t="s">
+      <c r="H231" s="138" t="s">
         <v>532</v>
       </c>
     </row>
@@ -33658,26 +33783,26 @@
       </c>
     </row>
     <row r="237" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A237" s="140" t="s">
+      <c r="A237" s="138" t="s">
         <v>553</v>
       </c>
-      <c r="B237" s="140"/>
-      <c r="C237" s="140" t="s">
+      <c r="B237" s="138"/>
+      <c r="C237" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="D237" s="140" t="s">
+      <c r="D237" s="138" t="s">
         <v>554</v>
       </c>
-      <c r="E237" s="140" t="s">
+      <c r="E237" s="138" t="s">
         <v>555</v>
       </c>
-      <c r="F237" s="140" t="s">
+      <c r="F237" s="138" t="s">
         <v>554</v>
       </c>
-      <c r="G237" s="140" t="s">
+      <c r="G237" s="138" t="s">
         <v>556</v>
       </c>
-      <c r="H237" s="140" t="s">
+      <c r="H237" s="138" t="s">
         <v>557</v>
       </c>
     </row>
@@ -33886,24 +34011,24 @@
       </c>
     </row>
     <row r="247" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A247" s="140" t="s">
+      <c r="A247" s="138" t="s">
         <v>583</v>
       </c>
-      <c r="B247" s="140"/>
-      <c r="C247" s="140"/>
-      <c r="D247" s="140" t="s">
+      <c r="B247" s="138"/>
+      <c r="C247" s="138"/>
+      <c r="D247" s="138" t="s">
         <v>584</v>
       </c>
-      <c r="E247" s="140" t="s">
+      <c r="E247" s="138" t="s">
         <v>584</v>
       </c>
-      <c r="F247" s="140" t="s">
+      <c r="F247" s="138" t="s">
         <v>584</v>
       </c>
-      <c r="G247" s="140" t="s">
+      <c r="G247" s="138" t="s">
         <v>585</v>
       </c>
-      <c r="H247" s="140" t="s">
+      <c r="H247" s="138" t="s">
         <v>586</v>
       </c>
     </row>
@@ -33956,24 +34081,24 @@
       </c>
     </row>
     <row r="250" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A250" s="140" t="s">
+      <c r="A250" s="138" t="s">
         <v>597</v>
       </c>
-      <c r="B250" s="140"/>
-      <c r="C250" s="140"/>
-      <c r="D250" s="140" t="s">
+      <c r="B250" s="138"/>
+      <c r="C250" s="138"/>
+      <c r="D250" s="138" t="s">
         <v>598</v>
       </c>
-      <c r="E250" s="140" t="s">
+      <c r="E250" s="138" t="s">
         <v>598</v>
       </c>
-      <c r="F250" s="140" t="s">
+      <c r="F250" s="138" t="s">
         <v>598</v>
       </c>
-      <c r="G250" s="140" t="s">
+      <c r="G250" s="138" t="s">
         <v>599</v>
       </c>
-      <c r="H250" s="140" t="s">
+      <c r="H250" s="138" t="s">
         <v>600</v>
       </c>
     </row>
@@ -34048,24 +34173,24 @@
       </c>
     </row>
     <row r="254" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A254" s="140" t="s">
+      <c r="A254" s="138" t="s">
         <v>612</v>
       </c>
-      <c r="B254" s="140"/>
-      <c r="C254" s="140"/>
-      <c r="D254" s="140" t="s">
+      <c r="B254" s="138"/>
+      <c r="C254" s="138"/>
+      <c r="D254" s="138" t="s">
         <v>613</v>
       </c>
-      <c r="E254" s="140" t="s">
+      <c r="E254" s="138" t="s">
         <v>613</v>
       </c>
-      <c r="F254" s="140" t="s">
+      <c r="F254" s="138" t="s">
         <v>613</v>
       </c>
-      <c r="G254" s="140" t="s">
+      <c r="G254" s="138" t="s">
         <v>614</v>
       </c>
-      <c r="H254" s="140" t="s">
+      <c r="H254" s="138" t="s">
         <v>615</v>
       </c>
     </row>
@@ -34182,26 +34307,26 @@
       </c>
     </row>
     <row r="260" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A260" s="140" t="s">
+      <c r="A260" s="138" t="s">
         <v>2055</v>
       </c>
-      <c r="B260" s="140"/>
-      <c r="C260" s="140" t="s">
+      <c r="B260" s="138"/>
+      <c r="C260" s="138" t="s">
         <v>8</v>
       </c>
-      <c r="D260" s="140" t="s">
+      <c r="D260" s="138" t="s">
         <v>2056</v>
       </c>
-      <c r="E260" s="140" t="s">
+      <c r="E260" s="138" t="s">
         <v>2057</v>
       </c>
-      <c r="F260" s="140" t="s">
+      <c r="F260" s="138" t="s">
         <v>2056</v>
       </c>
-      <c r="G260" s="140" t="s">
+      <c r="G260" s="138" t="s">
         <v>2058</v>
       </c>
-      <c r="H260" s="140" t="s">
+      <c r="H260" s="138" t="s">
         <v>2059</v>
       </c>
     </row>
@@ -34276,24 +34401,24 @@
       </c>
     </row>
     <row r="264" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A264" s="140" t="s">
+      <c r="A264" s="138" t="s">
         <v>633</v>
       </c>
-      <c r="B264" s="140"/>
-      <c r="C264" s="140"/>
-      <c r="D264" s="140" t="s">
+      <c r="B264" s="138"/>
+      <c r="C264" s="138"/>
+      <c r="D264" s="138" t="s">
         <v>634</v>
       </c>
-      <c r="E264" s="140" t="s">
+      <c r="E264" s="138" t="s">
         <v>634</v>
       </c>
-      <c r="F264" s="140" t="s">
+      <c r="F264" s="138" t="s">
         <v>634</v>
       </c>
-      <c r="G264" s="140" t="s">
+      <c r="G264" s="138" t="s">
         <v>635</v>
       </c>
-      <c r="H264" s="140" t="s">
+      <c r="H264" s="138" t="s">
         <v>636</v>
       </c>
     </row>
@@ -34408,24 +34533,24 @@
       </c>
     </row>
     <row r="270" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A270" s="140" t="s">
+      <c r="A270" s="138" t="s">
         <v>1370</v>
       </c>
-      <c r="B270" s="140"/>
-      <c r="C270" s="140"/>
-      <c r="D270" s="140" t="s">
+      <c r="B270" s="138"/>
+      <c r="C270" s="138"/>
+      <c r="D270" s="138" t="s">
         <v>2072</v>
       </c>
-      <c r="E270" s="140" t="s">
+      <c r="E270" s="138" t="s">
         <v>2072</v>
       </c>
-      <c r="F270" s="140" t="s">
+      <c r="F270" s="138" t="s">
         <v>2072</v>
       </c>
-      <c r="G270" s="140" t="s">
+      <c r="G270" s="138" t="s">
         <v>2073</v>
       </c>
-      <c r="H270" s="140" t="s">
+      <c r="H270" s="138" t="s">
         <v>2074</v>
       </c>
     </row>
@@ -34590,26 +34715,26 @@
       </c>
     </row>
     <row r="278" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A278" s="140" t="s">
+      <c r="A278" s="138" t="s">
         <v>653</v>
       </c>
-      <c r="B278" s="140"/>
-      <c r="C278" s="140" t="s">
+      <c r="B278" s="138"/>
+      <c r="C278" s="138" t="s">
         <v>8</v>
       </c>
-      <c r="D278" s="140" t="s">
+      <c r="D278" s="138" t="s">
         <v>654</v>
       </c>
-      <c r="E278" s="140" t="s">
+      <c r="E278" s="138" t="s">
         <v>655</v>
       </c>
-      <c r="F278" s="140" t="s">
+      <c r="F278" s="138" t="s">
         <v>654</v>
       </c>
-      <c r="G278" s="140" t="s">
+      <c r="G278" s="138" t="s">
         <v>656</v>
       </c>
-      <c r="H278" s="140" t="s">
+      <c r="H278" s="138" t="s">
         <v>657</v>
       </c>
     </row>
@@ -34704,24 +34829,24 @@
       </c>
     </row>
     <row r="283" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A283" s="140" t="s">
+      <c r="A283" s="138" t="s">
         <v>1845</v>
       </c>
-      <c r="B283" s="140"/>
-      <c r="C283" s="140"/>
-      <c r="D283" s="140" t="s">
+      <c r="B283" s="138"/>
+      <c r="C283" s="138"/>
+      <c r="D283" s="138" t="s">
         <v>2076</v>
       </c>
-      <c r="E283" s="140" t="s">
+      <c r="E283" s="138" t="s">
         <v>2076</v>
       </c>
-      <c r="F283" s="140" t="s">
+      <c r="F283" s="138" t="s">
         <v>2076</v>
       </c>
-      <c r="G283" s="140" t="s">
+      <c r="G283" s="138" t="s">
         <v>2077</v>
       </c>
-      <c r="H283" s="140" t="s">
+      <c r="H283" s="138" t="s">
         <v>2078</v>
       </c>
     </row>
@@ -34814,24 +34939,24 @@
       </c>
     </row>
     <row r="288" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A288" s="140" t="s">
+      <c r="A288" s="138" t="s">
         <v>2079</v>
       </c>
-      <c r="B288" s="140"/>
-      <c r="C288" s="140"/>
-      <c r="D288" s="140" t="s">
+      <c r="B288" s="138"/>
+      <c r="C288" s="138"/>
+      <c r="D288" s="138" t="s">
         <v>2080</v>
       </c>
-      <c r="E288" s="140" t="s">
+      <c r="E288" s="138" t="s">
         <v>2080</v>
       </c>
-      <c r="F288" s="140" t="s">
+      <c r="F288" s="138" t="s">
         <v>2080</v>
       </c>
-      <c r="G288" s="140" t="s">
+      <c r="G288" s="138" t="s">
         <v>2081</v>
       </c>
-      <c r="H288" s="140" t="s">
+      <c r="H288" s="138" t="s">
         <v>2082</v>
       </c>
     </row>
@@ -34902,26 +35027,26 @@
       </c>
     </row>
     <row r="292" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A292" s="140" t="s">
+      <c r="A292" s="138" t="s">
         <v>1844</v>
       </c>
-      <c r="B292" s="140"/>
-      <c r="C292" s="140" t="s">
+      <c r="B292" s="138"/>
+      <c r="C292" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="D292" s="140" t="s">
+      <c r="D292" s="138" t="s">
         <v>1877</v>
       </c>
-      <c r="E292" s="140" t="s">
+      <c r="E292" s="138" t="s">
         <v>2089</v>
       </c>
-      <c r="F292" s="140" t="s">
+      <c r="F292" s="138" t="s">
         <v>1877</v>
       </c>
-      <c r="G292" s="140" t="s">
+      <c r="G292" s="138" t="s">
         <v>2090</v>
       </c>
-      <c r="H292" s="140" t="s">
+      <c r="H292" s="138" t="s">
         <v>2091</v>
       </c>
     </row>
@@ -35040,26 +35165,26 @@
       </c>
     </row>
     <row r="298" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A298" s="140" t="s">
+      <c r="A298" s="138" t="s">
         <v>675</v>
       </c>
-      <c r="B298" s="140"/>
-      <c r="C298" s="140" t="s">
+      <c r="B298" s="138"/>
+      <c r="C298" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="D298" s="140" t="s">
+      <c r="D298" s="138" t="s">
         <v>676</v>
       </c>
-      <c r="E298" s="140" t="s">
+      <c r="E298" s="138" t="s">
         <v>677</v>
       </c>
-      <c r="F298" s="140" t="s">
+      <c r="F298" s="138" t="s">
         <v>676</v>
       </c>
-      <c r="G298" s="140" t="s">
+      <c r="G298" s="138" t="s">
         <v>678</v>
       </c>
-      <c r="H298" s="140" t="s">
+      <c r="H298" s="138" t="s">
         <v>679</v>
       </c>
     </row>
@@ -35312,26 +35437,26 @@
       </c>
     </row>
     <row r="310" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A310" s="140" t="s">
+      <c r="A310" s="138" t="s">
         <v>724</v>
       </c>
-      <c r="B310" s="140"/>
-      <c r="C310" s="140" t="s">
+      <c r="B310" s="138"/>
+      <c r="C310" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="D310" s="140" t="s">
+      <c r="D310" s="138" t="s">
         <v>725</v>
       </c>
-      <c r="E310" s="140" t="s">
+      <c r="E310" s="138" t="s">
         <v>726</v>
       </c>
-      <c r="F310" s="140" t="s">
+      <c r="F310" s="138" t="s">
         <v>725</v>
       </c>
-      <c r="G310" s="140" t="s">
+      <c r="G310" s="138" t="s">
         <v>727</v>
       </c>
-      <c r="H310" s="140" t="s">
+      <c r="H310" s="138" t="s">
         <v>728</v>
       </c>
     </row>
@@ -35744,26 +35869,26 @@
       </c>
     </row>
     <row r="328" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A328" s="140" t="s">
+      <c r="A328" s="138" t="s">
         <v>788</v>
       </c>
-      <c r="B328" s="140"/>
-      <c r="C328" s="140" t="s">
+      <c r="B328" s="138"/>
+      <c r="C328" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="D328" s="140" t="s">
+      <c r="D328" s="138" t="s">
         <v>789</v>
       </c>
-      <c r="E328" s="140" t="s">
+      <c r="E328" s="138" t="s">
         <v>790</v>
       </c>
-      <c r="F328" s="140" t="s">
+      <c r="F328" s="138" t="s">
         <v>789</v>
       </c>
-      <c r="G328" s="140" t="s">
+      <c r="G328" s="138" t="s">
         <v>791</v>
       </c>
-      <c r="H328" s="140" t="s">
+      <c r="H328" s="138" t="s">
         <v>792</v>
       </c>
     </row>
@@ -41039,9 +41164,9 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -41152,7 +41277,7 @@
       <c r="D3" s="75" t="s">
         <v>137</v>
       </c>
-      <c r="E3" s="141" t="s">
+      <c r="E3" s="139" t="s">
         <v>1338</v>
       </c>
       <c r="F3" s="16" t="s">
@@ -41226,7 +41351,7 @@
       <c r="D5" s="43" t="s">
         <v>914</v>
       </c>
-      <c r="E5" s="142" t="s">
+      <c r="E5" s="140" t="s">
         <v>2293</v>
       </c>
       <c r="F5" s="106" t="s">
@@ -41630,7 +41755,7 @@
       <c r="D17" s="88" t="s">
         <v>131</v>
       </c>
-      <c r="E17" s="143" t="s">
+      <c r="E17" s="141" t="s">
         <v>2488</v>
       </c>
       <c r="F17" s="85" t="s">
@@ -41737,7 +41862,7 @@
       </c>
       <c r="M20" s="13"/>
     </row>
-    <row r="21" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>2499</v>
       </c>
@@ -41767,10 +41892,150 @@
       <c r="K21" s="54" t="s">
         <v>2368</v>
       </c>
-      <c r="L21" s="144" t="s">
+      <c r="L21" s="16" t="s">
+        <v>2507</v>
+      </c>
+      <c r="M21" s="13"/>
+    </row>
+    <row r="22" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>2499</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>2503</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>2265</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>1338</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>2206</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>2188</v>
+      </c>
+      <c r="J22" s="13"/>
+      <c r="K22" s="16" t="s">
+        <v>2189</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>2508</v>
+      </c>
+      <c r="M22" s="13"/>
+    </row>
+    <row r="23" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>2499</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>2504</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>1470</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>1338</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>2206</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="15" t="s">
+        <v>913</v>
+      </c>
+      <c r="I23" s="54" t="s">
+        <v>1472</v>
+      </c>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L23" s="16" t="s">
         <v>2500</v>
       </c>
-      <c r="M21" s="13"/>
+      <c r="M23" s="13"/>
+    </row>
+    <row r="24" spans="1:13" ht="100" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>2499</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>2505</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>914</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>2132</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>2206</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>2367</v>
+      </c>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54" t="s">
+        <v>2368</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>2501</v>
+      </c>
+      <c r="M24" s="13"/>
+    </row>
+    <row r="25" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>2499</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>2506</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>1338</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>2206</v>
+      </c>
+      <c r="G25" s="13"/>
+      <c r="H25" s="15" t="s">
+        <v>913</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>1410</v>
+      </c>
+      <c r="J25" s="54"/>
+      <c r="K25" s="16" t="s">
+        <v>1411</v>
+      </c>
+      <c r="L25" s="16" t="s">
+        <v>2502</v>
+      </c>
+      <c r="M25" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
CT deliverable updates for post-PR sprint
CT deliverable updates for post-PR sprint
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C3ADCC-5CD7-4B6D-B1C7-32740B9E2501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B1FE23-8CF0-4164-9DB2-B4542208309C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="480" windowWidth="16590" windowHeight="9280" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2050" yWindow="780" windowWidth="16590" windowHeight="9280" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -14950,6 +14950,12 @@
     <t>Update Preferred Term and synonym of attribute in PopulationDefinition class</t>
   </si>
   <si>
+    <t>Sex of Participants; Sex of Study Subjects</t>
+  </si>
+  <si>
+    <t>Update definition of attribute in AdministrationDuration class</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <strike/>
@@ -14957,7 +14963,32 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Sex of Participants</t>
+      <t>The value representing the amount of time elapsed during the administration of an agent.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+The value representing the amount of time over which the administration of an agent occurs.</t>
+    </r>
+  </si>
+  <si>
+    <t>Update Definition</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The exploratory purpose of the trial.</t>
     </r>
     <r>
       <rPr>
@@ -14975,49 +15006,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Population Definition Planned Sex</t>
-    </r>
-  </si>
-  <si>
-    <t>Sex of Participants; Sex of Study Subjects</t>
-  </si>
-  <si>
-    <t>Update definition of attribute in AdministrationDuration class</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>The value representing the amount of time elapsed during the administration of an agent.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-The value representing the amount of time over which the administration of an agent occurs.</t>
-    </r>
-  </si>
-  <si>
-    <t>Update Definition</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>The exploratory purpose of the trial.</t>
+      <t>Additional scientific question(s) within the study that enable further discovery research, beyond the primary and secondary objectives.</t>
     </r>
     <r>
       <rPr>
@@ -15028,14 +15017,19 @@
       <t xml:space="preserve">
 </t>
     </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Additional scientific question(s) within the study that enable further discovery research, beyond the primary and secondary objectives.</t>
+  </si>
+  <si>
+    <t>Update Preferred term and Definition</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Study Primary Objective</t>
     </r>
     <r>
       <rPr>
@@ -15046,23 +15040,41 @@
       <t xml:space="preserve">
 </t>
     </r>
-  </si>
-  <si>
-    <t>Update Preferred term and Definition</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Primary Objective</t>
+    </r>
   </si>
   <si>
     <r>
       <rPr>
         <strike/>
         <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Study Primary Objective</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
+        <color rgb="FF444444"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A principle objective of the study.</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color rgb="FF172B4D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> {P378 : CDISC}"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444444"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -15076,7 +15088,25 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Primary Objective</t>
+      <t>The main scientific question(s) the study is designed to answer. [After ICH E8; ICH E6 6.3]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF444444"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(CDISC Glossary)</t>
     </r>
   </si>
   <si>
@@ -15084,26 +15114,14 @@
       <rPr>
         <strike/>
         <sz val="10"/>
-        <color rgb="FF444444"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A principle objective of the study.</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color rgb="FF172B4D"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> {P378 : CDISC}"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF444444"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Study Secondary Objective</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -15117,25 +15135,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>The main scientific question(s) the study is designed to answer. [After ICH E8; ICH E6 6.3]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF444444"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(CDISC Glossary)</t>
+      <t>Secondary Objective</t>
     </r>
   </si>
   <si>
@@ -15143,14 +15143,16 @@
       <rPr>
         <strike/>
         <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Study Secondary Objective</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
+        <color rgb="FF172B4D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>An auxiliary objective of the study. {P378 : CDISC}"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF172B4D"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -15164,24 +15166,43 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Secondary Objective</t>
-    </r>
+      <t>The supportive or ancillary scientific question(s) the study is designed to answer. [After ICH E8]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF172B4D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(CDISC Glossary)</t>
+    </r>
+  </si>
+  <si>
+    <t>Update definition of Class</t>
   </si>
   <si>
     <r>
       <rPr>
         <strike/>
         <sz val="10"/>
-        <color rgb="FF172B4D"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>An auxiliary objective of the study. {P378 : CDISC}"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF172B4D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A clinical study involves research using human volunteers (also called participants) that is intended to add to medical knowledge. There are two main types of clinical studies: clinical trials (also called interventional studies) and observational studies. [[http://ClinicalTrials.gov]](CDISC Glossary)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -15195,29 +15216,11 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>The supportive or ancillary scientific question(s) the study is designed to answer. [After ICH E8]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF172B4D"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(CDISC Glossary)</t>
-    </r>
-  </si>
-  <si>
-    <t>Update definition of Class</t>
+      <t>A clinical study involves research using human volunteers (also called subjects or participants) that is intended to add to medical knowledge. There are two main types of clinical studies: clinical trials (also called interventional studies) and observational studies. [[http://ClinicalTrials.gov]](CDISC Glossary)</t>
+    </r>
+  </si>
+  <si>
+    <t>Update definition of attribute in StudyDesign class</t>
   </si>
   <si>
     <r>
@@ -15227,7 +15230,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>A clinical study involves research using human volunteers (also called participants) that is intended to add to medical knowledge. There are two main types of clinical studies: clinical trials (also called interventional studies) and observational studies. [[http://ClinicalTrials.gov]](CDISC Glossary)</t>
+      <t>The general design of the strategy for assigning interventions to participants in a clinical study. (clinicaltrials.gov)</t>
     </r>
     <r>
       <rPr>
@@ -15245,25 +15248,27 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>A clinical study involves research using human volunteers (also called subjects or participants) that is intended to add to medical knowledge. There are two main types of clinical studies: clinical trials (also called interventional studies) and observational studies. [[http://ClinicalTrials.gov]](CDISC Glossary)</t>
-    </r>
-  </si>
-  <si>
-    <t>Update definition of attribute in StudyDesign class</t>
+      <t>The general design of the strategy for assigning interventions to subjects in a clinical study. (clinicaltrials.gov)</t>
+    </r>
+  </si>
+  <si>
+    <t>Update definition of attribute in StudyAmendment class</t>
   </si>
   <si>
     <r>
       <rPr>
         <strike/>
         <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>The general design of the strategy for assigning interventions to participants in a clinical study. (clinicaltrials.gov)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>An indication as to whether the amendment likely to have a substantial impact on the safety or rights of the participants.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -15277,27 +15282,22 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>The general design of the strategy for assigning interventions to subjects in a clinical study. (clinicaltrials.gov)</t>
-    </r>
-  </si>
-  <si>
-    <t>Update definition of attribute in StudyAmendment class</t>
+      <t>An indication as to whether the amendment is likely to have a substantial impact on the safety or rights of study subjects/participants.</t>
+    </r>
   </si>
   <si>
     <r>
       <rPr>
         <strike/>
         <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>An indication as to whether the amendment likely to have a substantial impact on the safety or rights of the participants.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The mechanism used to obscure the distinctive characteristics of the study intervention or procedure to make it indistinguishable from the comparator. NOTE: Blinding refers to study participants while masking refers to the study intervention. (CDISC Glossary)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -15311,18 +15311,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>An indication as to whether the amendment is likely to have a substantial impact on the safety or rights of study subjects/participants.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>The mechanism used to obscure the distinctive characteristics of the study intervention or procedure to make it indistinguishable from the comparator. NOTE: Blinding refers to study participants while masking refers to the study intervention. (CDISC Glossary)</t>
+      <t>The mechanism used to obscure the distinctive characteristics of the study intervention or procedure to make it indistinguishable from a comparator. (CDISC Glossary)</t>
     </r>
     <r>
       <rPr>
@@ -15333,46 +15322,60 @@
       <t xml:space="preserve">
 </t>
     </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>The mechanism used to obscure the distinctive characteristics of the study intervention or procedure to make it indistinguishable from a comparator. (CDISC Glossary)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
+  </si>
+  <si>
+    <t>Remove term from Masking Role Valid Value Set</t>
+  </si>
+  <si>
+    <t>DDF Study Amendment Reason Code Valid Value Set</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Challenges with participant recruitment necessitates a change(s) to, or formal clarification of, the protocol.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
     </r>
-  </si>
-  <si>
-    <t>Remove term from Masking Role Valid Value Set</t>
-  </si>
-  <si>
-    <t>DDF Study Amendment Reason Code Valid Value Set</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Challenges with subject recruitment necessitates a change(s) to, or formal clarification of, the protocol.</t>
+    </r>
+  </si>
+  <si>
+    <t>Update NCI C-code, Preferred term, and Definition of attribute in StudyDesignPopulation class</t>
   </si>
   <si>
     <r>
       <rPr>
         <strike/>
         <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Challenges with participant recruitment necessitates a change(s) to, or formal clarification of, the protocol.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>C49696</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -15386,11 +15389,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Challenges with subject recruitment necessitates a change(s) to, or formal clarification of, the protocol.</t>
-    </r>
-  </si>
-  <si>
-    <t>Update NCI C-code, Preferred term, and Definition of attribute in StudyDesignPopulation class</t>
+      <t>CNEW</t>
+    </r>
   </si>
   <si>
     <r>
@@ -15400,7 +15400,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>C49696</t>
+      <t>Sex of Participants</t>
     </r>
     <r>
       <rPr>
@@ -15418,7 +15418,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>CNEW</t>
+      <t>Study Design Population Planned Sex</t>
     </r>
   </si>
   <si>
@@ -15429,7 +15429,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Sex of Participants</t>
+      <t>The specific sex, either male, female, or mixed of the subject group being studied. (NCI)</t>
     </r>
     <r>
       <rPr>
@@ -15447,22 +15447,30 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Study Design Population Planned Sex</t>
-    </r>
+      <t>The protocol-defined sex within the study design population.</t>
+    </r>
+  </si>
+  <si>
+    <t>Update Preferred term and definition of attribute in StudyDesignParameter class</t>
+  </si>
+  <si>
+    <t>DDF Study Design Parameter Attribute Terminology</t>
   </si>
   <si>
     <r>
       <rPr>
         <strike/>
         <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>The specific sex, either male, female, or mixed of the subject group being studied. (NCI)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Study Population Includes Healthy Subjects Indicator</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -15476,30 +15484,22 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>The protocol-defined sex within the study design population.</t>
-    </r>
-  </si>
-  <si>
-    <t>Update Preferred term and definition of attribute in StudyDesignParameter class</t>
-  </si>
-  <si>
-    <t>DDF Study Design Parameter Attribute Terminology</t>
+      <t>Study Design Population Includes Healthy Subjects Indicator</t>
+    </r>
   </si>
   <si>
     <r>
       <rPr>
         <strike/>
         <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Study Population Includes Healthy Subjects Indicator</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>An indication as to whether the population definition includes healthy subjects, that is, subjects without the disease or condition under study.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -15513,8 +15513,11 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Study Design Population Includes Healthy Subjects Indicator</t>
-    </r>
+      <t>An indication as to whether the study design population includes healthy subjects, that is, subjects without the disease or condition under study.</t>
+    </r>
+  </si>
+  <si>
+    <t>Update definition of attribute in StudyDesignParameter class</t>
   </si>
   <si>
     <r>
@@ -15524,7 +15527,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>An indication as to whether the population definition includes healthy subjects, that is, subjects without the disease or condition under study.</t>
+      <t>The protocol-defined age of subjects within the study design population.</t>
     </r>
     <r>
       <rPr>
@@ -15542,11 +15545,11 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>An indication as to whether the study design population includes healthy subjects, that is, subjects without the disease or condition under study.</t>
-    </r>
-  </si>
-  <si>
-    <t>Update definition of attribute in StudyDesignParameter class</t>
+      <t>The anticipated age of subjects within the study design population.</t>
+    </r>
+  </si>
+  <si>
+    <t>Update NCI C-code, Preferred term, and Definition of attribute in StudyCohort class</t>
   </si>
   <si>
     <r>
@@ -15556,7 +15559,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>The protocol-defined age of subjects within the study design population.</t>
+      <t>C49692</t>
     </r>
     <r>
       <rPr>
@@ -15574,11 +15577,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>The anticipated age of subjects within the study design population.</t>
-    </r>
-  </si>
-  <si>
-    <t>Update NCI C-code, Preferred term, and Definition of attribute in StudyCohort class</t>
+      <t>CNEW</t>
+    </r>
   </si>
   <si>
     <r>
@@ -15588,7 +15588,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>C49692</t>
+      <t>Planned Number of Participants in Study Cohort</t>
     </r>
     <r>
       <rPr>
@@ -15606,7 +15606,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>CNEW</t>
+      <t>Study Cohort Planned Enrollment Number</t>
     </r>
   </si>
   <si>
@@ -15617,7 +15617,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Planned Number of Participants in Study Cohort</t>
+      <t>The protocol-defined number of subjects within a study cohort.</t>
     </r>
     <r>
       <rPr>
@@ -15635,8 +15635,11 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Study Cohort Planned Enrollment Number</t>
-    </r>
+      <t>The value representing the planned number of subjects to be entered in a clinical trial, within the study cohort.</t>
+    </r>
+  </si>
+  <si>
+    <t>Update Preferred term and definition of attribute in StudyCohort class</t>
   </si>
   <si>
     <r>
@@ -15646,7 +15649,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>The protocol-defined number of subjects within a study cohort.</t>
+      <t>Planned Sex of Study Cohort Participants</t>
     </r>
     <r>
       <rPr>
@@ -15664,11 +15667,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>The value representing the planned number of subjects to be entered in a clinical trial, within the study cohort.</t>
-    </r>
-  </si>
-  <si>
-    <t>Update Preferred term and definition of attribute in StudyCohort class</t>
+      <t>Study Cohort Planned Sex</t>
+    </r>
   </si>
   <si>
     <r>
@@ -15678,7 +15678,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Planned Sex of Study Cohort Participants</t>
+      <t>The protocol-defined sex of the study cohort.</t>
     </r>
     <r>
       <rPr>
@@ -15696,8 +15696,11 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Study Cohort Planned Sex</t>
-    </r>
+      <t>The protocol-defined sex within the study cohort.</t>
+    </r>
+  </si>
+  <si>
+    <t>Update definition of attribute in StudyCohort class</t>
   </si>
   <si>
     <r>
@@ -15707,7 +15710,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>The protocol-defined sex of the study cohort.</t>
+      <t>The protocol-defined age of subjects within the study cohort.</t>
     </r>
     <r>
       <rPr>
@@ -15725,11 +15728,14 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>The protocol-defined sex within the study cohort.</t>
-    </r>
-  </si>
-  <si>
-    <t>Update definition of attribute in StudyCohort class</t>
+      <t>The anticipated age of subjects within the study cohort.</t>
+    </r>
+  </si>
+  <si>
+    <t>Add 'Inherited From ' information to CT deliverable</t>
+  </si>
+  <si>
+    <t>Update Definition of attribute in Timing Class</t>
   </si>
   <si>
     <r>
@@ -15739,7 +15745,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>The protocol-defined age of subjects within the study cohort.</t>
+      <t>The textual representation of the chronological relationship between temporal events.</t>
     </r>
     <r>
       <rPr>
@@ -15757,14 +15763,11 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>The anticipated age of subjects within the study cohort.</t>
-    </r>
-  </si>
-  <si>
-    <t>Add 'Inherited From ' information to CT deliverable</t>
-  </si>
-  <si>
-    <t>Update Definition of attribute in Timing Class</t>
+      <t>A narrative representation of the chronological relationship between temporal events.</t>
+    </r>
+  </si>
+  <si>
+    <t>Update attribute name, NCI C-code, Preferred term, and Definition of attribute in Timing class</t>
   </si>
   <si>
     <r>
@@ -15774,7 +15777,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>The textual representation of the chronological relationship between temporal events.</t>
+      <t>window</t>
     </r>
     <r>
       <rPr>
@@ -15792,25 +15795,24 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>A narrative representation of the chronological relationship between temporal events.</t>
-    </r>
-  </si>
-  <si>
-    <t>Update attribute name, NCI C-code, Preferred term, and Definition of attribute in Timing class</t>
+      <t>windowLabel</t>
+    </r>
   </si>
   <si>
     <r>
       <rPr>
         <strike/>
         <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>window</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>C48921</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -15824,7 +15826,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>windowLabel</t>
+      <t>CNEW</t>
     </r>
   </si>
   <si>
@@ -15836,7 +15838,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>C48921</t>
+      <t>Timing Window</t>
     </r>
     <r>
       <rPr>
@@ -15855,7 +15857,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>CNEW</t>
+      <t>Timing Window Label</t>
     </r>
   </si>
   <si>
@@ -15867,7 +15869,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Timing Window</t>
+      <t>A time period, or other type of interval, during which a temporal event may be achieved, obtained, or observed.</t>
     </r>
     <r>
       <rPr>
@@ -15886,8 +15888,14 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Timing Window Label</t>
-    </r>
+      <t>The short descriptive designation for a time period, or other type of interval, during which a temporal event may be achieved, obtained, or observed.</t>
+    </r>
+  </si>
+  <si>
+    <t>Update NCI C-code</t>
+  </si>
+  <si>
+    <t>DDF Study Intervention Product Designation Valid Value Set</t>
   </si>
   <si>
     <r>
@@ -15898,7 +15906,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>A time period, or other type of interval, during which a temporal event may be achieved, obtained, or observed.</t>
+      <t>CNEW</t>
     </r>
     <r>
       <rPr>
@@ -15917,30 +15925,28 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>The short descriptive designation for a time period, or other type of interval, during which a temporal event may be achieved, obtained, or observed.</t>
-    </r>
-  </si>
-  <si>
-    <t>Update NCI C-code</t>
-  </si>
-  <si>
-    <t>DDF Study Intervention Product Designation Valid Value Set</t>
+      <t>C202579</t>
+    </r>
+  </si>
+  <si>
+    <t>Remove attribute from ScheduledDecisionInstance class.</t>
+  </si>
+  <si>
+    <t>Remove attribute from SyntaxTemplateDictionary class.</t>
   </si>
   <si>
     <r>
       <rPr>
         <strike/>
         <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>CNEW</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The specific sex, either male, female, or mixed of the subject group being studied. (NCI)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -15954,14 +15960,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>C202579</t>
-    </r>
-  </si>
-  <si>
-    <t>Remove attribute from ScheduledDecisionInstance class.</t>
-  </si>
-  <si>
-    <t>Remove attribute from SyntaxTemplateDictionary class.</t>
+      <t>The protocol-defined sex within the population definition.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -16146,12 +16146,14 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -16442,7 +16444,7 @@
     <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -16865,12 +16867,6 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -16896,6 +16892,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -17295,10 +17300,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="151" t="s">
         <v>908</v>
       </c>
-      <c r="B1" s="143"/>
+      <c r="B1" s="152"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -31576,7 +31581,7 @@
   </sheetData>
   <autoFilter ref="A1:K56" xr:uid="{56E2EBE1-9928-42D6-AA06-A82264CE5423}"/>
   <conditionalFormatting sqref="H48">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33754,7 +33759,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H39">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34079,7 +34084,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H8">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -48262,7 +48267,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D11:E11">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="participant">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="participant">
       <formula>NOT(ISERROR(SEARCH("participant",D11)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -48598,7 +48603,7 @@
       <c r="D9" s="88" t="s">
         <v>924</v>
       </c>
-      <c r="E9" s="144" t="s">
+      <c r="E9" s="142" t="s">
         <v>1102</v>
       </c>
       <c r="F9" s="88" t="s">
@@ -48615,7 +48620,7 @@
       <c r="K9" s="88" t="s">
         <v>2594</v>
       </c>
-      <c r="L9" s="145" t="s">
+      <c r="L9" s="143" t="s">
         <v>938</v>
       </c>
       <c r="M9" s="87"/>
@@ -48659,7 +48664,7 @@
       <c r="A11" s="15" t="s">
         <v>2597</v>
       </c>
-      <c r="B11" s="146" t="s">
+      <c r="B11" s="144" t="s">
         <v>913</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -48676,16 +48681,16 @@
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="58" t="s">
-        <v>1800</v>
+        <v>913</v>
       </c>
       <c r="I11" s="15" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J11" s="92" t="s">
         <v>2598</v>
       </c>
-      <c r="J11" s="92" t="s">
-        <v>2599</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>1802</v>
+      <c r="K11" s="153" t="s">
+        <v>2650</v>
       </c>
       <c r="L11" s="16" t="s">
         <v>2112</v>
@@ -48696,7 +48701,7 @@
     </row>
     <row r="12" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>2600</v>
+        <v>2599</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>913</v>
@@ -48722,7 +48727,7 @@
       </c>
       <c r="J12" s="92"/>
       <c r="K12" s="92" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="L12" s="89" t="s">
         <v>938</v>
@@ -48731,7 +48736,7 @@
     </row>
     <row r="13" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>583</v>
@@ -48759,7 +48764,7 @@
         <v>1320</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
       <c r="L13" s="16" t="s">
         <v>939</v>
@@ -48768,7 +48773,7 @@
     </row>
     <row r="14" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>583</v>
@@ -48790,13 +48795,13 @@
         <v>587</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>2605</v>
+        <v>2604</v>
       </c>
       <c r="J14" s="15" t="s">
         <v>1359</v>
       </c>
-      <c r="K14" s="147" t="s">
-        <v>2606</v>
+      <c r="K14" s="145" t="s">
+        <v>2605</v>
       </c>
       <c r="L14" s="16" t="s">
         <v>939</v>
@@ -48805,7 +48810,7 @@
     </row>
     <row r="15" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>583</v>
@@ -48827,13 +48832,13 @@
         <v>592</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>2607</v>
+        <v>2606</v>
       </c>
       <c r="J15" s="15" t="s">
         <v>1360</v>
       </c>
-      <c r="K15" s="148" t="s">
-        <v>2608</v>
+      <c r="K15" s="146" t="s">
+        <v>2607</v>
       </c>
       <c r="L15" s="16" t="s">
         <v>939</v>
@@ -48842,7 +48847,7 @@
     </row>
     <row r="16" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>2609</v>
+        <v>2608</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>118</v>
@@ -48868,7 +48873,7 @@
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15" t="s">
-        <v>2610</v>
+        <v>2609</v>
       </c>
       <c r="L16" s="15" t="s">
         <v>938</v>
@@ -48877,7 +48882,7 @@
     </row>
     <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>2611</v>
+        <v>2610</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>286</v>
@@ -48903,7 +48908,7 @@
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="15" t="s">
-        <v>2612</v>
+        <v>2611</v>
       </c>
       <c r="L17" s="15" t="s">
         <v>2238</v>
@@ -48914,7 +48919,7 @@
     </row>
     <row r="18" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>913</v>
@@ -48940,7 +48945,7 @@
       </c>
       <c r="J18" s="55"/>
       <c r="K18" s="55" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
       <c r="L18" s="16" t="s">
         <v>938</v>
@@ -48949,7 +48954,7 @@
     </row>
     <row r="19" spans="1:13" ht="137.5" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>2609</v>
+        <v>2608</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>118</v>
@@ -48960,7 +48965,7 @@
       <c r="D19" s="15" t="s">
         <v>2313</v>
       </c>
-      <c r="E19" s="149" t="s">
+      <c r="E19" s="147" t="s">
         <v>2313</v>
       </c>
       <c r="F19" s="15" t="s">
@@ -48975,7 +48980,7 @@
       </c>
       <c r="J19" s="15"/>
       <c r="K19" s="15" t="s">
-        <v>2615</v>
+        <v>2614</v>
       </c>
       <c r="L19" s="16" t="s">
         <v>939</v>
@@ -48984,9 +48989,9 @@
     </row>
     <row r="20" spans="1:13" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>2616</v>
-      </c>
-      <c r="B20" s="146" t="s">
+        <v>2615</v>
+      </c>
+      <c r="B20" s="144" t="s">
         <v>913</v>
       </c>
       <c r="C20" s="15" t="s">
@@ -49019,13 +49024,13 @@
     </row>
     <row r="21" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>2602</v>
-      </c>
-      <c r="B21" s="146" t="s">
+        <v>2601</v>
+      </c>
+      <c r="B21" s="144" t="s">
         <v>913</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>2617</v>
+        <v>2616</v>
       </c>
       <c r="D21" s="75" t="s">
         <v>1414</v>
@@ -49045,7 +49050,7 @@
       </c>
       <c r="J21" s="55"/>
       <c r="K21" s="55" t="s">
-        <v>2618</v>
+        <v>2617</v>
       </c>
       <c r="L21" s="16" t="s">
         <v>939</v>
@@ -49054,9 +49059,9 @@
     </row>
     <row r="22" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>2619</v>
-      </c>
-      <c r="B22" s="146" t="s">
+        <v>2618</v>
+      </c>
+      <c r="B22" s="144" t="s">
         <v>302</v>
       </c>
       <c r="C22" s="15" t="s">
@@ -49075,14 +49080,14 @@
         <v>2150</v>
       </c>
       <c r="H22" s="15" t="s">
+        <v>2619</v>
+      </c>
+      <c r="I22" s="15" t="s">
         <v>2620</v>
-      </c>
-      <c r="I22" s="15" t="s">
-        <v>2621</v>
       </c>
       <c r="J22" s="15"/>
       <c r="K22" s="15" t="s">
-        <v>2622</v>
+        <v>2621</v>
       </c>
       <c r="L22" s="16" t="s">
         <v>2112</v>
@@ -49093,13 +49098,13 @@
     </row>
     <row r="23" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
+        <v>2622</v>
+      </c>
+      <c r="B23" s="144" t="s">
+        <v>913</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>2623</v>
-      </c>
-      <c r="B23" s="146" t="s">
-        <v>913</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>2624</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>925</v>
@@ -49117,11 +49122,11 @@
         <v>913</v>
       </c>
       <c r="I23" s="55" t="s">
-        <v>2625</v>
+        <v>2624</v>
       </c>
       <c r="J23" s="55"/>
       <c r="K23" s="15" t="s">
-        <v>2626</v>
+        <v>2625</v>
       </c>
       <c r="L23" s="54" t="s">
         <v>938</v>
@@ -49130,13 +49135,13 @@
     </row>
     <row r="24" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>2627</v>
-      </c>
-      <c r="B24" s="146" t="s">
+        <v>2626</v>
+      </c>
+      <c r="B24" s="144" t="s">
         <v>913</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>2624</v>
+        <v>2623</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>925</v>
@@ -49158,7 +49163,7 @@
       </c>
       <c r="J24" s="15"/>
       <c r="K24" s="15" t="s">
-        <v>2628</v>
+        <v>2627</v>
       </c>
       <c r="L24" s="16" t="s">
         <v>938</v>
@@ -49167,9 +49172,9 @@
     </row>
     <row r="25" spans="1:13" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>2629</v>
-      </c>
-      <c r="B25" s="146" t="s">
+        <v>2628</v>
+      </c>
+      <c r="B25" s="144" t="s">
         <v>913</v>
       </c>
       <c r="C25" s="15" t="s">
@@ -49188,14 +49193,14 @@
         <v>2150</v>
       </c>
       <c r="H25" s="15" t="s">
+        <v>2629</v>
+      </c>
+      <c r="I25" s="15" t="s">
         <v>2630</v>
-      </c>
-      <c r="I25" s="15" t="s">
-        <v>2631</v>
       </c>
       <c r="J25" s="15"/>
       <c r="K25" s="15" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
       <c r="L25" s="16" t="s">
         <v>938</v>
@@ -49204,9 +49209,9 @@
     </row>
     <row r="26" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>2633</v>
-      </c>
-      <c r="B26" s="146" t="s">
+        <v>2632</v>
+      </c>
+      <c r="B26" s="144" t="s">
         <v>913</v>
       </c>
       <c r="C26" s="15" t="s">
@@ -49228,24 +49233,24 @@
         <v>913</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
       <c r="J26" s="15"/>
       <c r="K26" s="15" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
       <c r="L26" s="16" t="s">
         <v>2112</v>
       </c>
-      <c r="M26" s="150" t="s">
+      <c r="M26" s="148" t="s">
         <v>1832</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>2636</v>
-      </c>
-      <c r="B27" s="146" t="s">
+        <v>2635</v>
+      </c>
+      <c r="B27" s="144" t="s">
         <v>913</v>
       </c>
       <c r="C27" s="15" t="s">
@@ -49271,7 +49276,7 @@
       </c>
       <c r="J27" s="15"/>
       <c r="K27" s="15" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="L27" s="16" t="s">
         <v>938</v>
@@ -49280,9 +49285,9 @@
     </row>
     <row r="28" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>2638</v>
-      </c>
-      <c r="B28" s="146" t="s">
+        <v>2637</v>
+      </c>
+      <c r="B28" s="144" t="s">
         <v>913</v>
       </c>
       <c r="C28" s="15" t="s">
@@ -49317,7 +49322,7 @@
     </row>
     <row r="29" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>2639</v>
+        <v>2638</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>1736</v>
@@ -49343,7 +49348,7 @@
       </c>
       <c r="J29" s="55"/>
       <c r="K29" s="15" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
       <c r="L29" s="54" t="s">
         <v>938</v>
@@ -49352,7 +49357,7 @@
     </row>
     <row r="30" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>1736</v>
@@ -49364,21 +49369,21 @@
         <v>961</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
       <c r="F30" s="15" t="s">
         <v>909</v>
       </c>
       <c r="G30" s="15"/>
       <c r="H30" s="55" t="s">
+        <v>2642</v>
+      </c>
+      <c r="I30" s="55" t="s">
         <v>2643</v>
-      </c>
-      <c r="I30" s="55" t="s">
-        <v>2644</v>
       </c>
       <c r="J30" s="55"/>
       <c r="K30" s="55" t="s">
-        <v>2645</v>
+        <v>2644</v>
       </c>
       <c r="L30" s="54" t="s">
         <v>938</v>
@@ -49387,13 +49392,13 @@
     </row>
     <row r="31" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
+        <v>2645</v>
+      </c>
+      <c r="B31" s="144" t="s">
+        <v>913</v>
+      </c>
+      <c r="C31" s="15" t="s">
         <v>2646</v>
-      </c>
-      <c r="B31" s="146" t="s">
-        <v>913</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>2647</v>
       </c>
       <c r="D31" s="136" t="s">
         <v>1805</v>
@@ -49406,7 +49411,7 @@
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="55" t="s">
-        <v>2648</v>
+        <v>2647</v>
       </c>
       <c r="I31" s="55" t="s">
         <v>2442</v>
@@ -49422,7 +49427,7 @@
     </row>
     <row r="32" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>1992</v>
@@ -49440,7 +49445,7 @@
         <v>909</v>
       </c>
       <c r="G32" s="23"/>
-      <c r="H32" s="151" t="s">
+      <c r="H32" s="149" t="s">
         <v>1996</v>
       </c>
       <c r="I32" s="23" t="s">
@@ -49457,9 +49462,9 @@
     </row>
     <row r="33" spans="1:13" ht="50" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>2650</v>
-      </c>
-      <c r="B33" s="146" t="s">
+        <v>2649</v>
+      </c>
+      <c r="B33" s="144" t="s">
         <v>913</v>
       </c>
       <c r="C33" s="15" t="s">
@@ -49468,7 +49473,7 @@
       <c r="D33" s="23" t="s">
         <v>1183</v>
       </c>
-      <c r="E33" s="152" t="s">
+      <c r="E33" s="150" t="s">
         <v>1191</v>
       </c>
       <c r="F33" s="23" t="s">
@@ -49492,32 +49497,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E4">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="subject">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="subject">
       <formula>NOT(ISERROR(SEARCH("subject",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10:E11 H10:H11">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="participant">
+  <conditionalFormatting sqref="D10:E11 H10">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="participant">
       <formula>NOT(ISERROR(SEARCH("participant",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:F9">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="participant">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="participant">
       <formula>NOT(ISERROR(SEARCH("participant",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:J6 L5:M6 H7:M7 H8:J9 L8:M9">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="participant">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="participant">
       <formula>NOT(ISERROR(SEARCH("participant",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K4">
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="subject">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="subject">
       <formula>NOT(ISERROR(SEARCH("subject",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="M11" r:id="rId1" xr:uid="{D4EEC41E-B3C1-4528-95A1-DDD8E6B69861}"/>

</xml_diff>

<commit_message>
sprint 3 - 388, 353, 371
2nd part of sprint 3 items complete: 388, 353, 371
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F751F562-65D5-4F70-84B1-C737FA0FD77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0017EB3-DF5A-434D-9B42-C797C5D4DD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="16780" windowHeight="9930" tabRatio="668" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1030" yWindow="30" windowWidth="16780" windowHeight="9930" tabRatio="668" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -14588,7 +14588,7 @@
   </sheetPr>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14677,7 +14677,7 @@
         <v>1613</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M2" s="13"/>
     </row>
@@ -14710,7 +14710,7 @@
         <v>1616</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M3" s="13"/>
     </row>
@@ -14743,7 +14743,7 @@
         <v>1618</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M4" s="13"/>
     </row>
@@ -14776,7 +14776,7 @@
         <v>1620</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M5" s="13"/>
     </row>
@@ -14809,7 +14809,7 @@
         <v>1622</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M6" s="13"/>
     </row>
@@ -14840,7 +14840,7 @@
         <v>1624</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M7" s="13"/>
     </row>
@@ -14871,7 +14871,7 @@
         <v>1626</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M8" s="13"/>
     </row>
@@ -14904,7 +14904,7 @@
         <v>1628</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M9" s="13"/>
     </row>
@@ -14937,7 +14937,7 @@
         <v>1630</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M10" s="13"/>
     </row>
@@ -14968,7 +14968,7 @@
         <v>1632</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M11" s="13"/>
     </row>
@@ -14999,7 +14999,7 @@
         <v>1634</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M12" s="13"/>
     </row>
@@ -15030,7 +15030,7 @@
         <v>1636</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M13" s="13"/>
     </row>
@@ -15061,7 +15061,7 @@
         <v>1638</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M14" s="13"/>
     </row>
@@ -15092,7 +15092,7 @@
         <v>1640</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M15" s="13"/>
     </row>
@@ -15123,7 +15123,7 @@
         <v>1642</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M16" s="13"/>
     </row>
@@ -15154,7 +15154,7 @@
         <v>1644</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M17" s="13"/>
     </row>
@@ -15185,7 +15185,7 @@
         <v>1646</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M18" s="13"/>
     </row>
@@ -15216,7 +15216,7 @@
         <v>1648</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M19" s="13"/>
     </row>
@@ -15247,7 +15247,7 @@
         <v>1650</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M20" s="13"/>
     </row>
@@ -15278,7 +15278,7 @@
         <v>1652</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M21" s="13"/>
     </row>
@@ -15309,7 +15309,7 @@
         <v>1654</v>
       </c>
       <c r="L22" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M22" s="13"/>
     </row>
@@ -15340,7 +15340,7 @@
         <v>1656</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M23" s="13"/>
     </row>
@@ -15371,7 +15371,7 @@
         <v>1659</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M24" s="13"/>
     </row>
@@ -15402,7 +15402,7 @@
         <v>1661</v>
       </c>
       <c r="L25" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M25" s="13"/>
     </row>
@@ -15433,7 +15433,7 @@
         <v>1663</v>
       </c>
       <c r="L26" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M26" s="13"/>
     </row>
@@ -15464,7 +15464,7 @@
         <v>1666</v>
       </c>
       <c r="L27" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M27" s="13"/>
     </row>
@@ -15495,7 +15495,7 @@
         <v>1669</v>
       </c>
       <c r="L28" s="16" t="s">
-        <v>1614</v>
+        <v>928</v>
       </c>
       <c r="M28" s="13"/>
     </row>

</xml_diff>

<commit_message>
399 - update to changes file
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC84034-2A25-4726-989C-9E602385C08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE19C59-6ABF-4AE4-B985-2A8002F32395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="80" windowWidth="16370" windowHeight="9980" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="590" yWindow="150" windowWidth="16370" windowHeight="9980" tabRatio="668" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4269" uniqueCount="1833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4270" uniqueCount="1834">
   <si>
     <t>Code</t>
   </si>
@@ -5915,6 +5915,9 @@
       </rPr>
       <t>A USDM relationship between the StudyVersion and StudyDefinitionDocumentVersion classes which identifies the version of the study protocol document associated with the study version.</t>
     </r>
+  </si>
+  <si>
+    <t>Added NCI c-codes to all codeable model elements within the Phase 3 release of DDF</t>
   </si>
 </sst>
 </file>
@@ -6373,12 +6376,6 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6398,6 +6395,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6695,10 +6698,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="61" t="s">
         <v>903</v>
       </c>
-      <c r="B1" s="55"/>
+      <c r="B1" s="62"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -18812,7 +18815,7 @@
   </sheetPr>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19091,7 +19094,7 @@
       <c r="D8" s="15" t="s">
         <v>1761</v>
       </c>
-      <c r="E8" s="56" t="s">
+      <c r="E8" s="54" t="s">
         <v>1761</v>
       </c>
       <c r="F8" s="16" t="s">
@@ -19433,7 +19436,7 @@
       <c r="D18" s="15" t="s">
         <v>1793</v>
       </c>
-      <c r="E18" s="56" t="s">
+      <c r="E18" s="54" t="s">
         <v>1793</v>
       </c>
       <c r="F18" s="16" t="s">
@@ -19630,9 +19633,9 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19705,7 +19708,7 @@
       <c r="D2" s="39" t="s">
         <v>1144</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="55" t="s">
         <v>1144</v>
       </c>
       <c r="F2" s="39" t="s">
@@ -19741,7 +19744,7 @@
       <c r="D3" s="39" t="s">
         <v>1144</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="56" t="s">
         <v>1808</v>
       </c>
       <c r="F3" s="39" t="s">
@@ -19777,7 +19780,7 @@
       <c r="D4" s="39" t="s">
         <v>1144</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="56" t="s">
         <v>1809</v>
       </c>
       <c r="F4" s="38" t="s">
@@ -19813,7 +19816,7 @@
       <c r="D5" s="39" t="s">
         <v>1144</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="57" t="s">
         <v>1054</v>
       </c>
       <c r="F5" s="40" t="s">
@@ -19845,7 +19848,7 @@
       <c r="D6" s="39" t="s">
         <v>1144</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="57" t="s">
         <v>1055</v>
       </c>
       <c r="F6" s="40" t="s">
@@ -19877,7 +19880,7 @@
       <c r="D7" s="39" t="s">
         <v>1144</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="57" t="s">
         <v>1056</v>
       </c>
       <c r="F7" s="40" t="s">
@@ -19909,7 +19912,7 @@
       <c r="D8" s="39" t="s">
         <v>1057</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="55" t="s">
         <v>1057</v>
       </c>
       <c r="F8" s="38" t="s">
@@ -19945,7 +19948,7 @@
       <c r="D9" s="39" t="s">
         <v>1057</v>
       </c>
-      <c r="E9" s="60" t="s">
+      <c r="E9" s="58" t="s">
         <v>1670</v>
       </c>
       <c r="F9" s="40" t="s">
@@ -19981,7 +19984,7 @@
       <c r="D10" s="39" t="s">
         <v>1057</v>
       </c>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="58" t="s">
         <v>1675</v>
       </c>
       <c r="F10" s="40" t="s">
@@ -20017,7 +20020,7 @@
       <c r="D11" s="39" t="s">
         <v>1057</v>
       </c>
-      <c r="E11" s="60" t="s">
+      <c r="E11" s="58" t="s">
         <v>1678</v>
       </c>
       <c r="F11" s="40" t="s">
@@ -20053,7 +20056,7 @@
       <c r="D12" s="39" t="s">
         <v>1057</v>
       </c>
-      <c r="E12" s="59" t="s">
+      <c r="E12" s="57" t="s">
         <v>1058</v>
       </c>
       <c r="F12" s="40" t="s">
@@ -20085,7 +20088,7 @@
       <c r="D13" s="38" t="s">
         <v>1095</v>
       </c>
-      <c r="E13" s="60" t="s">
+      <c r="E13" s="58" t="s">
         <v>1689</v>
       </c>
       <c r="F13" s="40" t="s">
@@ -20118,24 +20121,24 @@
       <c r="C14" s="15" t="s">
         <v>608</v>
       </c>
-      <c r="D14" s="61" t="s">
+      <c r="D14" s="59" t="s">
         <v>1826</v>
       </c>
-      <c r="E14" s="62" t="s">
+      <c r="E14" s="60" t="s">
         <v>1827</v>
       </c>
       <c r="F14" s="16" t="s">
         <v>1701</v>
       </c>
       <c r="G14" s="13"/>
-      <c r="H14" s="62" t="s">
+      <c r="H14" s="60" t="s">
         <v>615</v>
       </c>
-      <c r="I14" s="62" t="s">
+      <c r="I14" s="60" t="s">
         <v>616</v>
       </c>
-      <c r="J14" s="62"/>
-      <c r="K14" s="62" t="s">
+      <c r="J14" s="60"/>
+      <c r="K14" s="60" t="s">
         <v>617</v>
       </c>
       <c r="L14" s="16" t="s">
@@ -20154,26 +20157,26 @@
       <c r="C15" s="15" t="s">
         <v>608</v>
       </c>
-      <c r="D15" s="61" t="s">
+      <c r="D15" s="59" t="s">
         <v>1826</v>
       </c>
-      <c r="E15" s="62" t="s">
+      <c r="E15" s="60" t="s">
         <v>1827</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>1701</v>
       </c>
       <c r="G15" s="13"/>
-      <c r="H15" s="62" t="s">
+      <c r="H15" s="60" t="s">
         <v>624</v>
       </c>
-      <c r="I15" s="62" t="s">
+      <c r="I15" s="60" t="s">
         <v>625</v>
       </c>
-      <c r="J15" s="62" t="s">
+      <c r="J15" s="60" t="s">
         <v>626</v>
       </c>
-      <c r="K15" s="62" t="s">
+      <c r="K15" s="60" t="s">
         <v>627</v>
       </c>
       <c r="L15" s="16" t="s">
@@ -20192,24 +20195,24 @@
       <c r="C16" s="15" t="s">
         <v>608</v>
       </c>
-      <c r="D16" s="61" t="s">
+      <c r="D16" s="59" t="s">
         <v>1826</v>
       </c>
-      <c r="E16" s="62" t="s">
+      <c r="E16" s="60" t="s">
         <v>1827</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>1701</v>
       </c>
       <c r="G16" s="13"/>
-      <c r="H16" s="62" t="s">
+      <c r="H16" s="60" t="s">
         <v>611</v>
       </c>
-      <c r="I16" s="62" t="s">
+      <c r="I16" s="60" t="s">
         <v>612</v>
       </c>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62" t="s">
+      <c r="J16" s="60"/>
+      <c r="K16" s="60" t="s">
         <v>613</v>
       </c>
       <c r="L16" s="16" t="s">
@@ -20228,24 +20231,24 @@
       <c r="C17" s="15" t="s">
         <v>608</v>
       </c>
-      <c r="D17" s="61" t="s">
+      <c r="D17" s="59" t="s">
         <v>1826</v>
       </c>
-      <c r="E17" s="62" t="s">
+      <c r="E17" s="60" t="s">
         <v>1827</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>1701</v>
       </c>
       <c r="G17" s="13"/>
-      <c r="H17" s="62" t="s">
+      <c r="H17" s="60" t="s">
         <v>618</v>
       </c>
-      <c r="I17" s="62" t="s">
+      <c r="I17" s="60" t="s">
         <v>619</v>
       </c>
-      <c r="J17" s="62"/>
-      <c r="K17" s="62" t="s">
+      <c r="J17" s="60"/>
+      <c r="K17" s="60" t="s">
         <v>620</v>
       </c>
       <c r="L17" s="16" t="s">
@@ -20264,24 +20267,24 @@
       <c r="C18" s="15" t="s">
         <v>608</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="59" t="s">
         <v>1826</v>
       </c>
-      <c r="E18" s="62" t="s">
+      <c r="E18" s="60" t="s">
         <v>1827</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>1701</v>
       </c>
       <c r="G18" s="13"/>
-      <c r="H18" s="62" t="s">
+      <c r="H18" s="60" t="s">
         <v>621</v>
       </c>
-      <c r="I18" s="62" t="s">
+      <c r="I18" s="60" t="s">
         <v>622</v>
       </c>
-      <c r="J18" s="62"/>
-      <c r="K18" s="62" t="s">
+      <c r="J18" s="60"/>
+      <c r="K18" s="60" t="s">
         <v>623</v>
       </c>
       <c r="L18" s="16" t="s">
@@ -20353,6 +20356,24 @@
       </c>
       <c r="M20" s="13"/>
       <c r="N20" s="13"/>
+    </row>
+    <row r="21" spans="1:14" ht="62.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>1833</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update CT changes file
tickets: 316, 444, 456
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097052F2-F836-4211-8B6D-86495733FFAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40D33BE-FED9-47F4-B073-F4C5C0ECC249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="650" windowWidth="16840" windowHeight="8820" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="300" windowWidth="16990" windowHeight="9810" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4804" uniqueCount="1990">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5244" uniqueCount="2131">
   <si>
     <t>Code</t>
   </si>
@@ -7806,6 +7806,690 @@
   </si>
   <si>
     <t>scope</t>
+  </si>
+  <si>
+    <t>Administration</t>
+  </si>
+  <si>
+    <t>administrableProduct</t>
+  </si>
+  <si>
+    <t>A USDM relationship between the Administration and AdministrableProductDefinition classes which identifies the administrable product associated with the administration.</t>
+  </si>
+  <si>
+    <t>AdministrableProduct</t>
+  </si>
+  <si>
+    <t>Administrable Product</t>
+  </si>
+  <si>
+    <t>Any study product that is formulated and presented in the form that is suitable for administration to a study participant.</t>
+  </si>
+  <si>
+    <t>DDF Administrable Product Attribute Terminology</t>
+  </si>
+  <si>
+    <t>Administrable Product Definition Name</t>
+  </si>
+  <si>
+    <t>The literal identifier (i.e., distinctive designation) of the administrable product.</t>
+  </si>
+  <si>
+    <t>Administrable Product Definition Description</t>
+  </si>
+  <si>
+    <t>A narrative representation of the administrable product.</t>
+  </si>
+  <si>
+    <t>Administrable Product Definition Label</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the administrable product.</t>
+  </si>
+  <si>
+    <t>Add Complex Datatype Relationship to new class</t>
+  </si>
+  <si>
+    <t>administrableDoseForm</t>
+  </si>
+  <si>
+    <t>C42636</t>
+  </si>
+  <si>
+    <t>Dose Form</t>
+  </si>
+  <si>
+    <t>The physical form in which active and/or inert ingredient(s) are presented.</t>
+  </si>
+  <si>
+    <t>Y (C66726)</t>
+  </si>
+  <si>
+    <t>https://ncit.nci.nih.gov/ncitbrowser/ajax?action=create_src_vs_tree&amp;vsd_uri=http://evs.nci.nih.gov/valueset/CDISC/C66726</t>
+  </si>
+  <si>
+    <t>pharmacologicClass</t>
+  </si>
+  <si>
+    <t>C98768</t>
+  </si>
+  <si>
+    <t>Pharmacologic Class</t>
+  </si>
+  <si>
+    <t>The pharmacological class of the investigational product.</t>
+  </si>
+  <si>
+    <t>Y (Points to external codelists; FDA requirement to use…)</t>
+  </si>
+  <si>
+    <t>A USDM relationship between the AdministrableProductn and CommentAnnotation classes which provides the set of notes related to the administrable product.</t>
+  </si>
+  <si>
+    <t>ingredients</t>
+  </si>
+  <si>
+    <t>A USDM relationship between the AdministrableProduct and Ingredient classes which provides the set of ingredients related to the administrable product.</t>
+  </si>
+  <si>
+    <t>A USDM relationship between the AdministrableProduct and AdministrableProductProperty classes which provides the set of properties related to the administrable product.</t>
+  </si>
+  <si>
+    <t>identifiers</t>
+  </si>
+  <si>
+    <t>A USDM relationship between the AdministrableProduct and AdministrableProductIdentifier classes which provides the set of identifiers related to the administrable product.</t>
+  </si>
+  <si>
+    <t>AdministrableProductIdentifier</t>
+  </si>
+  <si>
+    <t>Administrable Product Identifier</t>
+  </si>
+  <si>
+    <t>A sequence of characters used to identify, name, or characterize the administrable product.</t>
+  </si>
+  <si>
+    <t>DDF Administrable Product Identifier Attribute Terminology</t>
+  </si>
+  <si>
+    <t>Administrable Product Identifier Text</t>
+  </si>
+  <si>
+    <t>An instance of structured text that represents the administrable product.</t>
+  </si>
+  <si>
+    <t>A USDM relationship between the AdministrableProductIdentifier and Organization class which provides the details associated with which provides the details associated with each organization that has assigned the administrable product identifier.</t>
+  </si>
+  <si>
+    <t>AdministrableProductProperty</t>
+  </si>
+  <si>
+    <t>Administrable Product Property</t>
+  </si>
+  <si>
+    <t>A characteristic from a set of characteristics used to define an administrable product.</t>
+  </si>
+  <si>
+    <t>DDF Administrable Product Property Attribute Terminology</t>
+  </si>
+  <si>
+    <t>Administrable Product Property Name</t>
+  </si>
+  <si>
+    <t>The literal identifier (i.e., distinctive designation) of the administrable product property.</t>
+  </si>
+  <si>
+    <t>Administrable Product Property Text</t>
+  </si>
+  <si>
+    <t>An instance of structured text that represents the administrable product property.</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>Administrable Product Property Quantity Value</t>
+  </si>
+  <si>
+    <t>The numeric value associated with an administrable product property.</t>
+  </si>
+  <si>
+    <t>Administrable Product Property Type</t>
+  </si>
+  <si>
+    <t>A characterization or classification of the administrable product property.</t>
+  </si>
+  <si>
+    <t>Create new codelist to support AdministrableProductProperty.type responses</t>
+  </si>
+  <si>
+    <t>DDF Administrable Product Property Type Value Set</t>
+  </si>
+  <si>
+    <t>AdministrableProductProperty.type</t>
+  </si>
+  <si>
+    <t>C45997</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>The negative logarithm (base 10) of the concentration of hydronium ions, which is used as a measure of the acidity or alkalinity of a fluid.</t>
+  </si>
+  <si>
+    <t>Substance</t>
+  </si>
+  <si>
+    <t>C45306</t>
+  </si>
+  <si>
+    <t>Any matter of defined composition that has discrete existence, whose origin may be biological, mineral or chemical.</t>
+  </si>
+  <si>
+    <t>DDF Substance Attribute Terminology</t>
+  </si>
+  <si>
+    <t>Substance Name</t>
+  </si>
+  <si>
+    <t>The literal identifier (i.e., distinctive designation) of the substance.</t>
+  </si>
+  <si>
+    <t>Substance Description</t>
+  </si>
+  <si>
+    <t>A narrative representation of the substance.</t>
+  </si>
+  <si>
+    <t>Substance Label</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the substance.</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>Substance Code</t>
+  </si>
+  <si>
+    <t>A symbol or combination of symbols which is assigned to the substance.</t>
+  </si>
+  <si>
+    <t>Y (Point out to multiple Biomedical coding dictionaries such as WHODrug, ATC, UNII, etc.)</t>
+  </si>
+  <si>
+    <t>strengths</t>
+  </si>
+  <si>
+    <t>A USDM relationship between the Substance and Strength class which provides the values of the strengths of the substance.</t>
+  </si>
+  <si>
+    <t>referenceSubstance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A USDM relationship within the Substance class that identifies the association between two substances, one of which is used as a reference for the other. 
+</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Substance Strength</t>
+  </si>
+  <si>
+    <t>The content of an substance expressed quantitatively per dosage unit, per unit of volume, or per unit of weight, according to the pharmaceutical dose form of the product.</t>
+  </si>
+  <si>
+    <t>DDF Strength Attribute Terminology</t>
+  </si>
+  <si>
+    <t>Substance Strength Name</t>
+  </si>
+  <si>
+    <t>The literal identifier (i.e., distinctive designation) of the substance strength.</t>
+  </si>
+  <si>
+    <t>Substance Strength Description</t>
+  </si>
+  <si>
+    <t>A narrative representation of the substance strength.</t>
+  </si>
+  <si>
+    <t>Substance Strength Label</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the substance strength.</t>
+  </si>
+  <si>
+    <t>numerator</t>
+  </si>
+  <si>
+    <t>A USDM relationship between the Strength and the Quantity and Range classes that identifies the numerator's value or range of values associated with the substance  strength.</t>
+  </si>
+  <si>
+    <t>denominator</t>
+  </si>
+  <si>
+    <t>A USDM relationship between the Strength and Quantity classes that identifies the denominator associated with the substance strength.</t>
+  </si>
+  <si>
+    <t>Ingredient</t>
+  </si>
+  <si>
+    <t>C51981</t>
+  </si>
+  <si>
+    <t>Any component that constitutes a part of a compounded substance or mixture.</t>
+  </si>
+  <si>
+    <t>Add attribute to new class</t>
+  </si>
+  <si>
+    <t>DDF Ingredient Attribute Terminology</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>Ingredient Role</t>
+  </si>
+  <si>
+    <t>The intended use of the ingredient within the context of the compounded substance or mixture.</t>
+  </si>
+  <si>
+    <t>Y (Point to FHIR value set: Ingredient Role)</t>
+  </si>
+  <si>
+    <t>https://www.hl7.org/fhir/valueset-ingredient-role.html</t>
+  </si>
+  <si>
+    <t>substance</t>
+  </si>
+  <si>
+    <t>A USDM relationship between the Ingredient and Substance classes that identifies the substance associated with the ingredient.</t>
+  </si>
+  <si>
+    <t>Remove attribute from StudyIntervention class</t>
+  </si>
+  <si>
+    <t>CDISC DDF Study Intervention Attribute Terminology</t>
+  </si>
+  <si>
+    <t>Update codelist reference information</t>
+  </si>
+  <si>
+    <t>C207547</t>
+  </si>
+  <si>
+    <t>Study Design Characteristic</t>
+  </si>
+  <si>
+    <t>The distinguishing qualities or prominent aspect of a study design.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW - Study Design Characteristics Response)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (C207416)</t>
+    </r>
+  </si>
+  <si>
+    <t>C207496</t>
+  </si>
+  <si>
+    <t>Protocol Approval Date Type</t>
+  </si>
+  <si>
+    <t>A characterization or classification of the protocol approval date.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW - Governance Date Type Response)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (C207413)</t>
+    </r>
+  </si>
+  <si>
+    <t>C207540</t>
+  </si>
+  <si>
+    <t>Study Amendment Reason Code</t>
+  </si>
+  <si>
+    <t>A symbol or combination of symbols which is assigned to the study amendment reason.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW - Study Amendment Reason Response)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (C207415)</t>
+    </r>
+  </si>
+  <si>
+    <t>C207495</t>
+  </si>
+  <si>
+    <t>Geographic Scope Type</t>
+  </si>
+  <si>
+    <t>A characterization or classification of the geographic scope.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW - Geographic Scope Type Response)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (C207412)</t>
+    </r>
+  </si>
+  <si>
+    <t>C207560</t>
+  </si>
+  <si>
+    <t>Study Intervention Role</t>
+  </si>
+  <si>
+    <t>Study Intervention Use</t>
+  </si>
+  <si>
+    <t>The intended use of the trial intervention within the context of the study design.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW - Study Intervention Role Response)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (C207417)</t>
+    </r>
+  </si>
+  <si>
+    <t>productDesignation</t>
+  </si>
+  <si>
+    <t>C207559</t>
+  </si>
+  <si>
+    <t>Study Intervention Product Designation</t>
+  </si>
+  <si>
+    <t>An indication as to whether the investigational intervention is an investigational medicinal product or an auxiliary medicinal product.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW - Study Intervention Product Designation Response)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (C207418)</t>
+    </r>
+  </si>
+  <si>
+    <t>C207568</t>
+  </si>
+  <si>
+    <t>Study Title Type</t>
+  </si>
+  <si>
+    <t>A characterization or classification of the study title.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW-Study Title Type Response)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (C207419)</t>
+    </r>
+  </si>
+  <si>
+    <t>C207506</t>
+  </si>
+  <si>
+    <t>Masking Role</t>
+  </si>
+  <si>
+    <t>Blinded Roles; Blinding Roles</t>
+  </si>
+  <si>
+    <t>An identifying designation assigned to a masked individual within a study that corresponds with their function.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW - Masking Role Response)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (C207414)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW Study Definition Document Type Response)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y (CNEW Reference Identifier Type Response)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -23227,7 +23911,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -23691,10 +24375,1281 @@
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
     </row>
+    <row r="13" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>1955</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>1990</v>
+      </c>
+      <c r="E13" s="69" t="s">
+        <v>1991</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16" t="s">
+        <v>1992</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+    </row>
+    <row r="14" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>1993</v>
+      </c>
+      <c r="E14" s="71" t="s">
+        <v>1993</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>1683</v>
+      </c>
+      <c r="G14" s="13"/>
+      <c r="H14" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>1994</v>
+      </c>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16" t="s">
+        <v>1995</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+    </row>
+    <row r="15" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>1996</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>1993</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>1670</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>1671</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>1997</v>
+      </c>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16" t="s">
+        <v>1998</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>1614</v>
+      </c>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+    </row>
+    <row r="16" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>1996</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>1993</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>1675</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>1671</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>1999</v>
+      </c>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16" t="s">
+        <v>2000</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>1614</v>
+      </c>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+    </row>
+    <row r="17" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>1996</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>1993</v>
+      </c>
+      <c r="E17" s="44" t="s">
+        <v>1678</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>1671</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>2001</v>
+      </c>
+      <c r="J17" s="16"/>
+      <c r="K17" s="25" t="s">
+        <v>2002</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>1614</v>
+      </c>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+    </row>
+    <row r="18" spans="1:14" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>2003</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>1996</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>1993</v>
+      </c>
+      <c r="E18" s="70" t="s">
+        <v>2004</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="16" t="s">
+        <v>2005</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>2006</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>2006</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>2007</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>2008</v>
+      </c>
+      <c r="M18" s="63" t="s">
+        <v>2009</v>
+      </c>
+      <c r="N18" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>2003</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>1996</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>1993</v>
+      </c>
+      <c r="E19" s="70" t="s">
+        <v>2010</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="15" t="s">
+        <v>2011</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>2012</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>2012</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>2013</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>2014</v>
+      </c>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+    </row>
+    <row r="20" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>1993</v>
+      </c>
+      <c r="E20" s="69" t="s">
+        <v>1612</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="G20" s="13"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16" t="s">
+        <v>2015</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>928</v>
+      </c>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+    </row>
+    <row r="21" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>1993</v>
+      </c>
+      <c r="E21" s="69" t="s">
+        <v>2016</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16" t="s">
+        <v>2017</v>
+      </c>
+      <c r="L21" s="16" t="s">
+        <v>928</v>
+      </c>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+    </row>
+    <row r="22" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>1993</v>
+      </c>
+      <c r="E22" s="69" t="s">
+        <v>1527</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16" t="s">
+        <v>2018</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>928</v>
+      </c>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+    </row>
+    <row r="23" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>1993</v>
+      </c>
+      <c r="E23" s="69" t="s">
+        <v>2019</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16" t="s">
+        <v>2020</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>928</v>
+      </c>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+    </row>
+    <row r="24" spans="1:14" ht="25" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>2021</v>
+      </c>
+      <c r="E24" s="45" t="s">
+        <v>2021</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>1683</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>2022</v>
+      </c>
+      <c r="J24" s="16"/>
+      <c r="K24" s="15" t="s">
+        <v>2023</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>928</v>
+      </c>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+    </row>
+    <row r="25" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>2024</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>2021</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>1689</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>1671</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>1951</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>2025</v>
+      </c>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16" t="s">
+        <v>2026</v>
+      </c>
+      <c r="L25" s="16" t="s">
+        <v>1614</v>
+      </c>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+    </row>
+    <row r="26" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>2021</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>1989</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>1951</v>
+      </c>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16" t="s">
+        <v>2027</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>928</v>
+      </c>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+    </row>
+    <row r="27" spans="1:14" ht="25" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>2028</v>
+      </c>
+      <c r="E27" s="45" t="s">
+        <v>2028</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>1683</v>
+      </c>
+      <c r="G27" s="13"/>
+      <c r="H27" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>2029</v>
+      </c>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16" t="s">
+        <v>2030</v>
+      </c>
+      <c r="L27" s="16" t="s">
+        <v>928</v>
+      </c>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+    </row>
+    <row r="28" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>2031</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>2028</v>
+      </c>
+      <c r="E28" s="44" t="s">
+        <v>1670</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>1671</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>2032</v>
+      </c>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16" t="s">
+        <v>2033</v>
+      </c>
+      <c r="L28" s="16" t="s">
+        <v>1614</v>
+      </c>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+    </row>
+    <row r="29" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>2031</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>2028</v>
+      </c>
+      <c r="E29" s="44" t="s">
+        <v>1689</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>1671</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>2034</v>
+      </c>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16" t="s">
+        <v>2035</v>
+      </c>
+      <c r="L29" s="16" t="s">
+        <v>1614</v>
+      </c>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+    </row>
+    <row r="30" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>2031</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>2028</v>
+      </c>
+      <c r="E30" s="44" t="s">
+        <v>2036</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>2037</v>
+      </c>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16" t="s">
+        <v>2038</v>
+      </c>
+      <c r="L30" s="16" t="s">
+        <v>1614</v>
+      </c>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+    </row>
+    <row r="31" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>2031</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>2028</v>
+      </c>
+      <c r="E31" s="44" t="s">
+        <v>1778</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="H31" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>2039</v>
+      </c>
+      <c r="J31" s="16"/>
+      <c r="K31" s="15" t="s">
+        <v>2040</v>
+      </c>
+      <c r="L31" s="16" t="s">
+        <v>1781</v>
+      </c>
+      <c r="M31" s="13"/>
+      <c r="N31" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>2041</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>2042</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>2028</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>2043</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="H32" s="16" t="s">
+        <v>2044</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>2045</v>
+      </c>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16" t="s">
+        <v>2046</v>
+      </c>
+      <c r="L32" s="16" t="s">
+        <v>928</v>
+      </c>
+      <c r="M32" s="13"/>
+      <c r="N32" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>2047</v>
+      </c>
+      <c r="E33" s="45" t="s">
+        <v>2047</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>1683</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="16" t="s">
+        <v>2048</v>
+      </c>
+      <c r="I33" s="16" t="s">
+        <v>2047</v>
+      </c>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16" t="s">
+        <v>2049</v>
+      </c>
+      <c r="L33" s="16" t="s">
+        <v>928</v>
+      </c>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+    </row>
+    <row r="34" spans="1:14" ht="25" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>2050</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>2047</v>
+      </c>
+      <c r="E34" s="44" t="s">
+        <v>1670</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>1671</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>2051</v>
+      </c>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16" t="s">
+        <v>2052</v>
+      </c>
+      <c r="L34" s="16" t="s">
+        <v>1614</v>
+      </c>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+    </row>
+    <row r="35" spans="1:14" ht="25" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>2050</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>2047</v>
+      </c>
+      <c r="E35" s="44" t="s">
+        <v>1675</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>1671</v>
+      </c>
+      <c r="G35" s="13"/>
+      <c r="H35" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>2053</v>
+      </c>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16" t="s">
+        <v>2054</v>
+      </c>
+      <c r="L35" s="16" t="s">
+        <v>1614</v>
+      </c>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+    </row>
+    <row r="36" spans="1:14" ht="25" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>2050</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>2047</v>
+      </c>
+      <c r="E36" s="44" t="s">
+        <v>1678</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>1671</v>
+      </c>
+      <c r="G36" s="13"/>
+      <c r="H36" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I36" s="16" t="s">
+        <v>2055</v>
+      </c>
+      <c r="J36" s="16"/>
+      <c r="K36" s="25" t="s">
+        <v>2056</v>
+      </c>
+      <c r="L36" s="16" t="s">
+        <v>1614</v>
+      </c>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+    </row>
+    <row r="37" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>2050</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>2047</v>
+      </c>
+      <c r="E37" s="44" t="s">
+        <v>2057</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G37" s="13"/>
+      <c r="H37" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I37" s="16" t="s">
+        <v>2058</v>
+      </c>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16" t="s">
+        <v>2059</v>
+      </c>
+      <c r="L37" s="16" t="s">
+        <v>2060</v>
+      </c>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+    </row>
+    <row r="38" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>2047</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>2061</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="G38" s="13"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16" t="s">
+        <v>2062</v>
+      </c>
+      <c r="L38" s="16" t="s">
+        <v>928</v>
+      </c>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+    </row>
+    <row r="39" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>2047</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>2063</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="G39" s="13"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16" t="s">
+        <v>2064</v>
+      </c>
+      <c r="L39" s="16" t="s">
+        <v>928</v>
+      </c>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+    </row>
+    <row r="40" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>2065</v>
+      </c>
+      <c r="E40" s="45" t="s">
+        <v>2065</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>1683</v>
+      </c>
+      <c r="G40" s="13"/>
+      <c r="H40" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I40" s="16" t="s">
+        <v>2066</v>
+      </c>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16" t="s">
+        <v>2067</v>
+      </c>
+      <c r="L40" s="16" t="s">
+        <v>928</v>
+      </c>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+    </row>
+    <row r="41" spans="1:14" ht="25" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>2068</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>2065</v>
+      </c>
+      <c r="E41" s="44" t="s">
+        <v>1670</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>1671</v>
+      </c>
+      <c r="G41" s="13"/>
+      <c r="H41" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I41" s="16" t="s">
+        <v>2069</v>
+      </c>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16" t="s">
+        <v>2070</v>
+      </c>
+      <c r="L41" s="16" t="s">
+        <v>1614</v>
+      </c>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+    </row>
+    <row r="42" spans="1:14" ht="25" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>2068</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>2065</v>
+      </c>
+      <c r="E42" s="44" t="s">
+        <v>1675</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>1671</v>
+      </c>
+      <c r="G42" s="13"/>
+      <c r="H42" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I42" s="16" t="s">
+        <v>2071</v>
+      </c>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16" t="s">
+        <v>2072</v>
+      </c>
+      <c r="L42" s="16" t="s">
+        <v>1614</v>
+      </c>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+    </row>
+    <row r="43" spans="1:14" ht="25" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>2068</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>2065</v>
+      </c>
+      <c r="E43" s="44" t="s">
+        <v>1678</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>1671</v>
+      </c>
+      <c r="G43" s="13"/>
+      <c r="H43" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I43" s="16" t="s">
+        <v>2073</v>
+      </c>
+      <c r="J43" s="16"/>
+      <c r="K43" s="25" t="s">
+        <v>2074</v>
+      </c>
+      <c r="L43" s="16" t="s">
+        <v>1614</v>
+      </c>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+    </row>
+    <row r="44" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>2065</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>2075</v>
+      </c>
+      <c r="F44" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="G44" s="13"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16" t="s">
+        <v>2076</v>
+      </c>
+      <c r="L44" s="16" t="s">
+        <v>928</v>
+      </c>
+      <c r="M44" s="13"/>
+      <c r="N44" s="13"/>
+    </row>
+    <row r="45" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>2065</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>2077</v>
+      </c>
+      <c r="F45" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="G45" s="13"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16" t="s">
+        <v>2078</v>
+      </c>
+      <c r="L45" s="16" t="s">
+        <v>928</v>
+      </c>
+      <c r="M45" s="13"/>
+      <c r="N45" s="13"/>
+    </row>
+    <row r="46" spans="1:14" ht="25" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>2079</v>
+      </c>
+      <c r="E46" s="45" t="s">
+        <v>2079</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>1683</v>
+      </c>
+      <c r="G46" s="13"/>
+      <c r="H46" s="16" t="s">
+        <v>2080</v>
+      </c>
+      <c r="I46" s="16" t="s">
+        <v>2079</v>
+      </c>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16" t="s">
+        <v>2081</v>
+      </c>
+      <c r="L46" s="16" t="s">
+        <v>928</v>
+      </c>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+    </row>
+    <row r="47" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
+        <v>2082</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>2083</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>2079</v>
+      </c>
+      <c r="E47" s="44" t="s">
+        <v>2084</v>
+      </c>
+      <c r="F47" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G47" s="13"/>
+      <c r="H47" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I47" s="16" t="s">
+        <v>2085</v>
+      </c>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16" t="s">
+        <v>2086</v>
+      </c>
+      <c r="L47" s="16" t="s">
+        <v>2087</v>
+      </c>
+      <c r="M47" s="13" t="s">
+        <v>2088</v>
+      </c>
+      <c r="N47" s="13"/>
+    </row>
+    <row r="48" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>2079</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>2089</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="G48" s="13"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16" t="s">
+        <v>2090</v>
+      </c>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C12">
     <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="M18" r:id="rId1" xr:uid="{51B40971-21A8-4D77-9B34-E5A907A6FD59}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -23704,7 +25659,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -23839,6 +25794,348 @@
       </c>
       <c r="M3" s="13"/>
       <c r="N3" s="13"/>
+    </row>
+    <row r="4" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>2091</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>2092</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>2010</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G4" s="68"/>
+      <c r="H4" s="39" t="s">
+        <v>2011</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>2012</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>2012</v>
+      </c>
+      <c r="K4" s="38" t="s">
+        <v>2013</v>
+      </c>
+      <c r="L4" s="38" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="15" t="s">
+        <v>907</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="44" t="s">
+        <v>1407</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>2094</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>2095</v>
+      </c>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25" t="s">
+        <v>2096</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="16" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="F6" s="25"/>
+      <c r="G6" s="44" t="s">
+        <v>1778</v>
+      </c>
+      <c r="H6" s="62" t="s">
+        <v>2098</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>2099</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="16" t="s">
+        <v>2100</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>2101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="16" t="s">
+        <v>1717</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="F7" s="25"/>
+      <c r="G7" s="65" t="s">
+        <v>2057</v>
+      </c>
+      <c r="H7" s="62" t="s">
+        <v>2102</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>2103</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>2103</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>2104</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="15" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="44" t="s">
+        <v>1778</v>
+      </c>
+      <c r="H8" s="62" t="s">
+        <v>2106</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>2107</v>
+      </c>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="27" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="F9" s="16"/>
+      <c r="G9" s="44" t="s">
+        <v>2084</v>
+      </c>
+      <c r="H9" s="62" t="s">
+        <v>2110</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>2111</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>2112</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>2113</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>2114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="27" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="65" t="s">
+        <v>2115</v>
+      </c>
+      <c r="H10" s="62" t="s">
+        <v>2116</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>2117</v>
+      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="15" t="s">
+        <v>2118</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>2119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="15" t="s">
+        <v>1732</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="44" t="s">
+        <v>1778</v>
+      </c>
+      <c r="H11" s="62" t="s">
+        <v>2120</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>2121</v>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="16" t="s">
+        <v>2122</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>2123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="16" t="s">
+        <v>1711</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="F12" s="27"/>
+      <c r="G12" s="44" t="s">
+        <v>2084</v>
+      </c>
+      <c r="H12" s="62" t="s">
+        <v>2124</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>2125</v>
+      </c>
+      <c r="J12" s="25" t="s">
+        <v>2126</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>2127</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="15" t="s">
+        <v>1759</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="F13" s="27"/>
+      <c r="G13" s="44" t="s">
+        <v>1778</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>1779</v>
+      </c>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16" t="s">
+        <v>1780</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="27" t="s">
+        <v>1958</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>1603</v>
+      </c>
+      <c r="F14" s="27"/>
+      <c r="G14" s="65" t="s">
+        <v>1778</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>1962</v>
+      </c>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16" t="s">
+        <v>1963</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>2130</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3">

</xml_diff>

<commit_message>
Sprint 7 final changes
to support tickets 316, 444, 456
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40D33BE-FED9-47F4-B073-F4C5C0ECC249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B583ABD-6B35-4034-BEAF-F15F8033BFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="300" windowWidth="16990" windowHeight="9810" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="990" windowWidth="16990" windowHeight="9810" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5244" uniqueCount="2131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5244" uniqueCount="2132">
   <si>
     <t>Code</t>
   </si>
@@ -7808,13 +7808,7 @@
     <t>scope</t>
   </si>
   <si>
-    <t>Administration</t>
-  </si>
-  <si>
     <t>administrableProduct</t>
-  </si>
-  <si>
-    <t>A USDM relationship between the Administration and AdministrableProductDefinition classes which identifies the administrable product associated with the administration.</t>
   </si>
   <si>
     <t>AdministrableProduct</t>
@@ -8490,6 +8484,15 @@
       </rPr>
       <t>Y (CNEW Reference Identifier Type Response)</t>
     </r>
+  </si>
+  <si>
+    <t>A USDM relationship between the AgentAdministration and AdministrableProductDefinition classes which identifies the administrable product associated with the agent administration.</t>
+  </si>
+  <si>
+    <t>Y (CNEW Administrable Product Property Type)</t>
+  </si>
+  <si>
+    <t>Y (Points to external codelists such as UNII, MED-RT)</t>
   </si>
 </sst>
 </file>
@@ -24375,7 +24378,7 @@
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
     </row>
-    <row r="13" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>1955</v>
       </c>
@@ -24385,11 +24388,11 @@
       <c r="C13" s="13" t="s">
         <v>928</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="16" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E13" s="69" t="s">
         <v>1990</v>
-      </c>
-      <c r="E13" s="69" t="s">
-        <v>1991</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>913</v>
@@ -24399,7 +24402,7 @@
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
       <c r="K13" s="16" t="s">
-        <v>1992</v>
+        <v>2129</v>
       </c>
       <c r="L13" s="13" t="s">
         <v>928</v>
@@ -24418,10 +24421,10 @@
         <v>119</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="E14" s="71" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>1683</v>
@@ -24431,11 +24434,11 @@
         <v>1672</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="J14" s="16"/>
       <c r="K14" s="16" t="s">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="L14" s="13" t="s">
         <v>928</v>
@@ -24451,10 +24454,10 @@
         <v>1672</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="E15" s="44" t="s">
         <v>1670</v>
@@ -24467,11 +24470,11 @@
         <v>1672</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="J15" s="16"/>
       <c r="K15" s="16" t="s">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="L15" s="13" t="s">
         <v>1614</v>
@@ -24487,10 +24490,10 @@
         <v>1672</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="E16" s="44" t="s">
         <v>1675</v>
@@ -24503,11 +24506,11 @@
         <v>1672</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="J16" s="16"/>
       <c r="K16" s="16" t="s">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="L16" s="13" t="s">
         <v>1614</v>
@@ -24523,10 +24526,10 @@
         <v>1672</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="E17" s="44" t="s">
         <v>1678</v>
@@ -24539,11 +24542,11 @@
         <v>1672</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="J17" s="16"/>
       <c r="K17" s="25" t="s">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="L17" s="13" t="s">
         <v>1614</v>
@@ -24553,41 +24556,41 @@
     </row>
     <row r="18" spans="1:14" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="E18" s="70" t="s">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>1603</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="16" t="s">
+        <v>2003</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>2004</v>
+      </c>
+      <c r="K18" s="16" t="s">
         <v>2005</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="L18" s="16" t="s">
         <v>2006</v>
       </c>
-      <c r="J18" s="16" t="s">
-        <v>2006</v>
-      </c>
-      <c r="K18" s="16" t="s">
+      <c r="M18" s="63" t="s">
         <v>2007</v>
-      </c>
-      <c r="L18" s="16" t="s">
-        <v>2008</v>
-      </c>
-      <c r="M18" s="63" t="s">
-        <v>2009</v>
       </c>
       <c r="N18" s="16" t="s">
         <v>9</v>
@@ -24595,38 +24598,38 @@
     </row>
     <row r="19" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="E19" s="70" t="s">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>1603</v>
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="15" t="s">
+        <v>2009</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>2010</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>2010</v>
+      </c>
+      <c r="K19" s="13" t="s">
         <v>2011</v>
       </c>
-      <c r="I19" s="16" t="s">
-        <v>2012</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>2012</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>2013</v>
-      </c>
       <c r="L19" s="16" t="s">
-        <v>2014</v>
+        <v>2131</v>
       </c>
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
@@ -24642,7 +24645,7 @@
         <v>928</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="E20" s="69" t="s">
         <v>1612</v>
@@ -24655,7 +24658,7 @@
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
       <c r="K20" s="16" t="s">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="L20" s="16" t="s">
         <v>928</v>
@@ -24674,10 +24677,10 @@
         <v>928</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="E21" s="69" t="s">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>913</v>
@@ -24687,7 +24690,7 @@
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
       <c r="K21" s="16" t="s">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="L21" s="16" t="s">
         <v>928</v>
@@ -24706,7 +24709,7 @@
         <v>928</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="E22" s="69" t="s">
         <v>1527</v>
@@ -24719,7 +24722,7 @@
       <c r="I22" s="16"/>
       <c r="J22" s="16"/>
       <c r="K22" s="16" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="L22" s="16" t="s">
         <v>928</v>
@@ -24738,10 +24741,10 @@
         <v>928</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="E23" s="69" t="s">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>913</v>
@@ -24751,7 +24754,7 @@
       <c r="I23" s="16"/>
       <c r="J23" s="16"/>
       <c r="K23" s="16" t="s">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="L23" s="16" t="s">
         <v>928</v>
@@ -24770,10 +24773,10 @@
         <v>119</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="E24" s="45" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="F24" s="13" t="s">
         <v>1683</v>
@@ -24783,11 +24786,11 @@
         <v>1672</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="J24" s="16"/>
       <c r="K24" s="15" t="s">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="L24" s="16" t="s">
         <v>928</v>
@@ -24803,10 +24806,10 @@
         <v>1672</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="E25" s="44" t="s">
         <v>1689</v>
@@ -24821,11 +24824,11 @@
         <v>1672</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="J25" s="16"/>
       <c r="K25" s="16" t="s">
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="L25" s="16" t="s">
         <v>1614</v>
@@ -24844,7 +24847,7 @@
         <v>928</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="E26" s="17" t="s">
         <v>1989</v>
@@ -24859,7 +24862,7 @@
       <c r="I26" s="16"/>
       <c r="J26" s="16"/>
       <c r="K26" s="16" t="s">
-        <v>2027</v>
+        <v>2025</v>
       </c>
       <c r="L26" s="16" t="s">
         <v>928</v>
@@ -24878,10 +24881,10 @@
         <v>119</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="E27" s="45" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="F27" s="13" t="s">
         <v>1683</v>
@@ -24891,11 +24894,11 @@
         <v>1672</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>2029</v>
+        <v>2027</v>
       </c>
       <c r="J27" s="16"/>
       <c r="K27" s="16" t="s">
-        <v>2030</v>
+        <v>2028</v>
       </c>
       <c r="L27" s="16" t="s">
         <v>928</v>
@@ -24911,10 +24914,10 @@
         <v>1672</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>2031</v>
+        <v>2029</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="E28" s="44" t="s">
         <v>1670</v>
@@ -24927,11 +24930,11 @@
         <v>1672</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="J28" s="16"/>
       <c r="K28" s="16" t="s">
-        <v>2033</v>
+        <v>2031</v>
       </c>
       <c r="L28" s="16" t="s">
         <v>1614</v>
@@ -24947,10 +24950,10 @@
         <v>1672</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>2031</v>
+        <v>2029</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="E29" s="44" t="s">
         <v>1689</v>
@@ -24963,11 +24966,11 @@
         <v>1672</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>2034</v>
+        <v>2032</v>
       </c>
       <c r="J29" s="16"/>
       <c r="K29" s="16" t="s">
-        <v>2035</v>
+        <v>2033</v>
       </c>
       <c r="L29" s="16" t="s">
         <v>1614</v>
@@ -24983,13 +24986,13 @@
         <v>1672</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>2031</v>
+        <v>2029</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="E30" s="44" t="s">
-        <v>2036</v>
+        <v>2034</v>
       </c>
       <c r="F30" s="16" t="s">
         <v>1603</v>
@@ -24999,11 +25002,11 @@
         <v>1672</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>2037</v>
+        <v>2035</v>
       </c>
       <c r="J30" s="16"/>
       <c r="K30" s="16" t="s">
-        <v>2038</v>
+        <v>2036</v>
       </c>
       <c r="L30" s="16" t="s">
         <v>1614</v>
@@ -25011,7 +25014,7 @@
       <c r="M30" s="13"/>
       <c r="N30" s="13"/>
     </row>
-    <row r="31" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>1976</v>
       </c>
@@ -25019,10 +25022,10 @@
         <v>1672</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>2031</v>
+        <v>2029</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="E31" s="44" t="s">
         <v>1778</v>
@@ -25035,14 +25038,14 @@
         <v>1672</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>2039</v>
+        <v>2037</v>
       </c>
       <c r="J31" s="16"/>
       <c r="K31" s="15" t="s">
-        <v>2040</v>
+        <v>2038</v>
       </c>
       <c r="L31" s="16" t="s">
-        <v>1781</v>
+        <v>2130</v>
       </c>
       <c r="M31" s="13"/>
       <c r="N31" s="16" t="s">
@@ -25051,33 +25054,33 @@
     </row>
     <row r="32" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>2041</v>
+        <v>2039</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>2042</v>
+        <v>2040</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>2043</v>
+        <v>2041</v>
       </c>
       <c r="F32" s="17" t="s">
         <v>1701</v>
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="16" t="s">
-        <v>2044</v>
+        <v>2042</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>2045</v>
+        <v>2043</v>
       </c>
       <c r="J32" s="16"/>
       <c r="K32" s="16" t="s">
-        <v>2046</v>
+        <v>2044</v>
       </c>
       <c r="L32" s="16" t="s">
         <v>928</v>
@@ -25098,24 +25101,24 @@
         <v>119</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="E33" s="45" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="F33" s="13" t="s">
         <v>1683</v>
       </c>
       <c r="G33" s="13"/>
       <c r="H33" s="16" t="s">
-        <v>2048</v>
+        <v>2046</v>
       </c>
       <c r="I33" s="16" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="J33" s="16"/>
       <c r="K33" s="16" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="L33" s="16" t="s">
         <v>928</v>
@@ -25131,10 +25134,10 @@
         <v>1672</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="E34" s="44" t="s">
         <v>1670</v>
@@ -25147,11 +25150,11 @@
         <v>1672</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>2051</v>
+        <v>2049</v>
       </c>
       <c r="J34" s="16"/>
       <c r="K34" s="16" t="s">
-        <v>2052</v>
+        <v>2050</v>
       </c>
       <c r="L34" s="16" t="s">
         <v>1614</v>
@@ -25167,10 +25170,10 @@
         <v>1672</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="E35" s="44" t="s">
         <v>1675</v>
@@ -25183,11 +25186,11 @@
         <v>1672</v>
       </c>
       <c r="I35" s="16" t="s">
-        <v>2053</v>
+        <v>2051</v>
       </c>
       <c r="J35" s="16"/>
       <c r="K35" s="16" t="s">
-        <v>2054</v>
+        <v>2052</v>
       </c>
       <c r="L35" s="16" t="s">
         <v>1614</v>
@@ -25203,10 +25206,10 @@
         <v>1672</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="E36" s="44" t="s">
         <v>1678</v>
@@ -25219,11 +25222,11 @@
         <v>1672</v>
       </c>
       <c r="I36" s="16" t="s">
-        <v>2055</v>
+        <v>2053</v>
       </c>
       <c r="J36" s="16"/>
       <c r="K36" s="25" t="s">
-        <v>2056</v>
+        <v>2054</v>
       </c>
       <c r="L36" s="16" t="s">
         <v>1614</v>
@@ -25239,13 +25242,13 @@
         <v>1672</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="E37" s="44" t="s">
-        <v>2057</v>
+        <v>2055</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>1603</v>
@@ -25255,14 +25258,14 @@
         <v>1672</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>2058</v>
+        <v>2056</v>
       </c>
       <c r="J37" s="16"/>
       <c r="K37" s="16" t="s">
-        <v>2059</v>
+        <v>2057</v>
       </c>
       <c r="L37" s="16" t="s">
-        <v>2060</v>
+        <v>2058</v>
       </c>
       <c r="M37" s="13"/>
       <c r="N37" s="13"/>
@@ -25278,10 +25281,10 @@
         <v>928</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>2061</v>
+        <v>2059</v>
       </c>
       <c r="F38" s="16" t="s">
         <v>913</v>
@@ -25291,7 +25294,7 @@
       <c r="I38" s="16"/>
       <c r="J38" s="16"/>
       <c r="K38" s="16" t="s">
-        <v>2062</v>
+        <v>2060</v>
       </c>
       <c r="L38" s="16" t="s">
         <v>928</v>
@@ -25310,10 +25313,10 @@
         <v>928</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>2063</v>
+        <v>2061</v>
       </c>
       <c r="F39" s="16" t="s">
         <v>913</v>
@@ -25323,7 +25326,7 @@
       <c r="I39" s="16"/>
       <c r="J39" s="16"/>
       <c r="K39" s="16" t="s">
-        <v>2064</v>
+        <v>2062</v>
       </c>
       <c r="L39" s="16" t="s">
         <v>928</v>
@@ -25342,10 +25345,10 @@
         <v>119</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>2065</v>
+        <v>2063</v>
       </c>
       <c r="E40" s="45" t="s">
-        <v>2065</v>
+        <v>2063</v>
       </c>
       <c r="F40" s="13" t="s">
         <v>1683</v>
@@ -25355,11 +25358,11 @@
         <v>1672</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>2066</v>
+        <v>2064</v>
       </c>
       <c r="J40" s="16"/>
       <c r="K40" s="16" t="s">
-        <v>2067</v>
+        <v>2065</v>
       </c>
       <c r="L40" s="16" t="s">
         <v>928</v>
@@ -25375,10 +25378,10 @@
         <v>1672</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>2068</v>
+        <v>2066</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>2065</v>
+        <v>2063</v>
       </c>
       <c r="E41" s="44" t="s">
         <v>1670</v>
@@ -25391,11 +25394,11 @@
         <v>1672</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>2069</v>
+        <v>2067</v>
       </c>
       <c r="J41" s="16"/>
       <c r="K41" s="16" t="s">
-        <v>2070</v>
+        <v>2068</v>
       </c>
       <c r="L41" s="16" t="s">
         <v>1614</v>
@@ -25411,10 +25414,10 @@
         <v>1672</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>2068</v>
+        <v>2066</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>2065</v>
+        <v>2063</v>
       </c>
       <c r="E42" s="44" t="s">
         <v>1675</v>
@@ -25427,11 +25430,11 @@
         <v>1672</v>
       </c>
       <c r="I42" s="16" t="s">
-        <v>2071</v>
+        <v>2069</v>
       </c>
       <c r="J42" s="16"/>
       <c r="K42" s="16" t="s">
-        <v>2072</v>
+        <v>2070</v>
       </c>
       <c r="L42" s="16" t="s">
         <v>1614</v>
@@ -25447,10 +25450,10 @@
         <v>1672</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>2068</v>
+        <v>2066</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>2065</v>
+        <v>2063</v>
       </c>
       <c r="E43" s="44" t="s">
         <v>1678</v>
@@ -25463,11 +25466,11 @@
         <v>1672</v>
       </c>
       <c r="I43" s="16" t="s">
-        <v>2073</v>
+        <v>2071</v>
       </c>
       <c r="J43" s="16"/>
       <c r="K43" s="25" t="s">
-        <v>2074</v>
+        <v>2072</v>
       </c>
       <c r="L43" s="16" t="s">
         <v>1614</v>
@@ -25486,10 +25489,10 @@
         <v>928</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>2065</v>
+        <v>2063</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>2075</v>
+        <v>2073</v>
       </c>
       <c r="F44" s="16" t="s">
         <v>913</v>
@@ -25499,7 +25502,7 @@
       <c r="I44" s="16"/>
       <c r="J44" s="16"/>
       <c r="K44" s="16" t="s">
-        <v>2076</v>
+        <v>2074</v>
       </c>
       <c r="L44" s="16" t="s">
         <v>928</v>
@@ -25518,10 +25521,10 @@
         <v>928</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>2065</v>
+        <v>2063</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>2077</v>
+        <v>2075</v>
       </c>
       <c r="F45" s="16" t="s">
         <v>913</v>
@@ -25531,7 +25534,7 @@
       <c r="I45" s="16"/>
       <c r="J45" s="16"/>
       <c r="K45" s="16" t="s">
-        <v>2078</v>
+        <v>2076</v>
       </c>
       <c r="L45" s="16" t="s">
         <v>928</v>
@@ -25550,24 +25553,24 @@
         <v>119</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>2079</v>
+        <v>2077</v>
       </c>
       <c r="E46" s="45" t="s">
-        <v>2079</v>
+        <v>2077</v>
       </c>
       <c r="F46" s="13" t="s">
         <v>1683</v>
       </c>
       <c r="G46" s="13"/>
       <c r="H46" s="16" t="s">
-        <v>2080</v>
+        <v>2078</v>
       </c>
       <c r="I46" s="16" t="s">
-        <v>2079</v>
+        <v>2077</v>
       </c>
       <c r="J46" s="16"/>
       <c r="K46" s="16" t="s">
-        <v>2081</v>
+        <v>2079</v>
       </c>
       <c r="L46" s="16" t="s">
         <v>928</v>
@@ -25577,19 +25580,19 @@
     </row>
     <row r="47" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>2082</v>
+        <v>2080</v>
       </c>
       <c r="B47" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>2083</v>
+        <v>2081</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>2079</v>
+        <v>2077</v>
       </c>
       <c r="E47" s="44" t="s">
-        <v>2084</v>
+        <v>2082</v>
       </c>
       <c r="F47" s="16" t="s">
         <v>1603</v>
@@ -25599,17 +25602,17 @@
         <v>1672</v>
       </c>
       <c r="I47" s="16" t="s">
-        <v>2085</v>
+        <v>2083</v>
       </c>
       <c r="J47" s="16"/>
       <c r="K47" s="16" t="s">
+        <v>2084</v>
+      </c>
+      <c r="L47" s="16" t="s">
+        <v>2085</v>
+      </c>
+      <c r="M47" s="13" t="s">
         <v>2086</v>
-      </c>
-      <c r="L47" s="16" t="s">
-        <v>2087</v>
-      </c>
-      <c r="M47" s="13" t="s">
-        <v>2088</v>
       </c>
       <c r="N47" s="13"/>
     </row>
@@ -25624,10 +25627,10 @@
         <v>928</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>2079</v>
+        <v>2077</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>2089</v>
+        <v>2087</v>
       </c>
       <c r="F48" s="16" t="s">
         <v>913</v>
@@ -25637,7 +25640,7 @@
       <c r="I48" s="16"/>
       <c r="J48" s="16"/>
       <c r="K48" s="16" t="s">
-        <v>2090</v>
+        <v>2088</v>
       </c>
       <c r="L48" s="13"/>
       <c r="M48" s="13"/>
@@ -25797,43 +25800,43 @@
     </row>
     <row r="4" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>2091</v>
+        <v>2089</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>220</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>2092</v>
+        <v>2090</v>
       </c>
       <c r="D4" s="43" t="s">
         <v>1143</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="F4" s="38" t="s">
         <v>1603</v>
       </c>
       <c r="G4" s="68"/>
       <c r="H4" s="39" t="s">
+        <v>2009</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>2010</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>2010</v>
+      </c>
+      <c r="K4" s="38" t="s">
         <v>2011</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="L4" s="38" t="s">
         <v>2012</v>
-      </c>
-      <c r="J4" s="38" t="s">
-        <v>2012</v>
-      </c>
-      <c r="K4" s="38" t="s">
-        <v>2013</v>
-      </c>
-      <c r="L4" s="38" t="s">
-        <v>2014</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -25848,22 +25851,22 @@
         <v>1407</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>2094</v>
+        <v>2092</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>2095</v>
+        <v>2093</v>
       </c>
       <c r="J5" s="25"/>
       <c r="K5" s="25" t="s">
-        <v>2096</v>
+        <v>2094</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>2097</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -25878,22 +25881,22 @@
         <v>1778</v>
       </c>
       <c r="H6" s="62" t="s">
-        <v>2098</v>
+        <v>2096</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>2099</v>
+        <v>2097</v>
       </c>
       <c r="J6" s="25"/>
       <c r="K6" s="16" t="s">
-        <v>2100</v>
+        <v>2098</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>2101</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -25905,27 +25908,27 @@
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="65" t="s">
-        <v>2057</v>
+        <v>2055</v>
       </c>
       <c r="H7" s="62" t="s">
+        <v>2100</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>2101</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>2101</v>
+      </c>
+      <c r="K7" s="16" t="s">
         <v>2102</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="L7" s="16" t="s">
         <v>2103</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>2103</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>2104</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>2105</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -25940,22 +25943,22 @@
         <v>1778</v>
       </c>
       <c r="H8" s="62" t="s">
-        <v>2106</v>
+        <v>2104</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>2107</v>
+        <v>2105</v>
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="25" t="s">
-        <v>2108</v>
+        <v>2106</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>2109</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -25967,27 +25970,27 @@
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="44" t="s">
-        <v>2084</v>
+        <v>2082</v>
       </c>
       <c r="H9" s="62" t="s">
+        <v>2108</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>2109</v>
+      </c>
+      <c r="J9" s="16" t="s">
         <v>2110</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="K9" s="15" t="s">
         <v>2111</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="L9" s="16" t="s">
         <v>2112</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>2113</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>2114</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -25999,25 +26002,25 @@
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="65" t="s">
+        <v>2113</v>
+      </c>
+      <c r="H10" s="62" t="s">
+        <v>2114</v>
+      </c>
+      <c r="I10" s="16" t="s">
         <v>2115</v>
-      </c>
-      <c r="H10" s="62" t="s">
-        <v>2116</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>2117</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="15" t="s">
-        <v>2118</v>
+        <v>2116</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>2119</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -26032,22 +26035,22 @@
         <v>1778</v>
       </c>
       <c r="H11" s="62" t="s">
-        <v>2120</v>
+        <v>2118</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>2121</v>
+        <v>2119</v>
       </c>
       <c r="J11" s="13"/>
       <c r="K11" s="16" t="s">
-        <v>2122</v>
+        <v>2120</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>2123</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -26059,27 +26062,27 @@
       </c>
       <c r="F12" s="27"/>
       <c r="G12" s="44" t="s">
-        <v>2084</v>
+        <v>2082</v>
       </c>
       <c r="H12" s="62" t="s">
+        <v>2122</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>2123</v>
+      </c>
+      <c r="J12" s="25" t="s">
         <v>2124</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="K12" s="16" t="s">
         <v>2125</v>
       </c>
-      <c r="J12" s="25" t="s">
+      <c r="L12" s="16" t="s">
         <v>2126</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>2127</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>2128</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -26104,12 +26107,12 @@
         <v>1780</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>2129</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -26134,7 +26137,7 @@
         <v>1963</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>2130</v>
+        <v>2128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added rest of StudyRole.code values
And removed Masking.role
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9764DEC8-265A-40C2-A854-1D081C4FB73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC02AC5-CF9B-43C7-AD1C-6F6209400612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1070" yWindow="250" windowWidth="15120" windowHeight="9970" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1270" yWindow="350" windowWidth="16480" windowHeight="9970" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5786" uniqueCount="2272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5933" uniqueCount="2316">
   <si>
     <t>Code</t>
   </si>
@@ -9541,6 +9541,138 @@
   </si>
   <si>
     <t>An external committee whose purpose is to evaluate study data and decide whether a study endpoint or other criterion has been met. (NCI)</t>
+  </si>
+  <si>
+    <t>Co-Sponsor</t>
+  </si>
+  <si>
+    <t>An individual, company, institution, or organization that is designated by the study sponsor as a vested partner in the study.</t>
+  </si>
+  <si>
+    <t>C25392</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>The organization defined as being responsible for creating the product as stated on the package in which the product is supplied. (BRIDG)</t>
+  </si>
+  <si>
+    <t>Local Sponsor</t>
+  </si>
+  <si>
+    <t>The sponsor's legal representative at a geographical region within which the sponsor has no legal presence. (ICH M11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regulatory Agency </t>
+  </si>
+  <si>
+    <t>C51876</t>
+  </si>
+  <si>
+    <t>Medical Expert</t>
+  </si>
+  <si>
+    <t>A physician or health care provider selected by the sponsor to be readily available to advise clinical trial officials on trial related medical questions or problems.</t>
+  </si>
+  <si>
+    <t>C142578</t>
+  </si>
+  <si>
+    <t>Independent Data Monitoring Committee</t>
+  </si>
+  <si>
+    <t>A committee established by the sponsor to assess at intervals the progress of a clinical trial, safety data, and critical efficacy variables and recommend to the sponsor whether to continue, modify, or terminate the trial. [ICH E9] (CDISC Glossary)</t>
+  </si>
+  <si>
+    <t>Dose Escalation Committee</t>
+  </si>
+  <si>
+    <t>A committee established to assess whether a dose adjustment is appropriate and to determine whether the maximum-tolerated dose had been attained, based on a review of available safety and efficacy data at specified time points.</t>
+  </si>
+  <si>
+    <t>C142489</t>
+  </si>
+  <si>
+    <t>Data Safety Monitoring Board</t>
+  </si>
+  <si>
+    <t>A group of independent experts who are appointed to monitor the safety and scientific integrity of a research intervention, protect the confidentiality of participant data, and to make recommendations to the sponsor regarding the stopping of the trial for safety, efficacy, or for futility. (clinicaltrials.gov)</t>
+  </si>
+  <si>
+    <t>C19924</t>
+  </si>
+  <si>
+    <t>Principal investigator</t>
+  </si>
+  <si>
+    <t>A person who has the primary responsibility for the conduct of a clinical study and study-related personnel at a study site. While a single-center study would not include a coordinating investigator, the investigator at the site would fulfill the same responsibilities as a principal investigator.</t>
+  </si>
+  <si>
+    <t>Clinical Trial Physician</t>
+  </si>
+  <si>
+    <t>Study Doctor</t>
+  </si>
+  <si>
+    <t>Any physician that is associated with clinical trial.</t>
+  </si>
+  <si>
+    <t>C51851</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>Project Coordinator</t>
+  </si>
+  <si>
+    <t>A staff member who is responsible for the overall integration and interaction of different people and different components of subject matter associated with a specific project.</t>
+  </si>
+  <si>
+    <t>C37984</t>
+  </si>
+  <si>
+    <t>Laboratory</t>
+  </si>
+  <si>
+    <t>An organization with the capability and competency to perform scientific research, experiments, and measurements. (BRIDG)</t>
+  </si>
+  <si>
+    <t>Pharmacovigilance</t>
+  </si>
+  <si>
+    <t>A group that is responsible for monitoring the safety of medicines and taking action to reduce their risks and increase their benefits.</t>
+  </si>
+  <si>
+    <t>C54148</t>
+  </si>
+  <si>
+    <t>Contract Research Organization</t>
+  </si>
+  <si>
+    <t>CRO</t>
+  </si>
+  <si>
+    <t>A person or an organization (commercial, academic, or other) contracted by the sponsor to perform one or more of a sponsor's trial-related duties and functions. [ICH E6 Glossary] (CDISC Glossary)</t>
+  </si>
+  <si>
+    <t>C80403</t>
+  </si>
+  <si>
+    <t>Study Site</t>
+  </si>
+  <si>
+    <t>The location at which a study investigator conducts study activities.</t>
+  </si>
+  <si>
+    <t>C51877</t>
+  </si>
+  <si>
+    <t>Statistician</t>
+  </si>
+  <si>
+    <t>A professional who specializes in applying statistical principles to experimental design and data analysis.</t>
   </si>
 </sst>
 </file>
@@ -10142,12 +10274,6 @@
     <xf numFmtId="0" fontId="16" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -10165,6 +10291,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -10657,10 +10789,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="90" t="s">
         <v>903</v>
       </c>
-      <c r="B1" s="85"/>
+      <c r="B1" s="91"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -12578,13 +12710,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29 H33">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="CNEW">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="CNEW">
       <formula>NOT(ISERROR(SEARCH("CNEW",H29)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27136,7 +27268,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -27761,7 +27893,7 @@
       <c r="D18" s="16" t="s">
         <v>2197</v>
       </c>
-      <c r="E18" s="87" t="s">
+      <c r="E18" s="85" t="s">
         <v>2052</v>
       </c>
       <c r="F18" s="16" t="s">
@@ -27796,7 +27928,7 @@
       <c r="C19" s="16" t="s">
         <v>2267</v>
       </c>
-      <c r="D19" s="88" t="s">
+      <c r="D19" s="86" t="s">
         <v>2197</v>
       </c>
       <c r="E19" s="15" t="s">
@@ -27836,7 +27968,7 @@
       <c r="C20" s="16" t="s">
         <v>2267</v>
       </c>
-      <c r="D20" s="88" t="s">
+      <c r="D20" s="86" t="s">
         <v>2197</v>
       </c>
       <c r="E20" s="15" t="s">
@@ -27874,7 +28006,7 @@
       <c r="C21" s="16" t="s">
         <v>2267</v>
       </c>
-      <c r="D21" s="88" t="s">
+      <c r="D21" s="86" t="s">
         <v>2197</v>
       </c>
       <c r="E21" s="15" t="s">
@@ -27912,7 +28044,7 @@
       <c r="C22" s="16" t="s">
         <v>2267</v>
       </c>
-      <c r="D22" s="88" t="s">
+      <c r="D22" s="86" t="s">
         <v>2197</v>
       </c>
       <c r="E22" s="15" t="s">
@@ -27950,7 +28082,7 @@
       <c r="C23" s="16" t="s">
         <v>2267</v>
       </c>
-      <c r="D23" s="88" t="s">
+      <c r="D23" s="86" t="s">
         <v>2197</v>
       </c>
       <c r="E23" s="15" t="s">
@@ -27988,7 +28120,7 @@
       <c r="C24" s="16" t="s">
         <v>2267</v>
       </c>
-      <c r="D24" s="88" t="s">
+      <c r="D24" s="86" t="s">
         <v>2197</v>
       </c>
       <c r="E24" s="15" t="s">
@@ -27998,14 +28130,14 @@
         <v>1701</v>
       </c>
       <c r="G24" s="13"/>
-      <c r="H24" s="89" t="s">
+      <c r="H24" s="87" t="s">
         <v>2268</v>
       </c>
-      <c r="I24" s="90" t="s">
+      <c r="I24" s="88" t="s">
         <v>2269</v>
       </c>
-      <c r="J24" s="90"/>
-      <c r="K24" s="91" t="s">
+      <c r="J24" s="88"/>
+      <c r="K24" s="89" t="s">
         <v>2271</v>
       </c>
       <c r="L24" s="16" t="s">
@@ -28016,9 +28148,511 @@
         <v>9</v>
       </c>
     </row>
+    <row r="25" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D25" s="86" t="s">
+        <v>2197</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G25" s="13"/>
+      <c r="H25" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>2272</v>
+      </c>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16" t="s">
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D26" s="86" t="s">
+        <v>2197</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" s="16" t="s">
+        <v>2274</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>2275</v>
+      </c>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16" t="s">
+        <v>2276</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D27" s="86" t="s">
+        <v>2197</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G27" s="13"/>
+      <c r="H27" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>2277</v>
+      </c>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16" t="s">
+        <v>2278</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D28" s="86" t="s">
+        <v>2197</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>2279</v>
+      </c>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D29" s="86" t="s">
+        <v>2197</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="16" t="s">
+        <v>2280</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>2281</v>
+      </c>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16" t="s">
+        <v>2282</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D30" s="86" t="s">
+        <v>2197</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="16" t="s">
+        <v>2283</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>2284</v>
+      </c>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16" t="s">
+        <v>2285</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D31" s="86" t="s">
+        <v>2197</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="H31" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>2286</v>
+      </c>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16" t="s">
+        <v>2287</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D32" s="86" t="s">
+        <v>2197</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="H32" s="16" t="s">
+        <v>2288</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>2289</v>
+      </c>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D33" s="86" t="s">
+        <v>2197</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="16" t="s">
+        <v>2291</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>2292</v>
+      </c>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16" t="s">
+        <v>2293</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D34" s="86" t="s">
+        <v>2197</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>2294</v>
+      </c>
+      <c r="J34" s="16" t="s">
+        <v>2295</v>
+      </c>
+      <c r="K34" s="16" t="s">
+        <v>2296</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D35" s="86" t="s">
+        <v>2197</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G35" s="13"/>
+      <c r="H35" s="16" t="s">
+        <v>2297</v>
+      </c>
+      <c r="I35" s="15" t="s">
+        <v>2298</v>
+      </c>
+      <c r="J35" s="16" t="s">
+        <v>2299</v>
+      </c>
+      <c r="K35" s="16" t="s">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D36" s="86" t="s">
+        <v>2197</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G36" s="13"/>
+      <c r="H36" s="16" t="s">
+        <v>2301</v>
+      </c>
+      <c r="I36" s="15" t="s">
+        <v>2302</v>
+      </c>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16" t="s">
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D37" s="86" t="s">
+        <v>2197</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G37" s="13"/>
+      <c r="H37" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="I37" s="15" t="s">
+        <v>2304</v>
+      </c>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16" t="s">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D38" s="86" t="s">
+        <v>2197</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G38" s="13"/>
+      <c r="H38" s="16" t="s">
+        <v>2306</v>
+      </c>
+      <c r="I38" s="16" t="s">
+        <v>2307</v>
+      </c>
+      <c r="J38" s="16" t="s">
+        <v>2308</v>
+      </c>
+      <c r="K38" s="16" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D39" s="86" t="s">
+        <v>2197</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G39" s="13"/>
+      <c r="H39" s="16" t="s">
+        <v>2310</v>
+      </c>
+      <c r="I39" s="16" t="s">
+        <v>2311</v>
+      </c>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16" t="s">
+        <v>2312</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D40" s="86" t="s">
+        <v>2197</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G40" s="13"/>
+      <c r="H40" s="16" t="s">
+        <v>2313</v>
+      </c>
+      <c r="I40" s="16" t="s">
+        <v>2314</v>
+      </c>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16" t="s">
+        <v>2315</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="I20">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -28032,7 +28666,9 @@
   </sheetPr>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -28813,16 +29449,16 @@
       </c>
       <c r="M21" s="25"/>
       <c r="N21" s="13"/>
-      <c r="O21" s="86" t="s">
+      <c r="O21" s="84" t="s">
         <v>2263</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I18">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -30564,7 +31200,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C12">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="M18" r:id="rId1" xr:uid="{51B40971-21A8-4D77-9B34-E5A907A6FD59}"/>
@@ -31403,7 +32039,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="M19" r:id="rId1" xr:uid="{6B67868F-51ED-422D-93DE-65481C699D06}"/>

</xml_diff>

<commit_message>
updated valid value sets tab
Changed organizationType to type in valid value sets tab.
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC02AC5-CF9B-43C7-AD1C-6F6209400612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BF6D6C-7F92-4588-90D6-5368A355167F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1270" yWindow="350" windowWidth="16480" windowHeight="9970" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3320" yWindow="90" windowWidth="15280" windowHeight="9970" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5933" uniqueCount="2316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5970" uniqueCount="2317">
   <si>
     <t>Code</t>
   </si>
@@ -9516,9 +9516,6 @@
     </r>
   </si>
   <si>
-    <t>ok</t>
-  </si>
-  <si>
     <t>Study Role Code</t>
   </si>
   <si>
@@ -9673,6 +9670,12 @@
   </si>
   <si>
     <t>A professional who specializes in applying statistical principles to experimental design and data analysis.</t>
+  </si>
+  <si>
+    <t>Regulatory Body; Regulator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An organization (typically a government agency) that is responsible for implementing and enforcing laws, licensing and regulating products and services, promoting the use of standards, and ensuring safety and consumer protections. </t>
   </si>
 </sst>
 </file>
@@ -9807,7 +9810,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -9883,12 +9886,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10274,9 +10271,6 @@
     <xf numFmtId="0" fontId="16" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -10296,6 +10290,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -10789,10 +10786,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="89" t="s">
         <v>903</v>
       </c>
-      <c r="B1" s="91"/>
+      <c r="B1" s="90"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -27893,7 +27890,7 @@
       <c r="D18" s="16" t="s">
         <v>2197</v>
       </c>
-      <c r="E18" s="85" t="s">
+      <c r="E18" s="84" t="s">
         <v>2052</v>
       </c>
       <c r="F18" s="16" t="s">
@@ -27904,14 +27901,14 @@
         <v>1672</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>2264</v>
+        <v>2263</v>
       </c>
       <c r="J18" s="16"/>
       <c r="K18" s="16" t="s">
+        <v>2264</v>
+      </c>
+      <c r="L18" s="16" t="s">
         <v>2265</v>
-      </c>
-      <c r="L18" s="16" t="s">
-        <v>2266</v>
       </c>
       <c r="M18" s="13"/>
       <c r="N18" s="16" t="s">
@@ -27920,15 +27917,15 @@
     </row>
     <row r="19" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D19" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D19" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E19" s="15" t="s">
@@ -27960,15 +27957,15 @@
     </row>
     <row r="20" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D20" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D20" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E20" s="15" t="s">
@@ -27998,15 +27995,15 @@
     </row>
     <row r="21" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D21" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D21" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E21" s="15" t="s">
@@ -28036,15 +28033,15 @@
     </row>
     <row r="22" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D22" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D22" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E22" s="15" t="s">
@@ -28074,15 +28071,15 @@
     </row>
     <row r="23" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D23" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D23" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E23" s="15" t="s">
@@ -28112,15 +28109,15 @@
     </row>
     <row r="24" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D24" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D24" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E24" s="15" t="s">
@@ -28130,15 +28127,15 @@
         <v>1701</v>
       </c>
       <c r="G24" s="13"/>
-      <c r="H24" s="87" t="s">
+      <c r="H24" s="86" t="s">
+        <v>2267</v>
+      </c>
+      <c r="I24" s="87" t="s">
         <v>2268</v>
       </c>
-      <c r="I24" s="88" t="s">
-        <v>2269</v>
-      </c>
-      <c r="J24" s="88"/>
-      <c r="K24" s="89" t="s">
-        <v>2271</v>
+      <c r="J24" s="87"/>
+      <c r="K24" s="88" t="s">
+        <v>2270</v>
       </c>
       <c r="L24" s="16" t="s">
         <v>928</v>
@@ -28150,15 +28147,15 @@
     </row>
     <row r="25" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D25" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D25" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E25" s="15" t="s">
@@ -28172,24 +28169,24 @@
         <v>1672</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>2272</v>
+        <v>2271</v>
       </c>
       <c r="J25" s="16"/>
       <c r="K25" s="16" t="s">
-        <v>2273</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D26" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D26" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E26" s="15" t="s">
@@ -28200,27 +28197,27 @@
       </c>
       <c r="G26" s="13"/>
       <c r="H26" s="16" t="s">
+        <v>2273</v>
+      </c>
+      <c r="I26" s="16" t="s">
         <v>2274</v>
-      </c>
-      <c r="I26" s="16" t="s">
-        <v>2275</v>
       </c>
       <c r="J26" s="16"/>
       <c r="K26" s="16" t="s">
-        <v>2276</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D27" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D27" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E27" s="15" t="s">
@@ -28234,24 +28231,24 @@
         <v>1672</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>2277</v>
+        <v>2276</v>
       </c>
       <c r="J27" s="16"/>
       <c r="K27" s="16" t="s">
-        <v>2278</v>
+        <v>2277</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D28" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D28" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E28" s="15" t="s">
@@ -28265,7 +28262,7 @@
         <v>603</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>2279</v>
+        <v>2278</v>
       </c>
       <c r="J28" s="16"/>
       <c r="K28" s="16" t="s">
@@ -28274,15 +28271,15 @@
     </row>
     <row r="29" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D29" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D29" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E29" s="15" t="s">
@@ -28293,27 +28290,27 @@
       </c>
       <c r="G29" s="13"/>
       <c r="H29" s="16" t="s">
+        <v>2279</v>
+      </c>
+      <c r="I29" s="16" t="s">
         <v>2280</v>
-      </c>
-      <c r="I29" s="16" t="s">
-        <v>2281</v>
       </c>
       <c r="J29" s="16"/>
       <c r="K29" s="16" t="s">
-        <v>2282</v>
+        <v>2281</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D30" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D30" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E30" s="15" t="s">
@@ -28324,27 +28321,27 @@
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="16" t="s">
+        <v>2282</v>
+      </c>
+      <c r="I30" s="16" t="s">
         <v>2283</v>
-      </c>
-      <c r="I30" s="16" t="s">
-        <v>2284</v>
       </c>
       <c r="J30" s="16"/>
       <c r="K30" s="16" t="s">
-        <v>2285</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D31" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D31" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E31" s="15" t="s">
@@ -28358,24 +28355,24 @@
         <v>1672</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>2286</v>
+        <v>2285</v>
       </c>
       <c r="J31" s="16"/>
       <c r="K31" s="16" t="s">
-        <v>2287</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D32" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D32" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E32" s="15" t="s">
@@ -28386,27 +28383,27 @@
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="16" t="s">
+        <v>2287</v>
+      </c>
+      <c r="I32" s="16" t="s">
         <v>2288</v>
-      </c>
-      <c r="I32" s="16" t="s">
-        <v>2289</v>
       </c>
       <c r="J32" s="16"/>
       <c r="K32" s="16" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D33" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D33" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E33" s="15" t="s">
@@ -28417,27 +28414,27 @@
       </c>
       <c r="G33" s="13"/>
       <c r="H33" s="16" t="s">
+        <v>2290</v>
+      </c>
+      <c r="I33" s="15" t="s">
         <v>2291</v>
-      </c>
-      <c r="I33" s="15" t="s">
-        <v>2292</v>
       </c>
       <c r="J33" s="16"/>
       <c r="K33" s="16" t="s">
-        <v>2293</v>
+        <v>2292</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D34" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D34" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E34" s="15" t="s">
@@ -28451,26 +28448,26 @@
         <v>1672</v>
       </c>
       <c r="I34" s="15" t="s">
+        <v>2293</v>
+      </c>
+      <c r="J34" s="16" t="s">
         <v>2294</v>
       </c>
-      <c r="J34" s="16" t="s">
+      <c r="K34" s="16" t="s">
         <v>2295</v>
-      </c>
-      <c r="K34" s="16" t="s">
-        <v>2296</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D35" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D35" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E35" s="15" t="s">
@@ -28481,29 +28478,29 @@
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="16" t="s">
+        <v>2296</v>
+      </c>
+      <c r="I35" s="15" t="s">
         <v>2297</v>
       </c>
-      <c r="I35" s="15" t="s">
+      <c r="J35" s="16" t="s">
         <v>2298</v>
       </c>
-      <c r="J35" s="16" t="s">
+      <c r="K35" s="16" t="s">
         <v>2299</v>
-      </c>
-      <c r="K35" s="16" t="s">
-        <v>2300</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D36" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D36" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E36" s="15" t="s">
@@ -28514,27 +28511,27 @@
       </c>
       <c r="G36" s="13"/>
       <c r="H36" s="16" t="s">
+        <v>2300</v>
+      </c>
+      <c r="I36" s="15" t="s">
         <v>2301</v>
-      </c>
-      <c r="I36" s="15" t="s">
-        <v>2302</v>
       </c>
       <c r="J36" s="16"/>
       <c r="K36" s="16" t="s">
-        <v>2303</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D37" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D37" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E37" s="15" t="s">
@@ -28548,24 +28545,24 @@
         <v>1672</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>2304</v>
+        <v>2303</v>
       </c>
       <c r="J37" s="16"/>
       <c r="K37" s="16" t="s">
-        <v>2305</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D38" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D38" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E38" s="15" t="s">
@@ -28576,29 +28573,29 @@
       </c>
       <c r="G38" s="13"/>
       <c r="H38" s="16" t="s">
+        <v>2305</v>
+      </c>
+      <c r="I38" s="16" t="s">
         <v>2306</v>
       </c>
-      <c r="I38" s="16" t="s">
+      <c r="J38" s="16" t="s">
         <v>2307</v>
       </c>
-      <c r="J38" s="16" t="s">
+      <c r="K38" s="16" t="s">
         <v>2308</v>
-      </c>
-      <c r="K38" s="16" t="s">
-        <v>2309</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D39" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D39" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E39" s="15" t="s">
@@ -28609,27 +28606,27 @@
       </c>
       <c r="G39" s="13"/>
       <c r="H39" s="16" t="s">
+        <v>2309</v>
+      </c>
+      <c r="I39" s="16" t="s">
         <v>2310</v>
-      </c>
-      <c r="I39" s="16" t="s">
-        <v>2311</v>
       </c>
       <c r="J39" s="16"/>
       <c r="K39" s="16" t="s">
-        <v>2312</v>
+        <v>2311</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>2267</v>
-      </c>
-      <c r="D40" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D40" s="85" t="s">
         <v>2197</v>
       </c>
       <c r="E40" s="15" t="s">
@@ -28640,14 +28637,14 @@
       </c>
       <c r="G40" s="13"/>
       <c r="H40" s="16" t="s">
+        <v>2312</v>
+      </c>
+      <c r="I40" s="16" t="s">
         <v>2313</v>
-      </c>
-      <c r="I40" s="16" t="s">
-        <v>2314</v>
       </c>
       <c r="J40" s="16"/>
       <c r="K40" s="16" t="s">
-        <v>2315</v>
+        <v>2314</v>
       </c>
     </row>
   </sheetData>
@@ -28664,11 +28661,9 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -28765,6 +28760,8 @@
       <c r="L2" s="16" t="s">
         <v>2167</v>
       </c>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:14" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -29270,7 +29267,7 @@
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
     </row>
-    <row r="17" spans="1:15" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>2243</v>
       </c>
@@ -29306,7 +29303,7 @@
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
     </row>
-    <row r="18" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>2243</v>
       </c>
@@ -29342,7 +29339,7 @@
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
     </row>
-    <row r="19" spans="1:15" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>2243</v>
       </c>
@@ -29378,7 +29375,7 @@
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
     </row>
-    <row r="20" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>2243</v>
       </c>
@@ -29414,7 +29411,7 @@
       <c r="M20" s="13"/>
       <c r="N20" s="13"/>
     </row>
-    <row r="21" spans="1:15" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>2260</v>
       </c>
@@ -29449,9 +29446,146 @@
       </c>
       <c r="M21" s="25"/>
       <c r="N21" s="13"/>
-      <c r="O21" s="84" t="s">
-        <v>2263</v>
-      </c>
+    </row>
+    <row r="22" spans="1:14" ht="25" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B22" s="60" t="s">
+        <v>592</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="E22" s="60" t="s">
+        <v>2214</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="60" t="s">
+        <v>596</v>
+      </c>
+      <c r="I22" s="60" t="s">
+        <v>597</v>
+      </c>
+      <c r="J22" s="60"/>
+      <c r="K22" s="60" t="s">
+        <v>598</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+    </row>
+    <row r="23" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B23" s="60" t="s">
+        <v>592</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="E23" s="60" t="s">
+        <v>2214</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="60" t="s">
+        <v>600</v>
+      </c>
+      <c r="I23" s="91" t="s">
+        <v>601</v>
+      </c>
+      <c r="J23" s="60" t="s">
+        <v>602</v>
+      </c>
+      <c r="K23" s="60" t="s">
+        <v>927</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+    </row>
+    <row r="24" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B24" s="60" t="s">
+        <v>592</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" s="60" t="s">
+        <v>2214</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="60" t="s">
+        <v>603</v>
+      </c>
+      <c r="I24" s="60" t="s">
+        <v>604</v>
+      </c>
+      <c r="J24" s="60" t="s">
+        <v>2315</v>
+      </c>
+      <c r="K24" s="60" t="s">
+        <v>2316</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+    </row>
+    <row r="25" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B25" s="60" t="s">
+        <v>592</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="E25" s="60" t="s">
+        <v>2214</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>1701</v>
+      </c>
+      <c r="G25" s="13"/>
+      <c r="H25" s="60" t="s">
+        <v>2218</v>
+      </c>
+      <c r="I25" s="60" t="s">
+        <v>2219</v>
+      </c>
+      <c r="J25" s="91"/>
+      <c r="K25" s="60" t="s">
+        <v>2220</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I18">

</xml_diff>

<commit_message>
updated definition for StudyRole.appliesTo
updated definition for StudyRole.appliesTo
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BF6D6C-7F92-4588-90D6-5368A355167F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541856A8-51AB-4E0A-A804-305D16C7AF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="90" windowWidth="15280" windowHeight="9970" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="210" windowWidth="19160" windowHeight="9920" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -9308,9 +9308,6 @@
     <t>A USDM relationship between the StudyRole and Masking classes which describes the masking associated with the study role.</t>
   </si>
   <si>
-    <t>A USDM relationship between the StudyRole and StudyVersion and StudyDesign classes that identifies the study version or study design that applies to the study role.</t>
-  </si>
-  <si>
     <t>A USDM relationship between the StudyRole and Organization classes which identifies the set of organizations associated with the study role.</t>
   </si>
   <si>
@@ -9676,6 +9673,9 @@
   </si>
   <si>
     <t xml:space="preserve">An organization (typically a government agency) that is responsible for implementing and enforcing laws, licensing and regulating products and services, promoting the use of standards, and ensuring safety and consumer protections. </t>
+  </si>
+  <si>
+    <t>A USDM relationship between the StudyRole and either StudyVersion or StudyDesign classes that identifies the study version or study design to which the study role applies.</t>
   </si>
 </sst>
 </file>
@@ -10286,13 +10286,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -10786,10 +10786,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="90" t="s">
         <v>903</v>
       </c>
-      <c r="B1" s="90"/>
+      <c r="B1" s="91"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -27837,7 +27837,7 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
       <c r="K16" s="16" t="s">
-        <v>2211</v>
+        <v>2316</v>
       </c>
       <c r="L16" s="16" t="s">
         <v>928</v>
@@ -27869,7 +27869,7 @@
       <c r="I17" s="16"/>
       <c r="J17" s="16"/>
       <c r="K17" s="16" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
       <c r="L17" s="16" t="s">
         <v>928</v>
@@ -27901,14 +27901,14 @@
         <v>1672</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="J18" s="16"/>
       <c r="K18" s="16" t="s">
+        <v>2263</v>
+      </c>
+      <c r="L18" s="16" t="s">
         <v>2264</v>
-      </c>
-      <c r="L18" s="16" t="s">
-        <v>2265</v>
       </c>
       <c r="M18" s="13"/>
       <c r="N18" s="16" t="s">
@@ -27917,13 +27917,13 @@
     </row>
     <row r="19" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D19" s="85" t="s">
         <v>2197</v>
@@ -27936,16 +27936,16 @@
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="26" t="s">
+        <v>2245</v>
+      </c>
+      <c r="I19" s="26" t="s">
         <v>2246</v>
       </c>
-      <c r="I19" s="26" t="s">
+      <c r="J19" s="26" t="s">
         <v>2247</v>
       </c>
-      <c r="J19" s="26" t="s">
+      <c r="K19" s="26" t="s">
         <v>2248</v>
-      </c>
-      <c r="K19" s="26" t="s">
-        <v>2249</v>
       </c>
       <c r="L19" s="16" t="s">
         <v>928</v>
@@ -27957,13 +27957,13 @@
     </row>
     <row r="20" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D20" s="85" t="s">
         <v>2197</v>
@@ -27976,14 +27976,14 @@
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="26" t="s">
+        <v>2249</v>
+      </c>
+      <c r="I20" s="26" t="s">
         <v>2250</v>
-      </c>
-      <c r="I20" s="26" t="s">
-        <v>2251</v>
       </c>
       <c r="J20" s="26"/>
       <c r="K20" s="26" t="s">
-        <v>2252</v>
+        <v>2251</v>
       </c>
       <c r="L20" s="16" t="s">
         <v>928</v>
@@ -27995,13 +27995,13 @@
     </row>
     <row r="21" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D21" s="85" t="s">
         <v>2197</v>
@@ -28014,14 +28014,14 @@
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="62" t="s">
+        <v>2252</v>
+      </c>
+      <c r="I21" s="26" t="s">
         <v>2253</v>
-      </c>
-      <c r="I21" s="26" t="s">
-        <v>2254</v>
       </c>
       <c r="J21" s="26"/>
       <c r="K21" s="26" t="s">
-        <v>2255</v>
+        <v>2254</v>
       </c>
       <c r="L21" s="16" t="s">
         <v>928</v>
@@ -28033,13 +28033,13 @@
     </row>
     <row r="22" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D22" s="85" t="s">
         <v>2197</v>
@@ -28055,7 +28055,7 @@
         <v>600</v>
       </c>
       <c r="I22" s="26" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="J22" s="26"/>
       <c r="K22" s="26" t="s">
@@ -28071,13 +28071,13 @@
     </row>
     <row r="23" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D23" s="85" t="s">
         <v>2197</v>
@@ -28090,14 +28090,14 @@
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="15" t="s">
+        <v>2256</v>
+      </c>
+      <c r="I23" s="15" t="s">
         <v>2257</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>2258</v>
       </c>
       <c r="J23" s="15"/>
       <c r="K23" s="15" t="s">
-        <v>2259</v>
+        <v>2258</v>
       </c>
       <c r="L23" s="16" t="s">
         <v>928</v>
@@ -28109,13 +28109,13 @@
     </row>
     <row r="24" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D24" s="85" t="s">
         <v>2197</v>
@@ -28128,14 +28128,14 @@
       </c>
       <c r="G24" s="13"/>
       <c r="H24" s="86" t="s">
+        <v>2266</v>
+      </c>
+      <c r="I24" s="87" t="s">
         <v>2267</v>
-      </c>
-      <c r="I24" s="87" t="s">
-        <v>2268</v>
       </c>
       <c r="J24" s="87"/>
       <c r="K24" s="88" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="L24" s="16" t="s">
         <v>928</v>
@@ -28147,13 +28147,13 @@
     </row>
     <row r="25" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D25" s="85" t="s">
         <v>2197</v>
@@ -28169,22 +28169,22 @@
         <v>1672</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>2271</v>
+        <v>2270</v>
       </c>
       <c r="J25" s="16"/>
       <c r="K25" s="16" t="s">
-        <v>2272</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D26" s="85" t="s">
         <v>2197</v>
@@ -28197,25 +28197,25 @@
       </c>
       <c r="G26" s="13"/>
       <c r="H26" s="16" t="s">
+        <v>2272</v>
+      </c>
+      <c r="I26" s="16" t="s">
         <v>2273</v>
-      </c>
-      <c r="I26" s="16" t="s">
-        <v>2274</v>
       </c>
       <c r="J26" s="16"/>
       <c r="K26" s="16" t="s">
-        <v>2275</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D27" s="85" t="s">
         <v>2197</v>
@@ -28231,22 +28231,22 @@
         <v>1672</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>2276</v>
+        <v>2275</v>
       </c>
       <c r="J27" s="16"/>
       <c r="K27" s="16" t="s">
-        <v>2277</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D28" s="85" t="s">
         <v>2197</v>
@@ -28262,7 +28262,7 @@
         <v>603</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>2278</v>
+        <v>2277</v>
       </c>
       <c r="J28" s="16"/>
       <c r="K28" s="16" t="s">
@@ -28271,13 +28271,13 @@
     </row>
     <row r="29" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D29" s="85" t="s">
         <v>2197</v>
@@ -28290,25 +28290,25 @@
       </c>
       <c r="G29" s="13"/>
       <c r="H29" s="16" t="s">
+        <v>2278</v>
+      </c>
+      <c r="I29" s="16" t="s">
         <v>2279</v>
-      </c>
-      <c r="I29" s="16" t="s">
-        <v>2280</v>
       </c>
       <c r="J29" s="16"/>
       <c r="K29" s="16" t="s">
-        <v>2281</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D30" s="85" t="s">
         <v>2197</v>
@@ -28321,25 +28321,25 @@
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="16" t="s">
+        <v>2281</v>
+      </c>
+      <c r="I30" s="16" t="s">
         <v>2282</v>
-      </c>
-      <c r="I30" s="16" t="s">
-        <v>2283</v>
       </c>
       <c r="J30" s="16"/>
       <c r="K30" s="16" t="s">
-        <v>2284</v>
+        <v>2283</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D31" s="85" t="s">
         <v>2197</v>
@@ -28355,22 +28355,22 @@
         <v>1672</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>2285</v>
+        <v>2284</v>
       </c>
       <c r="J31" s="16"/>
       <c r="K31" s="16" t="s">
-        <v>2286</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D32" s="85" t="s">
         <v>2197</v>
@@ -28383,25 +28383,25 @@
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="16" t="s">
+        <v>2286</v>
+      </c>
+      <c r="I32" s="16" t="s">
         <v>2287</v>
-      </c>
-      <c r="I32" s="16" t="s">
-        <v>2288</v>
       </c>
       <c r="J32" s="16"/>
       <c r="K32" s="16" t="s">
-        <v>2289</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D33" s="85" t="s">
         <v>2197</v>
@@ -28414,25 +28414,25 @@
       </c>
       <c r="G33" s="13"/>
       <c r="H33" s="16" t="s">
+        <v>2289</v>
+      </c>
+      <c r="I33" s="15" t="s">
         <v>2290</v>
-      </c>
-      <c r="I33" s="15" t="s">
-        <v>2291</v>
       </c>
       <c r="J33" s="16"/>
       <c r="K33" s="16" t="s">
-        <v>2292</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D34" s="85" t="s">
         <v>2197</v>
@@ -28448,24 +28448,24 @@
         <v>1672</v>
       </c>
       <c r="I34" s="15" t="s">
+        <v>2292</v>
+      </c>
+      <c r="J34" s="16" t="s">
         <v>2293</v>
       </c>
-      <c r="J34" s="16" t="s">
+      <c r="K34" s="16" t="s">
         <v>2294</v>
-      </c>
-      <c r="K34" s="16" t="s">
-        <v>2295</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D35" s="85" t="s">
         <v>2197</v>
@@ -28478,27 +28478,27 @@
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="16" t="s">
+        <v>2295</v>
+      </c>
+      <c r="I35" s="15" t="s">
         <v>2296</v>
       </c>
-      <c r="I35" s="15" t="s">
+      <c r="J35" s="16" t="s">
         <v>2297</v>
       </c>
-      <c r="J35" s="16" t="s">
+      <c r="K35" s="16" t="s">
         <v>2298</v>
-      </c>
-      <c r="K35" s="16" t="s">
-        <v>2299</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D36" s="85" t="s">
         <v>2197</v>
@@ -28511,25 +28511,25 @@
       </c>
       <c r="G36" s="13"/>
       <c r="H36" s="16" t="s">
+        <v>2299</v>
+      </c>
+      <c r="I36" s="15" t="s">
         <v>2300</v>
-      </c>
-      <c r="I36" s="15" t="s">
-        <v>2301</v>
       </c>
       <c r="J36" s="16"/>
       <c r="K36" s="16" t="s">
-        <v>2302</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D37" s="85" t="s">
         <v>2197</v>
@@ -28545,22 +28545,22 @@
         <v>1672</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>2303</v>
+        <v>2302</v>
       </c>
       <c r="J37" s="16"/>
       <c r="K37" s="16" t="s">
-        <v>2304</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D38" s="85" t="s">
         <v>2197</v>
@@ -28573,27 +28573,27 @@
       </c>
       <c r="G38" s="13"/>
       <c r="H38" s="16" t="s">
+        <v>2304</v>
+      </c>
+      <c r="I38" s="16" t="s">
         <v>2305</v>
       </c>
-      <c r="I38" s="16" t="s">
+      <c r="J38" s="16" t="s">
         <v>2306</v>
       </c>
-      <c r="J38" s="16" t="s">
+      <c r="K38" s="16" t="s">
         <v>2307</v>
-      </c>
-      <c r="K38" s="16" t="s">
-        <v>2308</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D39" s="85" t="s">
         <v>2197</v>
@@ -28606,25 +28606,25 @@
       </c>
       <c r="G39" s="13"/>
       <c r="H39" s="16" t="s">
+        <v>2308</v>
+      </c>
+      <c r="I39" s="16" t="s">
         <v>2309</v>
-      </c>
-      <c r="I39" s="16" t="s">
-        <v>2310</v>
       </c>
       <c r="J39" s="16"/>
       <c r="K39" s="16" t="s">
-        <v>2311</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="50" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D40" s="85" t="s">
         <v>2197</v>
@@ -28637,14 +28637,14 @@
       </c>
       <c r="G40" s="13"/>
       <c r="H40" s="16" t="s">
+        <v>2311</v>
+      </c>
+      <c r="I40" s="16" t="s">
         <v>2312</v>
-      </c>
-      <c r="I40" s="16" t="s">
-        <v>2313</v>
       </c>
       <c r="J40" s="16"/>
       <c r="K40" s="16" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
   </sheetData>
@@ -28765,7 +28765,7 @@
     </row>
     <row r="3" spans="1:14" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>239</v>
@@ -28777,7 +28777,7 @@
         <v>137</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>1603</v>
@@ -28794,16 +28794,16 @@
         <v>254</v>
       </c>
       <c r="L3" s="15" t="s">
+        <v>2214</v>
+      </c>
+      <c r="M3" s="25" t="s">
         <v>2215</v>
-      </c>
-      <c r="M3" s="25" t="s">
-        <v>2216</v>
       </c>
       <c r="N3" s="13"/>
     </row>
     <row r="4" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A4" s="75" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>118</v>
@@ -28822,14 +28822,14 @@
       </c>
       <c r="G4" s="74"/>
       <c r="H4" s="76" t="s">
+        <v>2217</v>
+      </c>
+      <c r="I4" s="76" t="s">
         <v>2218</v>
-      </c>
-      <c r="I4" s="76" t="s">
-        <v>2219</v>
       </c>
       <c r="J4" s="78"/>
       <c r="K4" s="76" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
       <c r="L4" s="76" t="s">
         <v>928</v>
@@ -28839,19 +28839,19 @@
     </row>
     <row r="5" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>2221</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="C5" s="16" t="s">
         <v>2222</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>2223</v>
       </c>
       <c r="D5" s="38" t="s">
         <v>1416</v>
       </c>
       <c r="E5" s="56" t="s">
-        <v>2224</v>
+        <v>2223</v>
       </c>
       <c r="F5" s="38" t="s">
         <v>1671</v>
@@ -28860,14 +28860,14 @@
         <v>137</v>
       </c>
       <c r="H5" s="80" t="s">
+        <v>2224</v>
+      </c>
+      <c r="I5" s="38" t="s">
         <v>2225</v>
-      </c>
-      <c r="I5" s="38" t="s">
-        <v>2226</v>
       </c>
       <c r="J5" s="40"/>
       <c r="K5" s="39" t="s">
-        <v>2227</v>
+        <v>2226</v>
       </c>
       <c r="L5" s="38" t="s">
         <v>1614</v>
@@ -28877,19 +28877,19 @@
     </row>
     <row r="6" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>2221</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="C6" s="16" t="s">
         <v>2222</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>2223</v>
       </c>
       <c r="D6" s="38" t="s">
         <v>1416</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>2228</v>
+        <v>2227</v>
       </c>
       <c r="F6" s="38" t="s">
         <v>1671</v>
@@ -28898,14 +28898,14 @@
         <v>137</v>
       </c>
       <c r="H6" s="80" t="s">
+        <v>2228</v>
+      </c>
+      <c r="I6" s="38" t="s">
         <v>2229</v>
-      </c>
-      <c r="I6" s="38" t="s">
-        <v>2230</v>
       </c>
       <c r="J6" s="40"/>
       <c r="K6" s="38" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
       <c r="L6" s="38" t="s">
         <v>1614</v>
@@ -28915,13 +28915,13 @@
     </row>
     <row r="7" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>2221</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="C7" s="16" t="s">
         <v>2222</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>2223</v>
       </c>
       <c r="D7" s="38" t="s">
         <v>1416</v>
@@ -28936,14 +28936,14 @@
         <v>137</v>
       </c>
       <c r="H7" s="80" t="s">
+        <v>2231</v>
+      </c>
+      <c r="I7" s="38" t="s">
         <v>2232</v>
-      </c>
-      <c r="I7" s="38" t="s">
-        <v>2233</v>
       </c>
       <c r="J7" s="40"/>
       <c r="K7" s="38" t="s">
-        <v>2234</v>
+        <v>2233</v>
       </c>
       <c r="L7" s="38" t="s">
         <v>1614</v>
@@ -28953,19 +28953,19 @@
     </row>
     <row r="8" spans="1:14" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>2221</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="C8" s="16" t="s">
         <v>2222</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>2223</v>
       </c>
       <c r="D8" s="38" t="s">
         <v>1416</v>
       </c>
       <c r="E8" s="56" t="s">
-        <v>2235</v>
+        <v>2234</v>
       </c>
       <c r="F8" s="38" t="s">
         <v>1603</v>
@@ -28984,22 +28984,22 @@
         <v>254</v>
       </c>
       <c r="L8" s="39" t="s">
+        <v>2214</v>
+      </c>
+      <c r="M8" s="40" t="s">
         <v>2215</v>
-      </c>
-      <c r="M8" s="40" t="s">
-        <v>2216</v>
       </c>
       <c r="N8" s="13"/>
     </row>
     <row r="9" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>2221</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="C9" s="16" t="s">
         <v>2222</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>2223</v>
       </c>
       <c r="D9" s="38" t="s">
         <v>1416</v>
@@ -29014,14 +29014,14 @@
         <v>137</v>
       </c>
       <c r="H9" s="80" t="s">
+        <v>2235</v>
+      </c>
+      <c r="I9" s="38" t="s">
         <v>2236</v>
-      </c>
-      <c r="I9" s="38" t="s">
-        <v>2237</v>
       </c>
       <c r="J9" s="40"/>
       <c r="K9" s="38" t="s">
-        <v>2238</v>
+        <v>2237</v>
       </c>
       <c r="L9" s="38" t="s">
         <v>1614</v>
@@ -29031,7 +29031,7 @@
     </row>
     <row r="10" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>2239</v>
+        <v>2238</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>928</v>
@@ -29065,7 +29065,7 @@
     </row>
     <row r="11" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>2239</v>
+        <v>2238</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>928</v>
@@ -29097,7 +29097,7 @@
     </row>
     <row r="12" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>2239</v>
+        <v>2238</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>928</v>
@@ -29129,7 +29129,7 @@
     </row>
     <row r="13" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>2239</v>
+        <v>2238</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>928</v>
@@ -29161,7 +29161,7 @@
     </row>
     <row r="14" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>2239</v>
+        <v>2238</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>928</v>
@@ -29193,13 +29193,13 @@
     </row>
     <row r="15" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>2221</v>
+        <v>2220</v>
       </c>
       <c r="B15" s="16" t="s">
+        <v>2239</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>2240</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>2241</v>
       </c>
       <c r="D15" s="38" t="s">
         <v>1711</v>
@@ -29224,20 +29224,20 @@
         <v>2122</v>
       </c>
       <c r="L15" s="38" t="s">
-        <v>2242</v>
+        <v>2241</v>
       </c>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
     </row>
     <row r="16" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>2243</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="C16" s="16" t="s">
         <v>2244</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>2245</v>
       </c>
       <c r="D16" s="83" t="s">
         <v>1711</v>
@@ -29250,16 +29250,16 @@
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="36" t="s">
+        <v>2245</v>
+      </c>
+      <c r="I16" s="36" t="s">
         <v>2246</v>
       </c>
-      <c r="I16" s="36" t="s">
+      <c r="J16" s="36" t="s">
         <v>2247</v>
       </c>
-      <c r="J16" s="36" t="s">
+      <c r="K16" s="36" t="s">
         <v>2248</v>
-      </c>
-      <c r="K16" s="36" t="s">
-        <v>2249</v>
       </c>
       <c r="L16" s="38" t="s">
         <v>928</v>
@@ -29269,13 +29269,13 @@
     </row>
     <row r="17" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>2243</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="C17" s="16" t="s">
         <v>2244</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>2245</v>
       </c>
       <c r="D17" s="83" t="s">
         <v>1711</v>
@@ -29288,14 +29288,14 @@
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="36" t="s">
+        <v>2249</v>
+      </c>
+      <c r="I17" s="36" t="s">
         <v>2250</v>
-      </c>
-      <c r="I17" s="36" t="s">
-        <v>2251</v>
       </c>
       <c r="J17" s="36"/>
       <c r="K17" s="36" t="s">
-        <v>2252</v>
+        <v>2251</v>
       </c>
       <c r="L17" s="38" t="s">
         <v>928</v>
@@ -29305,13 +29305,13 @@
     </row>
     <row r="18" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>2243</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="C18" s="16" t="s">
         <v>2244</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>2245</v>
       </c>
       <c r="D18" s="83" t="s">
         <v>1711</v>
@@ -29324,14 +29324,14 @@
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="80" t="s">
+        <v>2252</v>
+      </c>
+      <c r="I18" s="36" t="s">
         <v>2253</v>
-      </c>
-      <c r="I18" s="36" t="s">
-        <v>2254</v>
       </c>
       <c r="J18" s="36"/>
       <c r="K18" s="36" t="s">
-        <v>2255</v>
+        <v>2254</v>
       </c>
       <c r="L18" s="38" t="s">
         <v>928</v>
@@ -29341,13 +29341,13 @@
     </row>
     <row r="19" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>2243</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="C19" s="16" t="s">
         <v>2244</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>2245</v>
       </c>
       <c r="D19" s="83" t="s">
         <v>1711</v>
@@ -29363,7 +29363,7 @@
         <v>600</v>
       </c>
       <c r="I19" s="36" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="J19" s="36"/>
       <c r="K19" s="36" t="s">
@@ -29377,13 +29377,13 @@
     </row>
     <row r="20" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>2243</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="C20" s="16" t="s">
         <v>2244</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>2245</v>
       </c>
       <c r="D20" s="83" t="s">
         <v>1711</v>
@@ -29396,14 +29396,14 @@
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="39" t="s">
+        <v>2256</v>
+      </c>
+      <c r="I20" s="39" t="s">
         <v>2257</v>
-      </c>
-      <c r="I20" s="39" t="s">
-        <v>2258</v>
       </c>
       <c r="J20" s="39"/>
       <c r="K20" s="39" t="s">
-        <v>2259</v>
+        <v>2258</v>
       </c>
       <c r="L20" s="38" t="s">
         <v>928</v>
@@ -29413,19 +29413,19 @@
     </row>
     <row r="21" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>2260</v>
+        <v>2259</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>1672</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>2261</v>
+        <v>2260</v>
       </c>
       <c r="D21" s="25" t="s">
         <v>2042</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>1603</v>
@@ -29449,7 +29449,7 @@
     </row>
     <row r="22" spans="1:14" ht="25" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>2260</v>
+        <v>2259</v>
       </c>
       <c r="B22" s="60" t="s">
         <v>592</v>
@@ -29459,7 +29459,7 @@
         <v>137</v>
       </c>
       <c r="E22" s="60" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>1701</v>
@@ -29483,7 +29483,7 @@
     </row>
     <row r="23" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>2260</v>
+        <v>2259</v>
       </c>
       <c r="B23" s="60" t="s">
         <v>592</v>
@@ -29493,7 +29493,7 @@
         <v>137</v>
       </c>
       <c r="E23" s="60" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
       <c r="F23" s="15" t="s">
         <v>1701</v>
@@ -29502,7 +29502,7 @@
       <c r="H23" s="60" t="s">
         <v>600</v>
       </c>
-      <c r="I23" s="91" t="s">
+      <c r="I23" s="89" t="s">
         <v>601</v>
       </c>
       <c r="J23" s="60" t="s">
@@ -29519,7 +29519,7 @@
     </row>
     <row r="24" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>2260</v>
+        <v>2259</v>
       </c>
       <c r="B24" s="60" t="s">
         <v>592</v>
@@ -29529,7 +29529,7 @@
         <v>137</v>
       </c>
       <c r="E24" s="60" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
       <c r="F24" s="15" t="s">
         <v>1701</v>
@@ -29542,10 +29542,10 @@
         <v>604</v>
       </c>
       <c r="J24" s="60" t="s">
+        <v>2314</v>
+      </c>
+      <c r="K24" s="60" t="s">
         <v>2315</v>
-      </c>
-      <c r="K24" s="60" t="s">
-        <v>2316</v>
       </c>
       <c r="L24" s="13" t="s">
         <v>928</v>
@@ -29555,7 +29555,7 @@
     </row>
     <row r="25" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>2260</v>
+        <v>2259</v>
       </c>
       <c r="B25" s="60" t="s">
         <v>592</v>
@@ -29565,21 +29565,21 @@
         <v>137</v>
       </c>
       <c r="E25" s="60" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>1701</v>
       </c>
       <c r="G25" s="13"/>
       <c r="H25" s="60" t="s">
+        <v>2217</v>
+      </c>
+      <c r="I25" s="60" t="s">
         <v>2218</v>
       </c>
-      <c r="I25" s="60" t="s">
+      <c r="J25" s="89"/>
+      <c r="K25" s="60" t="s">
         <v>2219</v>
-      </c>
-      <c r="J25" s="91"/>
-      <c r="K25" s="60" t="s">
-        <v>2220</v>
       </c>
       <c r="L25" s="13" t="s">
         <v>928</v>

</xml_diff>

<commit_message>
sprint 10 Berber fixes
sprint 10 Berber fixes
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5565BAEA-0880-4F38-88CA-07F08D10B954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A898BDCF-7C89-4F5C-8B15-80EA9717929F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1750" yWindow="120" windowWidth="16310" windowHeight="10060" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="16300" windowHeight="10060" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7125" uniqueCount="2469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7125" uniqueCount="2470">
   <si>
     <t>Code</t>
   </si>
@@ -10160,9 +10160,6 @@
     <t>Add relationship to existing Class</t>
   </si>
   <si>
-    <t>interventions</t>
-  </si>
-  <si>
     <t>A USDM relationship between the Estimand and StudyIntervention classes which identifies the set of study interventions associated with the Estimand.</t>
   </si>
   <si>
@@ -10228,10 +10225,42 @@
     <t>Update Inheritance relationship</t>
   </si>
   <si>
-    <t>A USDM relationship between the StudyDesign and StudyDefinitionDocumentVersion classes which identifies the version of the study definition document associated with the study design.</t>
-  </si>
-  <si>
     <t>Remove term from codelist; too generic. Instead add additional types of research organizations.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>intervention</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>interventions</t>
+    </r>
+  </si>
+  <si>
+    <t>Update UML Item Name and update definition</t>
+  </si>
+  <si>
+    <t>A USDM relationship between the StudyDesign and StudyDefinitionDocumentVersion classes which identifies the version of the study definition documents associated with the study design.</t>
   </si>
 </sst>
 </file>
@@ -10864,12 +10893,6 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -10881,6 +10904,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -12053,10 +12082,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="101" t="s">
         <v>410</v>
       </c>
-      <c r="B1" s="98"/>
+      <c r="B1" s="102"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -32405,13 +32434,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -32700,7 +32727,7 @@
         <v>1628</v>
       </c>
       <c r="G8" s="13"/>
-      <c r="H8" s="99" t="s">
+      <c r="H8" s="97" t="s">
         <v>980</v>
       </c>
       <c r="I8" s="16" t="s">
@@ -32714,7 +32741,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>2452</v>
       </c>
@@ -32724,155 +32751,125 @@
       <c r="C9" s="13" t="s">
         <v>434</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>118</v>
+      <c r="D9" s="16" t="s">
+        <v>976</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>2453</v>
+        <v>2454</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>420</v>
       </c>
       <c r="G9" s="13"/>
-      <c r="H9" s="73"/>
+      <c r="H9" s="16"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
       <c r="K9" s="16" t="s">
-        <v>2454</v>
+        <v>2455</v>
       </c>
       <c r="L9" s="27" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="50" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>2452</v>
+    <row r="10" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>2456</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>434</v>
+        <v>190</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>434</v>
+        <v>191</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>976</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>2455</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>420</v>
-      </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
+        <v>973</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>997</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>979</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>478</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>980</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>2457</v>
+      </c>
       <c r="J10" s="16"/>
       <c r="K10" s="16" t="s">
-        <v>2456</v>
-      </c>
-      <c r="L10" s="27" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>2457</v>
+        <v>2458</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>2452</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>190</v>
+        <v>434</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="D11" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>973</v>
       </c>
-      <c r="E11" s="42" t="s">
-        <v>997</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>979</v>
+      <c r="E11" s="28" t="s">
+        <v>480</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>420</v>
       </c>
       <c r="G11" s="16" t="s">
         <v>478</v>
       </c>
-      <c r="H11" s="16" t="s">
-        <v>980</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>2458</v>
-      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
       <c r="J11" s="16"/>
-      <c r="K11" s="16" t="s">
+      <c r="K11" s="15" t="s">
         <v>2459</v>
       </c>
-      <c r="L11" s="16" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="50" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>2452</v>
+      <c r="L11" s="27" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>1625</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>434</v>
+        <v>2394</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>434</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>973</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>480</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>420</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>478</v>
-      </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
+        <v>1033</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F12" s="89" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="16" t="s">
+        <v>2460</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>2461</v>
+      </c>
       <c r="J12" s="16"/>
-      <c r="K12" s="15" t="s">
-        <v>2460</v>
+      <c r="K12" s="16" t="s">
+        <v>2462</v>
       </c>
       <c r="L12" s="27" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>1625</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>2394</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>1033</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>572</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>1034</v>
-      </c>
-      <c r="F13" s="89" t="s">
-        <v>1628</v>
-      </c>
-      <c r="G13" s="13"/>
-      <c r="H13" s="16" t="s">
-        <v>2461</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>2462</v>
-      </c>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16" t="s">
-        <v>2463</v>
-      </c>
-      <c r="L13" s="27" t="s">
         <v>434</v>
       </c>
     </row>
@@ -32887,7 +32884,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -32958,7 +32955,7 @@
     </row>
     <row r="2" spans="1:14" ht="25" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>2464</v>
+        <v>2463</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>176</v>
@@ -32970,7 +32967,7 @@
         <v>118</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>2465</v>
+        <v>2464</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>979</v>
@@ -32992,43 +32989,37 @@
     </row>
     <row r="3" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>2466</v>
+        <v>2468</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>973</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>978</v>
+        <v>118</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>2467</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>979</v>
-      </c>
-      <c r="G3" s="64" t="s">
-        <v>478</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>197</v>
-      </c>
+        <v>420</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
       <c r="J3" s="15"/>
-      <c r="K3" s="15" t="s">
-        <v>198</v>
+      <c r="K3" s="64" t="s">
+        <v>2453</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>922</v>
+        <v>434</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>2466</v>
+        <v>2465</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>190</v>
@@ -33040,7 +33031,7 @@
         <v>973</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>983</v>
+        <v>978</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>979</v>
@@ -33049,14 +33040,14 @@
         <v>478</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="J4" s="15"/>
       <c r="K4" s="15" t="s">
-        <v>1970</v>
+        <v>198</v>
       </c>
       <c r="L4" s="16" t="s">
         <v>922</v>
@@ -33064,7 +33055,7 @@
     </row>
     <row r="5" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>2466</v>
+        <v>2465</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>190</v>
@@ -33075,8 +33066,8 @@
       <c r="D5" s="15" t="s">
         <v>973</v>
       </c>
-      <c r="E5" s="100" t="s">
-        <v>986</v>
+      <c r="E5" s="39" t="s">
+        <v>983</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>979</v>
@@ -33084,113 +33075,149 @@
       <c r="G5" s="64" t="s">
         <v>478</v>
       </c>
-      <c r="H5" s="60" t="s">
-        <v>1971</v>
-      </c>
-      <c r="I5" s="25" t="s">
-        <v>1972</v>
-      </c>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25" t="s">
-        <v>1973</v>
-      </c>
-      <c r="L5" s="25" t="s">
+      <c r="H5" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15" t="s">
+        <v>1970</v>
+      </c>
+      <c r="L5" s="16" t="s">
         <v>922</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>2466</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>434</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>434</v>
+        <v>2465</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>191</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>973</v>
       </c>
-      <c r="E6" s="23" t="s">
-        <v>920</v>
+      <c r="E6" s="98" t="s">
+        <v>986</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>420</v>
+        <v>979</v>
       </c>
       <c r="G6" s="64" t="s">
         <v>478</v>
       </c>
-      <c r="H6" s="101"/>
-      <c r="I6" s="25"/>
+      <c r="H6" s="60" t="s">
+        <v>1971</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>1972</v>
+      </c>
       <c r="J6" s="25"/>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="25" t="s">
+        <v>1973</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>2465</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>973</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>920</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>420</v>
+      </c>
+      <c r="G7" s="64" t="s">
+        <v>478</v>
+      </c>
+      <c r="H7" s="99"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="16" t="s">
         <v>974</v>
       </c>
-      <c r="L6" s="16" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="50" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>2464</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>434</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>434</v>
-      </c>
-      <c r="D7" s="26" t="s">
+      <c r="L7" s="16" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>2463</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="D8" s="26" t="s">
         <v>414</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E8" s="17" t="s">
         <v>1136</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F8" s="26" t="s">
         <v>420</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="15" t="s">
-        <v>2467</v>
-      </c>
-      <c r="L7" s="15" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>2468</v>
-      </c>
-      <c r="B8" s="102" t="s">
+      <c r="G8" s="13"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="15" t="s">
+        <v>2469</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>2466</v>
+      </c>
+      <c r="B9" s="100" t="s">
         <v>348</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C9" s="36" t="s">
         <v>351</v>
       </c>
-      <c r="D8" s="93" t="s">
+      <c r="D9" s="93" t="s">
         <v>124</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E9" s="41" t="s">
         <v>2436</v>
       </c>
-      <c r="F8" s="94" t="s">
+      <c r="F9" s="94" t="s">
         <v>1628</v>
       </c>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37" t="s">
+      <c r="G9" s="36"/>
+      <c r="H9" s="37" t="s">
         <v>1525</v>
       </c>
-      <c r="I8" s="37" t="s">
+      <c r="I9" s="37" t="s">
         <v>1526</v>
       </c>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37" t="s">
+      <c r="J9" s="37"/>
+      <c r="K9" s="37" t="s">
         <v>1527</v>
       </c>
-      <c r="L8" s="37" t="s">
+      <c r="L9" s="37" t="s">
         <v>434</v>
       </c>
     </row>

</xml_diff>

<commit_message>
QC for sprint 10
Updates to Study Role Code and Organization Type codelists
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A898BDCF-7C89-4F5C-8B15-80EA9717929F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE453C2-0C22-4697-BB91-2CE0F4C6D2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="16300" windowHeight="10060" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="740" yWindow="0" windowWidth="17700" windowHeight="10080" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7125" uniqueCount="2470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7157" uniqueCount="2476">
   <si>
     <t>Code</t>
   </si>
@@ -10261,6 +10261,24 @@
   </si>
   <si>
     <t>A USDM relationship between the StudyDesign and StudyDefinitionDocumentVersion classes which identifies the version of the study definition documents associated with the study design.</t>
+  </si>
+  <si>
+    <t>Study Role Code Value Set Terminology</t>
+  </si>
+  <si>
+    <t>StudyRole.code</t>
+  </si>
+  <si>
+    <t>Contract Research</t>
+  </si>
+  <si>
+    <t>Research that is conducted by an individual or organization on behalf of another organization through a contracting mechanism.</t>
+  </si>
+  <si>
+    <t>Remove term from codelist.</t>
+  </si>
+  <si>
+    <t>Remove term from codelist</t>
   </si>
 </sst>
 </file>
@@ -32434,7 +32452,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -32873,6 +32891,40 @@
         <v>434</v>
       </c>
     </row>
+    <row r="13" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>1625</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>980</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>2470</v>
+      </c>
+      <c r="D13" s="89" t="s">
+        <v>1505</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>2471</v>
+      </c>
+      <c r="F13" s="89" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="16" t="s">
+        <v>980</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>2472</v>
+      </c>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16" t="s">
+        <v>2473</v>
+      </c>
+      <c r="L13" s="27" t="s">
+        <v>434</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -32884,7 +32936,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -32986,6 +33038,8 @@
       <c r="L2" s="15" t="s">
         <v>922</v>
       </c>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -33016,6 +33070,8 @@
       <c r="L3" s="16" t="s">
         <v>434</v>
       </c>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
     </row>
     <row r="4" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
@@ -33052,6 +33108,8 @@
       <c r="L4" s="16" t="s">
         <v>922</v>
       </c>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
     </row>
     <row r="5" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
@@ -33088,6 +33146,8 @@
       <c r="L5" s="16" t="s">
         <v>922</v>
       </c>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
     </row>
     <row r="6" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
@@ -33124,6 +33184,8 @@
       <c r="L6" s="25" t="s">
         <v>922</v>
       </c>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
     </row>
     <row r="7" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
@@ -33156,6 +33218,8 @@
       <c r="L7" s="16" t="s">
         <v>434</v>
       </c>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
     </row>
     <row r="8" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
@@ -33186,6 +33250,8 @@
       <c r="L8" s="15" t="s">
         <v>434</v>
       </c>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
     </row>
     <row r="9" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
@@ -33220,6 +33286,84 @@
       <c r="L9" s="37" t="s">
         <v>434</v>
       </c>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+    </row>
+    <row r="10" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>2474</v>
+      </c>
+      <c r="B10" s="100" t="s">
+        <v>348</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>351</v>
+      </c>
+      <c r="D10" s="93" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>2436</v>
+      </c>
+      <c r="F10" s="94" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="37" t="s">
+        <v>356</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>357</v>
+      </c>
+      <c r="J10" s="37" t="s">
+        <v>358</v>
+      </c>
+      <c r="K10" s="37" t="s">
+        <v>433</v>
+      </c>
+      <c r="L10" s="36" t="s">
+        <v>434</v>
+      </c>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+    </row>
+    <row r="11" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>2475</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>980</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>2470</v>
+      </c>
+      <c r="D11" s="93" t="s">
+        <v>1505</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>2471</v>
+      </c>
+      <c r="F11" s="94" t="s">
+        <v>1628</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="37" t="s">
+        <v>1612</v>
+      </c>
+      <c r="I11" s="37" t="s">
+        <v>1613</v>
+      </c>
+      <c r="J11" s="37" t="s">
+        <v>1614</v>
+      </c>
+      <c r="K11" s="37" t="s">
+        <v>1615</v>
+      </c>
+      <c r="L11" s="36" t="s">
+        <v>434</v>
+      </c>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Resolution of Berber QC comments
for ticket 430
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296EC7C8-8E4F-4382-B6BE-E7353DDF776D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BB3FD4-0F67-4C7F-9BC0-2EF2449CBC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="180" windowWidth="16030" windowHeight="9900" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="670" yWindow="1670" windowWidth="18620" windowHeight="8400" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8992" uniqueCount="2822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9022" uniqueCount="2831">
   <si>
     <t>Code</t>
   </si>
@@ -11586,6 +11586,137 @@
   </si>
   <si>
     <t>A USDM relationship between the EligibilityCriterion and EligibilityCriterionItem classes which identifies the item belonging to the eligibility criterion.</t>
+  </si>
+  <si>
+    <t>Update role and assign NCI PT, CDISC PT, and update definition.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Relationship</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Complex Datatype Relationship</t>
+    </r>
+  </si>
+  <si>
+    <t>C80489</t>
+  </si>
+  <si>
+    <t>Denominator</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A USDM relationship between the Strength and Quantity classes that identifies the denominator associated with the substance strength.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The divisor of a fraction.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>N/A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>N</t>
+    </r>
+  </si>
+  <si>
+    <t>Update role</t>
+  </si>
+  <si>
+    <t>DDF Abbreviation Attribute Terminology</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Complex Datatype Relationship</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Attribute</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -12293,17 +12424,17 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -14396,10 +14527,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="115" t="s">
         <v>410</v>
       </c>
-      <c r="B1" s="114"/>
+      <c r="B1" s="116"/>
     </row>
     <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -42315,7 +42446,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -42449,7 +42580,7 @@
       <c r="L3" s="36" t="s">
         <v>2753</v>
       </c>
-      <c r="M3" s="115" t="s">
+      <c r="M3" s="113" t="s">
         <v>2754</v>
       </c>
       <c r="N3" s="13"/>
@@ -42652,7 +42783,7 @@
       <c r="G9" s="38" t="s">
         <v>723</v>
       </c>
-      <c r="H9" s="116" t="s">
+      <c r="H9" s="114" t="s">
         <v>2185</v>
       </c>
       <c r="I9" s="36" t="s">
@@ -42690,7 +42821,7 @@
       <c r="G10" s="38" t="s">
         <v>723</v>
       </c>
-      <c r="H10" s="116" t="s">
+      <c r="H10" s="114" t="s">
         <v>2182</v>
       </c>
       <c r="I10" s="36" t="s">
@@ -43009,6 +43140,114 @@
       </c>
       <c r="M18" s="27"/>
       <c r="N18" s="16"/>
+    </row>
+    <row r="19" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>2822</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>980</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>1380</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>2823</v>
+      </c>
+      <c r="G19" s="16"/>
+      <c r="H19" s="64" t="s">
+        <v>2824</v>
+      </c>
+      <c r="I19" s="64" t="s">
+        <v>2825</v>
+      </c>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16" t="s">
+        <v>2826</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>2827</v>
+      </c>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+    </row>
+    <row r="20" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>2828</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>980</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>2829</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>1255</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>2830</v>
+      </c>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16" t="s">
+        <v>1245</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>1244</v>
+      </c>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16" t="s">
+        <v>1246</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>922</v>
+      </c>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+    </row>
+    <row r="21" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>2828</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>980</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>2829</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>1256</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>2830</v>
+      </c>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16" t="s">
+        <v>980</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>1248</v>
+      </c>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16" t="s">
+        <v>1249</v>
+      </c>
+      <c r="L21" s="16" t="s">
+        <v>922</v>
+      </c>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Richard Marshall QC items
various tickets
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT_Changes.xlsx
+++ b/Deliverables/CT/USDM_CT_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5271967A-DCB2-477C-B3F7-0F238AAE8E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49936B56-218D-424C-BA3B-F5154AB31552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="920" windowWidth="16010" windowHeight="9880" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2410" yWindow="130" windowWidth="16600" windowHeight="9880" tabRatio="668" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10568" uniqueCount="3093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10617" uniqueCount="3106">
   <si>
     <t>Code</t>
   </si>
@@ -13262,6 +13262,83 @@
   </si>
   <si>
     <t>An expression that defines the lower and upper limits of a variation.</t>
+  </si>
+  <si>
+    <t>A USDM relationship between the InterventionalStudyDesign and EligibilityCriterion classes which identifies the set of eligibility criterion associated with the interventional study design.</t>
+  </si>
+  <si>
+    <t>A USDM relationship between the ObservationalStudyDesign and EligibilityCriterion classes which identifies the set of eligibility criterion associated with the observational study design.</t>
+  </si>
+  <si>
+    <t>plannedDuration</t>
+  </si>
+  <si>
+    <t>Scheduled Timeline Planned Duration</t>
+  </si>
+  <si>
+    <t>The period of time over which the scheduled timeline is intended to take place.</t>
+  </si>
+  <si>
+    <t>C215465</t>
+  </si>
+  <si>
+    <t>personName</t>
+  </si>
+  <si>
+    <t>Assigned Person Person Name</t>
+  </si>
+  <si>
+    <t>Assigned Person Human Name</t>
+  </si>
+  <si>
+    <t>A word or group of words indicating the identity of an assigned person usually consisting of a first (personal) name and a last (family) name with an optional middle name. In some cultural traditions the family name comes first.</t>
+  </si>
+  <si>
+    <t>Update role of existing model element</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Relationship
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Complex Datatype Relationship</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A USDM relationship between the Administration and AdministrationDuration classes which provides the duration of an instance of product, agent, or therapy administration.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The amount of time elapsed during the administration of an agent.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -13686,7 +13763,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -14102,6 +14179,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -17234,7 +17314,7 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1533525</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="264560"/>
@@ -17289,7 +17369,7 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1533525</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="264560"/>
@@ -17307,6 +17387,226 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9705975" y="7677150"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1533525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="TextBox 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6C6E03E-CC7C-43FD-9E9A-1D42DB26B9A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9705975" y="7677150"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1533525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="TextBox 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1F00A4F-B590-4F7B-9EA3-8F12E0C4441E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9705975" y="7677150"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1533525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="TextBox 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F617656-D259-47F7-8A41-D539DCA8CEB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10912475" y="7677150"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1533525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="TextBox 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAAE81E1-58E9-4618-A920-8814029E8D5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10912475" y="7677150"/>
           <a:ext cx="184731" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -49671,7 +49971,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -50287,76 +50587,76 @@
     </row>
     <row r="17" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>3024</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>106</v>
+        <v>3031</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>3098</v>
+      </c>
+      <c r="C17" s="129" t="s">
+        <v>1493</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>3035</v>
-      </c>
-      <c r="E17" s="43" t="s">
-        <v>3035</v>
+        <v>1490</v>
+      </c>
+      <c r="E17" s="68" t="s">
+        <v>3099</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>1068</v>
+        <v>911</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="16" t="s">
-        <v>3036</v>
+        <v>980</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>3037</v>
+        <v>3100</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>3038</v>
+        <v>3101</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>3039</v>
+        <v>3102</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>434</v>
+        <v>922</v>
       </c>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
     </row>
-    <row r="18" spans="1:14" ht="25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>3028</v>
+        <v>3024</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>980</v>
+        <v>105</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>3040</v>
+        <v>106</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>3035</v>
       </c>
-      <c r="E18" s="68" t="s">
-        <v>997</v>
+      <c r="E18" s="43" t="s">
+        <v>3035</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>911</v>
+        <v>1068</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="16" t="s">
-        <v>980</v>
+        <v>3036</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>3041</v>
+        <v>3037</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>3042</v>
+        <v>3038</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>3043</v>
+        <v>3039</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>922</v>
+        <v>434</v>
       </c>
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
@@ -50374,24 +50674,24 @@
       <c r="D19" s="16" t="s">
         <v>3035</v>
       </c>
-      <c r="E19" s="42" t="s">
-        <v>3044</v>
+      <c r="E19" s="68" t="s">
+        <v>997</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>911</v>
+        <v>979</v>
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="16" t="s">
-        <v>3045</v>
+        <v>980</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>3046</v>
+        <v>3041</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>3047</v>
+        <v>3042</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>3048</v>
+        <v>3043</v>
       </c>
       <c r="L19" s="16" t="s">
         <v>922</v>
@@ -50399,7 +50699,7 @@
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
     </row>
-    <row r="20" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="25" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>3028</v>
       </c>
@@ -50413,21 +50713,23 @@
         <v>3035</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>3049</v>
+        <v>3044</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>911</v>
+        <v>979</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="16" t="s">
-        <v>3050</v>
+        <v>3045</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>3051</v>
-      </c>
-      <c r="J20" s="16"/>
+        <v>3046</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>3047</v>
+      </c>
       <c r="K20" s="16" t="s">
-        <v>3052</v>
+        <v>3048</v>
       </c>
       <c r="L20" s="16" t="s">
         <v>922</v>
@@ -50435,7 +50737,7 @@
       <c r="M20" s="13"/>
       <c r="N20" s="13"/>
     </row>
-    <row r="21" spans="1:14" ht="25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>3028</v>
       </c>
@@ -50449,21 +50751,21 @@
         <v>3035</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>3053</v>
+        <v>3049</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>911</v>
+        <v>979</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="16" t="s">
-        <v>980</v>
+        <v>3050</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>3054</v>
+        <v>3051</v>
       </c>
       <c r="J21" s="16"/>
       <c r="K21" s="16" t="s">
-        <v>3055</v>
+        <v>3052</v>
       </c>
       <c r="L21" s="16" t="s">
         <v>922</v>
@@ -50471,7 +50773,7 @@
       <c r="M21" s="13"/>
       <c r="N21" s="13"/>
     </row>
-    <row r="22" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="25" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>3028</v>
       </c>
@@ -50485,21 +50787,21 @@
         <v>3035</v>
       </c>
       <c r="E22" s="42" t="s">
-        <v>3056</v>
+        <v>3053</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>911</v>
+        <v>979</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="16" t="s">
         <v>980</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>3057</v>
+        <v>3054</v>
       </c>
       <c r="J22" s="16"/>
       <c r="K22" s="16" t="s">
-        <v>3058</v>
+        <v>3055</v>
       </c>
       <c r="L22" s="16" t="s">
         <v>922</v>
@@ -50509,41 +50811,41 @@
     </row>
     <row r="23" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>3059</v>
+        <v>3028</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>2369</v>
+        <v>980</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>1030</v>
+        <v>3040</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>414</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>1031</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>2604</v>
+        <v>3035</v>
+      </c>
+      <c r="E23" s="42" t="s">
+        <v>3056</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>979</v>
       </c>
       <c r="G23" s="13"/>
-      <c r="H23" s="26" t="s">
+      <c r="H23" s="16" t="s">
         <v>980</v>
       </c>
-      <c r="I23" s="26" t="s">
-        <v>3060</v>
-      </c>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26" t="s">
-        <v>3061</v>
+      <c r="I23" s="16" t="s">
+        <v>3057</v>
+      </c>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16" t="s">
+        <v>3058</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>434</v>
+        <v>922</v>
       </c>
       <c r="M23" s="13"/>
       <c r="N23" s="13"/>
     </row>
-    <row r="24" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>3059</v>
       </c>
@@ -50567,11 +50869,11 @@
         <v>980</v>
       </c>
       <c r="I24" s="26" t="s">
-        <v>3062</v>
+        <v>3060</v>
       </c>
       <c r="J24" s="26"/>
       <c r="K24" s="26" t="s">
-        <v>3063</v>
+        <v>3061</v>
       </c>
       <c r="L24" s="16" t="s">
         <v>434</v>
@@ -50579,7 +50881,7 @@
       <c r="M24" s="13"/>
       <c r="N24" s="13"/>
     </row>
-    <row r="25" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="50" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>3059</v>
       </c>
@@ -50603,11 +50905,11 @@
         <v>980</v>
       </c>
       <c r="I25" s="26" t="s">
-        <v>3064</v>
-      </c>
-      <c r="J25" s="15"/>
+        <v>3062</v>
+      </c>
+      <c r="J25" s="26"/>
       <c r="K25" s="26" t="s">
-        <v>3065</v>
+        <v>3063</v>
       </c>
       <c r="L25" s="16" t="s">
         <v>434</v>
@@ -50639,11 +50941,11 @@
         <v>980</v>
       </c>
       <c r="I26" s="26" t="s">
-        <v>3066</v>
+        <v>3064</v>
       </c>
       <c r="J26" s="15"/>
       <c r="K26" s="26" t="s">
-        <v>3067</v>
+        <v>3065</v>
       </c>
       <c r="L26" s="16" t="s">
         <v>434</v>
@@ -50672,14 +50974,14 @@
       </c>
       <c r="G27" s="13"/>
       <c r="H27" s="26" t="s">
-        <v>3068</v>
+        <v>980</v>
       </c>
       <c r="I27" s="26" t="s">
-        <v>3069</v>
-      </c>
-      <c r="J27" s="26"/>
+        <v>3066</v>
+      </c>
+      <c r="J27" s="15"/>
       <c r="K27" s="26" t="s">
-        <v>3070</v>
+        <v>3067</v>
       </c>
       <c r="L27" s="16" t="s">
         <v>434</v>
@@ -50687,7 +50989,7 @@
       <c r="M27" s="13"/>
       <c r="N27" s="13"/>
     </row>
-    <row r="28" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>3059</v>
       </c>
@@ -50707,15 +51009,15 @@
         <v>2604</v>
       </c>
       <c r="G28" s="13"/>
-      <c r="H28" s="15" t="s">
-        <v>3071</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>3072</v>
+      <c r="H28" s="26" t="s">
+        <v>3068</v>
+      </c>
+      <c r="I28" s="26" t="s">
+        <v>3069</v>
       </c>
       <c r="J28" s="26"/>
-      <c r="K28" s="15" t="s">
-        <v>3073</v>
+      <c r="K28" s="26" t="s">
+        <v>3070</v>
       </c>
       <c r="L28" s="16" t="s">
         <v>434</v>
@@ -50723,31 +51025,35 @@
       <c r="M28" s="13"/>
       <c r="N28" s="13"/>
     </row>
-    <row r="29" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>1263</v>
+    <row r="29" spans="1:14" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>3059</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>434</v>
+        <v>2369</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>434</v>
-      </c>
-      <c r="D29" s="13" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D29" s="16" t="s">
         <v>414</v>
       </c>
-      <c r="E29" s="17" t="s">
-        <v>3074</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>420</v>
+      <c r="E29" s="16" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>2604</v>
       </c>
       <c r="G29" s="13"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
+      <c r="H29" s="15" t="s">
+        <v>3071</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>3072</v>
+      </c>
+      <c r="J29" s="26"/>
       <c r="K29" s="15" t="s">
-        <v>3075</v>
+        <v>3073</v>
       </c>
       <c r="L29" s="16" t="s">
         <v>434</v>
@@ -50755,35 +51061,31 @@
       <c r="M29" s="13"/>
       <c r="N29" s="13"/>
     </row>
-    <row r="30" spans="1:14" ht="25" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
-        <v>3024</v>
+    <row r="30" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>1263</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>105</v>
+        <v>434</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>3076</v>
-      </c>
-      <c r="E30" s="70" t="s">
-        <v>3076</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>1068</v>
+        <v>434</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>414</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>3074</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>420</v>
       </c>
       <c r="G30" s="13"/>
-      <c r="H30" s="15" t="s">
-        <v>3077</v>
-      </c>
-      <c r="I30" s="16" t="s">
-        <v>3076</v>
-      </c>
-      <c r="J30" s="25"/>
-      <c r="K30" s="16" t="s">
-        <v>3078</v>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="15" t="s">
+        <v>3075</v>
       </c>
       <c r="L30" s="16" t="s">
         <v>434</v>
@@ -50793,36 +51095,36 @@
     </row>
     <row r="31" spans="1:14" ht="25" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>3028</v>
+        <v>3024</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>980</v>
+        <v>105</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>3079</v>
+        <v>106</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>3076</v>
       </c>
-      <c r="E31" s="42" t="s">
-        <v>997</v>
+      <c r="E31" s="70" t="s">
+        <v>3076</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>979</v>
+        <v>1068</v>
       </c>
       <c r="G31" s="13"/>
-      <c r="H31" s="60" t="s">
-        <v>980</v>
+      <c r="H31" s="15" t="s">
+        <v>3077</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>3080</v>
+        <v>3076</v>
       </c>
       <c r="J31" s="25"/>
       <c r="K31" s="16" t="s">
-        <v>3081</v>
-      </c>
-      <c r="L31" s="25" t="s">
-        <v>922</v>
+        <v>3078</v>
+      </c>
+      <c r="L31" s="16" t="s">
+        <v>434</v>
       </c>
       <c r="M31" s="13"/>
       <c r="N31" s="13"/>
@@ -50841,7 +51143,7 @@
         <v>3076</v>
       </c>
       <c r="E32" s="42" t="s">
-        <v>3011</v>
+        <v>997</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>979</v>
@@ -50851,11 +51153,11 @@
         <v>980</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
       <c r="J32" s="25"/>
       <c r="K32" s="16" t="s">
-        <v>3083</v>
+        <v>3081</v>
       </c>
       <c r="L32" s="25" t="s">
         <v>922</v>
@@ -50876,22 +51178,22 @@
       <c r="D33" s="15" t="s">
         <v>3076</v>
       </c>
-      <c r="E33" s="130" t="s">
-        <v>3012</v>
-      </c>
-      <c r="F33" s="85" t="s">
+      <c r="E33" s="42" t="s">
+        <v>3011</v>
+      </c>
+      <c r="F33" s="16" t="s">
         <v>979</v>
       </c>
       <c r="G33" s="13"/>
       <c r="H33" s="60" t="s">
         <v>980</v>
       </c>
-      <c r="I33" s="85" t="s">
-        <v>3084</v>
-      </c>
-      <c r="J33" s="137"/>
-      <c r="K33" s="85" t="s">
-        <v>3085</v>
+      <c r="I33" s="16" t="s">
+        <v>3082</v>
+      </c>
+      <c r="J33" s="25"/>
+      <c r="K33" s="16" t="s">
+        <v>3083</v>
       </c>
       <c r="L33" s="25" t="s">
         <v>922</v>
@@ -50912,24 +51214,24 @@
       <c r="D34" s="15" t="s">
         <v>3076</v>
       </c>
-      <c r="E34" s="39" t="s">
-        <v>1339</v>
-      </c>
-      <c r="F34" s="15" t="s">
-        <v>911</v>
+      <c r="E34" s="130" t="s">
+        <v>3012</v>
+      </c>
+      <c r="F34" s="85" t="s">
+        <v>979</v>
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="60" t="s">
         <v>980</v>
       </c>
-      <c r="I34" s="16" t="s">
-        <v>3086</v>
-      </c>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16" t="s">
-        <v>3087</v>
-      </c>
-      <c r="L34" s="16" t="s">
+      <c r="I34" s="85" t="s">
+        <v>3084</v>
+      </c>
+      <c r="J34" s="137"/>
+      <c r="K34" s="85" t="s">
+        <v>3085</v>
+      </c>
+      <c r="L34" s="25" t="s">
         <v>922</v>
       </c>
       <c r="M34" s="13"/>
@@ -50937,33 +51239,33 @@
     </row>
     <row r="35" spans="1:14" ht="25" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>3031</v>
-      </c>
-      <c r="B35" s="26" t="s">
-        <v>3088</v>
+        <v>3028</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>980</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>1508</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>1505</v>
-      </c>
-      <c r="E35" s="42" t="s">
-        <v>920</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>979</v>
+        <v>3079</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>3076</v>
+      </c>
+      <c r="E35" s="39" t="s">
+        <v>1339</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>911</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="60" t="s">
         <v>980</v>
       </c>
       <c r="I35" s="16" t="s">
-        <v>3089</v>
+        <v>3086</v>
       </c>
       <c r="J35" s="16"/>
       <c r="K35" s="16" t="s">
-        <v>3090</v>
+        <v>3087</v>
       </c>
       <c r="L35" s="16" t="s">
         <v>922</v>
@@ -50971,44 +51273,184 @@
       <c r="M35" s="13"/>
       <c r="N35" s="13"/>
     </row>
-    <row r="36" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="25" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>1252</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>434</v>
+        <v>3031</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>3088</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>434</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>1067</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>504</v>
+        <v>1508</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>1505</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>920</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>420</v>
-      </c>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
+        <v>979</v>
+      </c>
+      <c r="G36" s="13"/>
+      <c r="H36" s="60" t="s">
+        <v>980</v>
+      </c>
+      <c r="I36" s="16" t="s">
+        <v>3089</v>
+      </c>
       <c r="J36" s="16"/>
-      <c r="K36" s="15" t="s">
-        <v>3091</v>
+      <c r="K36" s="16" t="s">
+        <v>3090</v>
       </c>
       <c r="L36" s="16" t="s">
-        <v>434</v>
+        <v>922</v>
       </c>
       <c r="M36" s="13"/>
       <c r="N36" s="13"/>
     </row>
+    <row r="37" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>504</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>420</v>
+      </c>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="15" t="s">
+        <v>3091</v>
+      </c>
+      <c r="L37" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+    </row>
+    <row r="38" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>2612</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>3074</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>420</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>414</v>
+      </c>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="15" t="s">
+        <v>3093</v>
+      </c>
+      <c r="L38" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+    </row>
+    <row r="39" spans="1:14" ht="50" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>2654</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>3074</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>420</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>414</v>
+      </c>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="15" t="s">
+        <v>3094</v>
+      </c>
+      <c r="L39" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+    </row>
+    <row r="40" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>3031</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>667</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>456</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>447</v>
+      </c>
+      <c r="E40" s="42" t="s">
+        <v>3095</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>911</v>
+      </c>
+      <c r="G40" s="13"/>
+      <c r="H40" s="16" t="s">
+        <v>980</v>
+      </c>
+      <c r="I40" s="16" t="s">
+        <v>3096</v>
+      </c>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16" t="s">
+        <v>3097</v>
+      </c>
+      <c r="L40" s="16" t="s">
+        <v>922</v>
+      </c>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="TESTCD must be 8 characters or less" sqref="H23:H28" xr:uid="{AF62AD00-E78B-4B54-A1C3-40562FEAE3CA}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="TESTCD must be 8 characters or less" sqref="H24:H29" xr:uid="{AF62AD00-E78B-4B54-A1C3-40562FEAE3CA}">
       <formula1>8</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="TEST must be 40 characters or less_x000a_" sqref="I23:I28" xr:uid="{F6AD1B3D-608B-4653-9DDE-4A65C2E6CAD3}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="TEST must be 40 characters or less_x000a_" sqref="I24:I29" xr:uid="{F6AD1B3D-608B-4653-9DDE-4A65C2E6CAD3}">
       <formula1>40</formula1>
     </dataValidation>
   </dataValidations>
@@ -59008,7 +59450,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -60178,6 +60620,42 @@
       </c>
       <c r="M31" s="13"/>
       <c r="N31" s="13"/>
+    </row>
+    <row r="32" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>3103</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>1444</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>1757</v>
+      </c>
+      <c r="D32" s="140" t="s">
+        <v>1436</v>
+      </c>
+      <c r="E32" s="39" t="s">
+        <v>517</v>
+      </c>
+      <c r="F32" s="36" t="s">
+        <v>3104</v>
+      </c>
+      <c r="G32" s="36"/>
+      <c r="H32" s="59" t="s">
+        <v>1871</v>
+      </c>
+      <c r="I32" s="64" t="s">
+        <v>1872</v>
+      </c>
+      <c r="J32" s="16"/>
+      <c r="K32" s="15" t="s">
+        <v>3105</v>
+      </c>
+      <c r="L32" s="16" t="s">
+        <v>2827</v>
+      </c>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H5">

</xml_diff>